<commit_message>
Wrote text introduction for CCPT section
</commit_message>
<xml_diff>
--- a/results/cptVSsd_cpt.xlsx
+++ b/results/cptVSsd_cpt.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="51220" yWindow="7640" windowWidth="38400" windowHeight="21160" tabRatio="500"/>
+    <workbookView xWindow="-800" yWindow="4040" windowWidth="38400" windowHeight="21160" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -448,7 +448,7 @@
   <dimension ref="A1:O28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="I19" sqref="I19:I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -993,7 +993,7 @@
         <v>2.2363600215853903</v>
       </c>
     </row>
-    <row r="18" spans="7:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="7:9" x14ac:dyDescent="0.2">
       <c r="G18" t="s">
         <v>25</v>
       </c>
@@ -1001,7 +1001,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="7:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="7:9" x14ac:dyDescent="0.2">
       <c r="G19" s="3">
         <f>L2/E2</f>
         <v>1.5788312499999999</v>
@@ -1010,8 +1010,12 @@
         <f>K2/E2</f>
         <v>40.962125</v>
       </c>
-    </row>
-    <row r="20" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="I19">
+        <f>H19/G19</f>
+        <v>25.944587174848486</v>
+      </c>
+    </row>
+    <row r="20" spans="7:9" x14ac:dyDescent="0.2">
       <c r="G20" s="3">
         <f t="shared" ref="G20:G32" si="1">L3/E3</f>
         <v>1.9901899999999999</v>
@@ -1020,8 +1024,12 @@
         <f t="shared" ref="H20:H28" si="2">K3/E3</f>
         <v>84.671800000000005</v>
       </c>
-    </row>
-    <row r="21" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="I20">
+        <f t="shared" ref="I20:I28" si="3">H20/G20</f>
+        <v>42.544581170642005</v>
+      </c>
+    </row>
+    <row r="21" spans="7:9" x14ac:dyDescent="0.2">
       <c r="G21" s="3">
         <f t="shared" si="1"/>
         <v>2.0750964912280705</v>
@@ -1030,8 +1038,12 @@
         <f t="shared" si="2"/>
         <v>179.27807017543861</v>
       </c>
-    </row>
-    <row r="22" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="I21">
+        <f t="shared" si="3"/>
+        <v>86.395052438905822</v>
+      </c>
+    </row>
+    <row r="22" spans="7:9" x14ac:dyDescent="0.2">
       <c r="G22" s="3">
         <f t="shared" si="1"/>
         <v>2.4303249999999998</v>
@@ -1040,8 +1052,12 @@
         <f t="shared" si="2"/>
         <v>37.733249999999998</v>
       </c>
-    </row>
-    <row r="23" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="I22">
+        <f t="shared" si="3"/>
+        <v>15.526009895795831</v>
+      </c>
+    </row>
+    <row r="23" spans="7:9" x14ac:dyDescent="0.2">
       <c r="G23" s="3">
         <f t="shared" si="1"/>
         <v>1.68912987012987</v>
@@ -1050,8 +1066,12 @@
         <f t="shared" si="2"/>
         <v>58.575324675324673</v>
       </c>
-    </row>
-    <row r="24" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="I23">
+        <f t="shared" si="3"/>
+        <v>34.677809984392177</v>
+      </c>
+    </row>
+    <row r="24" spans="7:9" x14ac:dyDescent="0.2">
       <c r="G24" s="3">
         <f t="shared" si="1"/>
         <v>2.3391571428571432</v>
@@ -1060,8 +1080,12 @@
         <f t="shared" si="2"/>
         <v>40.462000000000003</v>
       </c>
-    </row>
-    <row r="25" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="I24">
+        <f t="shared" si="3"/>
+        <v>17.297683536805074</v>
+      </c>
+    </row>
+    <row r="25" spans="7:9" x14ac:dyDescent="0.2">
       <c r="G25" s="3">
         <f t="shared" si="1"/>
         <v>1.1072310344827587</v>
@@ -1070,8 +1094,12 @@
         <f t="shared" si="2"/>
         <v>33.773000000000003</v>
       </c>
-    </row>
-    <row r="26" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="I25">
+        <f t="shared" si="3"/>
+        <v>30.502215841318979</v>
+      </c>
+    </row>
+    <row r="26" spans="7:9" x14ac:dyDescent="0.2">
       <c r="G26" s="3">
         <f t="shared" si="1"/>
         <v>1.7960854700854703</v>
@@ -1080,8 +1108,12 @@
         <f t="shared" si="2"/>
         <v>29.80769230769231</v>
       </c>
-    </row>
-    <row r="27" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="I26">
+        <f t="shared" si="3"/>
+        <v>16.595920853518098</v>
+      </c>
+    </row>
+    <row r="27" spans="7:9" x14ac:dyDescent="0.2">
       <c r="G27" s="3">
         <f t="shared" si="1"/>
         <v>1.1598733333333333</v>
@@ -1090,8 +1122,12 @@
         <f t="shared" si="2"/>
         <v>59.489466666666665</v>
       </c>
-    </row>
-    <row r="28" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="I27">
+        <f t="shared" si="3"/>
+        <v>51.289623579586276</v>
+      </c>
+    </row>
+    <row r="28" spans="7:9" x14ac:dyDescent="0.2">
       <c r="G28" s="3">
         <f t="shared" si="1"/>
         <v>1.1088165137614678</v>
@@ -1099,6 +1135,10 @@
       <c r="H28" s="3">
         <f t="shared" si="2"/>
         <v>59.461926605504587</v>
+      </c>
+      <c r="I28">
+        <f t="shared" si="3"/>
+        <v>53.626480005957262</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Writing CCPT section - about to end EF_II. Added relevant bib/images and structure changes. Also made a note in the excel about a memory calculation ommision (in regards of rank/select dictionaries); It should be corrected in master branch
</commit_message>
<xml_diff>
--- a/results/cptVSsd_cpt.xlsx
+++ b/results/cptVSsd_cpt.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26606"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27907"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,13 +9,16 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-800" yWindow="4040" windowWidth="38400" windowHeight="21160" tabRatio="500"/>
+    <workbookView xWindow="51200" yWindow="7640" windowWidth="38400" windowHeight="21160" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -24,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>Trie Node Number</t>
   </si>
@@ -105,6 +108,12 @@
   </si>
   <si>
     <t>CPT/CDS space</t>
+  </si>
+  <si>
+    <t>II-SD should contain rank/select dictionaries space!!!! -&gt; correct this!!</t>
+  </si>
+  <si>
+    <t>SD_Tree should contain space calculation for its select dictionary</t>
   </si>
 </sst>
 </file>
@@ -448,7 +457,7 @@
   <dimension ref="A1:O28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19:I28"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -993,6 +1002,16 @@
         <v>2.2363600215853903</v>
       </c>
     </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="G13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="I14" t="s">
+        <v>28</v>
+      </c>
+    </row>
     <row r="18" spans="7:9" x14ac:dyDescent="0.2">
       <c r="G18" t="s">
         <v>25</v>
@@ -1017,7 +1036,7 @@
     </row>
     <row r="20" spans="7:9" x14ac:dyDescent="0.2">
       <c r="G20" s="3">
-        <f t="shared" ref="G20:G32" si="1">L3/E3</f>
+        <f t="shared" ref="G20:G28" si="1">L3/E3</f>
         <v>1.9901899999999999</v>
       </c>
       <c r="H20" s="3">

</xml_diff>

<commit_message>
Updated spreadsheet with new memory results. Did some extra calculations too. Some graphs were created on Numbers icloud.
</commit_message>
<xml_diff>
--- a/results/cptVSsd_cpt.xlsx
+++ b/results/cptVSsd_cpt.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>Trie Node Number</t>
   </si>
@@ -101,19 +101,34 @@
     <t>SD_CPT Time per query (s)</t>
   </si>
   <si>
-    <t>SD_CPT / CPT Time</t>
-  </si>
-  <si>
     <t>SD/CDS space</t>
   </si>
   <si>
     <t>CPT/CDS space</t>
   </si>
   <si>
-    <t>II-SD should contain rank/select dictionaries space!!!! -&gt; correct this!!</t>
-  </si>
-  <si>
-    <t>SD_Tree should contain space calculation for its select dictionary</t>
+    <t>Trie Node Number with Dictionary</t>
+  </si>
+  <si>
+    <t>Trie with Dict MB</t>
+  </si>
+  <si>
+    <t>Dictionary MB</t>
+  </si>
+  <si>
+    <t>CPT+ Time per query (s)</t>
+  </si>
+  <si>
+    <t>CPT+/CDS space</t>
+  </si>
+  <si>
+    <t>SD_CPT / CPT+ Time</t>
+  </si>
+  <si>
+    <t>II /CDS</t>
+  </si>
+  <si>
+    <t>SD_II / CDS</t>
   </si>
 </sst>
 </file>
@@ -124,7 +139,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -141,6 +156,22 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -160,8 +191,34 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -178,7 +235,33 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="27">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -454,28 +537,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O28"/>
+  <dimension ref="A1:S30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="3" width="24.1640625" customWidth="1"/>
     <col min="4" max="4" width="27.1640625" customWidth="1"/>
-    <col min="5" max="5" width="17.5" customWidth="1"/>
-    <col min="7" max="7" width="23.6640625" customWidth="1"/>
-    <col min="8" max="8" width="14.1640625" customWidth="1"/>
-    <col min="9" max="9" width="14.83203125" customWidth="1"/>
-    <col min="11" max="11" width="15" customWidth="1"/>
-    <col min="12" max="12" width="17.83203125" customWidth="1"/>
-    <col min="13" max="13" width="30.1640625" customWidth="1"/>
-    <col min="14" max="14" width="26" customWidth="1"/>
-    <col min="15" max="15" width="23.5" customWidth="1"/>
+    <col min="5" max="5" width="34.6640625" customWidth="1"/>
+    <col min="6" max="6" width="17.5" customWidth="1"/>
+    <col min="8" max="8" width="23.6640625" customWidth="1"/>
+    <col min="9" max="9" width="14.1640625" customWidth="1"/>
+    <col min="10" max="10" width="14.83203125" customWidth="1"/>
+    <col min="12" max="12" width="20.33203125" customWidth="1"/>
+    <col min="13" max="13" width="17.6640625" customWidth="1"/>
+    <col min="14" max="14" width="15" customWidth="1"/>
+    <col min="15" max="15" width="17.83203125" customWidth="1"/>
+    <col min="16" max="17" width="30.1640625" customWidth="1"/>
+    <col min="18" max="18" width="26" customWidth="1"/>
+    <col min="19" max="19" width="23.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -488,41 +574,53 @@
       <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" t="s">
         <v>21</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>11</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>12</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>13</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>14</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>15</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M1" t="s">
+        <v>28</v>
+      </c>
+      <c r="N1" t="s">
         <v>16</v>
       </c>
-      <c r="L1" t="s">
+      <c r="O1" t="s">
         <v>17</v>
       </c>
-      <c r="M1" t="s">
+      <c r="P1" t="s">
         <v>22</v>
       </c>
-      <c r="N1" t="s">
+      <c r="Q1" t="s">
+        <v>29</v>
+      </c>
+      <c r="R1" t="s">
         <v>23</v>
       </c>
-      <c r="O1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="S1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -535,42 +633,54 @@
       <c r="D2" s="6">
         <v>59088</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="6">
+        <v>33464</v>
+      </c>
+      <c r="F2" s="4">
         <v>0.16</v>
       </c>
-      <c r="F2" s="5">
+      <c r="G2" s="5">
         <v>3.7136</v>
       </c>
-      <c r="G2" s="5">
-        <v>0.16256000000000001</v>
-      </c>
       <c r="H2" s="5">
+        <v>0.23282900000000001</v>
+      </c>
+      <c r="I2" s="5">
         <v>0.47681600000000002</v>
       </c>
-      <c r="I2" s="5">
-        <v>9.0052599999999997E-2</v>
-      </c>
       <c r="J2" s="5">
+        <v>9.4036599999999998E-2</v>
+      </c>
+      <c r="K2" s="5">
         <v>2.3635199999999998</v>
       </c>
-      <c r="K2" s="5">
+      <c r="L2" s="5">
+        <v>1.33856</v>
+      </c>
+      <c r="M2" s="5">
+        <v>0.54470600000000002</v>
+      </c>
+      <c r="N2" s="5">
         <v>6.5539399999999999</v>
       </c>
-      <c r="L2" s="5">
-        <v>0.25261299999999998</v>
-      </c>
-      <c r="M2" s="5">
+      <c r="O2" s="5">
+        <v>0.32686599999999999</v>
+      </c>
+      <c r="P2" s="5">
         <v>5.2630000000000005E-4</v>
       </c>
-      <c r="N2" s="5">
+      <c r="Q2" s="5">
+        <v>5.3398400000000004E-4</v>
+      </c>
+      <c r="R2" s="5">
         <v>8.5400000000000005E-4</v>
       </c>
-      <c r="O2" s="5">
-        <f>N2/M2</f>
-        <v>1.6226486794603838</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="S2" s="5">
+        <f>R2/Q2</f>
+        <v>1.5992988553964163</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -583,42 +693,54 @@
       <c r="D3" s="6">
         <v>231942</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="6">
+        <v>134957</v>
+      </c>
+      <c r="F3" s="4">
         <v>0.5</v>
       </c>
-      <c r="F3" s="5">
+      <c r="G3" s="5">
         <v>32.438099999999999</v>
       </c>
-      <c r="G3" s="5">
-        <v>0.58146299999999995</v>
-      </c>
       <c r="H3" s="5">
+        <v>0.983792</v>
+      </c>
+      <c r="I3" s="5">
         <v>0.62010399999999999</v>
       </c>
-      <c r="I3" s="5">
-        <v>0.413632</v>
-      </c>
       <c r="J3" s="5">
+        <v>0.44035999999999997</v>
+      </c>
+      <c r="K3" s="5">
         <v>9.2776800000000001</v>
       </c>
-      <c r="K3" s="5">
+      <c r="L3" s="5">
+        <v>5.3982799999999997</v>
+      </c>
+      <c r="M3" s="5">
+        <v>1.7113499999999999</v>
+      </c>
+      <c r="N3" s="5">
         <v>42.335900000000002</v>
       </c>
-      <c r="L3" s="5">
-        <v>0.99509499999999995</v>
-      </c>
-      <c r="M3" s="5">
+      <c r="O3" s="5">
+        <v>1.42415</v>
+      </c>
+      <c r="P3" s="5">
         <v>4.4799999999999999E-4</v>
       </c>
-      <c r="N3" s="5">
+      <c r="Q3" s="5">
+        <v>6.4504899999999997E-4</v>
+      </c>
+      <c r="R3" s="5">
         <v>5.5900000000000004E-4</v>
       </c>
-      <c r="O3" s="5">
-        <f t="shared" ref="O3:O11" si="0">N3/M3</f>
-        <v>1.2477678571428572</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="S3" s="5">
+        <f t="shared" ref="S3:S11" si="0">R3/Q3</f>
+        <v>0.86660083187478787</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>18</v>
       </c>
@@ -631,42 +753,54 @@
       <c r="D4" s="6">
         <v>460435</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="6">
+        <v>240517</v>
+      </c>
+      <c r="F4" s="4">
         <v>1.1399999999999999</v>
       </c>
-      <c r="F4" s="5">
+      <c r="G4" s="5">
         <v>185.399</v>
       </c>
-      <c r="G4" s="5">
-        <v>1.38802</v>
-      </c>
       <c r="H4" s="5">
+        <v>3.2960500000000001</v>
+      </c>
+      <c r="I4" s="5">
         <v>0.56000000000000005</v>
       </c>
-      <c r="I4" s="5">
-        <v>0.97759700000000005</v>
-      </c>
       <c r="J4" s="5">
+        <v>1.1467700000000001</v>
+      </c>
+      <c r="K4" s="5">
         <v>18.417400000000001</v>
       </c>
-      <c r="K4" s="5">
+      <c r="L4" s="5">
+        <v>9.6206800000000001</v>
+      </c>
+      <c r="M4" s="11">
+        <v>3.70669</v>
+      </c>
+      <c r="N4" s="5">
         <v>204.37700000000001</v>
       </c>
-      <c r="L4" s="5">
-        <v>2.3656100000000002</v>
-      </c>
-      <c r="M4" s="5">
+      <c r="O4" s="5">
+        <v>4.4428200000000002</v>
+      </c>
+      <c r="P4" s="5">
         <v>5.4831400000000002E-2</v>
       </c>
-      <c r="N4" s="5">
+      <c r="Q4" s="5">
+        <v>0.110252</v>
+      </c>
+      <c r="R4" s="5">
         <v>9.2287999999999995E-2</v>
       </c>
-      <c r="O4" s="5">
+      <c r="S4" s="5">
         <f t="shared" si="0"/>
-        <v>1.6831231739477743</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+        <v>0.83706418024162821</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -679,42 +813,54 @@
       <c r="D5" s="6">
         <v>36839</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="6">
+        <v>18872</v>
+      </c>
+      <c r="F5" s="4">
         <v>0.04</v>
       </c>
-      <c r="F5" s="5">
+      <c r="G5" s="5">
         <v>2.9919999999999999E-2</v>
       </c>
-      <c r="G5" s="5">
-        <v>4.6976999999999998E-2</v>
-      </c>
       <c r="H5" s="5">
+        <v>7.9620999999999997E-2</v>
+      </c>
+      <c r="I5" s="5">
         <v>5.8479999999999999E-3</v>
       </c>
-      <c r="I5" s="5">
-        <v>5.0236700000000002E-2</v>
-      </c>
       <c r="J5" s="5">
+        <v>5.2380700000000002E-2</v>
+      </c>
+      <c r="K5" s="5">
         <v>1.47356</v>
       </c>
-      <c r="K5" s="5">
+      <c r="L5" s="5">
+        <v>0.75488</v>
+      </c>
+      <c r="M5" s="5">
+        <v>0.28207500000000002</v>
+      </c>
+      <c r="N5" s="5">
         <v>1.5093300000000001</v>
       </c>
-      <c r="L5" s="5">
-        <v>9.7212999999999994E-2</v>
-      </c>
-      <c r="M5" s="5">
+      <c r="O5" s="5">
+        <v>0.13200200000000001</v>
+      </c>
+      <c r="P5" s="5">
         <v>4.9019999999999999E-4</v>
       </c>
-      <c r="N5" s="5">
+      <c r="Q5" s="5">
+        <v>1.04747E-3</v>
+      </c>
+      <c r="R5" s="5">
         <v>1.157E-3</v>
       </c>
-      <c r="O5" s="5">
+      <c r="S5" s="5">
         <f t="shared" si="0"/>
-        <v>2.3602611179110569</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+        <v>1.1045662405605889</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -727,42 +873,54 @@
       <c r="D6" s="6">
         <v>659811</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="9">
+        <v>283527</v>
+      </c>
+      <c r="F6" s="4">
         <v>1.54</v>
       </c>
-      <c r="F6" s="5">
+      <c r="G6" s="5">
         <v>63.522599999999997</v>
       </c>
-      <c r="G6" s="5">
-        <v>1.2390099999999999</v>
-      </c>
       <c r="H6" s="5">
+        <v>2.51044</v>
+      </c>
+      <c r="I6" s="5">
         <v>0.29096</v>
       </c>
-      <c r="I6" s="5">
-        <v>1.36226</v>
-      </c>
       <c r="J6" s="5">
+        <v>1.4735100000000001</v>
+      </c>
+      <c r="K6" s="5">
         <v>26.392399999999999</v>
       </c>
-      <c r="K6" s="5">
+      <c r="L6" s="5">
+        <v>11.341100000000001</v>
+      </c>
+      <c r="M6" s="5">
+        <v>6.8092499999999996</v>
+      </c>
+      <c r="N6" s="5">
         <v>90.206000000000003</v>
       </c>
-      <c r="L6" s="5">
-        <v>2.6012599999999999</v>
-      </c>
-      <c r="M6" s="5">
+      <c r="O6" s="5">
+        <v>3.9839600000000002</v>
+      </c>
+      <c r="P6" s="5">
         <v>1.7062899999999999E-2</v>
       </c>
-      <c r="N6" s="5">
+      <c r="Q6" s="11">
+        <v>3.2385999999999998E-2</v>
+      </c>
+      <c r="R6" s="5">
         <v>2.6141999999999999E-2</v>
       </c>
-      <c r="O6" s="5">
+      <c r="S6" s="5">
         <f t="shared" si="0"/>
-        <v>1.5320959508641556</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+        <v>0.80720064225282528</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -775,42 +933,54 @@
       <c r="D7" s="7">
         <v>183206</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="7">
+        <v>94388</v>
+      </c>
+      <c r="F7" s="4">
         <v>0.35</v>
       </c>
-      <c r="F7" s="5">
+      <c r="G7" s="5">
         <v>6.7868199999999996</v>
       </c>
-      <c r="G7" s="5">
-        <v>0.46009899999999998</v>
-      </c>
       <c r="H7" s="5">
+        <v>1.2236100000000001</v>
+      </c>
+      <c r="I7" s="5">
         <v>4.6679999999999999E-2</v>
       </c>
-      <c r="I7" s="5">
-        <v>0.35860500000000001</v>
-      </c>
       <c r="J7" s="5">
+        <v>0.430813</v>
+      </c>
+      <c r="K7" s="5">
         <v>7.3282400000000001</v>
       </c>
-      <c r="K7" s="5">
+      <c r="L7" s="5">
+        <v>3.7755200000000002</v>
+      </c>
+      <c r="M7" s="5">
+        <v>1.4720800000000001</v>
+      </c>
+      <c r="N7" s="5">
         <v>14.1617</v>
       </c>
-      <c r="L7" s="5">
-        <v>0.81870500000000002</v>
-      </c>
-      <c r="M7" s="5">
+      <c r="O7" s="5">
+        <v>1.65442</v>
+      </c>
+      <c r="P7" s="5">
         <v>1.6165999999999999E-3</v>
       </c>
-      <c r="N7" s="5">
+      <c r="Q7" s="11">
+        <v>3.5724200000000002E-3</v>
+      </c>
+      <c r="R7" s="5">
         <v>3.039E-3</v>
       </c>
-      <c r="O7" s="5">
+      <c r="S7" s="5">
         <f t="shared" si="0"/>
-        <v>1.8798713349004084</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.2">
+        <v>0.8506838501631947</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
@@ -823,42 +993,54 @@
       <c r="D8" s="9">
         <v>236799</v>
       </c>
-      <c r="E8" s="10">
+      <c r="E8" s="9">
+        <v>85184</v>
+      </c>
+      <c r="F8" s="10">
         <v>0.28999999999999998</v>
       </c>
-      <c r="F8" s="11">
+      <c r="G8" s="11">
         <v>6.7879999999999996E-2</v>
       </c>
-      <c r="G8" s="11">
-        <v>0.125611</v>
-      </c>
-      <c r="H8" s="11">
+      <c r="H8" s="5">
+        <v>0.14596300000000001</v>
+      </c>
+      <c r="I8" s="11">
         <v>0.254328</v>
       </c>
-      <c r="I8" s="11">
-        <v>0.19548599999999999</v>
-      </c>
-      <c r="J8" s="11">
+      <c r="J8" s="5">
+        <v>0.19563</v>
+      </c>
+      <c r="K8" s="11">
         <v>9.4719599999999993</v>
       </c>
-      <c r="K8" s="11">
+      <c r="L8" s="11">
+        <v>3.4073600000000002</v>
+      </c>
+      <c r="M8" s="5">
+        <v>0.769123</v>
+      </c>
+      <c r="N8" s="11">
         <v>9.7941699999999994</v>
       </c>
-      <c r="L8" s="11">
-        <v>0.32109700000000002</v>
-      </c>
-      <c r="M8" s="11">
+      <c r="O8" s="5">
+        <v>0.34159299999999998</v>
+      </c>
+      <c r="P8" s="11">
         <v>1.0145700000000001E-2</v>
       </c>
-      <c r="N8" s="11">
+      <c r="Q8" s="5">
+        <v>1.59825E-2</v>
+      </c>
+      <c r="R8" s="11">
         <v>1.8703000000000001E-2</v>
       </c>
-      <c r="O8" s="11">
+      <c r="S8" s="5">
         <f t="shared" si="0"/>
-        <v>1.8434410637018639</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+        <v>1.1702174253089317</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -871,42 +1053,54 @@
       <c r="D9" s="7">
         <v>675229</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9">
+        <v>253903</v>
+      </c>
+      <c r="F9" s="4">
         <v>1.17</v>
       </c>
-      <c r="F9" s="5">
+      <c r="G9" s="5">
         <v>7.7022599999999999</v>
       </c>
-      <c r="G9" s="5">
-        <v>0.95254300000000003</v>
-      </c>
       <c r="H9" s="5">
+        <v>1.3235600000000001</v>
+      </c>
+      <c r="I9" s="5">
         <v>0.163608</v>
       </c>
-      <c r="I9" s="5">
-        <v>1.1488700000000001</v>
-      </c>
       <c r="J9" s="5">
+        <v>1.1728000000000001</v>
+      </c>
+      <c r="K9" s="5">
         <v>27.0092</v>
       </c>
-      <c r="K9" s="5">
+      <c r="L9" s="5">
+        <v>10.1561</v>
+      </c>
+      <c r="M9" s="5">
+        <v>5.7599499999999999</v>
+      </c>
+      <c r="N9" s="5">
         <v>34.875</v>
       </c>
-      <c r="L9" s="5">
-        <v>2.1014200000000001</v>
-      </c>
-      <c r="M9" s="5">
+      <c r="O9" s="5">
+        <v>2.4963600000000001</v>
+      </c>
+      <c r="P9" s="5">
         <v>1.4539399999999999E-2</v>
       </c>
-      <c r="N9" s="5">
+      <c r="Q9" s="5">
+        <v>2.63515E-2</v>
+      </c>
+      <c r="R9" s="5">
         <v>2.5314E-2</v>
       </c>
-      <c r="O9" s="5">
+      <c r="S9" s="5">
         <f t="shared" si="0"/>
-        <v>1.7410622171478878</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.2">
+        <v>0.96062842722425668</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
@@ -919,42 +1113,54 @@
       <c r="D10" s="9">
         <v>210891</v>
       </c>
-      <c r="E10" s="10">
+      <c r="E10">
+        <v>102044</v>
+      </c>
+      <c r="F10" s="10">
         <v>0.75</v>
       </c>
-      <c r="F10" s="11">
+      <c r="G10" s="11">
         <v>35.615600000000001</v>
       </c>
-      <c r="G10" s="11">
-        <v>0.48945</v>
-      </c>
-      <c r="H10" s="11">
+      <c r="H10" s="5">
+        <v>0.86825799999999997</v>
+      </c>
+      <c r="I10" s="11">
         <v>0.56584800000000002</v>
       </c>
-      <c r="I10" s="11">
-        <v>0.38045499999999999</v>
-      </c>
-      <c r="J10" s="11">
+      <c r="J10" s="5">
+        <v>0.412607</v>
+      </c>
+      <c r="K10" s="11">
         <v>8.4356399999999994</v>
       </c>
-      <c r="K10" s="11">
+      <c r="L10" s="11">
+        <v>4.0817600000000001</v>
+      </c>
+      <c r="M10" s="5">
+        <v>1.9416800000000001</v>
+      </c>
+      <c r="N10" s="11">
         <v>44.617100000000001</v>
       </c>
-      <c r="L10" s="11">
-        <v>0.86990500000000004</v>
-      </c>
-      <c r="M10" s="11">
+      <c r="O10" s="5">
+        <v>1.28087</v>
+      </c>
+      <c r="P10" s="11">
         <v>2.3800000000000002E-3</v>
       </c>
-      <c r="N10" s="11">
+      <c r="Q10" s="5">
+        <v>4.5834200000000004E-3</v>
+      </c>
+      <c r="R10" s="11">
         <v>5.6490000000000004E-3</v>
       </c>
-      <c r="O10" s="11">
+      <c r="S10" s="5">
         <f t="shared" si="0"/>
-        <v>2.3735294117647059</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.2">
+        <v>1.2324857857233245</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>10</v>
       </c>
@@ -967,200 +1173,347 @@
       <c r="D11" s="9">
         <v>306281</v>
       </c>
-      <c r="E11" s="10">
+      <c r="E11">
+        <v>139398</v>
+      </c>
+      <c r="F11" s="10">
         <v>1.0900000000000001</v>
       </c>
-      <c r="F11" s="11">
+      <c r="G11" s="11">
         <v>51.860300000000002</v>
       </c>
-      <c r="G11" s="11">
-        <v>0.63880700000000001</v>
-      </c>
-      <c r="H11" s="11">
+      <c r="H11" s="5">
+        <v>1.0831999999999999</v>
+      </c>
+      <c r="I11" s="11">
         <v>0.70199999999999996</v>
       </c>
-      <c r="I11" s="11">
-        <v>0.56979999999999997</v>
-      </c>
-      <c r="J11" s="11">
+      <c r="J11" s="5">
+        <v>0.60755199999999998</v>
+      </c>
+      <c r="K11" s="11">
         <v>12.251200000000001</v>
       </c>
-      <c r="K11" s="11">
+      <c r="L11" s="11">
+        <v>5.57592</v>
+      </c>
+      <c r="M11" s="5">
+        <v>2.6741999999999999</v>
+      </c>
+      <c r="N11" s="11">
         <v>64.813500000000005</v>
       </c>
-      <c r="L11" s="11">
-        <v>1.20861</v>
-      </c>
-      <c r="M11" s="11">
+      <c r="O11" s="5">
+        <v>1.69075</v>
+      </c>
+      <c r="P11" s="11">
         <v>3.5209E-3</v>
       </c>
-      <c r="N11" s="11">
+      <c r="Q11" s="5">
+        <v>6.5778099999999999E-3</v>
+      </c>
+      <c r="R11" s="11">
         <v>7.8740000000000008E-3</v>
       </c>
-      <c r="O11" s="11">
+      <c r="S11" s="5">
         <f t="shared" si="0"/>
-        <v>2.2363600215853903</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="G13" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="I14" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="18" spans="7:9" x14ac:dyDescent="0.2">
-      <c r="G18" t="s">
+        <v>1.1970549468592131</v>
+      </c>
+    </row>
+    <row r="18" spans="8:15" x14ac:dyDescent="0.2">
+      <c r="H18" t="s">
+        <v>24</v>
+      </c>
+      <c r="I18" t="s">
         <v>25</v>
       </c>
-      <c r="H18" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="19" spans="7:9" x14ac:dyDescent="0.2">
-      <c r="G19" s="3">
-        <f>L2/E2</f>
-        <v>1.5788312499999999</v>
-      </c>
+      <c r="J18" t="s">
+        <v>30</v>
+      </c>
+      <c r="M18" t="s">
+        <v>32</v>
+      </c>
+      <c r="N18" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="8:15" x14ac:dyDescent="0.2">
       <c r="H19" s="3">
-        <f>K2/E2</f>
+        <f>O2/F2</f>
+        <v>2.0429124999999999</v>
+      </c>
+      <c r="I19" s="3">
+        <f>N2/F2</f>
         <v>40.962125</v>
       </c>
-      <c r="I19">
-        <f>H19/G19</f>
-        <v>25.944587174848486</v>
-      </c>
-    </row>
-    <row r="20" spans="7:9" x14ac:dyDescent="0.2">
-      <c r="G20" s="3">
-        <f t="shared" ref="G20:G28" si="1">L3/E3</f>
-        <v>1.9901899999999999</v>
-      </c>
+      <c r="J19" s="3">
+        <f>(M2+L2+I2+G2)/F2</f>
+        <v>37.9605125</v>
+      </c>
+      <c r="K19" s="3">
+        <f>I19/H19</f>
+        <v>20.050846524263768</v>
+      </c>
+      <c r="M19" s="3">
+        <f>G2/F2</f>
+        <v>23.21</v>
+      </c>
+      <c r="N19" s="3">
+        <f>H2/F2</f>
+        <v>1.4551812500000001</v>
+      </c>
+    </row>
+    <row r="20" spans="8:15" x14ac:dyDescent="0.2">
       <c r="H20" s="3">
-        <f t="shared" ref="H20:H28" si="2">K3/E3</f>
+        <f t="shared" ref="H20:H28" si="1">O3/F3</f>
+        <v>2.8483000000000001</v>
+      </c>
+      <c r="I20" s="3">
+        <f t="shared" ref="I20:I28" si="2">N3/F3</f>
         <v>84.671800000000005</v>
       </c>
-      <c r="I20">
-        <f t="shared" ref="I20:I28" si="3">H20/G20</f>
-        <v>42.544581170642005</v>
-      </c>
-    </row>
-    <row r="21" spans="7:9" x14ac:dyDescent="0.2">
-      <c r="G21" s="3">
+      <c r="J20" s="3">
+        <f>(M3+L3+I3+G3)/F3</f>
+        <v>80.335667999999998</v>
+      </c>
+      <c r="K20" s="3">
+        <f>I20/H20</f>
+        <v>29.727135484323984</v>
+      </c>
+      <c r="M20" s="3">
+        <f t="shared" ref="M20:M28" si="3">G3/F3</f>
+        <v>64.876199999999997</v>
+      </c>
+      <c r="N20" s="3">
+        <f t="shared" ref="N20:N28" si="4">H3/F3</f>
+        <v>1.967584</v>
+      </c>
+      <c r="O20" s="5"/>
+    </row>
+    <row r="21" spans="8:15" x14ac:dyDescent="0.2">
+      <c r="H21" s="3">
         <f t="shared" si="1"/>
-        <v>2.0750964912280705</v>
-      </c>
-      <c r="H21" s="3">
+        <v>3.8972105263157899</v>
+      </c>
+      <c r="I21" s="3">
         <f t="shared" si="2"/>
         <v>179.27807017543861</v>
       </c>
-      <c r="I21">
+      <c r="J21" s="3">
+        <f>(M4+L4+I4+G4)/F4</f>
+        <v>174.81260526315791</v>
+      </c>
+      <c r="K21" s="3">
+        <f>I21/H21</f>
+        <v>46.001638598907903</v>
+      </c>
+      <c r="M21" s="3">
         <f t="shared" si="3"/>
-        <v>86.395052438905822</v>
-      </c>
-    </row>
-    <row r="22" spans="7:9" x14ac:dyDescent="0.2">
-      <c r="G22" s="3">
+        <v>162.63070175438597</v>
+      </c>
+      <c r="N21" s="3">
+        <f t="shared" si="4"/>
+        <v>2.8912719298245619</v>
+      </c>
+      <c r="O21" s="5"/>
+    </row>
+    <row r="22" spans="8:15" x14ac:dyDescent="0.2">
+      <c r="H22" s="3">
         <f t="shared" si="1"/>
-        <v>2.4303249999999998</v>
-      </c>
-      <c r="H22" s="3">
+        <v>3.3000500000000001</v>
+      </c>
+      <c r="I22" s="3">
         <f t="shared" si="2"/>
         <v>37.733249999999998</v>
       </c>
-      <c r="I22">
+      <c r="J22" s="3">
+        <f>(M5+L5+I5+G5)/F5</f>
+        <v>26.818075</v>
+      </c>
+      <c r="K22" s="3">
+        <f>I22/H22</f>
+        <v>11.434144937197921</v>
+      </c>
+      <c r="M22" s="3">
         <f t="shared" si="3"/>
-        <v>15.526009895795831</v>
-      </c>
-    </row>
-    <row r="23" spans="7:9" x14ac:dyDescent="0.2">
-      <c r="G23" s="3">
+        <v>0.748</v>
+      </c>
+      <c r="N22" s="3">
+        <f t="shared" si="4"/>
+        <v>1.9905249999999999</v>
+      </c>
+      <c r="O22" s="5"/>
+    </row>
+    <row r="23" spans="8:15" x14ac:dyDescent="0.2">
+      <c r="H23" s="3">
         <f t="shared" si="1"/>
-        <v>1.68912987012987</v>
-      </c>
-      <c r="H23" s="3">
+        <v>2.5869870129870129</v>
+      </c>
+      <c r="I23" s="3">
         <f t="shared" si="2"/>
         <v>58.575324675324673</v>
       </c>
-      <c r="I23">
+      <c r="J23" s="3">
+        <f>(M6+L6+I6+G6)/F6</f>
+        <v>53.223318181818179</v>
+      </c>
+      <c r="K23" s="3">
+        <f>I23/H23</f>
+        <v>22.642295605377562</v>
+      </c>
+      <c r="M23" s="3">
         <f t="shared" si="3"/>
-        <v>34.677809984392177</v>
-      </c>
-    </row>
-    <row r="24" spans="7:9" x14ac:dyDescent="0.2">
-      <c r="G24" s="3">
+        <v>41.248441558441556</v>
+      </c>
+      <c r="N23" s="3">
+        <f t="shared" si="4"/>
+        <v>1.6301558441558441</v>
+      </c>
+      <c r="O23" s="5"/>
+    </row>
+    <row r="24" spans="8:15" x14ac:dyDescent="0.2">
+      <c r="H24" s="3">
         <f t="shared" si="1"/>
-        <v>2.3391571428571432</v>
-      </c>
-      <c r="H24" s="3">
+        <v>4.7269142857142858</v>
+      </c>
+      <c r="I24" s="3">
         <f t="shared" si="2"/>
         <v>40.462000000000003</v>
       </c>
-      <c r="I24">
+      <c r="J24" s="3">
+        <f>(M7+L7+I7+G7)/F7</f>
+        <v>34.517428571428574</v>
+      </c>
+      <c r="K24" s="3">
+        <f>I24/H24</f>
+        <v>8.5599182795178983</v>
+      </c>
+      <c r="M24" s="3">
         <f t="shared" si="3"/>
-        <v>17.297683536805074</v>
-      </c>
-    </row>
-    <row r="25" spans="7:9" x14ac:dyDescent="0.2">
-      <c r="G25" s="3">
+        <v>19.390914285714285</v>
+      </c>
+      <c r="N24" s="3">
+        <f t="shared" si="4"/>
+        <v>3.4960285714285719</v>
+      </c>
+      <c r="O24" s="5"/>
+    </row>
+    <row r="25" spans="8:15" x14ac:dyDescent="0.2">
+      <c r="H25" s="3">
         <f t="shared" si="1"/>
-        <v>1.1072310344827587</v>
-      </c>
-      <c r="H25" s="3">
+        <v>1.1779068965517241</v>
+      </c>
+      <c r="I25" s="3">
         <f t="shared" si="2"/>
         <v>33.773000000000003</v>
       </c>
-      <c r="I25">
+      <c r="J25" s="3">
+        <f>(M8+L8+I8+G8)/F8</f>
+        <v>15.512727586206898</v>
+      </c>
+      <c r="K25" s="3">
+        <f>I25/H25</f>
+        <v>28.672045387346934</v>
+      </c>
+      <c r="M25" s="3">
         <f t="shared" si="3"/>
-        <v>30.502215841318979</v>
-      </c>
-    </row>
-    <row r="26" spans="7:9" x14ac:dyDescent="0.2">
-      <c r="G26" s="3">
+        <v>0.23406896551724138</v>
+      </c>
+      <c r="N25" s="3">
+        <f t="shared" si="4"/>
+        <v>0.50332068965517252</v>
+      </c>
+      <c r="O25" s="5"/>
+    </row>
+    <row r="26" spans="8:15" x14ac:dyDescent="0.2">
+      <c r="H26" s="3">
         <f t="shared" si="1"/>
-        <v>1.7960854700854703</v>
-      </c>
-      <c r="H26" s="3">
+        <v>2.1336410256410261</v>
+      </c>
+      <c r="I26" s="3">
         <f t="shared" si="2"/>
         <v>29.80769230769231</v>
       </c>
-      <c r="I26">
+      <c r="J26" s="3">
+        <f>(M9+L9+I9+G9)/F9</f>
+        <v>20.326425641025644</v>
+      </c>
+      <c r="K26" s="3">
+        <f>I26/H26</f>
+        <v>13.970340816228427</v>
+      </c>
+      <c r="M26" s="3">
         <f t="shared" si="3"/>
-        <v>16.595920853518098</v>
-      </c>
-    </row>
-    <row r="27" spans="7:9" x14ac:dyDescent="0.2">
-      <c r="G27" s="3">
+        <v>6.5831282051282054</v>
+      </c>
+      <c r="N26" s="3">
+        <f t="shared" si="4"/>
+        <v>1.1312478632478633</v>
+      </c>
+      <c r="O26" s="5"/>
+    </row>
+    <row r="27" spans="8:15" x14ac:dyDescent="0.2">
+      <c r="H27" s="3">
         <f t="shared" si="1"/>
-        <v>1.1598733333333333</v>
-      </c>
-      <c r="H27" s="3">
+        <v>1.7078266666666666</v>
+      </c>
+      <c r="I27" s="3">
         <f t="shared" si="2"/>
         <v>59.489466666666665</v>
       </c>
-      <c r="I27">
+      <c r="J27" s="3">
+        <f>(M10+L10+I10+G10)/F10</f>
+        <v>56.273183999999993</v>
+      </c>
+      <c r="K27" s="3">
+        <f>I27/H27</f>
+        <v>34.833433525650534</v>
+      </c>
+      <c r="M27" s="3">
         <f t="shared" si="3"/>
-        <v>51.289623579586276</v>
-      </c>
-    </row>
-    <row r="28" spans="7:9" x14ac:dyDescent="0.2">
-      <c r="G28" s="3">
+        <v>47.48746666666667</v>
+      </c>
+      <c r="N27" s="3">
+        <f t="shared" si="4"/>
+        <v>1.1576773333333332</v>
+      </c>
+      <c r="O27" s="5"/>
+    </row>
+    <row r="28" spans="8:15" x14ac:dyDescent="0.2">
+      <c r="H28" s="3">
         <f t="shared" si="1"/>
-        <v>1.1088165137614678</v>
-      </c>
-      <c r="H28" s="3">
+        <v>1.5511467889908255</v>
+      </c>
+      <c r="I28" s="3">
         <f t="shared" si="2"/>
         <v>59.461926605504587</v>
       </c>
-      <c r="I28">
+      <c r="J28" s="3">
+        <f>(M11+L11+I11+G11)/F11</f>
+        <v>55.791211009174312</v>
+      </c>
+      <c r="K28" s="3">
+        <f>I28/H28</f>
+        <v>38.334171225787379</v>
+      </c>
+      <c r="M28" s="3">
         <f t="shared" si="3"/>
-        <v>53.626480005957262</v>
-      </c>
+        <v>47.578256880733946</v>
+      </c>
+      <c r="N28" s="3">
+        <f t="shared" si="4"/>
+        <v>0.99376146788990816</v>
+      </c>
+      <c r="O28" s="5"/>
+    </row>
+    <row r="29" spans="8:15" x14ac:dyDescent="0.2">
+      <c r="O29" s="5"/>
+    </row>
+    <row r="30" spans="8:15" x14ac:dyDescent="0.2">
+      <c r="O30" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added marisa memory results to spreadsheet
</commit_message>
<xml_diff>
--- a/results/cptVSsd_cpt.xlsx
+++ b/results/cptVSsd_cpt.xlsx
@@ -225,8 +225,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="37">
+  <cellStyleXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -281,7 +283,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="37">
+  <cellStyles count="39">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -300,6 +302,7 @@
     <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -318,6 +321,7 @@
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -593,10 +597,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W42"/>
+  <dimension ref="A1:W36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="N28" sqref="N28"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="P19" sqref="P19:P28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -736,7 +740,9 @@
       <c r="O2" s="14">
         <v>0.116872</v>
       </c>
-      <c r="P2" s="13"/>
+      <c r="P2" s="5">
+        <v>0.117176</v>
+      </c>
       <c r="Q2" s="5">
         <v>0.54470600000000002</v>
       </c>
@@ -806,7 +812,9 @@
       <c r="O3" s="14">
         <v>0.1686</v>
       </c>
-      <c r="P3" s="13"/>
+      <c r="P3" s="14">
+        <v>0.15879199999999999</v>
+      </c>
       <c r="Q3" s="5">
         <v>1.7113499999999999</v>
       </c>
@@ -876,7 +884,9 @@
       <c r="O4" s="14">
         <v>0.15803200000000001</v>
       </c>
-      <c r="P4" s="13"/>
+      <c r="P4" s="14">
+        <v>0.158192</v>
+      </c>
       <c r="Q4" s="11">
         <v>3.70669</v>
       </c>
@@ -946,7 +956,9 @@
       <c r="O5" s="14">
         <v>6.8240000000000002E-3</v>
       </c>
-      <c r="P5" s="13"/>
+      <c r="P5" s="14">
+        <v>6.6160000000000004E-3</v>
+      </c>
       <c r="Q5" s="5">
         <v>0.28207500000000002</v>
       </c>
@@ -1016,7 +1028,9 @@
       <c r="O6" s="5">
         <v>8.7903999999999996E-2</v>
       </c>
-      <c r="P6" s="13"/>
+      <c r="P6" s="14">
+        <v>8.856E-2</v>
+      </c>
       <c r="Q6" s="5">
         <v>6.8092499999999996</v>
       </c>
@@ -1086,7 +1100,9 @@
       <c r="O7" s="5">
         <v>2.1312000000000001E-2</v>
       </c>
-      <c r="P7" s="13"/>
+      <c r="P7" s="5">
+        <v>1.992E-2</v>
+      </c>
       <c r="Q7" s="5">
         <v>1.4720800000000001</v>
       </c>
@@ -1156,7 +1172,9 @@
       <c r="O8" s="5">
         <v>9.5512E-2</v>
       </c>
-      <c r="P8" s="13"/>
+      <c r="P8" s="5">
+        <v>8.8496000000000005E-2</v>
+      </c>
       <c r="Q8" s="5">
         <v>0.769123</v>
       </c>
@@ -1226,7 +1244,9 @@
       <c r="O9" s="5">
         <v>4.9327999999999997E-2</v>
       </c>
-      <c r="P9" s="13"/>
+      <c r="P9" s="5">
+        <v>4.9784000000000002E-2</v>
+      </c>
       <c r="Q9" s="5">
         <v>5.7599499999999999</v>
       </c>
@@ -1296,7 +1316,9 @@
       <c r="O10" s="5">
         <v>0.18827199999999999</v>
       </c>
-      <c r="P10" s="13"/>
+      <c r="P10" s="5">
+        <v>0.17586399999999999</v>
+      </c>
       <c r="Q10" s="5">
         <v>1.9416800000000001</v>
       </c>
@@ -1366,7 +1388,9 @@
       <c r="O11" s="5">
         <v>0.195024</v>
       </c>
-      <c r="P11" s="13"/>
+      <c r="P11" s="5">
+        <v>0.209616</v>
+      </c>
       <c r="Q11" s="5">
         <v>2.6741999999999999</v>
       </c>
@@ -1456,8 +1480,8 @@
         <v>0.73045000000000004</v>
       </c>
       <c r="P19" s="13">
-        <f t="shared" ref="N19:P19" si="3">P2/$F2</f>
-        <v>0</v>
+        <f>P2/$F2</f>
+        <v>0.73234999999999995</v>
       </c>
       <c r="Q19" s="3">
         <f>G2/F2</f>
@@ -1470,11 +1494,11 @@
     </row>
     <row r="20" spans="8:19" x14ac:dyDescent="0.2">
       <c r="H20" s="3">
-        <f t="shared" ref="H20:H28" si="4">S3/F3</f>
+        <f t="shared" ref="H20:H28" si="3">S3/F3</f>
         <v>2.8483000000000001</v>
       </c>
       <c r="I20" s="3">
-        <f t="shared" ref="I20:I28" si="5">R3/F3</f>
+        <f t="shared" ref="I20:I28" si="4">R3/F3</f>
         <v>84.671800000000005</v>
       </c>
       <c r="J20" s="3">
@@ -1486,42 +1510,42 @@
         <v>29.727135484323984</v>
       </c>
       <c r="L20" s="13">
-        <f t="shared" ref="L20:L28" si="6">J3/F3</f>
+        <f t="shared" ref="L20:L28" si="5">J3/F3</f>
         <v>0.88071999999999995</v>
       </c>
       <c r="M20" s="13">
-        <f t="shared" ref="M20:N28" si="7">M3/$F3</f>
+        <f t="shared" ref="M20:N28" si="6">M3/$F3</f>
         <v>0.35553600000000002</v>
       </c>
       <c r="N20" s="13">
+        <f t="shared" si="6"/>
+        <v>0.31630399999999997</v>
+      </c>
+      <c r="O20" s="13">
+        <f t="shared" ref="N20:P20" si="7">O3/$F3</f>
+        <v>0.3372</v>
+      </c>
+      <c r="P20" s="13">
         <f t="shared" si="7"/>
-        <v>0.31630399999999997</v>
-      </c>
-      <c r="O20" s="13">
-        <f t="shared" ref="N20:P20" si="8">O3/$F3</f>
-        <v>0.3372</v>
-      </c>
-      <c r="P20" s="13">
-        <f t="shared" si="8"/>
-        <v>0</v>
+        <v>0.31758399999999998</v>
       </c>
       <c r="Q20" s="3">
-        <f t="shared" ref="Q20:Q28" si="9">G3/F3</f>
+        <f t="shared" ref="Q20:Q28" si="8">G3/F3</f>
         <v>64.876199999999997</v>
       </c>
       <c r="R20" s="3">
-        <f t="shared" ref="R20:R28" si="10">H3/F3</f>
+        <f t="shared" ref="R20:R28" si="9">H3/F3</f>
         <v>1.967584</v>
       </c>
       <c r="S20" s="5"/>
     </row>
     <row r="21" spans="8:19" x14ac:dyDescent="0.2">
       <c r="H21" s="3">
+        <f t="shared" si="3"/>
+        <v>3.8972105263157899</v>
+      </c>
+      <c r="I21" s="3">
         <f t="shared" si="4"/>
-        <v>3.8972105263157899</v>
-      </c>
-      <c r="I21" s="3">
-        <f t="shared" si="5"/>
         <v>179.27807017543861</v>
       </c>
       <c r="J21" s="3">
@@ -1533,42 +1557,42 @@
         <v>46.001638598907903</v>
       </c>
       <c r="L21" s="13">
+        <f t="shared" si="5"/>
+        <v>1.0059385964912282</v>
+      </c>
+      <c r="M21" s="13">
         <f t="shared" si="6"/>
-        <v>1.0059385964912282</v>
-      </c>
-      <c r="M21" s="13">
-        <f t="shared" si="7"/>
         <v>0.1540982456140351</v>
       </c>
       <c r="N21" s="13">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0.13861052631578949</v>
       </c>
       <c r="O21" s="13">
-        <f t="shared" ref="N21:P21" si="11">O4/$F4</f>
+        <f t="shared" ref="N21:P21" si="10">O4/$F4</f>
         <v>0.13862456140350879</v>
       </c>
       <c r="P21" s="13">
-        <f t="shared" si="11"/>
-        <v>0</v>
+        <f t="shared" si="10"/>
+        <v>0.13876491228070176</v>
       </c>
       <c r="Q21" s="3">
+        <f t="shared" si="8"/>
+        <v>162.63070175438597</v>
+      </c>
+      <c r="R21" s="3">
         <f t="shared" si="9"/>
-        <v>162.63070175438597</v>
-      </c>
-      <c r="R21" s="3">
-        <f t="shared" si="10"/>
         <v>2.8912719298245619</v>
       </c>
       <c r="S21" s="5"/>
     </row>
     <row r="22" spans="8:19" x14ac:dyDescent="0.2">
       <c r="H22" s="3">
+        <f t="shared" si="3"/>
+        <v>3.3000500000000001</v>
+      </c>
+      <c r="I22" s="3">
         <f t="shared" si="4"/>
-        <v>3.3000500000000001</v>
-      </c>
-      <c r="I22" s="3">
-        <f t="shared" si="5"/>
         <v>37.733249999999998</v>
       </c>
       <c r="J22" s="3">
@@ -1580,42 +1604,42 @@
         <v>11.434144937197921</v>
       </c>
       <c r="L22" s="13">
+        <f t="shared" si="5"/>
+        <v>1.3095175000000001</v>
+      </c>
+      <c r="M22" s="13">
         <f t="shared" si="6"/>
-        <v>1.3095175000000001</v>
-      </c>
-      <c r="M22" s="13">
-        <f t="shared" si="7"/>
         <v>0.20119999999999999</v>
       </c>
       <c r="N22" s="13">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0.15360000000000001</v>
       </c>
       <c r="O22" s="13">
-        <f t="shared" ref="N22:P22" si="12">O5/$F5</f>
+        <f t="shared" ref="N22:P22" si="11">O5/$F5</f>
         <v>0.1706</v>
       </c>
       <c r="P22" s="13">
-        <f t="shared" si="12"/>
-        <v>0</v>
+        <f t="shared" si="11"/>
+        <v>0.16540000000000002</v>
       </c>
       <c r="Q22" s="3">
+        <f t="shared" si="8"/>
+        <v>0.748</v>
+      </c>
+      <c r="R22" s="3">
         <f t="shared" si="9"/>
-        <v>0.748</v>
-      </c>
-      <c r="R22" s="3">
-        <f t="shared" si="10"/>
         <v>1.9905249999999999</v>
       </c>
       <c r="S22" s="5"/>
     </row>
     <row r="23" spans="8:19" x14ac:dyDescent="0.2">
       <c r="H23" s="3">
+        <f t="shared" si="3"/>
+        <v>2.5869870129870129</v>
+      </c>
+      <c r="I23" s="3">
         <f t="shared" si="4"/>
-        <v>2.5869870129870129</v>
-      </c>
-      <c r="I23" s="3">
-        <f t="shared" si="5"/>
         <v>58.575324675324673</v>
       </c>
       <c r="J23" s="3">
@@ -1627,42 +1651,42 @@
         <v>22.642295605377562</v>
       </c>
       <c r="L23" s="13">
+        <f t="shared" si="5"/>
+        <v>0.95682467532467541</v>
+      </c>
+      <c r="M23" s="13">
         <f t="shared" si="6"/>
-        <v>0.95682467532467541</v>
-      </c>
-      <c r="M23" s="13">
-        <f t="shared" si="7"/>
         <v>6.1475324675324676E-2</v>
       </c>
       <c r="N23" s="13">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>5.6228571428571426E-2</v>
       </c>
       <c r="O23" s="13">
-        <f t="shared" ref="N23:P23" si="13">O6/$F6</f>
+        <f t="shared" ref="N23:P23" si="12">O6/$F6</f>
         <v>5.7080519480519475E-2</v>
       </c>
       <c r="P23" s="13">
-        <f t="shared" si="13"/>
-        <v>0</v>
+        <f t="shared" si="12"/>
+        <v>5.7506493506493506E-2</v>
       </c>
       <c r="Q23" s="3">
+        <f t="shared" si="8"/>
+        <v>41.248441558441556</v>
+      </c>
+      <c r="R23" s="3">
         <f t="shared" si="9"/>
-        <v>41.248441558441556</v>
-      </c>
-      <c r="R23" s="3">
-        <f t="shared" si="10"/>
         <v>1.6301558441558441</v>
       </c>
       <c r="S23" s="5"/>
     </row>
     <row r="24" spans="8:19" x14ac:dyDescent="0.2">
       <c r="H24" s="3">
+        <f t="shared" si="3"/>
+        <v>4.7269142857142858</v>
+      </c>
+      <c r="I24" s="3">
         <f t="shared" si="4"/>
-        <v>4.7269142857142858</v>
-      </c>
-      <c r="I24" s="3">
-        <f t="shared" si="5"/>
         <v>40.462000000000003</v>
       </c>
       <c r="J24" s="3">
@@ -1674,42 +1698,42 @@
         <v>8.5599182795178983</v>
       </c>
       <c r="L24" s="13">
+        <f t="shared" si="5"/>
+        <v>1.2308942857142857</v>
+      </c>
+      <c r="M24" s="13">
         <f t="shared" si="6"/>
-        <v>1.2308942857142857</v>
-      </c>
-      <c r="M24" s="13">
-        <f t="shared" si="7"/>
         <v>7.5085714285714297E-2</v>
       </c>
       <c r="N24" s="13">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>5.3074285714285713E-2</v>
       </c>
       <c r="O24" s="13">
-        <f t="shared" ref="N24:P24" si="14">O7/$F7</f>
+        <f t="shared" ref="N24:P24" si="13">O7/$F7</f>
         <v>6.0891428571428576E-2</v>
       </c>
       <c r="P24" s="13">
-        <f t="shared" si="14"/>
-        <v>0</v>
+        <f t="shared" si="13"/>
+        <v>5.6914285714285716E-2</v>
       </c>
       <c r="Q24" s="3">
+        <f t="shared" si="8"/>
+        <v>19.390914285714285</v>
+      </c>
+      <c r="R24" s="3">
         <f t="shared" si="9"/>
-        <v>19.390914285714285</v>
-      </c>
-      <c r="R24" s="3">
-        <f t="shared" si="10"/>
         <v>3.4960285714285719</v>
       </c>
       <c r="S24" s="5"/>
     </row>
     <row r="25" spans="8:19" x14ac:dyDescent="0.2">
       <c r="H25" s="3">
+        <f t="shared" si="3"/>
+        <v>1.1779068965517241</v>
+      </c>
+      <c r="I25" s="3">
         <f t="shared" si="4"/>
-        <v>1.1779068965517241</v>
-      </c>
-      <c r="I25" s="3">
-        <f t="shared" si="5"/>
         <v>33.773000000000003</v>
       </c>
       <c r="J25" s="3">
@@ -1721,42 +1745,42 @@
         <v>28.672045387346934</v>
       </c>
       <c r="L25" s="13">
+        <f t="shared" si="5"/>
+        <v>0.6745862068965518</v>
+      </c>
+      <c r="M25" s="13">
         <f t="shared" si="6"/>
-        <v>0.6745862068965518</v>
-      </c>
-      <c r="M25" s="13">
-        <f t="shared" si="7"/>
         <v>0.38714482758620689</v>
       </c>
       <c r="N25" s="13">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0.32852413793103447</v>
       </c>
       <c r="O25" s="13">
-        <f t="shared" ref="N25:P25" si="15">O8/$F8</f>
+        <f t="shared" ref="N25:P25" si="14">O8/$F8</f>
         <v>0.32935172413793107</v>
       </c>
       <c r="P25" s="13">
-        <f t="shared" si="15"/>
-        <v>0</v>
+        <f t="shared" si="14"/>
+        <v>0.30515862068965521</v>
       </c>
       <c r="Q25" s="3">
+        <f t="shared" si="8"/>
+        <v>0.23406896551724138</v>
+      </c>
+      <c r="R25" s="3">
         <f t="shared" si="9"/>
-        <v>0.23406896551724138</v>
-      </c>
-      <c r="R25" s="3">
-        <f t="shared" si="10"/>
         <v>0.50332068965517252</v>
       </c>
       <c r="S25" s="5"/>
     </row>
     <row r="26" spans="8:19" x14ac:dyDescent="0.2">
       <c r="H26" s="3">
+        <f t="shared" si="3"/>
+        <v>2.1336410256410261</v>
+      </c>
+      <c r="I26" s="3">
         <f t="shared" si="4"/>
-        <v>2.1336410256410261</v>
-      </c>
-      <c r="I26" s="3">
-        <f t="shared" si="5"/>
         <v>29.80769230769231</v>
       </c>
       <c r="J26" s="3">
@@ -1768,42 +1792,42 @@
         <v>13.970340816228427</v>
       </c>
       <c r="L26" s="13">
+        <f t="shared" si="5"/>
+        <v>1.0023931623931626</v>
+      </c>
+      <c r="M26" s="13">
         <f t="shared" si="6"/>
-        <v>1.0023931623931626</v>
-      </c>
-      <c r="M26" s="13">
-        <f t="shared" si="7"/>
         <v>4.6523076923076924E-2</v>
       </c>
       <c r="N26" s="13">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>4.1825641025641028E-2</v>
       </c>
       <c r="O26" s="13">
-        <f t="shared" ref="N26:P26" si="16">O9/$F9</f>
+        <f t="shared" ref="N26:P26" si="15">O9/$F9</f>
         <v>4.2160683760683763E-2</v>
       </c>
       <c r="P26" s="13">
-        <f t="shared" si="16"/>
-        <v>0</v>
+        <f t="shared" si="15"/>
+        <v>4.2550427350427356E-2</v>
       </c>
       <c r="Q26" s="3">
+        <f t="shared" si="8"/>
+        <v>6.5831282051282054</v>
+      </c>
+      <c r="R26" s="3">
         <f t="shared" si="9"/>
-        <v>6.5831282051282054</v>
-      </c>
-      <c r="R26" s="3">
-        <f t="shared" si="10"/>
         <v>1.1312478632478633</v>
       </c>
       <c r="S26" s="5"/>
     </row>
     <row r="27" spans="8:19" x14ac:dyDescent="0.2">
       <c r="H27" s="3">
+        <f t="shared" si="3"/>
+        <v>1.7078266666666666</v>
+      </c>
+      <c r="I27" s="3">
         <f t="shared" si="4"/>
-        <v>1.7078266666666666</v>
-      </c>
-      <c r="I27" s="3">
-        <f t="shared" si="5"/>
         <v>59.489466666666665</v>
       </c>
       <c r="J27" s="3">
@@ -1815,42 +1839,42 @@
         <v>34.833433525650534</v>
       </c>
       <c r="L27" s="13">
+        <f t="shared" si="5"/>
+        <v>0.55014266666666667</v>
+      </c>
+      <c r="M27" s="13">
         <f t="shared" si="6"/>
-        <v>0.55014266666666667</v>
-      </c>
-      <c r="M27" s="13">
-        <f t="shared" si="7"/>
         <v>0.27365333333333336</v>
       </c>
       <c r="N27" s="13">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0.25312000000000001</v>
       </c>
       <c r="O27" s="13">
-        <f t="shared" ref="N27:P27" si="17">O10/$F10</f>
+        <f t="shared" ref="N27:P27" si="16">O10/$F10</f>
         <v>0.25102933333333333</v>
       </c>
       <c r="P27" s="13">
-        <f t="shared" si="17"/>
-        <v>0</v>
+        <f t="shared" si="16"/>
+        <v>0.23448533333333332</v>
       </c>
       <c r="Q27" s="3">
+        <f t="shared" si="8"/>
+        <v>47.48746666666667</v>
+      </c>
+      <c r="R27" s="3">
         <f t="shared" si="9"/>
-        <v>47.48746666666667</v>
-      </c>
-      <c r="R27" s="3">
-        <f t="shared" si="10"/>
         <v>1.1576773333333332</v>
       </c>
       <c r="S27" s="5"/>
     </row>
     <row r="28" spans="8:19" x14ac:dyDescent="0.2">
       <c r="H28" s="3">
+        <f t="shared" si="3"/>
+        <v>1.5511467889908255</v>
+      </c>
+      <c r="I28" s="3">
         <f t="shared" si="4"/>
-        <v>1.5511467889908255</v>
-      </c>
-      <c r="I28" s="3">
-        <f t="shared" si="5"/>
         <v>59.461926605504587</v>
       </c>
       <c r="J28" s="3">
@@ -1862,31 +1886,31 @@
         <v>38.334171225787379</v>
       </c>
       <c r="L28" s="13">
+        <f t="shared" si="5"/>
+        <v>0.55738715596330268</v>
+      </c>
+      <c r="M28" s="13">
         <f t="shared" si="6"/>
-        <v>0.55738715596330268</v>
-      </c>
-      <c r="M28" s="13">
-        <f t="shared" si="7"/>
         <v>0.21320366972477062</v>
       </c>
       <c r="N28" s="13">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0.19119266055045869</v>
       </c>
       <c r="O28" s="13">
-        <f t="shared" ref="N28:P28" si="18">O11/$F11</f>
+        <f t="shared" ref="N28:P28" si="17">O11/$F11</f>
         <v>0.17892110091743119</v>
       </c>
       <c r="P28" s="13">
-        <f t="shared" si="18"/>
-        <v>0</v>
+        <f t="shared" si="17"/>
+        <v>0.19230825688073394</v>
       </c>
       <c r="Q28" s="3">
+        <f t="shared" si="8"/>
+        <v>47.578256880733946</v>
+      </c>
+      <c r="R28" s="3">
         <f t="shared" si="9"/>
-        <v>47.578256880733946</v>
-      </c>
-      <c r="R28" s="3">
-        <f t="shared" si="10"/>
         <v>0.99376146788990816</v>
       </c>
       <c r="S28" s="5"/>
@@ -1897,40 +1921,18 @@
     <row r="30" spans="8:19" x14ac:dyDescent="0.2">
       <c r="S30" s="5"/>
     </row>
-    <row r="33" spans="13:16" x14ac:dyDescent="0.2">
+    <row r="33" spans="13:15" x14ac:dyDescent="0.2">
       <c r="M33" s="14"/>
       <c r="O33" s="14"/>
-      <c r="P33" s="14"/>
-    </row>
-    <row r="34" spans="13:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="34" spans="13:15" x14ac:dyDescent="0.2">
       <c r="M34" s="14"/>
-      <c r="P34" s="14"/>
-    </row>
-    <row r="35" spans="13:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="35" spans="13:15" x14ac:dyDescent="0.2">
       <c r="M35" s="14"/>
-      <c r="P35" s="14"/>
-    </row>
-    <row r="36" spans="13:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="36" spans="13:15" x14ac:dyDescent="0.2">
       <c r="M36" s="14"/>
-      <c r="P36" s="14"/>
-    </row>
-    <row r="37" spans="13:16" x14ac:dyDescent="0.2">
-      <c r="P37" s="14"/>
-    </row>
-    <row r="38" spans="13:16" x14ac:dyDescent="0.2">
-      <c r="P38" s="14"/>
-    </row>
-    <row r="39" spans="13:16" x14ac:dyDescent="0.2">
-      <c r="P39" s="14"/>
-    </row>
-    <row r="40" spans="13:16" x14ac:dyDescent="0.2">
-      <c r="P40" s="14"/>
-    </row>
-    <row r="41" spans="13:16" x14ac:dyDescent="0.2">
-      <c r="P41" s="14"/>
-    </row>
-    <row r="42" spans="13:16" x14ac:dyDescent="0.2">
-      <c r="P42" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added exported data for training time for each CPT variation
</commit_message>
<xml_diff>
--- a/results/cptVSsd_cpt.xlsx
+++ b/results/cptVSsd_cpt.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafaelktistakis/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafaelktistakis/Repositories/C.CPT/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31285D8A-88A6-C74C-AA1F-DC810015DA6B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3C23D14-69A6-8C45-95CF-0C8FAF92EA53}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="51200" yWindow="0" windowWidth="38400" windowHeight="21600" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
   <si>
     <t>Trie Node Number</t>
   </si>
@@ -211,6 +211,15 @@
   </si>
   <si>
     <t>Total SD_CPT* MB</t>
+  </si>
+  <si>
+    <t>CPT+ Train Time (s)</t>
+  </si>
+  <si>
+    <t>CPT Train Time (s)</t>
+  </si>
+  <si>
+    <t>SD_CPT Train Time (s)</t>
   </si>
 </sst>
 </file>
@@ -220,7 +229,7 @@
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
-    <numFmt numFmtId="171" formatCode="0.000000"/>
+    <numFmt numFmtId="166" formatCode="0.000000"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -305,7 +314,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -320,9 +329,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="27">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -629,10 +639,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AL34"/>
+  <dimension ref="A1:AP34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+    <sheetView tabSelected="1" topLeftCell="AH1" workbookViewId="0">
+      <selection activeCell="AN26" sqref="AN26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -667,9 +677,12 @@
     <col min="36" max="36" width="48.5" customWidth="1"/>
     <col min="37" max="37" width="23.5" customWidth="1"/>
     <col min="38" max="38" width="33.83203125" customWidth="1"/>
+    <col min="40" max="40" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="19.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -784,8 +797,17 @@
       <c r="AL1" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="2" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="AN1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -894,7 +916,7 @@
         <v>0.27395999999999998</v>
       </c>
       <c r="AH2" s="7">
-        <f>1000*AG2</f>
+        <f t="shared" ref="AH2:AH11" si="2">1000*AG2</f>
         <v>273.95999999999998</v>
       </c>
       <c r="AI2" s="5">
@@ -905,15 +927,24 @@
         <v>218.67000000000002</v>
       </c>
       <c r="AK2" s="5">
-        <f>AF2/AD2</f>
+        <f t="shared" ref="AK2:AK11" si="3">AF2/AD2</f>
         <v>1.0041252145665296</v>
       </c>
       <c r="AL2" s="12">
-        <f>AH2/AD2</f>
+        <f t="shared" ref="AL2:AL11" si="4">AH2/AD2</f>
         <v>1.2641429336089629</v>
       </c>
-    </row>
-    <row r="3" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="AN2" s="3">
+        <v>4.0334599999999998</v>
+      </c>
+      <c r="AO2" s="3">
+        <v>0.14577200000000001</v>
+      </c>
+      <c r="AP2" s="3">
+        <v>0.17785500000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -939,7 +970,7 @@
         <v>134957</v>
       </c>
       <c r="I3" s="4">
-        <f t="shared" ref="I3:I11" si="2">CEILING(LOG(D3+1,2),1)*(C3+B3)*0.00000013</f>
+        <f t="shared" ref="I3:I11" si="5">CEILING(LOG(D3+1,2),1)*(C3+B3)*0.00000013</f>
         <v>0.67983084000000005</v>
       </c>
       <c r="J3" s="5">
@@ -987,7 +1018,7 @@
         <v>1.42415</v>
       </c>
       <c r="X3" s="3">
-        <f t="shared" ref="X3:X11" si="3">P3+L3</f>
+        <f t="shared" ref="X3:X11" si="6">P3+L3</f>
         <v>1.02182</v>
       </c>
       <c r="Y3" s="3">
@@ -1008,40 +1039,49 @@
         <v>0.24426</v>
       </c>
       <c r="AD3" s="7">
-        <f t="shared" ref="AD3:AD11" si="4">1000*AC3</f>
+        <f t="shared" ref="AD3:AD11" si="7">1000*AC3</f>
         <v>244.26</v>
       </c>
       <c r="AE3" s="5">
         <v>0.17918999999999999</v>
       </c>
       <c r="AF3" s="7">
-        <f t="shared" ref="AF3:AF11" si="5">1000*AE3</f>
+        <f t="shared" ref="AF3:AF11" si="8">1000*AE3</f>
         <v>179.19</v>
       </c>
       <c r="AG3" s="5">
         <v>0.26718999999999998</v>
       </c>
       <c r="AH3" s="7">
-        <f>1000*AG3</f>
+        <f t="shared" si="2"/>
         <v>267.19</v>
       </c>
       <c r="AI3" s="5">
         <v>0.18373</v>
       </c>
       <c r="AJ3" s="7">
-        <f t="shared" ref="AJ3:AJ11" si="6">1000*AI3</f>
+        <f t="shared" ref="AJ3:AJ11" si="9">1000*AI3</f>
         <v>183.73000000000002</v>
       </c>
       <c r="AK3" s="5">
-        <f>AF3/AD3</f>
+        <f t="shared" si="3"/>
         <v>0.7336035372144436</v>
       </c>
       <c r="AL3" s="12">
-        <f>AH3/AD3</f>
+        <f t="shared" si="4"/>
         <v>1.0938753786948334</v>
       </c>
-    </row>
-    <row r="4" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="AN3" s="3">
+        <v>18.540900000000001</v>
+      </c>
+      <c r="AO3" s="3">
+        <v>0.53732999999999997</v>
+      </c>
+      <c r="AP3" s="3">
+        <v>0.80908999999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>16</v>
       </c>
@@ -1067,7 +1107,7 @@
         <v>240517</v>
       </c>
       <c r="I4" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1.2253254</v>
       </c>
       <c r="J4" s="5">
@@ -1115,7 +1155,7 @@
         <v>4.4428200000000002</v>
       </c>
       <c r="X4" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>2.4882600000000004</v>
       </c>
       <c r="Y4" s="3">
@@ -1136,40 +1176,49 @@
         <v>0.47705599999999998</v>
       </c>
       <c r="AD4" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>477.05599999999998</v>
       </c>
       <c r="AE4" s="5">
         <v>0.52105000000000001</v>
       </c>
       <c r="AF4" s="7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>521.05000000000007</v>
       </c>
       <c r="AG4" s="5">
         <v>1.4073599999999999</v>
       </c>
       <c r="AH4" s="7">
-        <f>1000*AG4</f>
+        <f t="shared" si="2"/>
         <v>1407.36</v>
       </c>
       <c r="AI4" s="5">
         <v>0.53049999999999997</v>
       </c>
       <c r="AJ4" s="7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>530.5</v>
       </c>
       <c r="AK4" s="5">
-        <f>AF4/AD4</f>
+        <f t="shared" si="3"/>
         <v>1.092219781325463</v>
       </c>
       <c r="AL4" s="12">
-        <f>AH4/AD4</f>
+        <f t="shared" si="4"/>
         <v>2.950093909310437</v>
       </c>
-    </row>
-    <row r="5" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="AN4" s="3">
+        <v>30.8811</v>
+      </c>
+      <c r="AO4" s="3">
+        <v>1.1552100000000001</v>
+      </c>
+      <c r="AP4" s="3">
+        <v>3.0717300000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -1195,7 +1244,7 @@
         <v>18872</v>
       </c>
       <c r="I5" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>4.526496E-2</v>
       </c>
       <c r="J5" s="5">
@@ -1243,7 +1292,7 @@
         <v>0.13200200000000001</v>
       </c>
       <c r="X5" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>9.93507E-2</v>
       </c>
       <c r="Y5" s="3">
@@ -1264,40 +1313,49 @@
         <v>0.20355400000000001</v>
       </c>
       <c r="AD5" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>203.554</v>
       </c>
       <c r="AE5" s="5">
         <v>0.31065999999999999</v>
       </c>
       <c r="AF5" s="7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>310.65999999999997</v>
       </c>
       <c r="AG5" s="5">
         <v>0.32585999999999998</v>
       </c>
       <c r="AH5" s="7">
-        <f>1000*AG5</f>
+        <f t="shared" si="2"/>
         <v>325.85999999999996</v>
       </c>
       <c r="AI5" s="5">
         <v>0.31697999999999998</v>
       </c>
       <c r="AJ5" s="7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>316.97999999999996</v>
       </c>
       <c r="AK5" s="5">
-        <f>AF5/AD5</f>
+        <f t="shared" si="3"/>
         <v>1.5261797852166992</v>
       </c>
       <c r="AL5" s="12">
-        <f>AH5/AD5</f>
+        <f t="shared" si="4"/>
         <v>1.6008528449453214</v>
       </c>
-    </row>
-    <row r="6" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="AN5" s="3">
+        <v>0.77232000000000001</v>
+      </c>
+      <c r="AO5" s="3">
+        <v>1.338E-2</v>
+      </c>
+      <c r="AP5" s="3">
+        <v>2.5908E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -1323,7 +1381,7 @@
         <v>283527</v>
       </c>
       <c r="I6" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1.4986516999999999</v>
       </c>
       <c r="J6" s="5">
@@ -1371,7 +1429,7 @@
         <v>3.9839600000000002</v>
       </c>
       <c r="X6" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>2.71252</v>
       </c>
       <c r="Y6" s="3">
@@ -1392,40 +1450,49 @@
         <v>0.34389399999999998</v>
       </c>
       <c r="AD6" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>343.89400000000001</v>
       </c>
       <c r="AE6" s="5">
         <v>0.41846</v>
       </c>
       <c r="AF6" s="7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>418.46</v>
       </c>
       <c r="AG6" s="5">
         <v>2.1104400000000001</v>
       </c>
       <c r="AH6" s="7">
-        <f>1000*AG6</f>
+        <f t="shared" si="2"/>
         <v>2110.44</v>
       </c>
       <c r="AI6" s="5">
         <v>0.40916000000000002</v>
       </c>
       <c r="AJ6" s="7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>409.16</v>
       </c>
       <c r="AK6" s="5">
-        <f>AF6/AD6</f>
+        <f t="shared" si="3"/>
         <v>1.2168284413220352</v>
       </c>
       <c r="AL6" s="12">
-        <f>AH6/AD6</f>
+        <f t="shared" si="4"/>
         <v>6.1368910187441479</v>
       </c>
-    </row>
-    <row r="7" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="AN6" s="3">
+        <v>21.082799999999999</v>
+      </c>
+      <c r="AO6" s="3">
+        <v>1.2007000000000001</v>
+      </c>
+      <c r="AP6" s="3">
+        <v>3.2590499999999998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -1451,7 +1518,7 @@
         <v>94388</v>
       </c>
       <c r="I7" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.36961470000000002</v>
       </c>
       <c r="J7" s="5">
@@ -1499,7 +1566,7 @@
         <v>1.65442</v>
       </c>
       <c r="X7" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0.890903</v>
       </c>
       <c r="Y7" s="3">
@@ -1520,40 +1587,49 @@
         <v>0.100912</v>
       </c>
       <c r="AD7" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>100.91200000000001</v>
       </c>
       <c r="AE7" s="5">
         <v>0.12305000000000001</v>
       </c>
       <c r="AF7" s="7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>123.05000000000001</v>
       </c>
       <c r="AG7" s="5">
         <v>0.13725000000000001</v>
       </c>
       <c r="AH7" s="7">
-        <f>1000*AG7</f>
+        <f t="shared" si="2"/>
         <v>137.25</v>
       </c>
       <c r="AI7" s="5">
         <v>0.12254</v>
       </c>
       <c r="AJ7" s="7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>122.53999999999999</v>
       </c>
       <c r="AK7" s="5">
-        <f>AF7/AD7</f>
+        <f t="shared" si="3"/>
         <v>1.2193792611384178</v>
       </c>
       <c r="AL7" s="12">
-        <f>AH7/AD7</f>
+        <f t="shared" si="4"/>
         <v>1.3600959251625178</v>
       </c>
-    </row>
-    <row r="8" spans="1:38" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AN7" s="3">
+        <v>3.9022399999999999</v>
+      </c>
+      <c r="AO7" s="3">
+        <v>0.128326</v>
+      </c>
+      <c r="AP7" s="3">
+        <v>0.56225599999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:42" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
@@ -1579,7 +1655,7 @@
         <v>85184</v>
       </c>
       <c r="I8" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.29611789999999999</v>
       </c>
       <c r="J8" s="10">
@@ -1627,7 +1703,7 @@
         <v>0.34159299999999998</v>
       </c>
       <c r="X8" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0.32123999999999997</v>
       </c>
       <c r="Y8" s="3">
@@ -1648,40 +1724,49 @@
         <v>11.638400000000001</v>
       </c>
       <c r="AD8" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>11638.400000000001</v>
       </c>
       <c r="AE8" s="10">
         <v>11.8131</v>
       </c>
       <c r="AF8" s="7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>11813.1</v>
       </c>
       <c r="AG8" s="10">
         <v>47.792200000000001</v>
       </c>
       <c r="AH8" s="7">
-        <f>1000*AG8</f>
+        <f t="shared" si="2"/>
         <v>47792.200000000004</v>
       </c>
       <c r="AI8" s="5">
         <v>11.2453</v>
       </c>
       <c r="AJ8" s="7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>11245.300000000001</v>
       </c>
       <c r="AK8" s="5">
-        <f>AF8/AD8</f>
+        <f t="shared" si="3"/>
         <v>1.0150106543854824</v>
       </c>
       <c r="AL8" s="12">
-        <f>AH8/AD8</f>
+        <f t="shared" si="4"/>
         <v>4.106423563376409</v>
       </c>
-    </row>
-    <row r="9" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="AN8" s="17">
+        <v>6.31088</v>
+      </c>
+      <c r="AO8" s="17">
+        <v>1.07114</v>
+      </c>
+      <c r="AP8" s="17">
+        <v>1.1564300000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -1707,7 +1792,7 @@
         <v>253903</v>
       </c>
       <c r="I9" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1.1880055199999999</v>
       </c>
       <c r="J9" s="5">
@@ -1755,7 +1840,7 @@
         <v>2.4963600000000001</v>
       </c>
       <c r="X9" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>2.12534</v>
       </c>
       <c r="Y9" s="3">
@@ -1776,40 +1861,49 @@
         <v>13.6942</v>
       </c>
       <c r="AD9" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>13694.2</v>
       </c>
       <c r="AE9" s="5">
         <v>17.8782</v>
       </c>
       <c r="AF9" s="7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>17878.2</v>
       </c>
       <c r="AG9" s="5">
         <v>24.385200000000001</v>
       </c>
       <c r="AH9" s="7">
-        <f>1000*AG9</f>
+        <f t="shared" si="2"/>
         <v>24385.200000000001</v>
       </c>
       <c r="AI9" s="5">
         <v>17.973400000000002</v>
       </c>
       <c r="AJ9" s="7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>17973.400000000001</v>
       </c>
       <c r="AK9" s="5">
-        <f>AF9/AD9</f>
+        <f t="shared" si="3"/>
         <v>1.3055308086635218</v>
       </c>
       <c r="AL9" s="12">
-        <f>AH9/AD9</f>
+        <f t="shared" si="4"/>
         <v>1.780695476917235</v>
       </c>
-    </row>
-    <row r="10" spans="1:38" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AN9" s="3">
+        <v>17.220300000000002</v>
+      </c>
+      <c r="AO9" s="3">
+        <v>0.74445099999999997</v>
+      </c>
+      <c r="AP9" s="3">
+        <v>1.3640399999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:42" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
@@ -1835,7 +1929,7 @@
         <v>102044</v>
       </c>
       <c r="I10" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.76494600000000001</v>
       </c>
       <c r="J10" s="10">
@@ -1883,7 +1977,7 @@
         <v>1.28087</v>
       </c>
       <c r="X10" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0.902057</v>
       </c>
       <c r="Y10" s="3">
@@ -1904,40 +1998,49 @@
         <v>0.98205900000000002</v>
       </c>
       <c r="AD10" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>982.05899999999997</v>
       </c>
       <c r="AE10" s="10">
         <v>1.0914999999999999</v>
       </c>
       <c r="AF10" s="7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>1091.5</v>
       </c>
       <c r="AG10" s="10">
         <v>3.4292199999999999</v>
       </c>
       <c r="AH10" s="7">
-        <f>1000*AG10</f>
+        <f t="shared" si="2"/>
         <v>3429.22</v>
       </c>
       <c r="AI10" s="5">
         <v>1.0933900000000001</v>
       </c>
       <c r="AJ10" s="7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>1093.3900000000001</v>
       </c>
       <c r="AK10" s="5">
-        <f>AF10/AD10</f>
+        <f t="shared" si="3"/>
         <v>1.111440351343453</v>
       </c>
       <c r="AL10" s="12">
-        <f>AH10/AD10</f>
+        <f t="shared" si="4"/>
         <v>3.4918675965496981</v>
       </c>
-    </row>
-    <row r="11" spans="1:38" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AN10" s="17">
+        <v>13.514900000000001</v>
+      </c>
+      <c r="AO10" s="17">
+        <v>0.59297100000000003</v>
+      </c>
+      <c r="AP10" s="17">
+        <v>0.83881300000000003</v>
+      </c>
+    </row>
+    <row r="11" spans="1:42" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="11" t="s">
         <v>10</v>
       </c>
@@ -1963,7 +2066,7 @@
         <v>139398</v>
       </c>
       <c r="I11" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1.1107372900000001</v>
       </c>
       <c r="J11" s="10">
@@ -2011,7 +2114,7 @@
         <v>1.69075</v>
       </c>
       <c r="X11" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>1.2463519999999999</v>
       </c>
       <c r="Y11" s="3">
@@ -2032,51 +2135,62 @@
         <v>1.1633</v>
       </c>
       <c r="AD11" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>1163.3</v>
       </c>
       <c r="AE11" s="10">
         <v>1.4539</v>
       </c>
       <c r="AF11" s="7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>1453.8999999999999</v>
       </c>
       <c r="AG11" s="10">
         <v>4.7567199999999996</v>
       </c>
       <c r="AH11" s="7">
-        <f>1000*AG11</f>
+        <f t="shared" si="2"/>
         <v>4756.7199999999993</v>
       </c>
       <c r="AI11" s="5">
         <v>1.44573</v>
       </c>
       <c r="AJ11" s="7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>1445.73</v>
       </c>
       <c r="AK11" s="5">
-        <f>AF11/AD11</f>
+        <f t="shared" si="3"/>
         <v>1.2498065847158943</v>
       </c>
       <c r="AL11" s="12">
-        <f>AH11/AD11</f>
+        <f t="shared" si="4"/>
         <v>4.0889882231582559</v>
       </c>
-    </row>
-    <row r="12" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="AN11" s="17">
+        <v>22.862400000000001</v>
+      </c>
+      <c r="AO11" s="17">
+        <v>0.94706000000000001</v>
+      </c>
+      <c r="AP11" s="17">
+        <v>1.34745</v>
+      </c>
+    </row>
+    <row r="12" spans="1:42" x14ac:dyDescent="0.2">
       <c r="W12" s="3"/>
       <c r="X12" s="3"/>
       <c r="Y12" s="3"/>
-    </row>
-    <row r="15" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="AO12" s="3"/>
+      <c r="AP12" s="3"/>
+    </row>
+    <row r="15" spans="1:42" x14ac:dyDescent="0.2">
       <c r="W15" s="5"/>
       <c r="X15" s="5"/>
       <c r="Y15" s="5"/>
       <c r="Z15" s="5"/>
     </row>
-    <row r="16" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:42" x14ac:dyDescent="0.2">
       <c r="W16" s="5"/>
       <c r="X16" s="5"/>
       <c r="Y16" s="5"/>
@@ -2118,31 +2232,31 @@
     </row>
     <row r="19" spans="4:32" x14ac:dyDescent="0.2">
       <c r="E19" s="3">
-        <f>W2/I2</f>
+        <f t="shared" ref="E19:E28" si="10">W2/I2</f>
         <v>1.3351844043063175</v>
       </c>
       <c r="F19" s="3">
-        <f>V2/I2</f>
+        <f t="shared" ref="F19:F28" si="11">V2/I2</f>
         <v>26.771577572336511</v>
       </c>
       <c r="G19" s="3">
-        <f>Z2/I2</f>
+        <f t="shared" ref="G19:G28" si="12">Z2/I2</f>
         <v>24.264797099689254</v>
       </c>
       <c r="H19" s="3">
-        <f t="shared" ref="H19:H28" si="7">F19/E19</f>
+        <f t="shared" ref="H19:H28" si="13">F19/E19</f>
         <v>20.050846524263765</v>
       </c>
       <c r="J19" s="3">
-        <f>J2/I2</f>
+        <f t="shared" ref="J19:J28" si="14">J2/I2</f>
         <v>15.169337905539091</v>
       </c>
       <c r="K19" s="3">
-        <f>L2/I2</f>
+        <f t="shared" ref="K19:K28" si="15">L2/I2</f>
         <v>0.66402616596414121</v>
       </c>
       <c r="L19" s="13">
-        <f>J2/Z2</f>
+        <f t="shared" ref="L19:L28" si="16">J2/Z2</f>
         <v>0.62515824233837736</v>
       </c>
       <c r="M19" s="5">
@@ -2157,35 +2271,35 @@
     </row>
     <row r="20" spans="4:32" x14ac:dyDescent="0.2">
       <c r="E20" s="3">
-        <f>W3/I3</f>
+        <f t="shared" si="10"/>
         <v>2.0948593623672616</v>
       </c>
       <c r="F20" s="3">
-        <f>V3/I3</f>
+        <f t="shared" si="11"/>
         <v>62.274168085696139</v>
       </c>
       <c r="G20" s="3">
-        <f>Z3/I3</f>
+        <f t="shared" si="12"/>
         <v>57.018778377279844</v>
       </c>
       <c r="H20" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>29.727135484323984</v>
       </c>
       <c r="J20" s="3">
-        <f>J3/I3</f>
+        <f t="shared" si="14"/>
         <v>47.71495803279533</v>
       </c>
       <c r="K20" s="3">
-        <f>L3/I3</f>
+        <f t="shared" si="15"/>
         <v>0.85530100399681774</v>
       </c>
       <c r="L20" s="13">
-        <f>J3/Z3</f>
+        <f t="shared" si="16"/>
         <v>0.83682883763444871</v>
       </c>
       <c r="M20" s="5">
-        <f t="shared" ref="M20:M28" si="8">L3+O3</f>
+        <f t="shared" ref="M20:M28" si="17">L3+O3</f>
         <v>1.2015639999999999</v>
       </c>
       <c r="V20" s="5"/>
@@ -2196,35 +2310,35 @@
     </row>
     <row r="21" spans="4:32" x14ac:dyDescent="0.2">
       <c r="E21" s="3">
-        <f>W4/I4</f>
+        <f t="shared" si="10"/>
         <v>3.6258286982380357</v>
       </c>
       <c r="F21" s="3">
-        <f>V4/I4</f>
+        <f t="shared" si="11"/>
         <v>166.79406139789481</v>
       </c>
       <c r="G21" s="3">
-        <f>Z4/I4</f>
+        <f t="shared" si="12"/>
         <v>158.96988669295519</v>
       </c>
       <c r="H21" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>46.001638598907903</v>
       </c>
       <c r="J21" s="3">
-        <f>J4/I4</f>
+        <f t="shared" si="14"/>
         <v>151.3059306531963</v>
       </c>
       <c r="K21" s="3">
-        <f>L4/I4</f>
+        <f t="shared" si="15"/>
         <v>1.094803062109053</v>
       </c>
       <c r="L21" s="13">
-        <f>J4/Z4</f>
+        <f t="shared" si="16"/>
         <v>0.95178988801469322</v>
       </c>
       <c r="M21" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="17"/>
         <v>1.9014900000000001</v>
       </c>
       <c r="V21" s="5"/>
@@ -2236,35 +2350,35 @@
     </row>
     <row r="22" spans="4:32" x14ac:dyDescent="0.2">
       <c r="E22" s="3">
-        <f>W5/I5</f>
+        <f t="shared" si="10"/>
         <v>2.9162071500781179</v>
       </c>
       <c r="F22" s="3">
-        <f>V5/I5</f>
+        <f t="shared" si="11"/>
         <v>33.344335220886087</v>
       </c>
       <c r="G22" s="3">
-        <f>Z5/I5</f>
+        <f t="shared" si="12"/>
         <v>14.460810304482758</v>
       </c>
       <c r="H22" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>11.434144937197921</v>
       </c>
       <c r="J22" s="3">
-        <f>J5/I5</f>
+        <f t="shared" si="14"/>
         <v>0.66099693891257161</v>
       </c>
       <c r="K22" s="3">
-        <f>L5/I5</f>
+        <f t="shared" si="15"/>
         <v>1.0376679886605444</v>
       </c>
       <c r="L22" s="13">
-        <f>J5/Z5</f>
+        <f t="shared" si="16"/>
         <v>4.5709536671514658E-2</v>
       </c>
       <c r="M22" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="17"/>
         <v>5.2817999999999997E-2</v>
       </c>
       <c r="V22" s="5"/>
@@ -2275,35 +2389,35 @@
     </row>
     <row r="23" spans="4:32" x14ac:dyDescent="0.2">
       <c r="E23" s="3">
-        <f>W6/I6</f>
+        <f t="shared" si="10"/>
         <v>2.6583628470844829</v>
       </c>
       <c r="F23" s="3">
-        <f>V6/I6</f>
+        <f t="shared" si="11"/>
         <v>60.191437410039974</v>
       </c>
       <c r="G23" s="3">
-        <f>Z6/I6</f>
+        <f t="shared" si="12"/>
         <v>52.021346921369386</v>
       </c>
       <c r="H23" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>22.642295605377562</v>
       </c>
       <c r="J23" s="3">
-        <f>J6/I6</f>
+        <f t="shared" si="14"/>
         <v>42.386499811797499</v>
       </c>
       <c r="K23" s="3">
-        <f>L6/I6</f>
+        <f t="shared" si="15"/>
         <v>0.82674980450761171</v>
       </c>
       <c r="L23" s="13">
-        <f>J6/Z6</f>
+        <f t="shared" si="16"/>
         <v>0.81479051043920447</v>
       </c>
       <c r="M23" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="17"/>
         <v>1.5299700000000001</v>
       </c>
       <c r="V23" s="5"/>
@@ -2317,35 +2431,35 @@
     </row>
     <row r="24" spans="4:32" x14ac:dyDescent="0.2">
       <c r="E24" s="3">
-        <f>W7/I7</f>
+        <f t="shared" si="10"/>
         <v>4.4760665633699093</v>
       </c>
       <c r="F24" s="3">
-        <f>V7/I7</f>
+        <f t="shared" si="11"/>
         <v>38.314763996128939</v>
       </c>
       <c r="G24" s="3">
-        <f>Z7/I7</f>
+        <f t="shared" si="12"/>
         <v>27.323426259832193</v>
       </c>
       <c r="H24" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>8.5599182795178965</v>
       </c>
       <c r="J24" s="3">
-        <f>J7/I7</f>
+        <f t="shared" si="14"/>
         <v>18.361877923145371</v>
       </c>
       <c r="K24" s="3">
-        <f>L7/I7</f>
+        <f t="shared" si="15"/>
         <v>1.2447827426777127</v>
       </c>
       <c r="L24" s="13">
-        <f>J7/Z7</f>
+        <f t="shared" si="16"/>
         <v>0.67201959770831976</v>
       </c>
       <c r="M24" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="17"/>
         <v>0.50676999999999994</v>
       </c>
       <c r="V24" s="5"/>
@@ -2356,35 +2470,35 @@
     </row>
     <row r="25" spans="4:32" x14ac:dyDescent="0.2">
       <c r="E25" s="3">
-        <f>W8/I8</f>
+        <f t="shared" si="10"/>
         <v>1.153570925634688</v>
       </c>
       <c r="F25" s="3">
-        <f>V8/I8</f>
+        <f t="shared" si="11"/>
         <v>33.075237937321589</v>
       </c>
       <c r="G25" s="3">
-        <f>Z8/I8</f>
+        <f t="shared" si="12"/>
         <v>15.560720915554242</v>
       </c>
       <c r="H25" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>28.672045387346934</v>
       </c>
       <c r="J25" s="3">
-        <f>J8/I8</f>
+        <f t="shared" si="14"/>
         <v>0.22923301833492674</v>
       </c>
       <c r="K25" s="3">
-        <f>L8/I8</f>
+        <f t="shared" si="15"/>
         <v>0.42418914898423904</v>
       </c>
       <c r="L25" s="13">
-        <f>J8/Z8</f>
+        <f t="shared" si="16"/>
         <v>1.4731516590969069E-2</v>
       </c>
       <c r="M25" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="17"/>
         <v>0.379938</v>
       </c>
       <c r="V25" s="5"/>
@@ -2395,35 +2509,35 @@
     </row>
     <row r="26" spans="4:32" x14ac:dyDescent="0.2">
       <c r="E26" s="3">
-        <f>W9/I9</f>
+        <f t="shared" si="10"/>
         <v>2.101303367681322</v>
       </c>
       <c r="F26" s="3">
-        <f>V9/I9</f>
+        <f t="shared" si="11"/>
         <v>29.355924204796626</v>
       </c>
       <c r="G26" s="3">
-        <f>Z9/I9</f>
+        <f t="shared" si="12"/>
         <v>17.027217179933643</v>
       </c>
       <c r="H26" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>13.970340816228429</v>
       </c>
       <c r="J26" s="3">
-        <f>J9/I9</f>
+        <f t="shared" si="14"/>
         <v>6.4833537137100175</v>
       </c>
       <c r="K26" s="3">
-        <f>L9/I9</f>
+        <f t="shared" si="15"/>
         <v>0.80179762127704601</v>
       </c>
       <c r="L26" s="13">
-        <f>J9/Z9</f>
+        <f t="shared" si="16"/>
         <v>0.38076414044630652</v>
       </c>
       <c r="M26" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="17"/>
         <v>1.1161480000000001</v>
       </c>
       <c r="V26" s="5"/>
@@ -2435,35 +2549,35 @@
     </row>
     <row r="27" spans="4:32" x14ac:dyDescent="0.2">
       <c r="E27" s="3">
-        <f>W10/I10</f>
+        <f t="shared" si="10"/>
         <v>1.6744580663210213</v>
       </c>
       <c r="F27" s="3">
-        <f>V10/I10</f>
+        <f t="shared" si="11"/>
         <v>58.327123744682631</v>
       </c>
       <c r="G27" s="3">
-        <f>Z10/I10</f>
+        <f t="shared" si="12"/>
         <v>54.328551296431378</v>
       </c>
       <c r="H27" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>34.833433525650534</v>
       </c>
       <c r="J27" s="3">
-        <f>J10/I10</f>
+        <f t="shared" si="14"/>
         <v>46.559626431146775</v>
       </c>
       <c r="K27" s="3">
-        <f>L10/I10</f>
+        <f t="shared" si="15"/>
         <v>0.63984908738656066</v>
       </c>
       <c r="L27" s="13">
-        <f>J10/Z10</f>
+        <f t="shared" si="16"/>
         <v>0.85700106702836165</v>
       </c>
       <c r="M27" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="17"/>
         <v>1.0552980000000001</v>
       </c>
       <c r="V27" s="5"/>
@@ -2477,35 +2591,35 @@
         <v>49</v>
       </c>
       <c r="E28" s="3">
-        <f>W11/I11</f>
+        <f t="shared" si="10"/>
         <v>1.5221871231135131</v>
       </c>
       <c r="F28" s="3">
-        <f>V11/I11</f>
+        <f t="shared" si="11"/>
         <v>58.351781815122095</v>
       </c>
       <c r="G28" s="3">
-        <f>Z11/I11</f>
+        <f t="shared" si="12"/>
         <v>53.961724828739655</v>
       </c>
       <c r="H28" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>38.334171225787372</v>
       </c>
       <c r="J28" s="3">
-        <f>J11/I11</f>
+        <f t="shared" si="14"/>
         <v>46.689978329619237</v>
       </c>
       <c r="K28" s="3">
-        <f>L11/I11</f>
+        <f t="shared" si="15"/>
         <v>0.57511349060766648</v>
       </c>
       <c r="L28" s="13">
-        <f>J11/Z11</f>
+        <f t="shared" si="16"/>
         <v>0.86524251175812061</v>
       </c>
       <c r="M28" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="17"/>
         <v>1.3408</v>
       </c>
       <c r="V28" s="5"/>

</xml_diff>

<commit_message>
corrected some minor staff for timing experiments in Evaluator
</commit_message>
<xml_diff>
--- a/results/cptVSsd_cpt.xlsx
+++ b/results/cptVSsd_cpt.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafaelktistakis/Repositories/C.CPT/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3C23D14-69A6-8C45-95CF-0C8FAF92EA53}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80D33778-5D52-C145-8BE2-2F8A6A7B74B4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51200" yWindow="0" windowWidth="38400" windowHeight="21600" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="51200" yWindow="460" windowWidth="38400" windowHeight="21140" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="65">
   <si>
     <t>Trie Node Number</t>
   </si>
@@ -220,6 +220,9 @@
   </si>
   <si>
     <t>SD_CPT Train Time (s)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">run again </t>
   </si>
 </sst>
 </file>
@@ -642,7 +645,7 @@
   <dimension ref="A1:AP34"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="AH1" workbookViewId="0">
-      <selection activeCell="AN26" sqref="AN26"/>
+      <selection activeCell="AN14" sqref="AN14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2184,6 +2187,17 @@
       <c r="AO12" s="3"/>
       <c r="AP12" s="3"/>
     </row>
+    <row r="14" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="AN14" t="s">
+        <v>64</v>
+      </c>
+      <c r="AO14" t="s">
+        <v>64</v>
+      </c>
+      <c r="AP14" t="s">
+        <v>64</v>
+      </c>
+    </row>
     <row r="15" spans="1:42" x14ac:dyDescent="0.2">
       <c r="W15" s="5"/>
       <c r="X15" s="5"/>

</xml_diff>

<commit_message>
slightly updated some timing exports for SD_CPT (sCPT)
</commit_message>
<xml_diff>
--- a/results/cptVSsd_cpt.xlsx
+++ b/results/cptVSsd_cpt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafaelktistakis/Repositories/C.CPT/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9AEC12D-41DD-324C-A3DE-99E13A9515F7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A647C40-46E6-4B48-9C8F-F5932E772B5A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="51200" yWindow="460" windowWidth="38400" windowHeight="21140" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="97">
   <si>
     <t>Trie Node Number</t>
   </si>
@@ -320,9 +320,6 @@
     <t>Test Time (s)</t>
   </si>
   <si>
-    <t>Thismemory report for II contains a further array Sigma x uint64_t for CPT/+ implementation</t>
-  </si>
-  <si>
     <t>CPT/+ implementation uses an extra int per Sigma symbol within II to count the set-bits (cardinality)</t>
   </si>
   <si>
@@ -330,6 +327,9 @@
   </si>
   <si>
     <t>Or in O(n) time calculate it; At least in its ADMA and PAKDD version</t>
+  </si>
+  <si>
+    <t>This memory report for II contains a further array Sigma x uint64_t for CPT/+ implementation</t>
   </si>
 </sst>
 </file>
@@ -15106,8 +15106,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AP34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="Z2" sqref="Z2"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -15322,7 +15322,7 @@
         <v>0.47681600000000002</v>
       </c>
       <c r="P2" s="5">
-        <v>9.4036599999999998E-2</v>
+        <v>9.0051999999999993E-2</v>
       </c>
       <c r="Q2" s="5">
         <v>2.3635199999999998</v>
@@ -15344,14 +15344,13 @@
         <v>6.5539360000000002</v>
       </c>
       <c r="W2" s="3">
-        <v>0.32686599999999999</v>
+        <v>0.315695</v>
       </c>
       <c r="X2" s="3">
-        <f>P2+L2</f>
-        <v>0.25659660000000001</v>
+        <v>0.25261299999999998</v>
       </c>
       <c r="Y2" s="3">
-        <v>0.26355899999999999</v>
+        <v>0.259575</v>
       </c>
       <c r="Z2" s="12">
         <f>T2+O2+S2+J2</f>
@@ -15460,7 +15459,7 @@
         <v>0.62010399999999999</v>
       </c>
       <c r="P3" s="5">
-        <v>0.44035999999999997</v>
+        <v>0.413632</v>
       </c>
       <c r="Q3" s="5">
         <v>9.2776800000000001</v>
@@ -15482,14 +15481,13 @@
         <v>42.335883999999993</v>
       </c>
       <c r="W3" s="3">
-        <v>1.42415</v>
+        <v>1.38659</v>
       </c>
       <c r="X3" s="3">
-        <f t="shared" ref="X3:X11" si="5">P3+L3</f>
-        <v>1.02182</v>
+        <v>0.99509499999999995</v>
       </c>
       <c r="Y3" s="3">
-        <v>1.03057</v>
+        <v>1.0038499999999999</v>
       </c>
       <c r="Z3" s="12">
         <f>T3+O3+S3+J3</f>
@@ -15506,14 +15504,14 @@
         <v>0.24426</v>
       </c>
       <c r="AD3" s="7">
-        <f t="shared" ref="AD3:AD11" si="6">1000*AC3</f>
+        <f t="shared" ref="AD3:AD11" si="5">1000*AC3</f>
         <v>244.26</v>
       </c>
       <c r="AE3" s="5">
         <v>0.17918999999999999</v>
       </c>
       <c r="AF3" s="7">
-        <f t="shared" ref="AF3:AF11" si="7">1000*AE3</f>
+        <f t="shared" ref="AF3:AF11" si="6">1000*AE3</f>
         <v>179.19</v>
       </c>
       <c r="AG3" s="5">
@@ -15527,7 +15525,7 @@
         <v>0.18373</v>
       </c>
       <c r="AJ3" s="7">
-        <f t="shared" ref="AJ3:AJ11" si="8">1000*AI3</f>
+        <f t="shared" ref="AJ3:AJ11" si="7">1000*AI3</f>
         <v>183.73000000000002</v>
       </c>
       <c r="AK3" s="5">
@@ -15598,7 +15596,7 @@
         <v>0.56000000000000005</v>
       </c>
       <c r="P4" s="5">
-        <v>1.1467700000000001</v>
+        <v>0.88269900000000001</v>
       </c>
       <c r="Q4" s="5">
         <v>18.417400000000001</v>
@@ -15620,14 +15618,13 @@
         <v>204.37639999999999</v>
       </c>
       <c r="W4" s="3">
-        <v>4.4428200000000002</v>
+        <v>4.0879700000000003</v>
       </c>
       <c r="X4" s="3">
-        <f t="shared" si="5"/>
-        <v>2.4882600000000004</v>
+        <v>2.2241900000000001</v>
       </c>
       <c r="Y4" s="3">
-        <v>2.4087399999999999</v>
+        <v>2.2395800000000001</v>
       </c>
       <c r="Z4" s="12">
         <f>T4+O4+S4+J4</f>
@@ -15644,14 +15641,14 @@
         <v>0.47705599999999998</v>
       </c>
       <c r="AD4" s="7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>477.05599999999998</v>
       </c>
       <c r="AE4" s="5">
         <v>0.52105000000000001</v>
       </c>
       <c r="AF4" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>521.05000000000007</v>
       </c>
       <c r="AG4" s="5">
@@ -15665,7 +15662,7 @@
         <v>0.53049999999999997</v>
       </c>
       <c r="AJ4" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>530.5</v>
       </c>
       <c r="AK4" s="5">
@@ -15736,7 +15733,7 @@
         <v>5.8479999999999999E-3</v>
       </c>
       <c r="P5" s="5">
-        <v>5.2380700000000002E-2</v>
+        <v>5.0236000000000003E-2</v>
       </c>
       <c r="Q5" s="5">
         <v>1.47356</v>
@@ -15758,14 +15755,13 @@
         <v>1.509328</v>
       </c>
       <c r="W5" s="3">
-        <v>0.13200200000000001</v>
+        <v>0.12792000000000001</v>
       </c>
       <c r="X5" s="3">
-        <f t="shared" si="5"/>
-        <v>9.93507E-2</v>
+        <v>9.7212999999999994E-2</v>
       </c>
       <c r="Y5" s="3">
-        <v>9.9746000000000001E-2</v>
+        <v>9.7601999999999994E-2</v>
       </c>
       <c r="Z5" s="12">
         <f>T5+O5+S5+J5</f>
@@ -15782,14 +15778,14 @@
         <v>0.20355400000000001</v>
       </c>
       <c r="AD5" s="7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>203.554</v>
       </c>
       <c r="AE5" s="5">
         <v>0.31065999999999999</v>
       </c>
       <c r="AF5" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>310.65999999999997</v>
       </c>
       <c r="AG5" s="5">
@@ -15803,7 +15799,7 @@
         <v>0.31697999999999998</v>
       </c>
       <c r="AJ5" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>316.97999999999996</v>
       </c>
       <c r="AK5" s="5">
@@ -15874,7 +15870,7 @@
         <v>0.29096</v>
       </c>
       <c r="P6" s="5">
-        <v>1.4735100000000001</v>
+        <v>1.36226</v>
       </c>
       <c r="Q6" s="5">
         <v>26.392399999999999</v>
@@ -15896,14 +15892,13 @@
         <v>90.20595999999999</v>
       </c>
       <c r="W6" s="3">
-        <v>3.9839600000000002</v>
+        <v>3.8429500000000001</v>
       </c>
       <c r="X6" s="3">
-        <f t="shared" si="5"/>
-        <v>2.71252</v>
+        <v>2.6012599999999999</v>
       </c>
       <c r="Y6" s="3">
-        <v>2.7448199999999998</v>
+        <v>2.6335700000000002</v>
       </c>
       <c r="Z6" s="12">
         <f>T6+O6+S6+J6</f>
@@ -15920,14 +15915,14 @@
         <v>0.34389399999999998</v>
       </c>
       <c r="AD6" s="7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>343.89400000000001</v>
       </c>
       <c r="AE6" s="5">
         <v>0.41846</v>
       </c>
       <c r="AF6" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>418.46</v>
       </c>
       <c r="AG6" s="5">
@@ -15941,7 +15936,7 @@
         <v>0.40916000000000002</v>
       </c>
       <c r="AJ6" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>409.16</v>
       </c>
       <c r="AK6" s="5">
@@ -16012,7 +16007,7 @@
         <v>4.6679999999999999E-2</v>
       </c>
       <c r="P7" s="5">
-        <v>0.430813</v>
+        <v>0.35860500000000001</v>
       </c>
       <c r="Q7" s="5">
         <v>7.3282400000000001</v>
@@ -16034,14 +16029,13 @@
         <v>14.16174</v>
       </c>
       <c r="W7" s="3">
-        <v>1.65442</v>
+        <v>1.5772699999999999</v>
       </c>
       <c r="X7" s="3">
-        <f t="shared" si="5"/>
-        <v>0.890903</v>
+        <v>0.81870500000000002</v>
       </c>
       <c r="Y7" s="3">
-        <v>0.89632199999999995</v>
+        <v>0.82411400000000001</v>
       </c>
       <c r="Z7" s="12">
         <f>T7+O7+S7+J7</f>
@@ -16058,14 +16052,14 @@
         <v>0.100912</v>
       </c>
       <c r="AD7" s="7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>100.91200000000001</v>
       </c>
       <c r="AE7" s="5">
         <v>0.12305000000000001</v>
       </c>
       <c r="AF7" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>123.05000000000001</v>
       </c>
       <c r="AG7" s="5">
@@ -16079,7 +16073,7 @@
         <v>0.12254</v>
       </c>
       <c r="AJ7" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>122.53999999999999</v>
       </c>
       <c r="AK7" s="5">
@@ -16150,7 +16144,7 @@
         <v>0.254328</v>
       </c>
       <c r="P8" s="5">
-        <v>0.19563</v>
+        <v>0.19548599999999999</v>
       </c>
       <c r="Q8" s="10">
         <v>9.4719599999999993</v>
@@ -16172,14 +16166,13 @@
         <v>9.7941679999999991</v>
       </c>
       <c r="W8" s="3">
-        <v>0.34159299999999998</v>
+        <v>0.33217099999999999</v>
       </c>
       <c r="X8" s="3">
-        <f t="shared" si="5"/>
-        <v>0.32123999999999997</v>
+        <v>0.32109700000000002</v>
       </c>
       <c r="Y8" s="3">
-        <v>0.33217600000000003</v>
+        <v>0.33203199999999999</v>
       </c>
       <c r="Z8" s="12">
         <f>T8+O8+S8+J8</f>
@@ -16196,14 +16189,14 @@
         <v>11.638400000000001</v>
       </c>
       <c r="AD8" s="7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>11638.400000000001</v>
       </c>
       <c r="AE8" s="10">
         <v>11.8131</v>
       </c>
       <c r="AF8" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>11813.1</v>
       </c>
       <c r="AG8" s="10">
@@ -16217,7 +16210,7 @@
         <v>11.2453</v>
       </c>
       <c r="AJ8" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>11245.300000000001</v>
       </c>
       <c r="AK8" s="5">
@@ -16288,7 +16281,7 @@
         <v>0.163608</v>
       </c>
       <c r="P9" s="5">
-        <v>1.1728000000000001</v>
+        <v>1.1488700000000001</v>
       </c>
       <c r="Q9" s="5">
         <v>27.0092</v>
@@ -16310,14 +16303,13 @@
         <v>34.875068000000006</v>
       </c>
       <c r="W9" s="3">
-        <v>2.4963600000000001</v>
+        <v>2.4368599999999998</v>
       </c>
       <c r="X9" s="3">
-        <f t="shared" si="5"/>
-        <v>2.12534</v>
+        <v>2.1014200000000001</v>
       </c>
       <c r="Y9" s="3">
-        <v>2.1714000000000002</v>
+        <v>2.1474700000000002</v>
       </c>
       <c r="Z9" s="12">
         <f>T9+O9+S9+J9</f>
@@ -16334,14 +16326,14 @@
         <v>13.6942</v>
       </c>
       <c r="AD9" s="7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>13694.2</v>
       </c>
       <c r="AE9" s="5">
         <v>17.8782</v>
       </c>
       <c r="AF9" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>17878.2</v>
       </c>
       <c r="AG9" s="5">
@@ -16355,7 +16347,7 @@
         <v>17.973400000000002</v>
       </c>
       <c r="AJ9" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>17973.400000000001</v>
       </c>
       <c r="AK9" s="5">
@@ -16426,7 +16418,7 @@
         <v>0.56584800000000002</v>
       </c>
       <c r="P10" s="5">
-        <v>0.412607</v>
+        <v>0.38045499999999999</v>
       </c>
       <c r="Q10" s="10">
         <v>8.4356399999999994</v>
@@ -16448,14 +16440,13 @@
         <v>44.617088000000003</v>
       </c>
       <c r="W10" s="3">
-        <v>1.28087</v>
+        <v>1.23034</v>
       </c>
       <c r="X10" s="3">
-        <f t="shared" si="5"/>
-        <v>0.902057</v>
+        <v>0.86990500000000004</v>
       </c>
       <c r="Y10" s="3">
-        <v>0.92410400000000004</v>
+        <v>0.89195199999999997</v>
       </c>
       <c r="Z10" s="12">
         <f>T10+O10+S10+J10</f>
@@ -16472,14 +16463,14 @@
         <v>0.98205900000000002</v>
       </c>
       <c r="AD10" s="7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>982.05899999999997</v>
       </c>
       <c r="AE10" s="10">
         <v>1.0914999999999999</v>
       </c>
       <c r="AF10" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>1091.5</v>
       </c>
       <c r="AG10" s="10">
@@ -16493,7 +16484,7 @@
         <v>1.0933900000000001</v>
       </c>
       <c r="AJ10" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>1093.3900000000001</v>
       </c>
       <c r="AK10" s="5">
@@ -16564,7 +16555,7 @@
         <v>0.70199999999999996</v>
       </c>
       <c r="P11" s="5">
-        <v>0.60755199999999998</v>
+        <v>0.56979999999999997</v>
       </c>
       <c r="Q11" s="10">
         <v>12.251200000000001</v>
@@ -16586,14 +16577,13 @@
         <v>64.813500000000005</v>
       </c>
       <c r="W11" s="3">
-        <v>1.69075</v>
+        <v>1.62714</v>
       </c>
       <c r="X11" s="3">
-        <f t="shared" si="5"/>
-        <v>1.2463519999999999</v>
+        <v>1.20861</v>
       </c>
       <c r="Y11" s="3">
-        <v>1.2761400000000001</v>
+        <v>1.2383900000000001</v>
       </c>
       <c r="Z11" s="12">
         <f>T11+O11+S11+J11</f>
@@ -16610,14 +16600,14 @@
         <v>1.1633</v>
       </c>
       <c r="AD11" s="7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>1163.3</v>
       </c>
       <c r="AE11" s="10">
         <v>1.4539</v>
       </c>
       <c r="AF11" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>1453.8999999999999</v>
       </c>
       <c r="AG11" s="10">
@@ -16631,7 +16621,7 @@
         <v>1.44573</v>
       </c>
       <c r="AJ11" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>1445.73</v>
       </c>
       <c r="AK11" s="5">
@@ -16661,18 +16651,9 @@
     </row>
     <row r="13" spans="1:42" x14ac:dyDescent="0.2">
       <c r="J13" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="P13" t="s">
-        <v>64</v>
-      </c>
-      <c r="W13" t="s">
-        <v>64</v>
-      </c>
-      <c r="X13" t="s">
-        <v>64</v>
-      </c>
-      <c r="Y13" t="s">
         <v>64</v>
       </c>
       <c r="AF13" t="s">
@@ -16681,12 +16662,12 @@
     </row>
     <row r="14" spans="1:42" x14ac:dyDescent="0.2">
       <c r="J14" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="15" spans="1:42" x14ac:dyDescent="0.2">
       <c r="J15" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="W15" s="5"/>
       <c r="X15" s="5"/>
@@ -16695,16 +16676,14 @@
     </row>
     <row r="16" spans="1:42" x14ac:dyDescent="0.2">
       <c r="J16" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="W16" s="5"/>
-      <c r="X16" s="5"/>
       <c r="Y16" s="5"/>
       <c r="Z16" s="5"/>
     </row>
     <row r="17" spans="4:30" x14ac:dyDescent="0.2">
       <c r="W17" s="5"/>
-      <c r="X17" s="5"/>
       <c r="Y17" s="5"/>
       <c r="Z17" s="5"/>
     </row>
@@ -16731,7 +16710,6 @@
         <v>54</v>
       </c>
       <c r="W18" s="5"/>
-      <c r="X18" s="5"/>
       <c r="Y18" s="5"/>
       <c r="Z18" s="5"/>
       <c r="AD18" s="16"/>
@@ -16739,7 +16717,7 @@
     <row r="19" spans="4:30" x14ac:dyDescent="0.2">
       <c r="E19" s="3">
         <f>W2/I2</f>
-        <v>1.3351844043063175</v>
+        <v>1.2895530294294386</v>
       </c>
       <c r="F19" s="3" t="e">
         <f>#REF!/I2</f>
@@ -16750,11 +16728,11 @@
         <v>24.264797099689254</v>
       </c>
       <c r="H19" s="3" t="e">
-        <f t="shared" ref="H19:H28" si="9">F19/E19</f>
+        <f t="shared" ref="H19:H28" si="8">F19/E19</f>
         <v>#REF!</v>
       </c>
       <c r="J19" s="3">
-        <f t="shared" ref="J19:J28" si="10">J2/I2</f>
+        <f t="shared" ref="J19:J28" si="9">J2/I2</f>
         <v>15.169337905539091</v>
       </c>
       <c r="K19" s="3">
@@ -16770,14 +16748,13 @@
         <v>0.63937600000000006</v>
       </c>
       <c r="W19" s="5"/>
-      <c r="X19" s="5"/>
       <c r="Y19" s="5"/>
       <c r="Z19" s="5"/>
     </row>
     <row r="20" spans="4:30" x14ac:dyDescent="0.2">
       <c r="E20" s="3">
         <f>W3/I3</f>
-        <v>2.0948593623672616</v>
+        <v>2.0396103242388945</v>
       </c>
       <c r="F20" s="3">
         <f>V3/I3</f>
@@ -16788,11 +16765,11 @@
         <v>57.018778377279844</v>
       </c>
       <c r="H20" s="3">
+        <f t="shared" si="8"/>
+        <v>30.532373664890116</v>
+      </c>
+      <c r="J20" s="3">
         <f t="shared" si="9"/>
-        <v>29.727124249552361</v>
-      </c>
-      <c r="J20" s="3">
-        <f t="shared" si="10"/>
         <v>47.71495803279533</v>
       </c>
       <c r="K20" s="3">
@@ -16804,19 +16781,18 @@
         <v>0.83682883763444871</v>
       </c>
       <c r="M20" s="5">
-        <f t="shared" ref="M20:M28" si="11">L3+O3</f>
+        <f t="shared" ref="M20:M28" si="10">L3+O3</f>
         <v>1.2015639999999999</v>
       </c>
       <c r="V20" s="5"/>
       <c r="W20" s="5"/>
-      <c r="X20" s="5"/>
       <c r="Y20" s="5"/>
       <c r="Z20" s="5"/>
     </row>
     <row r="21" spans="4:30" x14ac:dyDescent="0.2">
       <c r="E21" s="3">
         <f>W4/I4</f>
-        <v>3.6258286982380357</v>
+        <v>3.3362321551483389</v>
       </c>
       <c r="F21" s="3">
         <f>V4/I4</f>
@@ -16827,11 +16803,11 @@
         <v>158.96988669295519</v>
       </c>
       <c r="H21" s="3">
+        <f t="shared" si="8"/>
+        <v>49.9945938937908</v>
+      </c>
+      <c r="J21" s="3">
         <f t="shared" si="9"/>
-        <v>46.001503549547358</v>
-      </c>
-      <c r="J21" s="3">
-        <f t="shared" si="10"/>
         <v>151.3059306531963</v>
       </c>
       <c r="K21" s="3">
@@ -16843,12 +16819,11 @@
         <v>0.95178988801469322</v>
       </c>
       <c r="M21" s="5">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>1.9014900000000001</v>
       </c>
       <c r="V21" s="5"/>
       <c r="W21" s="5"/>
-      <c r="X21" s="5"/>
       <c r="Y21" s="5"/>
       <c r="Z21" s="5"/>
       <c r="AD21" s="16"/>
@@ -16856,7 +16831,7 @@
     <row r="22" spans="4:30" x14ac:dyDescent="0.2">
       <c r="E22" s="3">
         <f>W5/I5</f>
-        <v>2.9162071500781179</v>
+        <v>2.8260270195754069</v>
       </c>
       <c r="F22" s="3">
         <f>V5/I5</f>
@@ -16867,11 +16842,11 @@
         <v>14.460810304482758</v>
       </c>
       <c r="H22" s="3">
+        <f t="shared" si="8"/>
+        <v>11.798999374609128</v>
+      </c>
+      <c r="J22" s="3">
         <f t="shared" si="9"/>
-        <v>11.434129785912333</v>
-      </c>
-      <c r="J22" s="3">
-        <f t="shared" si="10"/>
         <v>0.66099693891257161</v>
       </c>
       <c r="K22" s="3">
@@ -16883,19 +16858,18 @@
         <v>4.5709536671514658E-2</v>
       </c>
       <c r="M22" s="5">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>5.2817999999999997E-2</v>
       </c>
       <c r="V22" s="5"/>
       <c r="W22" s="5"/>
-      <c r="X22" s="5"/>
       <c r="Y22" s="5"/>
       <c r="Z22" s="5"/>
     </row>
     <row r="23" spans="4:30" x14ac:dyDescent="0.2">
       <c r="E23" s="3">
         <f>W6/I6</f>
-        <v>2.6583628470844829</v>
+        <v>2.5642716049366241</v>
       </c>
       <c r="F23" s="3">
         <f>V6/I6</f>
@@ -16906,11 +16880,11 @@
         <v>52.021346921369386</v>
       </c>
       <c r="H23" s="3">
+        <f t="shared" si="8"/>
+        <v>23.473102694544554</v>
+      </c>
+      <c r="J23" s="3">
         <f t="shared" si="9"/>
-        <v>22.642285565116111</v>
-      </c>
-      <c r="J23" s="3">
-        <f t="shared" si="10"/>
         <v>42.386499811797499</v>
       </c>
       <c r="K23" s="3">
@@ -16922,19 +16896,18 @@
         <v>0.81479051043920447</v>
       </c>
       <c r="M23" s="5">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>1.5299700000000001</v>
       </c>
       <c r="V23" s="5"/>
       <c r="W23" s="5"/>
-      <c r="X23" s="5"/>
       <c r="Y23" s="5"/>
       <c r="Z23" s="5"/>
     </row>
     <row r="24" spans="4:30" x14ac:dyDescent="0.2">
       <c r="E24" s="3">
         <f>W7/I7</f>
-        <v>4.4760665633699093</v>
+        <v>4.2673356876769235</v>
       </c>
       <c r="F24" s="3">
         <f>V7/I7</f>
@@ -16945,11 +16918,11 @@
         <v>27.323426259832193</v>
       </c>
       <c r="H24" s="3">
+        <f t="shared" si="8"/>
+        <v>8.9786403088881421</v>
+      </c>
+      <c r="J24" s="3">
         <f t="shared" si="9"/>
-        <v>8.5599424571753229</v>
-      </c>
-      <c r="J24" s="3">
-        <f t="shared" si="10"/>
         <v>18.361877923145371</v>
       </c>
       <c r="K24" s="3">
@@ -16961,19 +16934,18 @@
         <v>0.67201959770831976</v>
       </c>
       <c r="M24" s="5">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>0.50676999999999994</v>
       </c>
       <c r="V24" s="5"/>
       <c r="W24" s="5"/>
-      <c r="X24" s="5"/>
       <c r="Y24" s="5"/>
       <c r="Z24" s="5"/>
     </row>
     <row r="25" spans="4:30" x14ac:dyDescent="0.2">
       <c r="E25" s="3">
         <f>W8/I8</f>
-        <v>1.153570925634688</v>
+        <v>1.1217525181692833</v>
       </c>
       <c r="F25" s="3">
         <f>V8/I8</f>
@@ -16984,11 +16956,11 @@
         <v>15.560720915554242</v>
       </c>
       <c r="H25" s="3">
+        <f t="shared" si="8"/>
+        <v>29.485319308428487</v>
+      </c>
+      <c r="J25" s="3">
         <f t="shared" si="9"/>
-        <v>28.67203953242602</v>
-      </c>
-      <c r="J25" s="3">
-        <f t="shared" si="10"/>
         <v>0.22923301833492674</v>
       </c>
       <c r="K25" s="3">
@@ -17000,19 +16972,18 @@
         <v>1.4731516590969069E-2</v>
       </c>
       <c r="M25" s="5">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>0.379938</v>
       </c>
       <c r="V25" s="5"/>
       <c r="W25" s="5"/>
-      <c r="X25" s="5"/>
       <c r="Y25" s="5"/>
       <c r="Z25" s="5"/>
     </row>
     <row r="26" spans="4:30" x14ac:dyDescent="0.2">
       <c r="E26" s="3">
         <f>W9/I9</f>
-        <v>2.101303367681322</v>
+        <v>2.0512194253104141</v>
       </c>
       <c r="F26" s="3">
         <f>V9/I9</f>
@@ -17023,11 +16994,11 @@
         <v>17.027217179933643</v>
       </c>
       <c r="H26" s="3">
+        <f t="shared" si="8"/>
+        <v>14.311477885475576</v>
+      </c>
+      <c r="J26" s="3">
         <f t="shared" si="9"/>
-        <v>13.970368055889377</v>
-      </c>
-      <c r="J26" s="3">
-        <f t="shared" si="10"/>
         <v>6.4833537137100175</v>
       </c>
       <c r="K26" s="3">
@@ -17039,7 +17010,7 @@
         <v>0.38076414044630652</v>
       </c>
       <c r="M26" s="5">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>1.1161480000000001</v>
       </c>
       <c r="V26" s="5"/>
@@ -17052,7 +17023,7 @@
     <row r="27" spans="4:30" x14ac:dyDescent="0.2">
       <c r="E27" s="3">
         <f>W10/I10</f>
-        <v>1.6744580663210213</v>
+        <v>1.6084011158957625</v>
       </c>
       <c r="F27" s="3">
         <f>V10/I10</f>
@@ -17063,11 +17034,11 @@
         <v>54.328551296431378</v>
       </c>
       <c r="H27" s="3">
+        <f t="shared" si="8"/>
+        <v>36.264031080839445</v>
+      </c>
+      <c r="J27" s="3">
         <f t="shared" si="9"/>
-        <v>34.833424157018278</v>
-      </c>
-      <c r="J27" s="3">
-        <f t="shared" si="10"/>
         <v>46.559626431146775</v>
       </c>
       <c r="K27" s="3">
@@ -17079,7 +17050,7 @@
         <v>0.85700106702836165</v>
       </c>
       <c r="M27" s="5">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>1.0552980000000001</v>
       </c>
       <c r="V27" s="5"/>
@@ -17094,7 +17065,7 @@
       </c>
       <c r="E28" s="3">
         <f>W11/I11</f>
-        <v>1.5221871231135131</v>
+        <v>1.4649188558349382</v>
       </c>
       <c r="F28" s="3">
         <f>V11/I11</f>
@@ -17105,11 +17076,11 @@
         <v>53.961724828739655</v>
       </c>
       <c r="H28" s="3">
+        <f t="shared" si="8"/>
+        <v>39.832774069840333</v>
+      </c>
+      <c r="J28" s="3">
         <f t="shared" si="9"/>
-        <v>38.334171225787372</v>
-      </c>
-      <c r="J28" s="3">
-        <f t="shared" si="10"/>
         <v>46.689978329619237</v>
       </c>
       <c r="K28" s="3">
@@ -17121,7 +17092,7 @@
         <v>0.86524251175812061</v>
       </c>
       <c r="M28" s="5">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>1.3408</v>
       </c>
       <c r="V28" s="5"/>

</xml_diff>

<commit_message>
More data in the spreadSheet; some charts are prepared for Quest exports. Also execution now reports Average Sequence length
</commit_message>
<xml_diff>
--- a/results/cptVSsd_cpt.xlsx
+++ b/results/cptVSsd_cpt.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafaelktistakis/Repositories/C.CPT/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A647C40-46E6-4B48-9C8F-F5932E772B5A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C54858E9-4879-F74A-9B8F-DBDC3283CA06}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51200" yWindow="460" windowWidth="38400" windowHeight="21140" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="51200" yWindow="460" windowWidth="38400" windowHeight="21140" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="All RAW Data" sheetId="1" r:id="rId1"/>
     <sheet name="Datasets Attributes, Notes" sheetId="2" r:id="rId2"/>
     <sheet name="Scalability CPT+" sheetId="3" r:id="rId3"/>
     <sheet name="Scalability sCPT" sheetId="4" r:id="rId4"/>
@@ -281,9 +281,6 @@
     <t>QUEST_5_1200</t>
   </si>
   <si>
-    <t>QUEST50K</t>
-  </si>
-  <si>
     <t>QUEST100K</t>
   </si>
   <si>
@@ -330,6 +327,9 @@
   </si>
   <si>
     <t>This memory report for II contains a further array Sigma x uint64_t for CPT/+ implementation</t>
+  </si>
+  <si>
+    <t>QUEST1600K</t>
   </si>
 </sst>
 </file>
@@ -401,12 +401,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -456,7 +462,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -486,6 +492,13 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="27">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -725,24 +738,6 @@
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>3872.21</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4729.8050000000003</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4243.9790000000003</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3765.9119999999998</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>3226.8020000000001</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2920.9470000000001</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -757,7 +752,7 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>subSeq</c:v>
+            <c:v>sCPT</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
@@ -874,24 +869,6 @@
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>4.3860700000000001</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4.6304299999999996</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4.5821399999999999</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4.7274099999999999</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4.5145200000000001</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>4.5786499999999997</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -899,6 +876,52 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-6740-7940-B6E7-390A1160FA2C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>CPT</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Scalability CPT'!$B$2:$G$2</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="6"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-6740-7940-B6E7-390A1160FA2C}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1476,15 +1499,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>0.33200000000000002</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.156</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.258</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1499,7 +1513,7 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>subSeq</c:v>
+            <c:v>sCPT</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
@@ -1672,15 +1686,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>5.6391999999999998E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.39711999999999997</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.0847500000000001</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1688,6 +1693,52 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000007-959F-6341-8837-5B0DE9299CD8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>CPT</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Scalability CPT'!$B$19:$D$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000008-959F-6341-8837-5B0DE9299CD8}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2337,24 +2388,6 @@
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>2.2850000000000001</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.046</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.73699999999999999</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.69599999999999995</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.59099999999999997</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.64100000000000001</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2369,7 +2402,7 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>subSeq</c:v>
+            <c:v>sCPT</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
@@ -2619,24 +2652,6 @@
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>0.47705999999999998</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.70109100000000002</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.83188799999999996</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.761154</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.0216700000000001</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.97730600000000001</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2644,6 +2659,52 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{0000000D-ACF3-224E-A1E3-B8FC3A670BCF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>CPT</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Scalability CPT'!$B$3:$G$3</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="6"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000E-ACF3-224E-A1E3-B8FC3A670BCF}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3161,24 +3222,6 @@
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>44.527999999999999</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>75.564999999999998</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>103.515</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>130.916</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>152.86799999999999</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>174.76599999999999</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -3193,7 +3236,7 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>subSeq</c:v>
+            <c:v>sCPT</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
@@ -3310,24 +3353,6 @@
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>6.4744400000000004</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>7.2308899999999996</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>7.9577400000000003</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>7.9333999999999998</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>7.9303600000000003</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>8.70336</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -3335,6 +3360,52 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-FFAC-1941-9218-ECD12BA8EAF1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>CPT</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Scalability CPT'!$B$4:$G$4</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="6"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-FFAC-1941-9218-ECD12BA8EAF1}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3853,18 +3924,6 @@
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>1616.71</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3179.241</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4421.4040000000005</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1882.4839999999999</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -3879,7 +3938,7 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>subSeq</c:v>
+            <c:v>sCPT</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
@@ -3990,18 +4049,6 @@
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>4.2885</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4.1141300000000003</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4.2238699999999998</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4.3745700000000003</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4009,6 +4056,52 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-07DD-704D-8D46-D069D4C3CD52}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>CPT</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Scalability CPT'!$B$8:$E$8</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="4"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-07DD-704D-8D46-D069D4C3CD52}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4608,18 +4701,6 @@
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>0.96599999999999997</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.78500000000000003</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.3879999999999999</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.4510000000000001</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4634,7 +4715,7 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>subSeq</c:v>
+            <c:v>sCPT</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
@@ -4833,18 +4914,6 @@
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>1.0930200000000001</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.73525399999999996</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.36714999999999998</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>7.2503999999999999E-2</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4852,6 +4921,52 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000009-D8F2-F148-BCDC-3B4F9BBB0AC0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>CPT</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Scalability CPT'!$B$9:$E$9</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="4"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000A-D8F2-F148-BCDC-3B4F9BBB0AC0}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -5362,18 +5477,6 @@
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>20.472999999999999</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>40.835000000000001</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>75.563999999999993</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>110.43899999999999</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -5388,7 +5491,7 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>subSeq</c:v>
+            <c:v>sCPT</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
@@ -5499,18 +5602,6 @@
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>6.96333</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>7.07735</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>7.2179900000000004</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>6.6927099999999999</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -5518,6 +5609,52 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-DD42-DD40-80A3-E02A8D4EE55E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>CPT</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Scalability CPT'!$B$10:$E$10</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="4"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-DD42-DD40-80A3-E02A8D4EE55E}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -6166,19 +6303,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>50000</c:v>
+                  <c:v>100000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>100000</c:v>
+                  <c:v>200000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>200000</c:v>
+                  <c:v>400000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>400000</c:v>
+                  <c:v>800000</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>800000</c:v>
+                  <c:v>1600000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6189,21 +6326,6 @@
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>41.591999999999999</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>265.18200000000002</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1355.3979999999999</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>5013.1270000000004</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>19782.670999999998</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -6218,7 +6340,7 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>subSeq</c:v>
+            <c:v>sCPT</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
@@ -6357,19 +6479,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>50000</c:v>
+                  <c:v>100000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>100000</c:v>
+                  <c:v>200000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>200000</c:v>
+                  <c:v>400000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>400000</c:v>
+                  <c:v>800000</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>800000</c:v>
+                  <c:v>1600000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6380,21 +6502,6 @@
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>0.83922300000000005</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.56646</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2.9251100000000001</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>5.9265600000000003</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>12.366899999999999</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -6402,6 +6509,52 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000008-2108-9647-B270-DF955DFD0F2E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>CPT</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Scalability CPT'!$B$13:$F$13</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="5"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000009-2108-9647-B270-DF955DFD0F2E}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -6962,19 +7115,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>50000</c:v>
+                  <c:v>100000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>100000</c:v>
+                  <c:v>200000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>200000</c:v>
+                  <c:v>400000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>400000</c:v>
+                  <c:v>800000</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>800000</c:v>
+                  <c:v>1600000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6985,21 +7138,6 @@
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>5.44</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>5.4720000000000004</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>16.512</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>30.238</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>98.623999999999995</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -7014,7 +7152,7 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>subSeq</c:v>
+            <c:v>sCPT</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
@@ -7215,19 +7353,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>50000</c:v>
+                  <c:v>100000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>100000</c:v>
+                  <c:v>200000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>200000</c:v>
+                  <c:v>400000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>400000</c:v>
+                  <c:v>800000</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>800000</c:v>
+                  <c:v>1600000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7238,21 +7376,6 @@
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>2.7061199999999999</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3.7662900000000001</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>6.4118700000000004</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>9.7641500000000008</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>14.345499999999999</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -7260,6 +7383,52 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000009-582D-434C-8CBA-20DF4D95CEE3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>CPT</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Scalability CPT'!$B$14:$F$14</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="5"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000A-582D-434C-8CBA-20DF4D95CEE3}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -7770,19 +7939,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>50000</c:v>
+                  <c:v>100000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>100000</c:v>
+                  <c:v>200000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>200000</c:v>
+                  <c:v>400000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>400000</c:v>
+                  <c:v>800000</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>800000</c:v>
+                  <c:v>1600000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7793,21 +7962,6 @@
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>6.7569999999999997</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>13.551</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>27.187999999999999</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>54.642000000000003</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>109.44799999999999</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -7822,7 +7976,7 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>subSeq</c:v>
+            <c:v>sCPT</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
@@ -7933,19 +8087,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>50000</c:v>
+                  <c:v>100000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>100000</c:v>
+                  <c:v>200000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>200000</c:v>
+                  <c:v>400000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>400000</c:v>
+                  <c:v>800000</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>800000</c:v>
+                  <c:v>1600000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7956,21 +8110,6 @@
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>1.2015</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2.37825</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4.7284499999999996</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>9.4307200000000009</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>18.892600000000002</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -7978,6 +8117,52 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-26C6-6941-AF0D-D5970E4763F5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>CPT</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Scalability CPT'!$B$15:$F$15</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="5"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-26C6-6941-AF0D-D5970E4763F5}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -15106,7 +15291,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AP34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView topLeftCell="N1" workbookViewId="0">
       <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
@@ -16651,7 +16836,7 @@
     </row>
     <row r="13" spans="1:42" x14ac:dyDescent="0.2">
       <c r="J13" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="P13" t="s">
         <v>64</v>
@@ -16662,12 +16847,12 @@
     </row>
     <row r="14" spans="1:42" x14ac:dyDescent="0.2">
       <c r="J14" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="15" spans="1:42" x14ac:dyDescent="0.2">
       <c r="J15" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="W15" s="5"/>
       <c r="X15" s="5"/>
@@ -16676,7 +16861,7 @@
     </row>
     <row r="16" spans="1:42" x14ac:dyDescent="0.2">
       <c r="J16" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="W16" s="5"/>
       <c r="Y16" s="5"/>
@@ -17142,8 +17327,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0F963C1-4776-254D-AB58-DB95BED4690B}">
   <dimension ref="A1:P29"/>
   <sheetViews>
-    <sheetView zoomScale="119" zoomScaleNormal="142" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView tabSelected="1" zoomScale="119" zoomScaleNormal="142" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -17184,7 +17369,9 @@
       <c r="B2" s="6">
         <v>149638</v>
       </c>
-      <c r="C2" s="7"/>
+      <c r="C2" s="7">
+        <v>2.5106600000000001</v>
+      </c>
       <c r="D2" s="6">
         <v>497</v>
       </c>
@@ -17211,7 +17398,9 @@
       <c r="B3" s="6">
         <v>358278</v>
       </c>
-      <c r="C3" s="7"/>
+      <c r="C3" s="7">
+        <v>4.6222300000000001</v>
+      </c>
       <c r="D3" s="6">
         <v>3340</v>
       </c>
@@ -17237,7 +17426,9 @@
       <c r="B4" s="6">
         <v>558373</v>
       </c>
-      <c r="C4" s="7"/>
+      <c r="C4" s="7">
+        <v>7.9768699999999999</v>
+      </c>
       <c r="D4" s="6">
         <v>21144</v>
       </c>
@@ -17263,7 +17454,9 @@
       <c r="B5" s="6">
         <v>37958</v>
       </c>
-      <c r="C5" s="7"/>
+      <c r="C5" s="7">
+        <v>51.997300000000003</v>
+      </c>
       <c r="D5" s="6">
         <v>267</v>
       </c>
@@ -17289,7 +17482,9 @@
       <c r="B6" s="6">
         <v>787066</v>
       </c>
-      <c r="C6" s="7"/>
+      <c r="C6" s="7">
+        <v>21.641100000000002</v>
+      </c>
       <c r="D6" s="6">
         <v>13905</v>
       </c>
@@ -17315,7 +17510,9 @@
       <c r="B7" s="6">
         <v>197251</v>
       </c>
-      <c r="C7" s="7"/>
+      <c r="C7" s="7">
+        <v>33.810600000000001</v>
+      </c>
       <c r="D7" s="6">
         <v>9025</v>
       </c>
@@ -17341,7 +17538,9 @@
       <c r="B8" s="8">
         <v>423776</v>
       </c>
-      <c r="C8" s="7"/>
+      <c r="C8" s="7">
+        <v>13.330500000000001</v>
+      </c>
       <c r="D8" s="8">
         <v>17</v>
       </c>
@@ -17367,7 +17566,9 @@
       <c r="B9" s="6">
         <v>741092</v>
       </c>
-      <c r="C9" s="7"/>
+      <c r="C9" s="7">
+        <v>36.239199999999997</v>
+      </c>
       <c r="D9" s="6">
         <v>2990</v>
       </c>
@@ -17392,7 +17593,9 @@
       <c r="B10" s="8">
         <v>419621</v>
       </c>
-      <c r="C10" s="7"/>
+      <c r="C10" s="7">
+        <v>5.9327199999999998</v>
+      </c>
       <c r="D10" s="8">
         <v>4018</v>
       </c>
@@ -17417,7 +17620,9 @@
       <c r="B11" s="8">
         <v>569493</v>
       </c>
-      <c r="C11" s="7"/>
+      <c r="C11" s="7">
+        <v>6.4900200000000003</v>
+      </c>
       <c r="D11" s="8">
         <v>4719</v>
       </c>
@@ -17439,244 +17644,261 @@
       <c r="H12" s="12"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A13" s="20" t="s">
+      <c r="A13" s="31" t="s">
         <v>70</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="26">
         <v>4035001</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="26">
         <v>6</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="26">
         <v>475</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="26">
         <v>567538</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="26">
         <v>100</v>
       </c>
-      <c r="H13" s="3">
+      <c r="G13" s="26"/>
+      <c r="H13" s="27">
         <f t="shared" ref="H3:H29" si="1">(_xlfn.CEILING.MATH(LOG(D13, 2)))*(B13)*0.000000125</f>
         <v>4.5393761249999995</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A14" s="20" t="s">
+      <c r="A14" s="31" t="s">
         <v>71</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="26">
         <v>4036466</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="26">
         <v>6</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="26">
         <v>912</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="26">
         <v>567639</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="26">
         <v>100</v>
       </c>
-      <c r="H14" s="3">
+      <c r="G14" s="26"/>
+      <c r="H14" s="27">
         <f t="shared" si="1"/>
         <v>5.0455825000000001</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A15" s="20" t="s">
+      <c r="A15" s="31" t="s">
         <v>72</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="26">
         <v>4036352</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="26">
         <v>6</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="26">
         <v>1307</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="26">
         <v>567812</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="26">
         <v>100</v>
       </c>
-      <c r="H15" s="3">
+      <c r="G15" s="26"/>
+      <c r="H15" s="27">
         <f t="shared" si="1"/>
         <v>5.5499839999999994</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A16" s="20" t="s">
+      <c r="A16" s="31" t="s">
         <v>73</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="26">
         <v>4033355</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="26">
         <v>6</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="26">
         <v>1695</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="26">
         <v>567595</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="26">
         <v>100</v>
       </c>
-      <c r="H16" s="3">
+      <c r="G16" s="26"/>
+      <c r="H16" s="27">
         <f t="shared" si="1"/>
         <v>5.5458631249999994</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A17" s="20" t="s">
+      <c r="A17" s="31" t="s">
         <v>74</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="26">
         <v>4036295</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="26">
         <v>6</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="26">
         <v>2005</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="26">
         <v>567746</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="26">
         <v>100</v>
       </c>
-      <c r="H17" s="3">
+      <c r="G17" s="26"/>
+      <c r="H17" s="27">
         <f t="shared" si="1"/>
         <v>5.5499056250000001</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A18" s="20" t="s">
+      <c r="A18" s="31" t="s">
         <v>75</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="26">
         <v>4035948</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="26">
         <v>6</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="26">
         <v>2313</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="26">
         <v>567988</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="26">
         <v>100</v>
       </c>
-      <c r="H18" s="3">
+      <c r="G18" s="26"/>
+      <c r="H18" s="27">
         <f t="shared" si="1"/>
         <v>6.053922</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="H19" s="3"/>
+      <c r="A19" s="25"/>
+      <c r="B19" s="26"/>
+      <c r="C19" s="26"/>
+      <c r="D19" s="26"/>
+      <c r="E19" s="26"/>
+      <c r="F19" s="26"/>
+      <c r="G19" s="26"/>
+      <c r="H19" s="27"/>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A20" s="18" t="s">
+      <c r="A20" s="25" t="s">
         <v>76</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="26">
         <v>3918478</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="26">
         <v>25</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="26">
         <v>915</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="26">
         <v>150000</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="26">
         <v>100</v>
       </c>
-      <c r="H20" s="3">
+      <c r="G20" s="26"/>
+      <c r="H20" s="27">
         <f t="shared" ref="H20:H23" si="2">(_xlfn.CEILING.MATH(LOG(D20, 2)))*(B20)*0.000000125</f>
         <v>4.8980974999999995</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A21" s="18" t="s">
+      <c r="A21" s="25" t="s">
         <v>77</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="26">
         <v>3983033</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="26">
         <v>12</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="26">
         <v>912</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="26">
         <v>299844</v>
       </c>
-      <c r="F21">
+      <c r="F21" s="26">
         <v>100</v>
       </c>
-      <c r="H21" s="3">
+      <c r="G21" s="26"/>
+      <c r="H21" s="27">
         <f t="shared" si="2"/>
         <v>4.9787912499999996</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A22" s="18" t="s">
+      <c r="A22" s="25" t="s">
         <v>78</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="26">
         <v>4036428</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="26">
         <v>6</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="26">
         <v>912</v>
       </c>
-      <c r="E22">
+      <c r="E22" s="26">
         <v>567639</v>
       </c>
-      <c r="F22">
+      <c r="F22" s="26">
         <v>100</v>
       </c>
-      <c r="H22" s="3">
+      <c r="G22" s="26"/>
+      <c r="H22" s="27">
         <f t="shared" si="2"/>
         <v>5.0455350000000001</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A23" s="18" t="s">
+      <c r="A23" s="25" t="s">
         <v>79</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="26">
         <v>3733343</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="26">
         <v>3</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="26">
         <v>908</v>
       </c>
-      <c r="E23">
+      <c r="E23" s="26">
         <v>872472</v>
       </c>
-      <c r="F23">
+      <c r="F23" s="26">
         <v>100</v>
       </c>
-      <c r="H23" s="3">
+      <c r="G23" s="26"/>
+      <c r="H23" s="27">
         <f t="shared" si="2"/>
         <v>4.66667875</v>
       </c>
@@ -17689,138 +17911,138 @@
       <c r="P24" s="2"/>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A25" s="18" t="s">
+      <c r="A25" s="28" t="s">
         <v>80</v>
       </c>
-      <c r="B25">
-        <v>662696</v>
-      </c>
-      <c r="C25">
+      <c r="B25" s="29">
+        <v>1783405</v>
+      </c>
+      <c r="C25" s="29">
         <v>20</v>
       </c>
-      <c r="D25">
-        <v>910</v>
-      </c>
-      <c r="E25">
-        <v>50000</v>
-      </c>
-      <c r="F25">
-        <v>100</v>
-      </c>
-      <c r="G25">
+      <c r="D25" s="29">
+        <v>917</v>
+      </c>
+      <c r="E25" s="29">
+        <v>100000</v>
+      </c>
+      <c r="F25" s="29">
+        <v>1000</v>
+      </c>
+      <c r="G25" s="29">
         <v>5</v>
       </c>
-      <c r="H25" s="3">
-        <f t="shared" si="1"/>
-        <v>0.82836999999999994</v>
+      <c r="H25" s="30">
+        <f>(_xlfn.CEILING.MATH(LOG(D25 + 1, 2)))*(B25+E25)*0.000000125</f>
+        <v>2.3542562499999997</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A26" s="18" t="s">
+      <c r="A26" s="28" t="s">
         <v>81</v>
       </c>
-      <c r="B26">
-        <v>1327559</v>
-      </c>
-      <c r="C26">
+      <c r="B26" s="29">
+        <v>3565014</v>
+      </c>
+      <c r="C26" s="29">
         <v>20</v>
       </c>
-      <c r="D26">
-        <v>910</v>
-      </c>
-      <c r="E26">
-        <v>100000</v>
-      </c>
-      <c r="F26">
-        <v>100</v>
-      </c>
-      <c r="G26">
+      <c r="D26" s="29">
+        <v>917</v>
+      </c>
+      <c r="E26" s="29">
+        <v>200000</v>
+      </c>
+      <c r="F26" s="29">
+        <v>1000</v>
+      </c>
+      <c r="G26" s="29">
         <v>5</v>
       </c>
-      <c r="H26" s="3">
-        <f t="shared" si="1"/>
-        <v>1.6594487499999999</v>
+      <c r="H26" s="30">
+        <f t="shared" ref="H26:H29" si="3">(_xlfn.CEILING.MATH(LOG(D26 + 1, 2)))*(B26+E26)*0.000000125</f>
+        <v>4.7062675</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A27" s="18" t="s">
+      <c r="A27" s="28" t="s">
         <v>82</v>
       </c>
-      <c r="B27">
-        <v>2655899</v>
-      </c>
-      <c r="C27">
+      <c r="B27" s="29">
+        <v>7129393</v>
+      </c>
+      <c r="C27" s="29">
         <v>20</v>
       </c>
-      <c r="D27">
-        <v>911</v>
-      </c>
-      <c r="E27">
-        <v>200000</v>
-      </c>
-      <c r="F27">
-        <v>100</v>
-      </c>
-      <c r="G27">
+      <c r="D27" s="29">
+        <v>917</v>
+      </c>
+      <c r="E27" s="29">
+        <v>400000</v>
+      </c>
+      <c r="F27" s="29">
+        <v>1000</v>
+      </c>
+      <c r="G27" s="29">
         <v>5</v>
       </c>
-      <c r="H27" s="3">
-        <f t="shared" si="1"/>
-        <v>3.3198737499999997</v>
+      <c r="H27" s="30">
+        <f t="shared" si="3"/>
+        <v>9.4117412500000004</v>
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A28" s="18" t="s">
+      <c r="A28" s="28" t="s">
         <v>83</v>
       </c>
-      <c r="B28">
-        <v>5313658</v>
-      </c>
-      <c r="C28">
+      <c r="B28" s="29">
+        <v>14261856</v>
+      </c>
+      <c r="C28" s="29">
         <v>20</v>
       </c>
-      <c r="D28">
-        <v>915</v>
-      </c>
-      <c r="E28">
-        <v>400000</v>
-      </c>
-      <c r="F28">
-        <v>100</v>
-      </c>
-      <c r="G28">
+      <c r="D28" s="29">
+        <v>917</v>
+      </c>
+      <c r="E28" s="29">
+        <v>800000</v>
+      </c>
+      <c r="F28" s="29">
+        <v>1000</v>
+      </c>
+      <c r="G28" s="29">
         <v>5</v>
       </c>
-      <c r="H28" s="3">
-        <f t="shared" si="1"/>
-        <v>6.6420724999999994</v>
+      <c r="H28" s="30">
+        <f t="shared" si="3"/>
+        <v>18.82732</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A29" s="18" t="s">
-        <v>84</v>
-      </c>
-      <c r="B29">
-        <v>10632846</v>
-      </c>
-      <c r="C29">
+      <c r="A29" s="28" t="s">
+        <v>96</v>
+      </c>
+      <c r="B29" s="29">
+        <v>28525176</v>
+      </c>
+      <c r="C29" s="29">
         <v>20</v>
       </c>
-      <c r="D29">
+      <c r="D29" s="29">
         <v>917</v>
       </c>
-      <c r="E29">
-        <v>800000</v>
-      </c>
-      <c r="F29">
-        <v>100</v>
-      </c>
-      <c r="G29">
+      <c r="E29" s="29">
+        <v>1600000</v>
+      </c>
+      <c r="F29" s="29">
+        <v>1000</v>
+      </c>
+      <c r="G29" s="29">
         <v>5</v>
       </c>
-      <c r="H29" s="3">
-        <f t="shared" si="1"/>
-        <v>13.291057499999999</v>
+      <c r="H29" s="30">
+        <f t="shared" si="3"/>
+        <v>37.656469999999999</v>
       </c>
     </row>
   </sheetData>
@@ -17835,17 +18057,18 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="B12" sqref="B12:F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21.6640625" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="21" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B1" s="21" t="s">
         <v>70</v>
@@ -17868,76 +18091,40 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>86</v>
-      </c>
-      <c r="B2" s="7">
-        <v>3872.21</v>
-      </c>
-      <c r="C2" s="7">
-        <v>4729.8050000000003</v>
-      </c>
-      <c r="D2" s="7">
-        <v>4243.9790000000003</v>
-      </c>
-      <c r="E2" s="7">
-        <v>3765.9119999999998</v>
-      </c>
-      <c r="F2" s="7">
-        <v>3226.8020000000001</v>
-      </c>
-      <c r="G2" s="7">
-        <v>2920.9470000000001</v>
-      </c>
+        <v>85</v>
+      </c>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>87</v>
-      </c>
-      <c r="B3" s="7">
-        <v>2.2850000000000001</v>
-      </c>
-      <c r="C3" s="7">
-        <v>1.046</v>
-      </c>
-      <c r="D3" s="7">
-        <v>0.73699999999999999</v>
-      </c>
-      <c r="E3" s="7">
-        <v>0.69599999999999995</v>
-      </c>
-      <c r="F3" s="7">
-        <v>0.59099999999999997</v>
-      </c>
-      <c r="G3" s="7">
-        <v>0.64100000000000001</v>
-      </c>
+        <v>86</v>
+      </c>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>88</v>
-      </c>
-      <c r="B4" s="7">
-        <v>44.527999999999999</v>
-      </c>
-      <c r="C4" s="7">
-        <v>75.564999999999998</v>
-      </c>
-      <c r="D4" s="7">
-        <v>103.515</v>
-      </c>
-      <c r="E4" s="7">
-        <v>130.916</v>
-      </c>
-      <c r="F4" s="7">
-        <v>152.86799999999999</v>
-      </c>
-      <c r="G4" s="7">
-        <v>174.76599999999999</v>
-      </c>
+        <v>87</v>
+      </c>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
     </row>
     <row r="7" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" s="21" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B7" s="22" t="s">
         <v>76</v>
@@ -17954,58 +18141,34 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>86</v>
-      </c>
-      <c r="B8" s="7">
-        <v>1616.71</v>
-      </c>
-      <c r="C8" s="7">
-        <v>3179.241</v>
-      </c>
-      <c r="D8" s="7">
-        <v>4421.4040000000005</v>
-      </c>
-      <c r="E8" s="7">
-        <v>1882.4839999999999</v>
-      </c>
+        <v>85</v>
+      </c>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>87</v>
-      </c>
-      <c r="B9" s="12">
-        <v>0.96599999999999997</v>
-      </c>
-      <c r="C9" s="12">
-        <v>0.78500000000000003</v>
-      </c>
-      <c r="D9" s="12">
-        <v>1.3879999999999999</v>
-      </c>
-      <c r="E9" s="12">
-        <v>1.4510000000000001</v>
-      </c>
+        <v>86</v>
+      </c>
+      <c r="B9" s="12"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>88</v>
-      </c>
-      <c r="B10" s="7">
-        <v>20.472999999999999</v>
-      </c>
-      <c r="C10" s="7">
-        <v>40.835000000000001</v>
-      </c>
-      <c r="D10" s="7">
-        <v>75.563999999999993</v>
-      </c>
-      <c r="E10" s="7">
-        <v>110.43899999999999</v>
-      </c>
+        <v>87</v>
+      </c>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
     </row>
     <row r="12" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A12" s="23" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B12" s="22" t="s">
         <v>80</v>
@@ -18020,72 +18183,42 @@
         <v>83</v>
       </c>
       <c r="F12" s="22" t="s">
-        <v>84</v>
+        <v>96</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="20" t="s">
-        <v>86</v>
-      </c>
-      <c r="B13" s="7">
-        <v>41.591999999999999</v>
-      </c>
-      <c r="C13" s="7">
-        <v>265.18200000000002</v>
-      </c>
-      <c r="D13" s="7">
-        <v>1355.3979999999999</v>
-      </c>
-      <c r="E13" s="7">
-        <v>5013.1270000000004</v>
-      </c>
-      <c r="F13" s="7">
-        <v>19782.670999999998</v>
-      </c>
+        <v>85</v>
+      </c>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="20" t="s">
-        <v>87</v>
-      </c>
-      <c r="B14" s="7">
-        <v>5.44</v>
-      </c>
-      <c r="C14" s="7">
-        <v>5.4720000000000004</v>
-      </c>
-      <c r="D14" s="7">
-        <v>16.512</v>
-      </c>
-      <c r="E14" s="7">
-        <v>30.238</v>
-      </c>
-      <c r="F14" s="7">
-        <v>98.623999999999995</v>
-      </c>
+        <v>86</v>
+      </c>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="20" t="s">
-        <v>88</v>
-      </c>
-      <c r="B15" s="7">
-        <v>6.7569999999999997</v>
-      </c>
-      <c r="C15" s="7">
-        <v>13.551</v>
-      </c>
-      <c r="D15" s="7">
-        <v>27.187999999999999</v>
-      </c>
-      <c r="E15" s="7">
-        <v>54.642000000000003</v>
-      </c>
-      <c r="F15" s="7">
-        <v>109.44799999999999</v>
-      </c>
+        <v>87</v>
+      </c>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="23" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B18" s="7">
         <v>3</v>
@@ -18099,16 +18232,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="20" t="s">
-        <v>92</v>
-      </c>
-      <c r="B19">
-        <v>0.33200000000000002</v>
-      </c>
-      <c r="C19">
-        <v>0.156</v>
-      </c>
-      <c r="D19">
-        <v>1.258</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -18122,17 +18246,18 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="B12" sqref="B12:F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21.6640625" customWidth="1"/>
+    <col min="6" max="6" width="13.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="21" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B1" s="21" t="s">
         <v>70</v>
@@ -18155,76 +18280,40 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>86</v>
-      </c>
-      <c r="B2" s="7">
-        <v>4.3860700000000001</v>
-      </c>
-      <c r="C2" s="7">
-        <v>4.6304299999999996</v>
-      </c>
-      <c r="D2" s="7">
-        <v>4.5821399999999999</v>
-      </c>
-      <c r="E2" s="7">
-        <v>4.7274099999999999</v>
-      </c>
-      <c r="F2" s="7">
-        <v>4.5145200000000001</v>
-      </c>
-      <c r="G2" s="7">
-        <v>4.5786499999999997</v>
-      </c>
+        <v>85</v>
+      </c>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>87</v>
-      </c>
-      <c r="B3" s="7">
-        <v>0.47705999999999998</v>
-      </c>
-      <c r="C3" s="7">
-        <v>0.70109100000000002</v>
-      </c>
-      <c r="D3" s="7">
-        <v>0.83188799999999996</v>
-      </c>
-      <c r="E3" s="7">
-        <v>0.761154</v>
-      </c>
-      <c r="F3" s="7">
-        <v>1.0216700000000001</v>
-      </c>
-      <c r="G3" s="7">
-        <v>0.97730600000000001</v>
-      </c>
+        <v>86</v>
+      </c>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>88</v>
-      </c>
-      <c r="B4" s="7">
-        <v>6.4744400000000004</v>
-      </c>
-      <c r="C4" s="7">
-        <v>7.2308899999999996</v>
-      </c>
-      <c r="D4" s="7">
-        <v>7.9577400000000003</v>
-      </c>
-      <c r="E4" s="7">
-        <v>7.9333999999999998</v>
-      </c>
-      <c r="F4" s="7">
-        <v>7.9303600000000003</v>
-      </c>
-      <c r="G4" s="7">
-        <v>8.70336</v>
-      </c>
+        <v>87</v>
+      </c>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
     </row>
     <row r="7" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" s="21" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B7" s="22" t="s">
         <v>76</v>
@@ -18241,58 +18330,34 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>86</v>
-      </c>
-      <c r="B8" s="3">
-        <v>4.2885</v>
-      </c>
-      <c r="C8" s="3">
-        <v>4.1141300000000003</v>
-      </c>
-      <c r="D8" s="3">
-        <v>4.2238699999999998</v>
-      </c>
-      <c r="E8" s="3">
-        <v>4.3745700000000003</v>
-      </c>
+        <v>85</v>
+      </c>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>87</v>
-      </c>
-      <c r="B9" s="3">
-        <v>1.0930200000000001</v>
-      </c>
-      <c r="C9" s="3">
-        <v>0.73525399999999996</v>
-      </c>
-      <c r="D9" s="3">
-        <v>0.36714999999999998</v>
-      </c>
-      <c r="E9" s="3">
-        <v>7.2503999999999999E-2</v>
-      </c>
+        <v>86</v>
+      </c>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>88</v>
-      </c>
-      <c r="B10" s="3">
-        <v>6.96333</v>
-      </c>
-      <c r="C10" s="3">
-        <v>7.07735</v>
-      </c>
-      <c r="D10" s="3">
-        <v>7.2179900000000004</v>
-      </c>
-      <c r="E10" s="3">
-        <v>6.6927099999999999</v>
-      </c>
+        <v>87</v>
+      </c>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
     </row>
     <row r="12" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A12" s="23" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B12" s="22" t="s">
         <v>80</v>
@@ -18307,72 +18372,42 @@
         <v>83</v>
       </c>
       <c r="F12" s="22" t="s">
-        <v>84</v>
+        <v>96</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="20" t="s">
-        <v>86</v>
-      </c>
-      <c r="B13" s="7">
-        <v>0.83922300000000005</v>
-      </c>
-      <c r="C13" s="7">
-        <v>1.56646</v>
-      </c>
-      <c r="D13" s="7">
-        <v>2.9251100000000001</v>
-      </c>
-      <c r="E13" s="7">
-        <v>5.9265600000000003</v>
-      </c>
-      <c r="F13" s="7">
-        <v>12.366899999999999</v>
-      </c>
+        <v>85</v>
+      </c>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="20" t="s">
-        <v>87</v>
-      </c>
-      <c r="B14" s="7">
-        <v>2.7061199999999999</v>
-      </c>
-      <c r="C14" s="7">
-        <v>3.7662900000000001</v>
-      </c>
-      <c r="D14" s="7">
-        <v>6.4118700000000004</v>
-      </c>
-      <c r="E14" s="7">
-        <v>9.7641500000000008</v>
-      </c>
-      <c r="F14" s="7">
-        <v>14.345499999999999</v>
-      </c>
+        <v>86</v>
+      </c>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="20" t="s">
-        <v>88</v>
-      </c>
-      <c r="B15" s="7">
-        <v>1.2015</v>
-      </c>
-      <c r="C15" s="7">
-        <v>2.37825</v>
-      </c>
-      <c r="D15" s="7">
-        <v>4.7284499999999996</v>
-      </c>
-      <c r="E15" s="7">
-        <v>9.4307200000000009</v>
-      </c>
-      <c r="F15" s="7">
-        <v>18.892600000000002</v>
-      </c>
+        <v>87</v>
+      </c>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="23" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B18" s="7">
         <v>3</v>
@@ -18386,16 +18421,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="20" t="s">
-        <v>92</v>
-      </c>
-      <c r="B19">
-        <v>5.6391999999999998E-2</v>
-      </c>
-      <c r="C19">
-        <v>0.39711999999999997</v>
-      </c>
-      <c r="D19">
-        <v>1.0847500000000001</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -18409,17 +18435,18 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="B12" sqref="B12:F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21.6640625" customWidth="1"/>
+    <col min="6" max="6" width="16.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="21" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B1" s="21" t="s">
         <v>70</v>
@@ -18442,76 +18469,40 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>86</v>
-      </c>
-      <c r="B2" s="7">
-        <v>4.3860700000000001</v>
-      </c>
-      <c r="C2" s="7">
-        <v>4.6304299999999996</v>
-      </c>
-      <c r="D2" s="7">
-        <v>4.5821399999999999</v>
-      </c>
-      <c r="E2" s="7">
-        <v>4.7274099999999999</v>
-      </c>
-      <c r="F2" s="7">
-        <v>4.5145200000000001</v>
-      </c>
-      <c r="G2" s="7">
-        <v>4.5786499999999997</v>
-      </c>
+        <v>85</v>
+      </c>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>87</v>
-      </c>
-      <c r="B3" s="7">
-        <v>0.47705999999999998</v>
-      </c>
-      <c r="C3" s="7">
-        <v>0.70109100000000002</v>
-      </c>
-      <c r="D3" s="7">
-        <v>0.83188799999999996</v>
-      </c>
-      <c r="E3" s="7">
-        <v>0.761154</v>
-      </c>
-      <c r="F3" s="7">
-        <v>1.0216700000000001</v>
-      </c>
-      <c r="G3" s="7">
-        <v>0.97730600000000001</v>
-      </c>
+        <v>86</v>
+      </c>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>88</v>
-      </c>
-      <c r="B4" s="7">
-        <v>6.4744400000000004</v>
-      </c>
-      <c r="C4" s="7">
-        <v>7.2308899999999996</v>
-      </c>
-      <c r="D4" s="7">
-        <v>7.9577400000000003</v>
-      </c>
-      <c r="E4" s="7">
-        <v>7.9333999999999998</v>
-      </c>
-      <c r="F4" s="7">
-        <v>7.9303600000000003</v>
-      </c>
-      <c r="G4" s="7">
-        <v>8.70336</v>
-      </c>
+        <v>87</v>
+      </c>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
     </row>
     <row r="7" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" s="21" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B7" s="22" t="s">
         <v>76</v>
@@ -18528,58 +18519,34 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>86</v>
-      </c>
-      <c r="B8" s="3">
-        <v>4.2885</v>
-      </c>
-      <c r="C8" s="3">
-        <v>4.1141300000000003</v>
-      </c>
-      <c r="D8" s="3">
-        <v>4.2238699999999998</v>
-      </c>
-      <c r="E8" s="3">
-        <v>4.3745700000000003</v>
-      </c>
+        <v>85</v>
+      </c>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>87</v>
-      </c>
-      <c r="B9" s="3">
-        <v>1.0930200000000001</v>
-      </c>
-      <c r="C9" s="3">
-        <v>0.73525399999999996</v>
-      </c>
-      <c r="D9" s="3">
-        <v>0.36714999999999998</v>
-      </c>
-      <c r="E9" s="3">
-        <v>7.2503999999999999E-2</v>
-      </c>
+        <v>86</v>
+      </c>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>88</v>
-      </c>
-      <c r="B10" s="3">
-        <v>6.96333</v>
-      </c>
-      <c r="C10" s="3">
-        <v>7.07735</v>
-      </c>
-      <c r="D10" s="3">
-        <v>7.2179900000000004</v>
-      </c>
-      <c r="E10" s="3">
-        <v>6.6927099999999999</v>
-      </c>
+        <v>87</v>
+      </c>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
     </row>
     <row r="12" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A12" s="23" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B12" s="22" t="s">
         <v>80</v>
@@ -18594,72 +18561,42 @@
         <v>83</v>
       </c>
       <c r="F12" s="22" t="s">
-        <v>84</v>
+        <v>96</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="20" t="s">
-        <v>86</v>
-      </c>
-      <c r="B13" s="7">
-        <v>0.83922300000000005</v>
-      </c>
-      <c r="C13" s="7">
-        <v>1.56646</v>
-      </c>
-      <c r="D13" s="7">
-        <v>2.9251100000000001</v>
-      </c>
-      <c r="E13" s="7">
-        <v>5.9265600000000003</v>
-      </c>
-      <c r="F13" s="7">
-        <v>12.366899999999999</v>
-      </c>
+        <v>85</v>
+      </c>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="20" t="s">
-        <v>87</v>
-      </c>
-      <c r="B14" s="7">
-        <v>2.7061199999999999</v>
-      </c>
-      <c r="C14" s="7">
-        <v>3.7662900000000001</v>
-      </c>
-      <c r="D14" s="7">
-        <v>6.4118700000000004</v>
-      </c>
-      <c r="E14" s="7">
-        <v>9.7641500000000008</v>
-      </c>
-      <c r="F14" s="7">
-        <v>14.345499999999999</v>
-      </c>
+        <v>86</v>
+      </c>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="20" t="s">
-        <v>88</v>
-      </c>
-      <c r="B15" s="7">
-        <v>1.2015</v>
-      </c>
-      <c r="C15" s="7">
-        <v>2.37825</v>
-      </c>
-      <c r="D15" s="7">
-        <v>4.7284499999999996</v>
-      </c>
-      <c r="E15" s="7">
-        <v>9.4307200000000009</v>
-      </c>
-      <c r="F15" s="7">
-        <v>18.892600000000002</v>
-      </c>
+        <v>87</v>
+      </c>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="23" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B18" s="7">
         <v>3</v>
@@ -18673,16 +18610,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="20" t="s">
-        <v>92</v>
-      </c>
-      <c r="B19">
-        <v>5.6391999999999998E-2</v>
-      </c>
-      <c r="C19">
-        <v>0.39711999999999997</v>
-      </c>
-      <c r="D19">
-        <v>1.0847500000000001</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -18698,8 +18626,8 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A35" zoomScale="75" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView topLeftCell="A67" zoomScale="75" workbookViewId="0">
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Draft calculations in the spreadsheet, a chart was added. Also, have started to export data into Thesis sCPT chapter
</commit_message>
<xml_diff>
--- a/results/cptVSsd_cpt.xlsx
+++ b/results/cptVSsd_cpt.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafaelktistakis/Repositories/C.CPT/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59CA2F3F-8898-A547-9263-872663F6E409}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71F73CFF-6552-D640-BF2B-F2700D18D8EF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="All RAW Data" sheetId="1" r:id="rId1"/>
@@ -19,8 +19,13 @@
     <sheet name="Scalability sCPT" sheetId="4" r:id="rId4"/>
     <sheet name="Scalability CPT" sheetId="6" r:id="rId5"/>
     <sheet name="TBU.Scalability Charts" sheetId="5" r:id="rId6"/>
+    <sheet name="Charts" sheetId="7" r:id="rId7"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId8"/>
+  </externalReferences>
   <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="6">Charts!$B$7:$M$38</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="5">'TBU.Scalability Charts'!$L$92:$V$119</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
@@ -36,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="106">
   <si>
     <t>Trie Node Number</t>
   </si>
@@ -328,6 +333,33 @@
   <si>
     <t>QUEST1600K</t>
   </si>
+  <si>
+    <t>CPT+</t>
+  </si>
+  <si>
+    <t>CPT</t>
+  </si>
+  <si>
+    <t>sCPT_Fast</t>
+  </si>
+  <si>
+    <t>scPT_slow</t>
+  </si>
+  <si>
+    <t>sCPT_Hybrid</t>
+  </si>
+  <si>
+    <t>sCPT-H to CPT+</t>
+  </si>
+  <si>
+    <t>sCPT-F to CPT+</t>
+  </si>
+  <si>
+    <t>sCPT-S to CPT+</t>
+  </si>
+  <si>
+    <t>Draft Calculations</t>
+  </si>
 </sst>
 </file>
 
@@ -412,7 +444,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -427,6 +459,21 @@
       </right>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -459,7 +506,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -496,6 +543,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="6" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="27">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -2040,6 +2096,1118 @@
     <a:p>
       <a:pPr>
         <a:defRPr sz="1200">
+          <a:latin typeface="CMU Concrete Roman" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+          <a:ea typeface="CMU Concrete Roman" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+          <a:cs typeface="CMU Concrete Roman" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>CPT+</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:pattFill prst="pct60">
+              <a:fgClr>
+                <a:schemeClr val="accent1"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="bg1"/>
+              </a:bgClr>
+            </a:pattFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-6.3173770648371807E-3"/>
+                  <c:y val="-3.7894221744520007E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000000-3611-BD49-B087-B03F0D55FF8A}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-4.7380327986278857E-3"/>
+                  <c:y val="-2.5262814496346674E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-3611-BD49-B087-B03F0D55FF8A}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-9.4760655972558287E-3"/>
+                  <c:y val="-4.210469082724445E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-3611-BD49-B087-B03F0D55FF8A}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0"/>
+                  <c:y val="-2.7368049037708893E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000003-3611-BD49-B087-B03F0D55FF8A}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="6"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-5.2118360784906802E-2"/>
+                  <c:y val="4.2104690827244554E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000004-3611-BD49-B087-B03F0D55FF8A}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="8"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-6.3173770648372969E-3"/>
+                  <c:y val="-2.315757995498445E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000005-3611-BD49-B087-B03F0D55FF8A}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="9"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-7.8967213310464756E-3"/>
+                  <c:y val="-4.6315159909968935E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000006-3611-BD49-B087-B03F0D55FF8A}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:numFmt formatCode="#,##0" sourceLinked="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="CMU Concrete Roman" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                    <a:ea typeface="CMU Concrete Roman" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                    <a:cs typeface="CMU Concrete Roman" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'All RAW Data'!$A$2:$A$11</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>BMS1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>BMS2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Kosarak</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>SIGN</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>BIBLE</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>LEVIATHAN</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>MSNB</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>FIFA</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>NASA_08</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>NASA_07</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'All RAW Data'!$AD$2:$AD$11</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>216.71599999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>244.26</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>477.05599999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>203.554</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>343.89400000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100.91200000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>11638.400000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>13694.2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>982.05899999999997</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1163.3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-3611-BD49-B087-B03F0D55FF8A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>sCPT-F</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:pattFill prst="openDmnd">
+              <a:fgClr>
+                <a:schemeClr val="accent2"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="bg1"/>
+              </a:bgClr>
+            </a:pattFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'All RAW Data'!$A$2:$A$11</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>BMS1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>BMS2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Kosarak</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>SIGN</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>BIBLE</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>LEVIATHAN</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>MSNB</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>FIFA</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>NASA_08</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>NASA_07</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'All RAW Data'!$AF$2:$AF$11</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>217.60999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>179.19</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>521.05000000000007</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>310.65999999999997</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>418.46</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>123.05000000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>11813.1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>17878.2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1091.5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1453.8999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000008-3611-BD49-B087-B03F0D55FF8A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>sCPT-H</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="1.1055409863465038E-2"/>
+                  <c:y val="-2.5262814496346712E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000009-3611-BD49-B087-B03F0D55FF8A}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="1.1055409863465067E-2"/>
+                  <c:y val="-2.1052345413622227E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000A-3611-BD49-B087-B03F0D55FF8A}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="3.1586885324185903E-3"/>
+                  <c:y val="-5.2630863534055564E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000B-3611-BD49-B087-B03F0D55FF8A}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="6"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-3.3166229590395196E-2"/>
+                  <c:y val="-4.6315159909968907E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000C-3611-BD49-B087-B03F0D55FF8A}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="7"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="3.6324918122813674E-2"/>
+                  <c:y val="-2.9473283579071127E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000D-3611-BD49-B087-B03F0D55FF8A}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="8"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.1055409863465067E-2"/>
+                  <c:y val="-8.2104147113126691E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000E-3611-BD49-B087-B03F0D55FF8A}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="9"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="4.7380327986278857E-3"/>
+                  <c:y val="-8.4209381654488921E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000F-3611-BD49-B087-B03F0D55FF8A}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="CMU Concrete Roman" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                    <a:ea typeface="CMU Concrete Roman" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                    <a:cs typeface="CMU Concrete Roman" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>'All RAW Data'!$AJ$2:$AJ$11</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>218.67000000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>183.73000000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>530.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>316.97999999999996</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>409.16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>122.53999999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>11245.300000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>17973.400000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1093.3900000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1445.73</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000010-3611-BD49-B087-B03F0D55FF8A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>sCPT-S</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill flip="none" rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="5000"/>
+                    <a:lumOff val="95000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="45000">
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="45000"/>
+                    <a:lumOff val="55000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="83000">
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="45000"/>
+                    <a:lumOff val="55000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="30000"/>
+                    <a:lumOff val="70000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="16200000" scaled="1"/>
+              <a:tileRect/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'All RAW Data'!$AH$2:$AH$11</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>273.95999999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>267.19</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1407.36</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>325.85999999999996</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2110.44</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>137.25</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>47792.200000000004</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>24385.200000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3429.22</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4756.7199999999993</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000011-3611-BD49-B087-B03F0D55FF8A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1087849711"/>
+        <c:axId val="1021367279"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1087849711"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="CMU Concrete Roman" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                    <a:ea typeface="CMU Concrete Roman" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                    <a:cs typeface="CMU Concrete Roman" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Datasets</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="CMU Concrete Roman" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                  <a:ea typeface="CMU Concrete Roman" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                  <a:cs typeface="CMU Concrete Roman" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="CMU Concrete Roman" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                <a:ea typeface="CMU Concrete Roman" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                <a:cs typeface="CMU Concrete Roman" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1021367279"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1021367279"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="CMU Concrete Roman" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                    <a:ea typeface="CMU Concrete Roman" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                    <a:cs typeface="CMU Concrete Roman" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time (ms)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="CMU Concrete Roman" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                  <a:ea typeface="CMU Concrete Roman" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                  <a:cs typeface="CMU Concrete Roman" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="CMU Concrete Roman" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                <a:ea typeface="CMU Concrete Roman" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                <a:cs typeface="CMU Concrete Roman" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1087849711"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="CMU Concrete Roman" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+              <a:ea typeface="CMU Concrete Roman" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+              <a:cs typeface="CMU Concrete Roman" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1600">
           <a:latin typeface="CMU Concrete Roman" panose="02000603000000000000" pitchFamily="2" charset="0"/>
           <a:ea typeface="CMU Concrete Roman" panose="02000603000000000000" pitchFamily="2" charset="0"/>
           <a:cs typeface="CMU Concrete Roman" panose="02000603000000000000" pitchFamily="2" charset="0"/>
@@ -8560,6 +9728,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors11.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -9385,6 +10593,509 @@
 
 <file path=xl/charts/style10.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style11.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -14295,6 +16006,166 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>611812</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>139782</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DD8CD7BA-2E25-7C45-9947-E5E3F23F30F6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Accuracy %"/>
+      <sheetName val="Execution Time per Query (μs)"/>
+      <sheetName val="Exec. Time of Test Phase (ms)"/>
+      <sheetName val="Memory (MB)"/>
+      <sheetName val="Memory - Input Ratio"/>
+      <sheetName val="Datasets Attributes, Notes"/>
+      <sheetName val="Scalability CPT+"/>
+      <sheetName val="Scalability subSeq"/>
+      <sheetName val="Scalability Charts"/>
+      <sheetName val="Performance Charts"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1">
+        <row r="1">
+          <cell r="D1" t="str">
+            <v>CPT+</v>
+          </cell>
+          <cell r="F1" t="str">
+            <v>subSeq</v>
+          </cell>
+        </row>
+        <row r="2">
+          <cell r="A2" t="str">
+            <v>BMS</v>
+          </cell>
+          <cell r="D2">
+            <v>393.37175792507207</v>
+          </cell>
+          <cell r="F2">
+            <v>233.4293948126801</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="A3" t="str">
+            <v>SIGN</v>
+          </cell>
+          <cell r="D3">
+            <v>623.46153846153857</v>
+          </cell>
+          <cell r="F3">
+            <v>2250</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="A4" t="str">
+            <v>MSNBC</v>
+          </cell>
+          <cell r="D4">
+            <v>139.21568627450981</v>
+          </cell>
+          <cell r="F4">
+            <v>58.823529411764703</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="A5" t="str">
+            <v>BIBLE_WORD</v>
+          </cell>
+          <cell r="D5">
+            <v>197.21590909090912</v>
+          </cell>
+          <cell r="F5">
+            <v>267.0454545454545</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="A6" t="str">
+            <v>BIBLE_CHAR</v>
+          </cell>
+          <cell r="D6">
+            <v>43.977591036414559</v>
+          </cell>
+          <cell r="F6">
+            <v>44.817927170868344</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="A7" t="str">
+            <v>KOSARAK</v>
+          </cell>
+          <cell r="D7">
+            <v>1863.72121966397</v>
+          </cell>
+          <cell r="F7">
+            <v>10295.270690728064</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="A8" t="str">
+            <v>FIFA</v>
+          </cell>
+          <cell r="D8">
+            <v>183.6901408450704</v>
+          </cell>
+          <cell r="F8">
+            <v>498.59154929577466</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="6" refreshError="1"/>
+      <sheetData sheetId="7" refreshError="1"/>
+      <sheetData sheetId="8" refreshError="1"/>
+      <sheetData sheetId="9" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -14558,10 +16429,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AP34"/>
+  <dimension ref="A1:AP70"/>
   <sheetViews>
-    <sheetView topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="E49" sqref="E49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -16581,10 +18452,552 @@
         <v>36</v>
       </c>
     </row>
-    <row r="34" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D34" t="s">
         <v>59</v>
       </c>
+    </row>
+    <row r="42" spans="4:13" x14ac:dyDescent="0.2">
+      <c r="F42" s="32" t="s">
+        <v>105</v>
+      </c>
+      <c r="G42" s="32"/>
+      <c r="H42" s="32"/>
+      <c r="I42" s="32"/>
+      <c r="J42" s="32"/>
+      <c r="K42" s="32"/>
+      <c r="L42" s="32"/>
+      <c r="M42" s="32"/>
+    </row>
+    <row r="43" spans="4:13" x14ac:dyDescent="0.2">
+      <c r="F43" s="32"/>
+      <c r="G43" s="32"/>
+      <c r="H43" s="32"/>
+      <c r="I43" s="32"/>
+      <c r="J43" s="32"/>
+      <c r="K43" s="32"/>
+      <c r="L43" s="32"/>
+      <c r="M43" s="32"/>
+    </row>
+    <row r="44" spans="4:13" x14ac:dyDescent="0.2">
+      <c r="F44" s="32"/>
+      <c r="G44" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="H44" s="32" t="s">
+        <v>101</v>
+      </c>
+      <c r="I44" s="32" t="s">
+        <v>99</v>
+      </c>
+      <c r="J44" s="32" t="s">
+        <v>100</v>
+      </c>
+      <c r="K44" s="32" t="s">
+        <v>97</v>
+      </c>
+      <c r="L44" s="33" t="s">
+        <v>98</v>
+      </c>
+      <c r="M44" s="32"/>
+    </row>
+    <row r="45" spans="4:13" x14ac:dyDescent="0.2">
+      <c r="F45" s="32"/>
+      <c r="G45" s="34" t="s">
+        <v>2</v>
+      </c>
+      <c r="H45" s="35">
+        <v>218.67000000000002</v>
+      </c>
+      <c r="I45" s="36">
+        <v>217.60999999999999</v>
+      </c>
+      <c r="J45" s="36">
+        <v>273.95999999999998</v>
+      </c>
+      <c r="K45" s="37">
+        <v>216.71599999999998</v>
+      </c>
+      <c r="L45" s="35">
+        <v>213.28299999999999</v>
+      </c>
+      <c r="M45" s="32"/>
+    </row>
+    <row r="46" spans="4:13" x14ac:dyDescent="0.2">
+      <c r="F46" s="32"/>
+      <c r="G46" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="H46" s="35">
+        <v>183.73000000000002</v>
+      </c>
+      <c r="I46" s="36">
+        <v>179.19</v>
+      </c>
+      <c r="J46" s="36">
+        <v>267.19</v>
+      </c>
+      <c r="K46" s="37">
+        <v>244.26</v>
+      </c>
+      <c r="L46" s="35">
+        <v>244.25200000000001</v>
+      </c>
+      <c r="M46" s="32"/>
+    </row>
+    <row r="47" spans="4:13" x14ac:dyDescent="0.2">
+      <c r="F47" s="32"/>
+      <c r="G47" s="34" t="s">
+        <v>16</v>
+      </c>
+      <c r="H47" s="35">
+        <v>530.5</v>
+      </c>
+      <c r="I47" s="36">
+        <v>521.05000000000007</v>
+      </c>
+      <c r="J47" s="36">
+        <v>1407.36</v>
+      </c>
+      <c r="K47" s="37">
+        <v>477.05599999999998</v>
+      </c>
+      <c r="L47" s="35">
+        <v>465.22</v>
+      </c>
+      <c r="M47" s="32"/>
+    </row>
+    <row r="48" spans="4:13" x14ac:dyDescent="0.2">
+      <c r="F48" s="32"/>
+      <c r="G48" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="H48" s="35">
+        <v>316.97999999999996</v>
+      </c>
+      <c r="I48" s="36">
+        <v>310.65999999999997</v>
+      </c>
+      <c r="J48" s="36">
+        <v>325.85999999999996</v>
+      </c>
+      <c r="K48" s="37">
+        <v>203.554</v>
+      </c>
+      <c r="L48" s="35">
+        <v>161.61800000000002</v>
+      </c>
+      <c r="M48" s="32"/>
+    </row>
+    <row r="49" spans="6:13" x14ac:dyDescent="0.2">
+      <c r="F49" s="32"/>
+      <c r="G49" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="H49" s="35">
+        <v>409.16</v>
+      </c>
+      <c r="I49" s="36">
+        <v>418.46</v>
+      </c>
+      <c r="J49" s="36">
+        <v>2110.44</v>
+      </c>
+      <c r="K49" s="37">
+        <v>343.89400000000001</v>
+      </c>
+      <c r="L49" s="35">
+        <v>271.78699999999998</v>
+      </c>
+      <c r="M49" s="32"/>
+    </row>
+    <row r="50" spans="6:13" x14ac:dyDescent="0.2">
+      <c r="F50" s="32"/>
+      <c r="G50" s="34" t="s">
+        <v>8</v>
+      </c>
+      <c r="H50" s="35">
+        <v>122.53999999999999</v>
+      </c>
+      <c r="I50" s="36">
+        <v>123.05000000000001</v>
+      </c>
+      <c r="J50" s="36">
+        <v>137.25</v>
+      </c>
+      <c r="K50" s="37">
+        <v>100.91200000000001</v>
+      </c>
+      <c r="L50" s="35">
+        <v>85.619</v>
+      </c>
+      <c r="M50" s="32"/>
+    </row>
+    <row r="51" spans="6:13" x14ac:dyDescent="0.2">
+      <c r="F51" s="32"/>
+      <c r="G51" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="H51" s="35">
+        <v>11245.300000000001</v>
+      </c>
+      <c r="I51" s="36">
+        <v>11813.1</v>
+      </c>
+      <c r="J51" s="36">
+        <v>47792.200000000004</v>
+      </c>
+      <c r="K51" s="37">
+        <v>11638.400000000001</v>
+      </c>
+      <c r="L51" s="35">
+        <v>6594.35</v>
+      </c>
+      <c r="M51" s="32"/>
+    </row>
+    <row r="52" spans="6:13" x14ac:dyDescent="0.2">
+      <c r="F52" s="32"/>
+      <c r="G52" s="34" t="s">
+        <v>6</v>
+      </c>
+      <c r="H52" s="35">
+        <v>17973.400000000001</v>
+      </c>
+      <c r="I52" s="36">
+        <v>17878.2</v>
+      </c>
+      <c r="J52" s="36">
+        <v>24385.200000000001</v>
+      </c>
+      <c r="K52" s="37">
+        <v>13694.2</v>
+      </c>
+      <c r="L52" s="35">
+        <v>10074</v>
+      </c>
+      <c r="M52" s="32"/>
+    </row>
+    <row r="53" spans="6:13" x14ac:dyDescent="0.2">
+      <c r="F53" s="32"/>
+      <c r="G53" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="H53" s="35">
+        <v>1093.3900000000001</v>
+      </c>
+      <c r="I53" s="36">
+        <v>1091.5</v>
+      </c>
+      <c r="J53" s="36">
+        <v>3429.22</v>
+      </c>
+      <c r="K53" s="37">
+        <v>982.05899999999997</v>
+      </c>
+      <c r="L53" s="35">
+        <v>627.42600000000004</v>
+      </c>
+      <c r="M53" s="32"/>
+    </row>
+    <row r="54" spans="6:13" x14ac:dyDescent="0.2">
+      <c r="F54" s="32"/>
+      <c r="G54" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="H54" s="35">
+        <v>1445.73</v>
+      </c>
+      <c r="I54" s="36">
+        <v>1453.8999999999999</v>
+      </c>
+      <c r="J54" s="36">
+        <v>4756.7199999999993</v>
+      </c>
+      <c r="K54" s="37">
+        <v>1163.3</v>
+      </c>
+      <c r="L54" s="35">
+        <v>831.09500000000003</v>
+      </c>
+      <c r="M54" s="32"/>
+    </row>
+    <row r="55" spans="6:13" x14ac:dyDescent="0.2">
+      <c r="F55" s="32"/>
+      <c r="G55" s="32"/>
+      <c r="H55" s="32"/>
+      <c r="I55" s="32"/>
+      <c r="J55" s="32"/>
+      <c r="K55" s="32"/>
+      <c r="L55" s="32"/>
+      <c r="M55" s="32"/>
+    </row>
+    <row r="56" spans="6:13" x14ac:dyDescent="0.2">
+      <c r="F56" s="32"/>
+      <c r="G56" s="32"/>
+      <c r="H56" s="32"/>
+      <c r="I56" s="32"/>
+      <c r="J56" s="32"/>
+      <c r="K56" s="32"/>
+      <c r="L56" s="32"/>
+      <c r="M56" s="32"/>
+    </row>
+    <row r="57" spans="6:13" x14ac:dyDescent="0.2">
+      <c r="F57" s="32"/>
+      <c r="G57" s="32"/>
+      <c r="H57" s="32"/>
+      <c r="I57" s="32"/>
+      <c r="J57" s="32"/>
+      <c r="K57" s="32"/>
+      <c r="L57" s="32"/>
+      <c r="M57" s="32"/>
+    </row>
+    <row r="58" spans="6:13" x14ac:dyDescent="0.2">
+      <c r="F58" s="32"/>
+      <c r="G58" s="32"/>
+      <c r="H58" s="32"/>
+      <c r="I58" s="32"/>
+      <c r="J58" s="32"/>
+      <c r="K58" s="32"/>
+      <c r="L58" s="32"/>
+      <c r="M58" s="32"/>
+    </row>
+    <row r="59" spans="6:13" x14ac:dyDescent="0.2">
+      <c r="F59" s="32"/>
+      <c r="G59" s="32"/>
+      <c r="H59" s="32"/>
+      <c r="I59" s="32"/>
+      <c r="J59" s="32"/>
+      <c r="K59" s="32"/>
+      <c r="L59" s="32"/>
+      <c r="M59" s="32"/>
+    </row>
+    <row r="60" spans="6:13" x14ac:dyDescent="0.2">
+      <c r="F60" s="32"/>
+      <c r="G60" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="H60" s="32" t="s">
+        <v>102</v>
+      </c>
+      <c r="I60" s="32" t="s">
+        <v>103</v>
+      </c>
+      <c r="J60" s="32" t="s">
+        <v>104</v>
+      </c>
+      <c r="K60" s="32"/>
+      <c r="L60" s="33"/>
+      <c r="M60" s="32"/>
+    </row>
+    <row r="61" spans="6:13" x14ac:dyDescent="0.2">
+      <c r="F61" s="32"/>
+      <c r="G61" s="34" t="s">
+        <v>2</v>
+      </c>
+      <c r="H61" s="39">
+        <f>H45/K45</f>
+        <v>1.0090164085715869</v>
+      </c>
+      <c r="I61" s="40">
+        <f>I45/K45</f>
+        <v>1.0041252145665296</v>
+      </c>
+      <c r="J61" s="40">
+        <f>J45/K45</f>
+        <v>1.2641429336089629</v>
+      </c>
+      <c r="K61" s="37"/>
+      <c r="L61" s="35"/>
+      <c r="M61" s="32"/>
+    </row>
+    <row r="62" spans="6:13" x14ac:dyDescent="0.2">
+      <c r="F62" s="32"/>
+      <c r="G62" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="H62" s="39">
+        <f t="shared" ref="H62:H70" si="18">H46/K46</f>
+        <v>0.75219028903627294</v>
+      </c>
+      <c r="I62" s="40">
+        <f t="shared" ref="I62:I70" si="19">I46/K46</f>
+        <v>0.7336035372144436</v>
+      </c>
+      <c r="J62" s="40">
+        <f t="shared" ref="J62:J70" si="20">J46/K46</f>
+        <v>1.0938753786948334</v>
+      </c>
+      <c r="K62" s="37"/>
+      <c r="L62" s="35"/>
+      <c r="M62" s="32"/>
+    </row>
+    <row r="63" spans="6:13" x14ac:dyDescent="0.2">
+      <c r="F63" s="32"/>
+      <c r="G63" s="34" t="s">
+        <v>16</v>
+      </c>
+      <c r="H63" s="39">
+        <f t="shared" si="18"/>
+        <v>1.1120287764958412</v>
+      </c>
+      <c r="I63" s="40">
+        <f t="shared" si="19"/>
+        <v>1.092219781325463</v>
+      </c>
+      <c r="J63" s="40">
+        <f t="shared" si="20"/>
+        <v>2.950093909310437</v>
+      </c>
+      <c r="K63" s="37"/>
+      <c r="L63" s="35"/>
+      <c r="M63" s="32"/>
+    </row>
+    <row r="64" spans="6:13" x14ac:dyDescent="0.2">
+      <c r="F64" s="32"/>
+      <c r="G64" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="H64" s="39">
+        <f t="shared" si="18"/>
+        <v>1.5572280574196526</v>
+      </c>
+      <c r="I64" s="40">
+        <f t="shared" si="19"/>
+        <v>1.5261797852166992</v>
+      </c>
+      <c r="J64" s="40">
+        <f t="shared" si="20"/>
+        <v>1.6008528449453214</v>
+      </c>
+      <c r="K64" s="37"/>
+      <c r="L64" s="35"/>
+      <c r="M64" s="32"/>
+    </row>
+    <row r="65" spans="6:13" x14ac:dyDescent="0.2">
+      <c r="F65" s="32"/>
+      <c r="G65" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="H65" s="39">
+        <f t="shared" si="18"/>
+        <v>1.189785224516857</v>
+      </c>
+      <c r="I65" s="40">
+        <f t="shared" si="19"/>
+        <v>1.2168284413220352</v>
+      </c>
+      <c r="J65" s="40">
+        <f t="shared" si="20"/>
+        <v>6.1368910187441479</v>
+      </c>
+      <c r="K65" s="37"/>
+      <c r="L65" s="35"/>
+      <c r="M65" s="32"/>
+    </row>
+    <row r="66" spans="6:13" x14ac:dyDescent="0.2">
+      <c r="F66" s="32"/>
+      <c r="G66" s="34" t="s">
+        <v>8</v>
+      </c>
+      <c r="H66" s="39">
+        <f t="shared" si="18"/>
+        <v>1.2143253527826223</v>
+      </c>
+      <c r="I66" s="40">
+        <f t="shared" si="19"/>
+        <v>1.2193792611384178</v>
+      </c>
+      <c r="J66" s="40">
+        <f t="shared" si="20"/>
+        <v>1.3600959251625178</v>
+      </c>
+      <c r="K66" s="37"/>
+      <c r="L66" s="35"/>
+      <c r="M66" s="32"/>
+    </row>
+    <row r="67" spans="6:13" x14ac:dyDescent="0.2">
+      <c r="F67" s="32"/>
+      <c r="G67" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="H67" s="39">
+        <f t="shared" si="18"/>
+        <v>0.96622387957107503</v>
+      </c>
+      <c r="I67" s="40">
+        <f t="shared" si="19"/>
+        <v>1.0150106543854824</v>
+      </c>
+      <c r="J67" s="40">
+        <f t="shared" si="20"/>
+        <v>4.106423563376409</v>
+      </c>
+      <c r="K67" s="37"/>
+      <c r="L67" s="35"/>
+      <c r="M67" s="32"/>
+    </row>
+    <row r="68" spans="6:13" x14ac:dyDescent="0.2">
+      <c r="F68" s="32"/>
+      <c r="G68" s="34" t="s">
+        <v>6</v>
+      </c>
+      <c r="H68" s="39">
+        <f t="shared" si="18"/>
+        <v>1.3124826568912387</v>
+      </c>
+      <c r="I68" s="40">
+        <f t="shared" si="19"/>
+        <v>1.3055308086635218</v>
+      </c>
+      <c r="J68" s="40">
+        <f t="shared" si="20"/>
+        <v>1.780695476917235</v>
+      </c>
+      <c r="K68" s="37"/>
+      <c r="L68" s="35"/>
+      <c r="M68" s="32"/>
+    </row>
+    <row r="69" spans="6:13" x14ac:dyDescent="0.2">
+      <c r="F69" s="32"/>
+      <c r="G69" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="H69" s="39">
+        <f t="shared" si="18"/>
+        <v>1.1133648792995128</v>
+      </c>
+      <c r="I69" s="40">
+        <f t="shared" si="19"/>
+        <v>1.111440351343453</v>
+      </c>
+      <c r="J69" s="40">
+        <f t="shared" si="20"/>
+        <v>3.4918675965496981</v>
+      </c>
+      <c r="K69" s="37"/>
+      <c r="L69" s="35"/>
+      <c r="M69" s="32"/>
+    </row>
+    <row r="70" spans="6:13" x14ac:dyDescent="0.2">
+      <c r="F70" s="32"/>
+      <c r="G70" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="H70" s="39">
+        <f t="shared" si="18"/>
+        <v>1.2427834608441504</v>
+      </c>
+      <c r="I70" s="40">
+        <f t="shared" si="19"/>
+        <v>1.2498065847158943</v>
+      </c>
+      <c r="J70" s="40">
+        <f t="shared" si="20"/>
+        <v>4.0889882231582559</v>
+      </c>
+      <c r="K70" s="37"/>
+      <c r="L70" s="35"/>
+      <c r="M70" s="32"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -16596,8 +19009,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0F963C1-4776-254D-AB58-DB95BED4690B}">
   <dimension ref="A1:P29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="119" zoomScaleNormal="142" workbookViewId="0">
-      <selection activeCell="J44" sqref="J44"/>
+    <sheetView zoomScale="119" zoomScaleNormal="142" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -17908,7 +20321,7 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A67" zoomScale="75" workbookViewId="0">
+    <sheetView topLeftCell="A18" zoomScale="75" workbookViewId="0">
       <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
@@ -17918,4 +20331,20 @@
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B007799-6C31-A447-9B6F-EA553D67BBB0}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7:M38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Organising previous II implementations results into the C.CPT cetral results spreadsheet
</commit_message>
<xml_diff>
--- a/results/cptVSsd_cpt.xlsx
+++ b/results/cptVSsd_cpt.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafaelktistakis/Repositories/C.CPT/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05DCC875-23B0-884B-8715-A039070A8602}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7878F905-F628-2140-B83B-5126A45A1AD5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" tabRatio="500" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" tabRatio="500" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="All RAW Data" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="Scalability Charts" sheetId="5" r:id="rId6"/>
     <sheet name="Charts" sheetId="7" r:id="rId7"/>
     <sheet name="Scalability LATEX" sheetId="8" r:id="rId8"/>
+    <sheet name="II Implementations" sheetId="9" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="6">Charts!$B$7:$M$38</definedName>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="126">
   <si>
     <t>Trie Node Number</t>
   </si>
@@ -333,21 +334,6 @@
     <t>QUEST1600K</t>
   </si>
   <si>
-    <t>CPT+</t>
-  </si>
-  <si>
-    <t>CPT</t>
-  </si>
-  <si>
-    <t>sCPT_Fast</t>
-  </si>
-  <si>
-    <t>scPT_slow</t>
-  </si>
-  <si>
-    <t>sCPT_Hybrid</t>
-  </si>
-  <si>
     <t>sCPT-H to CPT+</t>
   </si>
   <si>
@@ -359,6 +345,84 @@
   <si>
     <t>Draft Calculations</t>
   </si>
+  <si>
+    <t>CPTPlus to sCPT</t>
+  </si>
+  <si>
+    <t>II</t>
+  </si>
+  <si>
+    <t>sII</t>
+  </si>
+  <si>
+    <t>sII+Dict</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alphabet size: 1000 +Sequence Length: 20 +Transaction Length: 1 +Sequence Number: Variable </t>
+  </si>
+  <si>
+    <t>Exported queries (~9 items) through CPT+ execution during its II usage</t>
+  </si>
+  <si>
+    <t>Time Results (sec)</t>
+  </si>
+  <si>
+    <t>Number of Sequences</t>
+  </si>
+  <si>
+    <t>RAW</t>
+  </si>
+  <si>
+    <t>SMBT</t>
+  </si>
+  <si>
+    <t>RRR</t>
+  </si>
+  <si>
+    <t>RRR-selective</t>
+  </si>
+  <si>
+    <t>WAH 64</t>
+  </si>
+  <si>
+    <t>WAH 32</t>
+  </si>
+  <si>
+    <t>WT</t>
+  </si>
+  <si>
+    <t>Elias -Fano</t>
+  </si>
+  <si>
+    <t>Elias -Fano 256</t>
+  </si>
+  <si>
+    <t>Elias-Fano128</t>
+  </si>
+  <si>
+    <t>Elias-Fano 64</t>
+  </si>
+  <si>
+    <t>BV+Helper 64</t>
+  </si>
+  <si>
+    <t>BV+Helper 32</t>
+  </si>
+  <si>
+    <t>BV+Helper 16</t>
+  </si>
+  <si>
+    <t>Memory (Bytes)</t>
+  </si>
+  <si>
+    <t>RESULTS WERE COPIED OVER HERE</t>
+  </si>
+  <si>
+    <t>Original file in iCloud (numbers file): IIs execution time Analysis with CPT+ queries</t>
+  </si>
 </sst>
 </file>
 
@@ -369,7 +433,7 @@
     <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="0.000000"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -424,6 +488,20 @@
       <b/>
       <sz val="12"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -505,7 +583,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -537,7 +615,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="6" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -560,6 +637,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="27">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -31529,8 +31610,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AP70"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="E49" sqref="E49"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D56" sqref="D56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -33550,14 +33631,14 @@
         <v>36</v>
       </c>
     </row>
-    <row r="34" spans="4:13" x14ac:dyDescent="0.2">
+    <row r="34" spans="4:15" x14ac:dyDescent="0.2">
       <c r="D34" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="42" spans="4:13" x14ac:dyDescent="0.2">
+    <row r="42" spans="4:15" x14ac:dyDescent="0.2">
       <c r="F42" s="25" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="G42" s="25"/>
       <c r="H42" s="25"/>
@@ -33567,7 +33648,7 @@
       <c r="L42" s="25"/>
       <c r="M42" s="25"/>
     </row>
-    <row r="43" spans="4:13" x14ac:dyDescent="0.2">
+    <row r="43" spans="4:15" x14ac:dyDescent="0.2">
       <c r="F43" s="25"/>
       <c r="G43" s="25"/>
       <c r="H43" s="25"/>
@@ -33576,250 +33657,262 @@
       <c r="K43" s="25"/>
       <c r="L43" s="25"/>
       <c r="M43" s="25"/>
+      <c r="N43" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="O43" s="25" t="s">
+        <v>101</v>
+      </c>
     </row>
-    <row r="44" spans="4:13" x14ac:dyDescent="0.2">
+    <row r="44" spans="4:15" x14ac:dyDescent="0.2">
       <c r="F44" s="25"/>
       <c r="G44" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="H44" s="25" t="s">
-        <v>101</v>
-      </c>
-      <c r="I44" s="25" t="s">
-        <v>99</v>
+      <c r="H44" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="I44" s="19" t="s">
+        <v>103</v>
       </c>
       <c r="J44" s="25" t="s">
-        <v>100</v>
-      </c>
-      <c r="K44" s="25" t="s">
-        <v>97</v>
-      </c>
-      <c r="L44" s="26" t="s">
-        <v>98</v>
-      </c>
+        <v>104</v>
+      </c>
+      <c r="K44" s="25"/>
+      <c r="L44" s="26"/>
       <c r="M44" s="25"/>
+      <c r="N44" s="27"/>
+      <c r="O44" s="29"/>
     </row>
-    <row r="45" spans="4:13" x14ac:dyDescent="0.2">
+    <row r="45" spans="4:15" x14ac:dyDescent="0.2">
       <c r="F45" s="25"/>
       <c r="G45" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="H45" s="28">
-        <v>218.67000000000002</v>
-      </c>
-      <c r="I45" s="29">
-        <v>217.60999999999999</v>
-      </c>
-      <c r="J45" s="29">
-        <v>273.95999999999998</v>
-      </c>
-      <c r="K45" s="30">
-        <v>216.71599999999998</v>
-      </c>
-      <c r="L45" s="28">
-        <v>213.28299999999999</v>
-      </c>
+      <c r="H45" s="49">
+        <f>J2/I2</f>
+        <v>15.169337905539091</v>
+      </c>
+      <c r="I45" s="49">
+        <f>K2/I2</f>
+        <v>0.66423040629570007</v>
+      </c>
+      <c r="J45" s="50">
+        <f>(K2+M2+N2)/I2</f>
+        <v>0.95126976826851128</v>
+      </c>
+      <c r="K45" s="29"/>
+      <c r="L45" s="28"/>
       <c r="M45" s="25"/>
+      <c r="N45" s="27"/>
+      <c r="O45" s="29"/>
     </row>
-    <row r="46" spans="4:13" x14ac:dyDescent="0.2">
+    <row r="46" spans="4:15" x14ac:dyDescent="0.2">
       <c r="F46" s="25"/>
       <c r="G46" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="H46" s="28">
-        <v>183.73000000000002</v>
-      </c>
-      <c r="I46" s="29">
-        <v>179.19</v>
-      </c>
-      <c r="J46" s="29">
-        <v>267.19</v>
-      </c>
-      <c r="K46" s="30">
-        <v>244.26</v>
-      </c>
-      <c r="L46" s="28">
-        <v>244.25200000000001</v>
-      </c>
+      <c r="H46" s="49">
+        <f t="shared" ref="H46:H54" si="18">J3/I3</f>
+        <v>47.71495803279533</v>
+      </c>
+      <c r="I46" s="49">
+        <f t="shared" ref="I46:I54" si="19">K3/I3</f>
+        <v>0.75098093519852671</v>
+      </c>
+      <c r="J46" s="50">
+        <f t="shared" ref="J46:J54" si="20">(K3+M3+N3)/I3</f>
+        <v>1.3427899210927237</v>
+      </c>
+      <c r="K46" s="29"/>
+      <c r="L46" s="28"/>
       <c r="M46" s="25"/>
+      <c r="N46" s="27"/>
+      <c r="O46" s="29"/>
     </row>
-    <row r="47" spans="4:13" x14ac:dyDescent="0.2">
+    <row r="47" spans="4:15" x14ac:dyDescent="0.2">
       <c r="F47" s="25"/>
       <c r="G47" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="H47" s="28">
-        <v>530.5</v>
-      </c>
-      <c r="I47" s="29">
-        <v>521.05000000000007</v>
-      </c>
-      <c r="J47" s="29">
-        <v>1407.36</v>
-      </c>
-      <c r="K47" s="30">
-        <v>477.05599999999998</v>
-      </c>
-      <c r="L47" s="28">
-        <v>465.22</v>
-      </c>
+      <c r="H47" s="49">
+        <f t="shared" si="18"/>
+        <v>151.3059306531963</v>
+      </c>
+      <c r="I47" s="49">
+        <f t="shared" si="19"/>
+        <v>0.97665485429421439</v>
+      </c>
+      <c r="J47" s="50">
+        <f t="shared" si="20"/>
+        <v>2.5111778471253428</v>
+      </c>
+      <c r="K47" s="29"/>
+      <c r="L47" s="28"/>
       <c r="M47" s="25"/>
+      <c r="N47" s="27"/>
+      <c r="O47" s="29"/>
     </row>
-    <row r="48" spans="4:13" x14ac:dyDescent="0.2">
+    <row r="48" spans="4:15" x14ac:dyDescent="0.2">
       <c r="F48" s="25"/>
       <c r="G48" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="H48" s="28">
-        <v>316.97999999999996</v>
-      </c>
-      <c r="I48" s="29">
-        <v>310.65999999999997</v>
-      </c>
-      <c r="J48" s="29">
-        <v>325.85999999999996</v>
-      </c>
-      <c r="K48" s="30">
-        <v>203.554</v>
-      </c>
-      <c r="L48" s="28">
-        <v>161.61800000000002</v>
-      </c>
+      <c r="H48" s="49">
+        <f t="shared" si="18"/>
+        <v>0.66099693891257161</v>
+      </c>
+      <c r="I48" s="49">
+        <f t="shared" si="19"/>
+        <v>0.48713176814913789</v>
+      </c>
+      <c r="J48" s="50">
+        <f t="shared" si="20"/>
+        <v>1.2084402593087455</v>
+      </c>
+      <c r="K48" s="29"/>
+      <c r="L48" s="28"/>
       <c r="M48" s="25"/>
+      <c r="N48" s="27"/>
+      <c r="O48" s="29"/>
     </row>
-    <row r="49" spans="6:13" x14ac:dyDescent="0.2">
+    <row r="49" spans="6:15" x14ac:dyDescent="0.2">
       <c r="F49" s="25"/>
       <c r="G49" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="H49" s="28">
-        <v>409.16</v>
-      </c>
-      <c r="I49" s="29">
-        <v>418.46</v>
-      </c>
-      <c r="J49" s="29">
-        <v>2110.44</v>
-      </c>
-      <c r="K49" s="30">
-        <v>343.89400000000001</v>
-      </c>
-      <c r="L49" s="28">
-        <v>271.78699999999998</v>
-      </c>
+      <c r="H49" s="49">
+        <f t="shared" si="18"/>
+        <v>42.386499811797499</v>
+      </c>
+      <c r="I49" s="49">
+        <f t="shared" si="19"/>
+        <v>0.60997495281925751</v>
+      </c>
+      <c r="J49" s="50">
+        <f t="shared" si="20"/>
+        <v>1.458357535643539</v>
+      </c>
+      <c r="K49" s="29"/>
+      <c r="L49" s="28"/>
       <c r="M49" s="25"/>
+      <c r="N49" s="27"/>
+      <c r="O49" s="29"/>
     </row>
-    <row r="50" spans="6:13" x14ac:dyDescent="0.2">
+    <row r="50" spans="6:15" x14ac:dyDescent="0.2">
       <c r="F50" s="25"/>
       <c r="G50" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="H50" s="28">
-        <v>122.53999999999999</v>
-      </c>
-      <c r="I50" s="29">
-        <v>123.05000000000001</v>
-      </c>
-      <c r="J50" s="29">
-        <v>137.25</v>
-      </c>
-      <c r="K50" s="30">
-        <v>100.91200000000001</v>
-      </c>
-      <c r="L50" s="28">
-        <v>85.619</v>
-      </c>
+      <c r="H50" s="49">
+        <f t="shared" si="18"/>
+        <v>18.361877923145371</v>
+      </c>
+      <c r="I50" s="49">
+        <f t="shared" si="19"/>
+        <v>1.0072110227217694</v>
+      </c>
+      <c r="J50" s="50">
+        <f t="shared" si="20"/>
+        <v>3.0729567844568955</v>
+      </c>
+      <c r="K50" s="29"/>
+      <c r="L50" s="28"/>
       <c r="M50" s="25"/>
+      <c r="N50" s="26"/>
+      <c r="O50" s="29"/>
     </row>
-    <row r="51" spans="6:13" x14ac:dyDescent="0.2">
+    <row r="51" spans="6:15" x14ac:dyDescent="0.2">
       <c r="F51" s="25"/>
       <c r="G51" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="H51" s="28">
-        <v>11245.300000000001</v>
-      </c>
-      <c r="I51" s="29">
-        <v>11813.1</v>
-      </c>
-      <c r="J51" s="29">
-        <v>47792.200000000004</v>
-      </c>
-      <c r="K51" s="30">
-        <v>11638.400000000001</v>
-      </c>
-      <c r="L51" s="28">
-        <v>6594.35</v>
-      </c>
+      <c r="H51" s="49">
+        <f t="shared" si="18"/>
+        <v>0.22923301833492674</v>
+      </c>
+      <c r="I51" s="49">
+        <f t="shared" si="19"/>
+        <v>0.23183333395245612</v>
+      </c>
+      <c r="J51" s="50">
+        <f t="shared" si="20"/>
+        <v>0.30055596098716092</v>
+      </c>
+      <c r="K51" s="29"/>
+      <c r="L51" s="28"/>
       <c r="M51" s="25"/>
+      <c r="N51" s="27"/>
+      <c r="O51" s="29"/>
     </row>
-    <row r="52" spans="6:13" x14ac:dyDescent="0.2">
+    <row r="52" spans="6:15" x14ac:dyDescent="0.2">
       <c r="F52" s="25"/>
       <c r="G52" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="H52" s="28">
-        <v>17973.400000000001</v>
-      </c>
-      <c r="I52" s="29">
-        <v>17878.2</v>
-      </c>
-      <c r="J52" s="29">
-        <v>24385.200000000001</v>
-      </c>
-      <c r="K52" s="30">
-        <v>13694.2</v>
-      </c>
-      <c r="L52" s="28">
-        <v>10074</v>
-      </c>
+      <c r="H52" s="49">
+        <f t="shared" si="18"/>
+        <v>6.4833537137100175</v>
+      </c>
+      <c r="I52" s="49">
+        <f t="shared" si="19"/>
+        <v>0.4418750512203008</v>
+      </c>
+      <c r="J52" s="50">
+        <f t="shared" si="20"/>
+        <v>0.75418841488211275</v>
+      </c>
+      <c r="K52" s="29"/>
+      <c r="L52" s="28"/>
       <c r="M52" s="25"/>
+      <c r="N52" s="26"/>
+      <c r="O52" s="29"/>
     </row>
-    <row r="53" spans="6:13" x14ac:dyDescent="0.2">
+    <row r="53" spans="6:15" x14ac:dyDescent="0.2">
       <c r="F53" s="25"/>
       <c r="G53" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="H53" s="28">
-        <v>1093.3900000000001</v>
-      </c>
-      <c r="I53" s="29">
-        <v>1091.5</v>
-      </c>
-      <c r="J53" s="29">
-        <v>3429.22</v>
-      </c>
-      <c r="K53" s="30">
-        <v>982.05899999999997</v>
-      </c>
-      <c r="L53" s="28">
-        <v>627.42600000000004</v>
-      </c>
+      <c r="H53" s="49">
+        <f t="shared" si="18"/>
+        <v>46.559626431146775</v>
+      </c>
+      <c r="I53" s="49">
+        <f t="shared" si="19"/>
+        <v>0.54996038936081759</v>
+      </c>
+      <c r="J53" s="50">
+        <f t="shared" si="20"/>
+        <v>1.0451587432315481</v>
+      </c>
+      <c r="K53" s="29"/>
+      <c r="L53" s="28"/>
       <c r="M53" s="25"/>
+      <c r="N53" s="30"/>
+      <c r="O53" s="29"/>
     </row>
-    <row r="54" spans="6:13" x14ac:dyDescent="0.2">
+    <row r="54" spans="6:15" x14ac:dyDescent="0.2">
       <c r="F54" s="25"/>
-      <c r="G54" s="31" t="s">
+      <c r="G54" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="H54" s="28">
-        <v>1445.73</v>
-      </c>
-      <c r="I54" s="29">
-        <v>1453.8999999999999</v>
-      </c>
-      <c r="J54" s="29">
-        <v>4756.7199999999993</v>
-      </c>
-      <c r="K54" s="30">
-        <v>1163.3</v>
-      </c>
-      <c r="L54" s="28">
-        <v>831.09500000000003</v>
-      </c>
+      <c r="H54" s="49">
+        <f t="shared" si="18"/>
+        <v>46.689978329619237</v>
+      </c>
+      <c r="I54" s="49">
+        <f t="shared" si="19"/>
+        <v>0.48137395297136371</v>
+      </c>
+      <c r="J54" s="50">
+        <f t="shared" si="20"/>
+        <v>0.88145955737202264</v>
+      </c>
+      <c r="K54" s="29"/>
+      <c r="L54" s="28"/>
       <c r="M54" s="25"/>
     </row>
-    <row r="55" spans="6:13" x14ac:dyDescent="0.2">
+    <row r="55" spans="6:15" x14ac:dyDescent="0.2">
       <c r="F55" s="25"/>
       <c r="G55" s="25"/>
       <c r="H55" s="25"/>
@@ -33829,7 +33922,7 @@
       <c r="L55" s="25"/>
       <c r="M55" s="25"/>
     </row>
-    <row r="56" spans="6:13" x14ac:dyDescent="0.2">
+    <row r="56" spans="6:15" x14ac:dyDescent="0.2">
       <c r="F56" s="25"/>
       <c r="G56" s="25"/>
       <c r="H56" s="25"/>
@@ -33839,7 +33932,7 @@
       <c r="L56" s="25"/>
       <c r="M56" s="25"/>
     </row>
-    <row r="57" spans="6:13" x14ac:dyDescent="0.2">
+    <row r="57" spans="6:15" x14ac:dyDescent="0.2">
       <c r="F57" s="25"/>
       <c r="G57" s="25"/>
       <c r="H57" s="25"/>
@@ -33849,7 +33942,7 @@
       <c r="L57" s="25"/>
       <c r="M57" s="25"/>
     </row>
-    <row r="58" spans="6:13" x14ac:dyDescent="0.2">
+    <row r="58" spans="6:15" x14ac:dyDescent="0.2">
       <c r="F58" s="25"/>
       <c r="G58" s="25"/>
       <c r="H58" s="25"/>
@@ -33859,7 +33952,7 @@
       <c r="L58" s="25"/>
       <c r="M58" s="25"/>
     </row>
-    <row r="59" spans="6:13" x14ac:dyDescent="0.2">
+    <row r="59" spans="6:15" x14ac:dyDescent="0.2">
       <c r="F59" s="25"/>
       <c r="G59" s="25"/>
       <c r="H59" s="25"/>
@@ -33869,105 +33962,105 @@
       <c r="L59" s="25"/>
       <c r="M59" s="25"/>
     </row>
-    <row r="60" spans="6:13" x14ac:dyDescent="0.2">
+    <row r="60" spans="6:15" x14ac:dyDescent="0.2">
       <c r="F60" s="25"/>
       <c r="G60" s="25" t="s">
         <v>1</v>
       </c>
       <c r="H60" s="25" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="I60" s="25" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="J60" s="25" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="K60" s="25"/>
       <c r="L60" s="26"/>
       <c r="M60" s="25"/>
     </row>
-    <row r="61" spans="6:13" x14ac:dyDescent="0.2">
+    <row r="61" spans="6:15" x14ac:dyDescent="0.2">
       <c r="F61" s="25"/>
       <c r="G61" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="H61" s="32">
+      <c r="H61" s="31" t="e">
         <f>H45/K45</f>
-        <v>1.0090164085715869</v>
-      </c>
-      <c r="I61" s="33">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I61" s="32" t="e">
         <f>I45/K45</f>
-        <v>1.0041252145665296</v>
-      </c>
-      <c r="J61" s="33">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J61" s="32" t="e">
         <f>J45/K45</f>
-        <v>1.2641429336089629</v>
-      </c>
-      <c r="K61" s="30"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K61" s="29"/>
       <c r="L61" s="28"/>
       <c r="M61" s="25"/>
     </row>
-    <row r="62" spans="6:13" x14ac:dyDescent="0.2">
+    <row r="62" spans="6:15" x14ac:dyDescent="0.2">
       <c r="F62" s="25"/>
       <c r="G62" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="H62" s="32">
-        <f t="shared" ref="H62:H70" si="18">H46/K46</f>
-        <v>0.75219028903627294</v>
-      </c>
-      <c r="I62" s="33">
-        <f t="shared" ref="I62:I70" si="19">I46/K46</f>
-        <v>0.7336035372144436</v>
-      </c>
-      <c r="J62" s="33">
-        <f t="shared" ref="J62:J70" si="20">J46/K46</f>
-        <v>1.0938753786948334</v>
-      </c>
-      <c r="K62" s="30"/>
+      <c r="H62" s="31" t="e">
+        <f t="shared" ref="H62:H70" si="21">H46/K46</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I62" s="32" t="e">
+        <f t="shared" ref="I62:I70" si="22">I46/K46</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J62" s="32" t="e">
+        <f>J46/K46</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K62" s="29"/>
       <c r="L62" s="28"/>
       <c r="M62" s="25"/>
     </row>
-    <row r="63" spans="6:13" x14ac:dyDescent="0.2">
+    <row r="63" spans="6:15" x14ac:dyDescent="0.2">
       <c r="F63" s="25"/>
       <c r="G63" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="H63" s="32">
-        <f t="shared" si="18"/>
-        <v>1.1120287764958412</v>
-      </c>
-      <c r="I63" s="33">
-        <f t="shared" si="19"/>
-        <v>1.092219781325463</v>
-      </c>
-      <c r="J63" s="33">
-        <f t="shared" si="20"/>
-        <v>2.950093909310437</v>
-      </c>
-      <c r="K63" s="30"/>
+      <c r="H63" s="31" t="e">
+        <f t="shared" si="21"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I63" s="32" t="e">
+        <f t="shared" si="22"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J63" s="32" t="e">
+        <f t="shared" ref="J62:J70" si="23">J47/K47</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K63" s="29"/>
       <c r="L63" s="28"/>
       <c r="M63" s="25"/>
     </row>
-    <row r="64" spans="6:13" x14ac:dyDescent="0.2">
+    <row r="64" spans="6:15" x14ac:dyDescent="0.2">
       <c r="F64" s="25"/>
       <c r="G64" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="H64" s="32">
-        <f t="shared" si="18"/>
-        <v>1.5572280574196526</v>
-      </c>
-      <c r="I64" s="33">
-        <f t="shared" si="19"/>
-        <v>1.5261797852166992</v>
-      </c>
-      <c r="J64" s="33">
-        <f t="shared" si="20"/>
-        <v>1.6008528449453214</v>
-      </c>
-      <c r="K64" s="30"/>
+      <c r="H64" s="31" t="e">
+        <f t="shared" si="21"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I64" s="32" t="e">
+        <f t="shared" si="22"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J64" s="32" t="e">
+        <f t="shared" si="23"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K64" s="29"/>
       <c r="L64" s="28"/>
       <c r="M64" s="25"/>
     </row>
@@ -33976,19 +34069,19 @@
       <c r="G65" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="H65" s="32">
-        <f t="shared" si="18"/>
-        <v>1.189785224516857</v>
-      </c>
-      <c r="I65" s="33">
-        <f t="shared" si="19"/>
-        <v>1.2168284413220352</v>
-      </c>
-      <c r="J65" s="33">
-        <f t="shared" si="20"/>
-        <v>6.1368910187441479</v>
-      </c>
-      <c r="K65" s="30"/>
+      <c r="H65" s="31" t="e">
+        <f t="shared" si="21"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I65" s="32" t="e">
+        <f t="shared" si="22"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J65" s="32" t="e">
+        <f t="shared" si="23"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K65" s="29"/>
       <c r="L65" s="28"/>
       <c r="M65" s="25"/>
     </row>
@@ -33997,19 +34090,19 @@
       <c r="G66" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="H66" s="32">
-        <f t="shared" si="18"/>
-        <v>1.2143253527826223</v>
-      </c>
-      <c r="I66" s="33">
-        <f t="shared" si="19"/>
-        <v>1.2193792611384178</v>
-      </c>
-      <c r="J66" s="33">
-        <f t="shared" si="20"/>
-        <v>1.3600959251625178</v>
-      </c>
-      <c r="K66" s="30"/>
+      <c r="H66" s="31" t="e">
+        <f t="shared" si="21"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I66" s="32" t="e">
+        <f t="shared" si="22"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J66" s="32" t="e">
+        <f t="shared" si="23"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K66" s="29"/>
       <c r="L66" s="28"/>
       <c r="M66" s="25"/>
     </row>
@@ -34018,19 +34111,19 @@
       <c r="G67" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="H67" s="32">
-        <f t="shared" si="18"/>
-        <v>0.96622387957107503</v>
-      </c>
-      <c r="I67" s="33">
-        <f t="shared" si="19"/>
-        <v>1.0150106543854824</v>
-      </c>
-      <c r="J67" s="33">
-        <f t="shared" si="20"/>
-        <v>4.106423563376409</v>
-      </c>
-      <c r="K67" s="30"/>
+      <c r="H67" s="31" t="e">
+        <f t="shared" si="21"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I67" s="32" t="e">
+        <f t="shared" si="22"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J67" s="32" t="e">
+        <f t="shared" si="23"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K67" s="29"/>
       <c r="L67" s="28"/>
       <c r="M67" s="25"/>
     </row>
@@ -34039,19 +34132,19 @@
       <c r="G68" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="H68" s="32">
-        <f t="shared" si="18"/>
-        <v>1.3124826568912387</v>
-      </c>
-      <c r="I68" s="33">
-        <f t="shared" si="19"/>
-        <v>1.3055308086635218</v>
-      </c>
-      <c r="J68" s="33">
-        <f t="shared" si="20"/>
-        <v>1.780695476917235</v>
-      </c>
-      <c r="K68" s="30"/>
+      <c r="H68" s="31" t="e">
+        <f t="shared" si="21"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I68" s="32" t="e">
+        <f t="shared" si="22"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J68" s="32" t="e">
+        <f t="shared" si="23"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K68" s="29"/>
       <c r="L68" s="28"/>
       <c r="M68" s="25"/>
     </row>
@@ -34060,40 +34153,40 @@
       <c r="G69" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="H69" s="32">
-        <f t="shared" si="18"/>
-        <v>1.1133648792995128</v>
-      </c>
-      <c r="I69" s="33">
-        <f t="shared" si="19"/>
-        <v>1.111440351343453</v>
-      </c>
-      <c r="J69" s="33">
-        <f t="shared" si="20"/>
-        <v>3.4918675965496981</v>
-      </c>
-      <c r="K69" s="30"/>
+      <c r="H69" s="31" t="e">
+        <f t="shared" si="21"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I69" s="32" t="e">
+        <f t="shared" si="22"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J69" s="32" t="e">
+        <f t="shared" si="23"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K69" s="29"/>
       <c r="L69" s="28"/>
       <c r="M69" s="25"/>
     </row>
     <row r="70" spans="6:13" x14ac:dyDescent="0.2">
       <c r="F70" s="25"/>
-      <c r="G70" s="31" t="s">
+      <c r="G70" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="H70" s="32">
-        <f t="shared" si="18"/>
-        <v>1.2427834608441504</v>
-      </c>
-      <c r="I70" s="33">
-        <f t="shared" si="19"/>
-        <v>1.2498065847158943</v>
-      </c>
-      <c r="J70" s="33">
-        <f t="shared" si="20"/>
-        <v>4.0889882231582559</v>
-      </c>
-      <c r="K70" s="30"/>
+      <c r="H70" s="31" t="e">
+        <f t="shared" si="21"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I70" s="32" t="e">
+        <f t="shared" si="22"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J70" s="32" t="e">
+        <f t="shared" si="23"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K70" s="29"/>
       <c r="L70" s="28"/>
       <c r="M70" s="25"/>
     </row>
@@ -34113,7 +34206,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="27.6640625" style="37" customWidth="1"/>
+    <col min="1" max="1" width="27.6640625" style="36" customWidth="1"/>
     <col min="14" max="14" width="18.5" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="15" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="13.83203125" bestFit="1" customWidth="1"/>
@@ -34143,7 +34236,7 @@
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="37" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="6">
@@ -34172,7 +34265,7 @@
       <c r="M2" s="19"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="37" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="6">
@@ -34200,7 +34293,7 @@
       <c r="J3" s="7"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="37" t="s">
         <v>16</v>
       </c>
       <c r="B4" s="6">
@@ -34228,7 +34321,7 @@
       <c r="J4" s="7"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="38" t="s">
+      <c r="A5" s="37" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="6">
@@ -34256,7 +34349,7 @@
       <c r="J5" s="7"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A6" s="38" t="s">
+      <c r="A6" s="37" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="6">
@@ -34284,7 +34377,7 @@
       <c r="J6" s="7"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7" s="38" t="s">
+      <c r="A7" s="37" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="6">
@@ -34312,7 +34405,7 @@
       <c r="J7" s="7"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8" s="39" t="s">
+      <c r="A8" s="38" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="8">
@@ -34340,7 +34433,7 @@
       <c r="J8" s="7"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A9" s="38" t="s">
+      <c r="A9" s="37" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="6">
@@ -34367,7 +34460,7 @@
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A10" s="39" t="s">
+      <c r="A10" s="38" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="8">
@@ -34394,7 +34487,7 @@
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A11" s="40" t="s">
+      <c r="A11" s="39" t="s">
         <v>10</v>
       </c>
       <c r="B11" s="8">
@@ -34426,13 +34519,13 @@
       <c r="H12" s="22"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A13" s="41" t="s">
+      <c r="A13" s="40" t="s">
         <v>70</v>
       </c>
       <c r="B13" s="23">
         <v>4761705</v>
       </c>
-      <c r="C13" s="34">
+      <c r="C13" s="33">
         <v>8.3901000000000003</v>
       </c>
       <c r="D13" s="23">
@@ -34441,10 +34534,10 @@
       <c r="E13" s="23">
         <v>567538</v>
       </c>
-      <c r="F13" s="36">
+      <c r="F13" s="35">
         <v>1000</v>
       </c>
-      <c r="G13" s="36">
+      <c r="G13" s="35">
         <v>5</v>
       </c>
       <c r="H13" s="24">
@@ -34453,13 +34546,13 @@
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A14" s="41" t="s">
+      <c r="A14" s="40" t="s">
         <v>71</v>
       </c>
       <c r="B14" s="23">
         <v>4766822</v>
       </c>
-      <c r="C14" s="34">
+      <c r="C14" s="33">
         <v>8.3976000000000006</v>
       </c>
       <c r="D14" s="23">
@@ -34468,10 +34561,10 @@
       <c r="E14" s="23">
         <v>567639</v>
       </c>
-      <c r="F14" s="36">
+      <c r="F14" s="35">
         <v>1000</v>
       </c>
-      <c r="G14" s="36">
+      <c r="G14" s="35">
         <v>5</v>
       </c>
       <c r="H14" s="24">
@@ -34480,13 +34573,13 @@
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A15" s="41" t="s">
+      <c r="A15" s="40" t="s">
         <v>72</v>
       </c>
       <c r="B15" s="23">
         <v>4765510</v>
       </c>
-      <c r="C15" s="34">
+      <c r="C15" s="33">
         <v>8.3926999999999996</v>
       </c>
       <c r="D15" s="23">
@@ -34495,10 +34588,10 @@
       <c r="E15" s="23">
         <v>567812</v>
       </c>
-      <c r="F15" s="36">
+      <c r="F15" s="35">
         <v>1000</v>
       </c>
-      <c r="G15" s="36">
+      <c r="G15" s="35">
         <v>5</v>
       </c>
       <c r="H15" s="24">
@@ -34507,13 +34600,13 @@
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A16" s="41" t="s">
+      <c r="A16" s="40" t="s">
         <v>73</v>
       </c>
       <c r="B16" s="23">
         <v>4761937</v>
       </c>
-      <c r="C16" s="34">
+      <c r="C16" s="33">
         <v>8.3895999999999997</v>
       </c>
       <c r="D16" s="23">
@@ -34522,10 +34615,10 @@
       <c r="E16" s="23">
         <v>567595</v>
       </c>
-      <c r="F16" s="36">
+      <c r="F16" s="35">
         <v>1000</v>
       </c>
-      <c r="G16" s="36">
+      <c r="G16" s="35">
         <v>5</v>
       </c>
       <c r="H16" s="24">
@@ -34534,13 +34627,13 @@
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A17" s="41" t="s">
+      <c r="A17" s="40" t="s">
         <v>74</v>
       </c>
       <c r="B17" s="23">
         <v>4768081</v>
       </c>
-      <c r="C17" s="34">
+      <c r="C17" s="33">
         <v>8.3981999999999992</v>
       </c>
       <c r="D17" s="23">
@@ -34549,10 +34642,10 @@
       <c r="E17" s="23">
         <v>567746</v>
       </c>
-      <c r="F17" s="36">
+      <c r="F17" s="35">
         <v>1000</v>
       </c>
-      <c r="G17" s="36">
+      <c r="G17" s="35">
         <v>5</v>
       </c>
       <c r="H17" s="24">
@@ -34561,13 +34654,13 @@
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A18" s="41" t="s">
+      <c r="A18" s="40" t="s">
         <v>75</v>
       </c>
       <c r="B18" s="23">
         <v>4767858</v>
       </c>
-      <c r="C18" s="34">
+      <c r="C18" s="33">
         <v>8.3941999999999997</v>
       </c>
       <c r="D18" s="23">
@@ -34576,10 +34669,10 @@
       <c r="E18" s="23">
         <v>567988</v>
       </c>
-      <c r="F18" s="36">
+      <c r="F18" s="35">
         <v>1000</v>
       </c>
-      <c r="G18" s="36">
+      <c r="G18" s="35">
         <v>5</v>
       </c>
       <c r="H18" s="24">
@@ -34588,7 +34681,7 @@
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A19" s="42"/>
+      <c r="A19" s="41"/>
       <c r="B19" s="23"/>
       <c r="C19" s="23"/>
       <c r="D19" s="23"/>
@@ -34598,13 +34691,13 @@
       <c r="H19" s="24"/>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A20" s="42" t="s">
+      <c r="A20" s="41" t="s">
         <v>76</v>
       </c>
       <c r="B20" s="23">
         <v>5654658</v>
       </c>
-      <c r="C20" s="34">
+      <c r="C20" s="33">
         <v>37.6</v>
       </c>
       <c r="D20" s="23">
@@ -34623,19 +34716,19 @@
         <f>(_xlfn.CEILING.MATH(LOG(D20, 2)))*(B20)*0.000000125</f>
         <v>7.0683224999999998</v>
       </c>
-      <c r="O20" s="42"/>
-      <c r="P20" s="42"/>
-      <c r="Q20" s="42"/>
-      <c r="R20" s="42"/>
+      <c r="O20" s="41"/>
+      <c r="P20" s="41"/>
+      <c r="Q20" s="41"/>
+      <c r="R20" s="41"/>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A21" s="42" t="s">
+      <c r="A21" s="41" t="s">
         <v>77</v>
       </c>
       <c r="B21" s="23">
         <v>5345385</v>
       </c>
-      <c r="C21" s="34">
+      <c r="C21" s="33">
         <v>17.8</v>
       </c>
       <c r="D21" s="23">
@@ -34656,13 +34749,13 @@
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A22" s="42" t="s">
+      <c r="A22" s="41" t="s">
         <v>78</v>
       </c>
       <c r="B22" s="23">
         <v>4766822</v>
       </c>
-      <c r="C22" s="34">
+      <c r="C22" s="33">
         <v>8.39</v>
       </c>
       <c r="D22" s="23">
@@ -34683,13 +34776,13 @@
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A23" s="42" t="s">
+      <c r="A23" s="41" t="s">
         <v>79</v>
       </c>
       <c r="B23" s="23">
         <v>3690240</v>
       </c>
-      <c r="C23" s="34">
+      <c r="C23" s="33">
         <v>4.22</v>
       </c>
       <c r="D23" s="23">
@@ -34715,7 +34808,7 @@
       <c r="N24" s="2"/>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A25" s="42" t="s">
+      <c r="A25" s="41" t="s">
         <v>80</v>
       </c>
       <c r="B25" s="23">
@@ -34742,7 +34835,7 @@
       </c>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A26" s="42" t="s">
+      <c r="A26" s="41" t="s">
         <v>81</v>
       </c>
       <c r="B26" s="23">
@@ -34769,7 +34862,7 @@
       </c>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A27" s="42" t="s">
+      <c r="A27" s="41" t="s">
         <v>82</v>
       </c>
       <c r="B27" s="23">
@@ -34794,10 +34887,10 @@
         <f t="shared" si="2"/>
         <v>9.4117412500000004</v>
       </c>
-      <c r="O27" s="42"/>
+      <c r="O27" s="41"/>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A28" s="42" t="s">
+      <c r="A28" s="41" t="s">
         <v>83</v>
       </c>
       <c r="B28" s="23">
@@ -34822,10 +34915,10 @@
         <f t="shared" si="2"/>
         <v>18.82732</v>
       </c>
-      <c r="O28" s="42"/>
+      <c r="O28" s="41"/>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A29" s="42" t="s">
+      <c r="A29" s="41" t="s">
         <v>96</v>
       </c>
       <c r="B29" s="23">
@@ -34850,13 +34943,13 @@
         <f t="shared" si="2"/>
         <v>37.656469999999999</v>
       </c>
-      <c r="O29" s="42"/>
+      <c r="O29" s="41"/>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="O30" s="42"/>
+      <c r="O30" s="41"/>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A34" s="42"/>
+      <c r="A34" s="41"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -34879,30 +34972,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="44" t="s">
         <v>84</v>
       </c>
-      <c r="B1" s="45" t="s">
+      <c r="B1" s="44" t="s">
         <v>70</v>
       </c>
-      <c r="C1" s="45" t="s">
+      <c r="C1" s="44" t="s">
         <v>71</v>
       </c>
-      <c r="D1" s="45" t="s">
+      <c r="D1" s="44" t="s">
         <v>72</v>
       </c>
-      <c r="E1" s="45" t="s">
+      <c r="E1" s="44" t="s">
         <v>73</v>
       </c>
-      <c r="F1" s="45" t="s">
+      <c r="F1" s="44" t="s">
         <v>74</v>
       </c>
-      <c r="G1" s="45" t="s">
+      <c r="G1" s="44" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="36" t="s">
         <v>85</v>
       </c>
       <c r="B2" s="3">
@@ -34925,7 +35018,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="36" t="s">
         <v>86</v>
       </c>
       <c r="B3" s="3">
@@ -34948,7 +35041,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="37" t="s">
+      <c r="A4" s="36" t="s">
         <v>87</v>
       </c>
       <c r="B4" s="3">
@@ -34971,44 +35064,44 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="37"/>
-      <c r="B5" s="37"/>
-      <c r="C5" s="37"/>
-      <c r="D5" s="37"/>
-      <c r="E5" s="37"/>
-      <c r="F5" s="37"/>
-      <c r="G5" s="37"/>
+      <c r="A5" s="36"/>
+      <c r="B5" s="36"/>
+      <c r="C5" s="36"/>
+      <c r="D5" s="36"/>
+      <c r="E5" s="36"/>
+      <c r="F5" s="36"/>
+      <c r="G5" s="36"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="37"/>
-      <c r="B6" s="37"/>
-      <c r="C6" s="37"/>
-      <c r="D6" s="37"/>
-      <c r="E6" s="37"/>
-      <c r="F6" s="37"/>
-      <c r="G6" s="37"/>
+      <c r="A6" s="36"/>
+      <c r="B6" s="36"/>
+      <c r="C6" s="36"/>
+      <c r="D6" s="36"/>
+      <c r="E6" s="36"/>
+      <c r="F6" s="36"/>
+      <c r="G6" s="36"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="45" t="s">
+      <c r="A7" s="44" t="s">
         <v>88</v>
       </c>
-      <c r="B7" s="47" t="s">
+      <c r="B7" s="46" t="s">
         <v>76</v>
       </c>
-      <c r="C7" s="47" t="s">
+      <c r="C7" s="46" t="s">
         <v>77</v>
       </c>
-      <c r="D7" s="47" t="s">
+      <c r="D7" s="46" t="s">
         <v>78</v>
       </c>
-      <c r="E7" s="47" t="s">
+      <c r="E7" s="46" t="s">
         <v>79</v>
       </c>
-      <c r="F7" s="37"/>
-      <c r="G7" s="37"/>
+      <c r="F7" s="36"/>
+      <c r="G7" s="36"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="37" t="s">
+      <c r="A8" s="36" t="s">
         <v>85</v>
       </c>
       <c r="B8" s="3">
@@ -35023,11 +35116,11 @@
       <c r="E8" s="3">
         <v>1581</v>
       </c>
-      <c r="F8" s="37"/>
-      <c r="G8" s="37"/>
+      <c r="F8" s="36"/>
+      <c r="G8" s="36"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="37" t="s">
+      <c r="A9" s="36" t="s">
         <v>86</v>
       </c>
       <c r="B9" s="3">
@@ -35042,11 +35135,11 @@
       <c r="E9" s="3">
         <v>1.8303</v>
       </c>
-      <c r="F9" s="37"/>
-      <c r="G9" s="37"/>
+      <c r="F9" s="36"/>
+      <c r="G9" s="36"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="37" t="s">
+      <c r="A10" s="36" t="s">
         <v>87</v>
       </c>
       <c r="B10" s="3">
@@ -35061,41 +35154,41 @@
       <c r="E10" s="3">
         <v>145.6</v>
       </c>
-      <c r="F10" s="37"/>
-      <c r="G10" s="37"/>
+      <c r="F10" s="36"/>
+      <c r="G10" s="36"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="37"/>
-      <c r="B11" s="37"/>
-      <c r="C11" s="37"/>
-      <c r="D11" s="37"/>
-      <c r="E11" s="37"/>
-      <c r="F11" s="37"/>
-      <c r="G11" s="37"/>
+      <c r="A11" s="36"/>
+      <c r="B11" s="36"/>
+      <c r="C11" s="36"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
+      <c r="G11" s="36"/>
     </row>
     <row r="12" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A12" s="43" t="s">
+      <c r="A12" s="42" t="s">
         <v>89</v>
       </c>
-      <c r="B12" s="44" t="s">
+      <c r="B12" s="43" t="s">
         <v>80</v>
       </c>
-      <c r="C12" s="44" t="s">
+      <c r="C12" s="43" t="s">
         <v>81</v>
       </c>
-      <c r="D12" s="44" t="s">
+      <c r="D12" s="43" t="s">
         <v>82</v>
       </c>
-      <c r="E12" s="44" t="s">
+      <c r="E12" s="43" t="s">
         <v>83</v>
       </c>
-      <c r="F12" s="44" t="s">
+      <c r="F12" s="43" t="s">
         <v>96</v>
       </c>
-      <c r="G12" s="37"/>
+      <c r="G12" s="36"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="48" t="s">
+      <c r="A13" s="47" t="s">
         <v>85</v>
       </c>
       <c r="B13" s="3">
@@ -35113,10 +35206,10 @@
       <c r="F13" s="3">
         <v>35947</v>
       </c>
-      <c r="G13" s="37"/>
+      <c r="G13" s="36"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="48" t="s">
+      <c r="A14" s="47" t="s">
         <v>86</v>
       </c>
       <c r="B14" s="3">
@@ -35134,10 +35227,10 @@
       <c r="F14" s="3">
         <v>3.2633000000000001</v>
       </c>
-      <c r="G14" s="37"/>
+      <c r="G14" s="36"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="48" t="s">
+      <c r="A15" s="47" t="s">
         <v>87</v>
       </c>
       <c r="B15" s="3">
@@ -35155,45 +35248,45 @@
       <c r="F15" s="3">
         <v>628.12</v>
       </c>
-      <c r="G15" s="37"/>
+      <c r="G15" s="36"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="37"/>
-      <c r="B16" s="37"/>
-      <c r="C16" s="37"/>
-      <c r="D16" s="37"/>
-      <c r="E16" s="37"/>
-      <c r="F16" s="37"/>
-      <c r="G16" s="37"/>
+      <c r="A16" s="36"/>
+      <c r="B16" s="36"/>
+      <c r="C16" s="36"/>
+      <c r="D16" s="36"/>
+      <c r="E16" s="36"/>
+      <c r="F16" s="36"/>
+      <c r="G16" s="36"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="37"/>
-      <c r="B17" s="37"/>
-      <c r="C17" s="37"/>
-      <c r="D17" s="37"/>
-      <c r="E17" s="37"/>
-      <c r="F17" s="37"/>
-      <c r="G17" s="37"/>
+      <c r="A17" s="36"/>
+      <c r="B17" s="36"/>
+      <c r="C17" s="36"/>
+      <c r="D17" s="36"/>
+      <c r="E17" s="36"/>
+      <c r="F17" s="36"/>
+      <c r="G17" s="36"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" s="43" t="s">
+      <c r="A18" s="42" t="s">
         <v>90</v>
       </c>
-      <c r="B18" s="46">
+      <c r="B18" s="45">
         <v>3</v>
       </c>
-      <c r="C18" s="46">
+      <c r="C18" s="45">
         <v>6</v>
       </c>
-      <c r="D18" s="46">
+      <c r="D18" s="45">
         <v>12</v>
       </c>
-      <c r="E18" s="37"/>
-      <c r="F18" s="37"/>
-      <c r="G18" s="37"/>
+      <c r="E18" s="36"/>
+      <c r="F18" s="36"/>
+      <c r="G18" s="36"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="48" t="s">
+      <c r="A19" s="47" t="s">
         <v>91</v>
       </c>
       <c r="B19" s="3">
@@ -35205,18 +35298,18 @@
       <c r="D19" s="3">
         <v>0.251</v>
       </c>
-      <c r="E19" s="37"/>
-      <c r="F19" s="37"/>
-      <c r="G19" s="37"/>
+      <c r="E19" s="36"/>
+      <c r="F19" s="36"/>
+      <c r="G19" s="36"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20" s="37"/>
-      <c r="B20" s="37"/>
-      <c r="C20" s="37"/>
-      <c r="D20" s="37"/>
-      <c r="E20" s="37"/>
-      <c r="F20" s="37"/>
-      <c r="G20" s="37"/>
+      <c r="A20" s="36"/>
+      <c r="B20" s="36"/>
+      <c r="C20" s="36"/>
+      <c r="D20" s="36"/>
+      <c r="E20" s="36"/>
+      <c r="F20" s="36"/>
+      <c r="G20" s="36"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -35334,16 +35427,16 @@
       <c r="A7" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="B7" s="35" t="s">
+      <c r="B7" s="34" t="s">
         <v>76</v>
       </c>
-      <c r="C7" s="35" t="s">
+      <c r="C7" s="34" t="s">
         <v>77</v>
       </c>
-      <c r="D7" s="35" t="s">
+      <c r="D7" s="34" t="s">
         <v>78</v>
       </c>
-      <c r="E7" s="35" t="s">
+      <c r="E7" s="34" t="s">
         <v>79</v>
       </c>
     </row>
@@ -35399,22 +35492,22 @@
       </c>
     </row>
     <row r="12" spans="1:13" ht="34" x14ac:dyDescent="0.2">
-      <c r="A12" s="43" t="s">
+      <c r="A12" s="42" t="s">
         <v>89</v>
       </c>
-      <c r="B12" s="44" t="s">
+      <c r="B12" s="43" t="s">
         <v>80</v>
       </c>
-      <c r="C12" s="44" t="s">
+      <c r="C12" s="43" t="s">
         <v>81</v>
       </c>
-      <c r="D12" s="44" t="s">
+      <c r="D12" s="43" t="s">
         <v>82</v>
       </c>
-      <c r="E12" s="44" t="s">
+      <c r="E12" s="43" t="s">
         <v>83</v>
       </c>
-      <c r="F12" s="44" t="s">
+      <c r="F12" s="43" t="s">
         <v>96</v>
       </c>
     </row>
@@ -35532,32 +35625,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="44" t="s">
         <v>84</v>
       </c>
-      <c r="B1" s="45" t="s">
+      <c r="B1" s="44" t="s">
         <v>70</v>
       </c>
-      <c r="C1" s="45" t="s">
+      <c r="C1" s="44" t="s">
         <v>71</v>
       </c>
-      <c r="D1" s="45" t="s">
+      <c r="D1" s="44" t="s">
         <v>72</v>
       </c>
-      <c r="E1" s="45" t="s">
+      <c r="E1" s="44" t="s">
         <v>73</v>
       </c>
-      <c r="F1" s="45" t="s">
+      <c r="F1" s="44" t="s">
         <v>74</v>
       </c>
-      <c r="G1" s="45" t="s">
+      <c r="G1" s="44" t="s">
         <v>75</v>
       </c>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="36" t="s">
         <v>85</v>
       </c>
       <c r="B2" s="3">
@@ -35578,11 +35671,11 @@
       <c r="G2" s="3">
         <v>8.1449999999999996</v>
       </c>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="36"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="36" t="s">
         <v>86</v>
       </c>
       <c r="B3" s="3">
@@ -35603,11 +35696,11 @@
       <c r="G3" s="3">
         <v>1.24</v>
       </c>
-      <c r="H3" s="37"/>
-      <c r="I3" s="37"/>
+      <c r="H3" s="36"/>
+      <c r="I3" s="36"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="37" t="s">
+      <c r="A4" s="36" t="s">
         <v>87</v>
       </c>
       <c r="B4" s="3">
@@ -35628,54 +35721,54 @@
       <c r="G4" s="3">
         <v>308.55</v>
       </c>
-      <c r="H4" s="37"/>
-      <c r="I4" s="37"/>
+      <c r="H4" s="36"/>
+      <c r="I4" s="36"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="37"/>
-      <c r="B5" s="37"/>
-      <c r="C5" s="37"/>
-      <c r="D5" s="37"/>
-      <c r="E5" s="37"/>
-      <c r="F5" s="37"/>
-      <c r="G5" s="37"/>
-      <c r="H5" s="37"/>
-      <c r="I5" s="37"/>
+      <c r="A5" s="36"/>
+      <c r="B5" s="36"/>
+      <c r="C5" s="36"/>
+      <c r="D5" s="36"/>
+      <c r="E5" s="36"/>
+      <c r="F5" s="36"/>
+      <c r="G5" s="36"/>
+      <c r="H5" s="36"/>
+      <c r="I5" s="36"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="37"/>
-      <c r="B6" s="37"/>
-      <c r="C6" s="37"/>
-      <c r="D6" s="37"/>
-      <c r="E6" s="37"/>
-      <c r="F6" s="37"/>
-      <c r="G6" s="37"/>
-      <c r="H6" s="37"/>
-      <c r="I6" s="37"/>
+      <c r="A6" s="36"/>
+      <c r="B6" s="36"/>
+      <c r="C6" s="36"/>
+      <c r="D6" s="36"/>
+      <c r="E6" s="36"/>
+      <c r="F6" s="36"/>
+      <c r="G6" s="36"/>
+      <c r="H6" s="36"/>
+      <c r="I6" s="36"/>
     </row>
     <row r="7" spans="1:9" ht="34" x14ac:dyDescent="0.2">
-      <c r="A7" s="45" t="s">
+      <c r="A7" s="44" t="s">
         <v>88</v>
       </c>
-      <c r="B7" s="44" t="s">
+      <c r="B7" s="43" t="s">
         <v>76</v>
       </c>
-      <c r="C7" s="44" t="s">
+      <c r="C7" s="43" t="s">
         <v>77</v>
       </c>
-      <c r="D7" s="44" t="s">
+      <c r="D7" s="43" t="s">
         <v>78</v>
       </c>
-      <c r="E7" s="44" t="s">
+      <c r="E7" s="43" t="s">
         <v>79</v>
       </c>
-      <c r="F7" s="37"/>
-      <c r="G7" s="37"/>
-      <c r="H7" s="37"/>
-      <c r="I7" s="37"/>
+      <c r="F7" s="36"/>
+      <c r="G7" s="36"/>
+      <c r="H7" s="36"/>
+      <c r="I7" s="36"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="37" t="s">
+      <c r="A8" s="36" t="s">
         <v>85</v>
       </c>
       <c r="B8" s="3">
@@ -35690,34 +35783,34 @@
       <c r="E8" s="3">
         <v>25.302</v>
       </c>
-      <c r="F8" s="37"/>
-      <c r="G8" s="37"/>
-      <c r="H8" s="37"/>
-      <c r="I8" s="37"/>
+      <c r="F8" s="36"/>
+      <c r="G8" s="36"/>
+      <c r="H8" s="36"/>
+      <c r="I8" s="36"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="37" t="s">
+      <c r="A9" s="36" t="s">
         <v>86</v>
       </c>
-      <c r="B9" s="49">
+      <c r="B9" s="48">
         <v>2.0158</v>
       </c>
-      <c r="C9" s="49">
+      <c r="C9" s="48">
         <v>1.3463000000000001</v>
       </c>
-      <c r="D9" s="49">
+      <c r="D9" s="48">
         <v>0.7278</v>
       </c>
       <c r="E9" s="3">
         <v>0.40110000000000001</v>
       </c>
-      <c r="F9" s="37"/>
-      <c r="G9" s="37"/>
-      <c r="H9" s="37"/>
-      <c r="I9" s="37"/>
+      <c r="F9" s="36"/>
+      <c r="G9" s="36"/>
+      <c r="H9" s="36"/>
+      <c r="I9" s="36"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="37" t="s">
+      <c r="A10" s="36" t="s">
         <v>87</v>
       </c>
       <c r="B10" s="3">
@@ -35732,47 +35825,47 @@
       <c r="E10" s="3">
         <v>235.94</v>
       </c>
-      <c r="F10" s="37"/>
-      <c r="G10" s="37"/>
-      <c r="H10" s="37"/>
-      <c r="I10" s="37"/>
+      <c r="F10" s="36"/>
+      <c r="G10" s="36"/>
+      <c r="H10" s="36"/>
+      <c r="I10" s="36"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" s="37"/>
-      <c r="B11" s="37"/>
-      <c r="C11" s="37"/>
-      <c r="D11" s="37"/>
-      <c r="E11" s="37"/>
-      <c r="F11" s="37"/>
-      <c r="G11" s="37"/>
-      <c r="H11" s="37"/>
-      <c r="I11" s="37"/>
+      <c r="A11" s="36"/>
+      <c r="B11" s="36"/>
+      <c r="C11" s="36"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
+      <c r="G11" s="36"/>
+      <c r="H11" s="36"/>
+      <c r="I11" s="36"/>
     </row>
     <row r="12" spans="1:9" ht="34" x14ac:dyDescent="0.2">
-      <c r="A12" s="43" t="s">
+      <c r="A12" s="42" t="s">
         <v>89</v>
       </c>
-      <c r="B12" s="44" t="s">
+      <c r="B12" s="43" t="s">
         <v>80</v>
       </c>
-      <c r="C12" s="44" t="s">
+      <c r="C12" s="43" t="s">
         <v>81</v>
       </c>
-      <c r="D12" s="44" t="s">
+      <c r="D12" s="43" t="s">
         <v>82</v>
       </c>
-      <c r="E12" s="44" t="s">
+      <c r="E12" s="43" t="s">
         <v>83</v>
       </c>
-      <c r="F12" s="44" t="s">
+      <c r="F12" s="43" t="s">
         <v>96</v>
       </c>
-      <c r="G12" s="37"/>
-      <c r="H12" s="37"/>
-      <c r="I12" s="37"/>
+      <c r="G12" s="36"/>
+      <c r="H12" s="36"/>
+      <c r="I12" s="36"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" s="48" t="s">
+      <c r="A13" s="47" t="s">
         <v>85</v>
       </c>
       <c r="B13" s="3">
@@ -35790,12 +35883,12 @@
       <c r="F13" s="3">
         <v>516.45000000000005</v>
       </c>
-      <c r="G13" s="37"/>
-      <c r="H13" s="37"/>
-      <c r="I13" s="37"/>
+      <c r="G13" s="36"/>
+      <c r="H13" s="36"/>
+      <c r="I13" s="36"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" s="48" t="s">
+      <c r="A14" s="47" t="s">
         <v>86</v>
       </c>
       <c r="B14" s="3">
@@ -35813,12 +35906,12 @@
       <c r="F14" s="3">
         <v>3.3256999999999999</v>
       </c>
-      <c r="G14" s="37"/>
-      <c r="H14" s="37"/>
-      <c r="I14" s="37"/>
+      <c r="G14" s="36"/>
+      <c r="H14" s="36"/>
+      <c r="I14" s="36"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15" s="48" t="s">
+      <c r="A15" s="47" t="s">
         <v>87</v>
       </c>
       <c r="B15" s="3">
@@ -35836,53 +35929,53 @@
       <c r="F15" s="3">
         <v>1203.2</v>
       </c>
-      <c r="G15" s="37"/>
-      <c r="H15" s="37"/>
-      <c r="I15" s="37"/>
+      <c r="G15" s="36"/>
+      <c r="H15" s="36"/>
+      <c r="I15" s="36"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16" s="37"/>
-      <c r="B16" s="37"/>
-      <c r="C16" s="37"/>
-      <c r="D16" s="37"/>
-      <c r="E16" s="37"/>
-      <c r="F16" s="37"/>
-      <c r="G16" s="37"/>
-      <c r="H16" s="37"/>
-      <c r="I16" s="37"/>
+      <c r="A16" s="36"/>
+      <c r="B16" s="36"/>
+      <c r="C16" s="36"/>
+      <c r="D16" s="36"/>
+      <c r="E16" s="36"/>
+      <c r="F16" s="36"/>
+      <c r="G16" s="36"/>
+      <c r="H16" s="36"/>
+      <c r="I16" s="36"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" s="37"/>
-      <c r="B17" s="37"/>
-      <c r="C17" s="37"/>
-      <c r="D17" s="37"/>
-      <c r="E17" s="37"/>
-      <c r="F17" s="37"/>
-      <c r="G17" s="37"/>
-      <c r="H17" s="37"/>
-      <c r="I17" s="37"/>
+      <c r="A17" s="36"/>
+      <c r="B17" s="36"/>
+      <c r="C17" s="36"/>
+      <c r="D17" s="36"/>
+      <c r="E17" s="36"/>
+      <c r="F17" s="36"/>
+      <c r="G17" s="36"/>
+      <c r="H17" s="36"/>
+      <c r="I17" s="36"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A18" s="43" t="s">
+      <c r="A18" s="42" t="s">
         <v>90</v>
       </c>
-      <c r="B18" s="46">
+      <c r="B18" s="45">
         <v>3</v>
       </c>
-      <c r="C18" s="46">
+      <c r="C18" s="45">
         <v>6</v>
       </c>
-      <c r="D18" s="46">
+      <c r="D18" s="45">
         <v>12</v>
       </c>
-      <c r="E18" s="37"/>
-      <c r="F18" s="37"/>
-      <c r="G18" s="37"/>
-      <c r="H18" s="37"/>
-      <c r="I18" s="37"/>
+      <c r="E18" s="36"/>
+      <c r="F18" s="36"/>
+      <c r="G18" s="36"/>
+      <c r="H18" s="36"/>
+      <c r="I18" s="36"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A19" s="48" t="s">
+      <c r="A19" s="47" t="s">
         <v>91</v>
       </c>
       <c r="B19" s="3">
@@ -35894,22 +35987,22 @@
       <c r="D19" s="3">
         <v>0.248</v>
       </c>
-      <c r="E19" s="37"/>
-      <c r="F19" s="37"/>
-      <c r="G19" s="37"/>
-      <c r="H19" s="37"/>
-      <c r="I19" s="37"/>
+      <c r="E19" s="36"/>
+      <c r="F19" s="36"/>
+      <c r="G19" s="36"/>
+      <c r="H19" s="36"/>
+      <c r="I19" s="36"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A20" s="37"/>
-      <c r="B20" s="37"/>
-      <c r="C20" s="37"/>
-      <c r="D20" s="37"/>
-      <c r="E20" s="37"/>
-      <c r="F20" s="37"/>
-      <c r="G20" s="37"/>
-      <c r="H20" s="37"/>
-      <c r="I20" s="37"/>
+      <c r="A20" s="36"/>
+      <c r="B20" s="36"/>
+      <c r="C20" s="36"/>
+      <c r="D20" s="36"/>
+      <c r="E20" s="36"/>
+      <c r="F20" s="36"/>
+      <c r="G20" s="36"/>
+      <c r="H20" s="36"/>
+      <c r="I20" s="36"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -35940,7 +36033,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B007799-6C31-A447-9B6F-EA553D67BBB0}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7:M38"/>
     </sheetView>
   </sheetViews>
@@ -35969,4 +36062,248 @@
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB8FAB47-5DB0-2942-8AE1-E91249C6140C}">
+  <dimension ref="A1:O41"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="34.33203125" customWidth="1"/>
+    <col min="4" max="5" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="15" width="12.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>105</v>
+      </c>
+      <c r="K1" s="52" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>106</v>
+      </c>
+      <c r="K2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A6" s="51" t="s">
+        <v>108</v>
+      </c>
+      <c r="B6" t="s">
+        <v>109</v>
+      </c>
+      <c r="C6" t="s">
+        <v>110</v>
+      </c>
+      <c r="D6" t="s">
+        <v>111</v>
+      </c>
+      <c r="E6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F6" t="s">
+        <v>113</v>
+      </c>
+      <c r="G6" t="s">
+        <v>114</v>
+      </c>
+      <c r="H6" t="s">
+        <v>115</v>
+      </c>
+      <c r="I6" t="s">
+        <v>116</v>
+      </c>
+      <c r="J6" t="s">
+        <v>117</v>
+      </c>
+      <c r="K6" t="s">
+        <v>118</v>
+      </c>
+      <c r="L6" t="s">
+        <v>119</v>
+      </c>
+      <c r="M6" t="s">
+        <v>120</v>
+      </c>
+      <c r="N6" t="s">
+        <v>121</v>
+      </c>
+      <c r="O6" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A7" s="51">
+        <v>44972</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A8" s="51">
+        <v>89937</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A9" s="51">
+        <v>134921</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A10" s="51">
+        <v>179903</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A11" s="51">
+        <v>224883</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A12" s="51">
+        <v>269860</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A13" s="51">
+        <v>314838</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A14" s="51">
+        <v>359814</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A15" s="51">
+        <v>404787</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A16" s="51">
+        <v>449757</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A31" s="51" t="s">
+        <v>108</v>
+      </c>
+      <c r="B31" t="s">
+        <v>109</v>
+      </c>
+      <c r="C31" t="s">
+        <v>110</v>
+      </c>
+      <c r="D31" t="s">
+        <v>111</v>
+      </c>
+      <c r="E31" t="s">
+        <v>112</v>
+      </c>
+      <c r="F31" t="s">
+        <v>113</v>
+      </c>
+      <c r="G31" t="s">
+        <v>114</v>
+      </c>
+      <c r="H31" t="s">
+        <v>115</v>
+      </c>
+      <c r="I31" t="s">
+        <v>116</v>
+      </c>
+      <c r="J31" t="s">
+        <v>117</v>
+      </c>
+      <c r="K31" t="s">
+        <v>118</v>
+      </c>
+      <c r="L31" t="s">
+        <v>119</v>
+      </c>
+      <c r="M31" t="s">
+        <v>120</v>
+      </c>
+      <c r="N31" t="s">
+        <v>121</v>
+      </c>
+      <c r="O31" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A32" s="51">
+        <v>44972</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33" s="51">
+        <v>89937</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34" s="51">
+        <v>134921</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A35" s="51">
+        <v>179903</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A36" s="51">
+        <v>224883</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A37" s="51">
+        <v>269860</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A38" s="51">
+        <v>314838</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A39" s="51">
+        <v>359814</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A40" s="51">
+        <v>404787</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A41" s="51">
+        <v>449757</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added exported data (orgamised) for diff. II implementations; these data will be used into my Thesis section of sCPT CHapter
</commit_message>
<xml_diff>
--- a/results/cptVSsd_cpt.xlsx
+++ b/results/cptVSsd_cpt.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafaelktistakis/Repositories/C.CPT/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7878F905-F628-2140-B83B-5126A45A1AD5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77FA15EC-A19F-B444-A512-74BA00120B4B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" tabRatio="500" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25780" yWindow="0" windowWidth="25420" windowHeight="28800" tabRatio="500" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="All RAW Data" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="127">
   <si>
     <t>Trie Node Number</t>
   </si>
@@ -367,9 +367,6 @@
     <t>Exported queries (~9 items) through CPT+ execution during its II usage</t>
   </si>
   <si>
-    <t>Time Results (sec)</t>
-  </si>
-  <si>
     <t>Number of Sequences</t>
   </si>
   <si>
@@ -415,13 +412,19 @@
     <t>BV+Helper 16</t>
   </si>
   <si>
-    <t>Memory (Bytes)</t>
-  </si>
-  <si>
     <t>RESULTS WERE COPIED OVER HERE</t>
   </si>
   <si>
     <t>Original file in iCloud (numbers file): IIs execution time Analysis with CPT+ queries</t>
+  </si>
+  <si>
+    <t>WT similarity</t>
+  </si>
+  <si>
+    <t>Time Results (sec) * 10^6 = nano sec</t>
+  </si>
+  <si>
+    <t>Refer to original file if something is not clear here</t>
   </si>
 </sst>
 </file>
@@ -583,7 +586,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -641,6 +644,9 @@
     <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="27">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -36069,13 +36075,15 @@
   <dimension ref="A1:O41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="L37" sqref="L37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="34.33203125" customWidth="1"/>
+    <col min="3" max="3" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12.1640625" bestFit="1" customWidth="1"/>
@@ -36087,7 +36095,7 @@
         <v>105</v>
       </c>
       <c r="K1" s="52" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
@@ -36095,211 +36103,1056 @@
         <v>106</v>
       </c>
       <c r="K2" t="s">
-        <v>125</v>
+        <v>123</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="K3" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>107</v>
+        <v>125</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="51" t="s">
+        <v>107</v>
+      </c>
+      <c r="B6" t="s">
         <v>108</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>109</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>110</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>111</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>112</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>113</v>
       </c>
-      <c r="G6" t="s">
-        <v>114</v>
-      </c>
       <c r="H6" t="s">
+        <v>124</v>
+      </c>
+      <c r="I6" t="s">
         <v>115</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>116</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>117</v>
       </c>
-      <c r="K6" t="s">
+      <c r="L6" t="s">
         <v>118</v>
       </c>
-      <c r="L6" t="s">
+      <c r="M6" t="s">
         <v>119</v>
       </c>
-      <c r="M6" t="s">
+      <c r="N6" t="s">
         <v>120</v>
       </c>
-      <c r="N6" t="s">
+      <c r="O6" t="s">
         <v>121</v>
-      </c>
-      <c r="O6" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="51">
         <v>44972</v>
       </c>
+      <c r="B7" s="55">
+        <v>2.6</v>
+      </c>
+      <c r="C7" s="53">
+        <v>17500</v>
+      </c>
+      <c r="D7" s="55">
+        <v>504</v>
+      </c>
+      <c r="E7" s="55">
+        <v>19.399999999999999</v>
+      </c>
+      <c r="F7" s="55">
+        <v>10.1</v>
+      </c>
+      <c r="G7" s="55">
+        <v>20.2</v>
+      </c>
+      <c r="H7" s="55">
+        <v>261</v>
+      </c>
+      <c r="I7" s="55">
+        <v>87.626400000000004</v>
+      </c>
+      <c r="J7" s="55">
+        <v>2.78</v>
+      </c>
+      <c r="K7" s="55">
+        <v>5.07</v>
+      </c>
+      <c r="L7" s="55">
+        <v>44.8962</v>
+      </c>
+      <c r="M7" s="55">
+        <v>5.21</v>
+      </c>
+      <c r="N7" s="55">
+        <v>10.4</v>
+      </c>
+      <c r="O7" s="55">
+        <v>20.2</v>
+      </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="51">
         <v>89937</v>
       </c>
+      <c r="B8" s="55">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="C8" s="53">
+        <v>29600</v>
+      </c>
+      <c r="D8" s="55">
+        <v>1010</v>
+      </c>
+      <c r="E8" s="55">
+        <v>78.900000000000006</v>
+      </c>
+      <c r="F8" s="55">
+        <v>22.8</v>
+      </c>
+      <c r="G8" s="55">
+        <v>45.4</v>
+      </c>
+      <c r="H8" s="55">
+        <v>484</v>
+      </c>
+      <c r="I8" s="55">
+        <v>148.56299999999999</v>
+      </c>
+      <c r="J8" s="55">
+        <v>5.0599999999999996</v>
+      </c>
+      <c r="K8" s="55">
+        <v>32</v>
+      </c>
+      <c r="L8" s="55">
+        <v>79.006799999999998</v>
+      </c>
+      <c r="M8" s="55">
+        <v>10.6</v>
+      </c>
+      <c r="N8" s="55">
+        <v>21.8</v>
+      </c>
+      <c r="O8" s="55">
+        <v>42.2</v>
+      </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="51">
         <v>134921</v>
       </c>
+      <c r="B9" s="55">
+        <v>7.7</v>
+      </c>
+      <c r="C9" s="53">
+        <v>75300</v>
+      </c>
+      <c r="D9" s="55">
+        <v>2040</v>
+      </c>
+      <c r="E9" s="55">
+        <v>73.5</v>
+      </c>
+      <c r="F9" s="55">
+        <v>34.700000000000003</v>
+      </c>
+      <c r="G9" s="55">
+        <v>84.3</v>
+      </c>
+      <c r="H9" s="55">
+        <v>1170</v>
+      </c>
+      <c r="I9" s="55">
+        <v>397.91300000000001</v>
+      </c>
+      <c r="J9" s="55">
+        <v>7.77</v>
+      </c>
+      <c r="K9" s="55">
+        <v>7.56</v>
+      </c>
+      <c r="L9" s="55">
+        <v>71.266400000000004</v>
+      </c>
+      <c r="M9" s="55">
+        <v>16.7</v>
+      </c>
+      <c r="N9" s="55">
+        <v>33.700000000000003</v>
+      </c>
+      <c r="O9" s="55">
+        <v>65.900000000000006</v>
+      </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="51">
         <v>179903</v>
       </c>
+      <c r="B10" s="55">
+        <v>11</v>
+      </c>
+      <c r="C10" s="53">
+        <v>63000</v>
+      </c>
+      <c r="D10" s="55">
+        <v>2300</v>
+      </c>
+      <c r="E10" s="55">
+        <v>186</v>
+      </c>
+      <c r="F10" s="55">
+        <v>58.3</v>
+      </c>
+      <c r="G10" s="55">
+        <v>105</v>
+      </c>
+      <c r="H10" s="55">
+        <v>1120</v>
+      </c>
+      <c r="I10" s="55">
+        <v>348.62700000000001</v>
+      </c>
+      <c r="J10" s="55">
+        <v>7.05</v>
+      </c>
+      <c r="K10" s="55">
+        <v>62.2</v>
+      </c>
+      <c r="L10" s="55">
+        <v>253.42099999999999</v>
+      </c>
+      <c r="M10" s="55">
+        <v>22.2</v>
+      </c>
+      <c r="N10" s="55">
+        <v>45</v>
+      </c>
+      <c r="O10" s="55">
+        <v>86.5</v>
+      </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="51">
         <v>224883</v>
       </c>
+      <c r="B11" s="55">
+        <v>14</v>
+      </c>
+      <c r="C11" s="53">
+        <v>103000</v>
+      </c>
+      <c r="D11" s="55">
+        <v>3010</v>
+      </c>
+      <c r="E11" s="55">
+        <v>139</v>
+      </c>
+      <c r="F11" s="55">
+        <v>58.5</v>
+      </c>
+      <c r="G11" s="55">
+        <v>128</v>
+      </c>
+      <c r="H11" s="55">
+        <v>1790</v>
+      </c>
+      <c r="I11" s="55">
+        <v>548.89800000000002</v>
+      </c>
+      <c r="J11" s="55">
+        <v>18.899999999999999</v>
+      </c>
+      <c r="K11" s="55">
+        <v>48.1</v>
+      </c>
+      <c r="L11" s="55">
+        <v>294.65100000000001</v>
+      </c>
+      <c r="M11" s="55">
+        <v>26.6</v>
+      </c>
+      <c r="N11" s="55">
+        <v>53.5</v>
+      </c>
+      <c r="O11" s="55">
+        <v>105</v>
+      </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="51">
         <v>269860</v>
       </c>
+      <c r="B12" s="55">
+        <v>17</v>
+      </c>
+      <c r="C12" s="53">
+        <v>138000</v>
+      </c>
+      <c r="D12" s="55">
+        <v>4200</v>
+      </c>
+      <c r="E12" s="55">
+        <v>99.4</v>
+      </c>
+      <c r="F12" s="55">
+        <v>75.5</v>
+      </c>
+      <c r="G12" s="55">
+        <v>164</v>
+      </c>
+      <c r="H12" s="55">
+        <v>2350</v>
+      </c>
+      <c r="I12" s="55">
+        <v>884.90599999999995</v>
+      </c>
+      <c r="J12" s="55">
+        <v>18.7</v>
+      </c>
+      <c r="K12" s="55">
+        <v>18.7</v>
+      </c>
+      <c r="L12" s="55">
+        <v>389.85899999999998</v>
+      </c>
+      <c r="M12" s="55">
+        <v>34.700000000000003</v>
+      </c>
+      <c r="N12" s="55">
+        <v>68.8</v>
+      </c>
+      <c r="O12" s="55">
+        <v>135</v>
+      </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="51">
         <v>314838</v>
       </c>
+      <c r="B13" s="55">
+        <v>20</v>
+      </c>
+      <c r="C13" s="53">
+        <v>148000</v>
+      </c>
+      <c r="D13" s="55">
+        <v>4210</v>
+      </c>
+      <c r="E13" s="55">
+        <v>345</v>
+      </c>
+      <c r="F13" s="55">
+        <v>88.1</v>
+      </c>
+      <c r="G13" s="55">
+        <v>187</v>
+      </c>
+      <c r="H13" s="55">
+        <v>2440</v>
+      </c>
+      <c r="I13" s="55">
+        <v>885.56700000000001</v>
+      </c>
+      <c r="J13" s="55">
+        <v>13.1</v>
+      </c>
+      <c r="K13" s="55">
+        <v>111</v>
+      </c>
+      <c r="L13" s="55">
+        <v>383.44600000000003</v>
+      </c>
+      <c r="M13" s="55">
+        <v>38.1</v>
+      </c>
+      <c r="N13" s="55">
+        <v>77.5</v>
+      </c>
+      <c r="O13" s="55">
+        <v>152</v>
+      </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" s="51">
         <v>359814</v>
       </c>
+      <c r="B14" s="55">
+        <v>23</v>
+      </c>
+      <c r="C14" s="53">
+        <v>95300</v>
+      </c>
+      <c r="D14" s="55">
+        <v>4090</v>
+      </c>
+      <c r="E14" s="55">
+        <v>522</v>
+      </c>
+      <c r="F14" s="55">
+        <v>95.3</v>
+      </c>
+      <c r="G14" s="55">
+        <v>190</v>
+      </c>
+      <c r="H14" s="55">
+        <v>1750</v>
+      </c>
+      <c r="I14" s="55">
+        <v>587.96</v>
+      </c>
+      <c r="J14" s="55">
+        <v>66.5</v>
+      </c>
+      <c r="K14" s="55">
+        <v>178</v>
+      </c>
+      <c r="L14" s="55">
+        <v>229.12899999999999</v>
+      </c>
+      <c r="M14" s="55">
+        <v>44</v>
+      </c>
+      <c r="N14" s="55">
+        <v>88.1</v>
+      </c>
+      <c r="O14" s="55">
+        <v>170</v>
+      </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" s="51">
         <v>404787</v>
       </c>
+      <c r="B15" s="55">
+        <v>25</v>
+      </c>
+      <c r="C15" s="53">
+        <v>118000</v>
+      </c>
+      <c r="D15" s="55">
+        <v>5100</v>
+      </c>
+      <c r="E15" s="55">
+        <v>361</v>
+      </c>
+      <c r="F15" s="55">
+        <v>110</v>
+      </c>
+      <c r="G15" s="55">
+        <v>225</v>
+      </c>
+      <c r="H15" s="55">
+        <v>2270</v>
+      </c>
+      <c r="I15" s="55">
+        <v>656.274</v>
+      </c>
+      <c r="J15" s="55">
+        <v>54.3</v>
+      </c>
+      <c r="K15" s="55">
+        <v>143</v>
+      </c>
+      <c r="L15" s="55">
+        <v>456.24299999999999</v>
+      </c>
+      <c r="M15" s="55">
+        <v>49.3</v>
+      </c>
+      <c r="N15" s="55">
+        <v>99.4</v>
+      </c>
+      <c r="O15" s="55">
+        <v>195</v>
+      </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" s="51">
         <v>449757</v>
       </c>
+      <c r="B16" s="55">
+        <v>28</v>
+      </c>
+      <c r="C16" s="53">
+        <v>199000</v>
+      </c>
+      <c r="D16" s="55">
+        <v>6280</v>
+      </c>
+      <c r="E16" s="55">
+        <v>286</v>
+      </c>
+      <c r="F16" s="55">
+        <v>122</v>
+      </c>
+      <c r="G16" s="55">
+        <v>277</v>
+      </c>
+      <c r="H16" s="55">
+        <v>3280</v>
+      </c>
+      <c r="I16" s="55">
+        <v>1164.77</v>
+      </c>
+      <c r="J16" s="55">
+        <v>65.2</v>
+      </c>
+      <c r="K16" s="55">
+        <v>105</v>
+      </c>
+      <c r="L16" s="55">
+        <v>439.85700000000003</v>
+      </c>
+      <c r="M16" s="55">
+        <v>55.7</v>
+      </c>
+      <c r="N16" s="55">
+        <v>129</v>
+      </c>
+      <c r="O16" s="55">
+        <v>231</v>
+      </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>123</v>
+        <v>87</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A31" s="51" t="s">
+        <v>107</v>
+      </c>
+      <c r="B31" t="s">
         <v>108</v>
       </c>
-      <c r="B31" t="s">
+      <c r="C31" t="s">
         <v>109</v>
       </c>
-      <c r="C31" t="s">
+      <c r="D31" t="s">
         <v>110</v>
       </c>
-      <c r="D31" t="s">
+      <c r="E31" t="s">
         <v>111</v>
       </c>
-      <c r="E31" t="s">
+      <c r="F31" t="s">
         <v>112</v>
       </c>
-      <c r="F31" t="s">
+      <c r="G31" t="s">
         <v>113</v>
       </c>
-      <c r="G31" t="s">
+      <c r="H31" t="s">
         <v>114</v>
       </c>
-      <c r="H31" t="s">
+      <c r="I31" t="s">
         <v>115</v>
       </c>
-      <c r="I31" t="s">
+      <c r="J31" t="s">
         <v>116</v>
       </c>
-      <c r="J31" t="s">
+      <c r="K31" t="s">
         <v>117</v>
       </c>
-      <c r="K31" t="s">
+      <c r="L31" t="s">
         <v>118</v>
       </c>
-      <c r="L31" t="s">
+      <c r="M31" t="s">
         <v>119</v>
       </c>
-      <c r="M31" t="s">
+      <c r="N31" t="s">
         <v>120</v>
       </c>
-      <c r="N31" t="s">
+      <c r="O31" t="s">
         <v>121</v>
-      </c>
-      <c r="O31" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A32" s="51">
         <v>44972</v>
       </c>
+      <c r="B32" s="54">
+        <v>4.8899999999999997</v>
+      </c>
+      <c r="C32" s="54">
+        <v>0.92841099999999999</v>
+      </c>
+      <c r="D32" s="54">
+        <v>0.93</v>
+      </c>
+      <c r="E32" s="54">
+        <v>2.78</v>
+      </c>
+      <c r="F32" s="54">
+        <v>3.06</v>
+      </c>
+      <c r="G32" s="54">
+        <v>2.2599999999999998</v>
+      </c>
+      <c r="H32" s="54">
+        <v>1.6</v>
+      </c>
+      <c r="I32" s="54">
+        <v>0.509718</v>
+      </c>
+      <c r="J32" s="54">
+        <v>3.6</v>
+      </c>
+      <c r="K32" s="54">
+        <v>2.76</v>
+      </c>
+      <c r="L32" s="54">
+        <v>1.69208</v>
+      </c>
+      <c r="M32" s="54">
+        <v>2.31</v>
+      </c>
+      <c r="N32" s="54">
+        <v>1.62</v>
+      </c>
+      <c r="O32" s="54">
+        <v>1.18</v>
+      </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A33" s="51">
         <v>89937</v>
       </c>
+      <c r="B33" s="54">
+        <v>9.77</v>
+      </c>
+      <c r="C33" s="54">
+        <v>1.9160489999999999</v>
+      </c>
+      <c r="D33" s="54">
+        <v>1.8</v>
+      </c>
+      <c r="E33" s="54">
+        <v>5.53</v>
+      </c>
+      <c r="F33" s="54">
+        <v>6.12</v>
+      </c>
+      <c r="G33" s="54">
+        <v>4.5199999999999996</v>
+      </c>
+      <c r="H33" s="54">
+        <v>3.36</v>
+      </c>
+      <c r="I33" s="54">
+        <v>0.99899099999999996</v>
+      </c>
+      <c r="J33" s="54">
+        <v>7.25</v>
+      </c>
+      <c r="K33" s="54">
+        <v>5.49</v>
+      </c>
+      <c r="L33" s="54">
+        <v>3.3683200000000002</v>
+      </c>
+      <c r="M33" s="54">
+        <v>4.6100000000000003</v>
+      </c>
+      <c r="N33" s="54">
+        <v>3.23</v>
+      </c>
+      <c r="O33" s="54">
+        <v>2.34</v>
+      </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A34" s="51">
         <v>134921</v>
       </c>
+      <c r="B34" s="54">
+        <v>14.65</v>
+      </c>
+      <c r="C34" s="54">
+        <v>2.9083640000000002</v>
+      </c>
+      <c r="D34" s="54">
+        <v>2.69</v>
+      </c>
+      <c r="E34" s="54">
+        <v>8.2899999999999991</v>
+      </c>
+      <c r="F34" s="54">
+        <v>9.18</v>
+      </c>
+      <c r="G34" s="54">
+        <v>6.78</v>
+      </c>
+      <c r="H34" s="54">
+        <v>5.32</v>
+      </c>
+      <c r="I34" s="54">
+        <v>1.4875100000000001</v>
+      </c>
+      <c r="J34" s="54">
+        <v>10.89</v>
+      </c>
+      <c r="K34" s="54">
+        <v>8.2100000000000009</v>
+      </c>
+      <c r="L34" s="54">
+        <v>5.0148900000000003</v>
+      </c>
+      <c r="M34" s="54">
+        <v>6.91</v>
+      </c>
+      <c r="N34" s="54">
+        <v>4.83</v>
+      </c>
+      <c r="O34" s="54">
+        <v>3.51</v>
+      </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A35" s="51">
         <v>179903</v>
       </c>
+      <c r="B35" s="54">
+        <v>19.54</v>
+      </c>
+      <c r="C35" s="54">
+        <v>3.8546860000000001</v>
+      </c>
+      <c r="D35" s="54">
+        <v>3.57</v>
+      </c>
+      <c r="E35" s="54">
+        <v>11.05</v>
+      </c>
+      <c r="F35" s="54">
+        <v>12.23</v>
+      </c>
+      <c r="G35" s="54">
+        <v>9.0299999999999994</v>
+      </c>
+      <c r="H35" s="54">
+        <v>7.09</v>
+      </c>
+      <c r="I35" s="54">
+        <v>1.9766600000000001</v>
+      </c>
+      <c r="J35" s="54">
+        <v>14.51</v>
+      </c>
+      <c r="K35" s="54">
+        <v>11</v>
+      </c>
+      <c r="L35" s="54">
+        <v>6.6793899999999997</v>
+      </c>
+      <c r="M35" s="54">
+        <v>9.2100000000000009</v>
+      </c>
+      <c r="N35" s="54">
+        <v>6.44</v>
+      </c>
+      <c r="O35" s="54">
+        <v>4.68</v>
+      </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A36" s="51">
         <v>224883</v>
       </c>
+      <c r="B36" s="54">
+        <v>24.43</v>
+      </c>
+      <c r="C36" s="54">
+        <v>4.8074339999999998</v>
+      </c>
+      <c r="D36" s="54">
+        <v>4.45</v>
+      </c>
+      <c r="E36" s="54">
+        <v>13.81</v>
+      </c>
+      <c r="F36" s="54">
+        <v>15.28</v>
+      </c>
+      <c r="G36" s="54">
+        <v>11.29</v>
+      </c>
+      <c r="H36" s="54">
+        <v>8.84</v>
+      </c>
+      <c r="I36" s="54">
+        <v>2.4655999999999998</v>
+      </c>
+      <c r="J36" s="54">
+        <v>18.11</v>
+      </c>
+      <c r="K36" s="54">
+        <v>13.77</v>
+      </c>
+      <c r="L36" s="54">
+        <v>8.3453999999999997</v>
+      </c>
+      <c r="M36" s="54">
+        <v>11.5</v>
+      </c>
+      <c r="N36" s="54">
+        <v>8.0500000000000007</v>
+      </c>
+      <c r="O36" s="54">
+        <v>5.84</v>
+      </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A37" s="51">
         <v>269860</v>
       </c>
+      <c r="B37" s="54">
+        <v>29.35</v>
+      </c>
+      <c r="C37" s="54">
+        <v>5.7389200000000002</v>
+      </c>
+      <c r="D37" s="54">
+        <v>5.35</v>
+      </c>
+      <c r="E37" s="54">
+        <v>16.600000000000001</v>
+      </c>
+      <c r="F37" s="54">
+        <v>18.329999999999998</v>
+      </c>
+      <c r="G37" s="54">
+        <v>13.54</v>
+      </c>
+      <c r="H37" s="54">
+        <v>11.19</v>
+      </c>
+      <c r="I37" s="54">
+        <v>2.95438</v>
+      </c>
+      <c r="J37" s="54">
+        <v>21.73</v>
+      </c>
+      <c r="K37" s="54">
+        <v>16.489999999999998</v>
+      </c>
+      <c r="L37" s="54">
+        <v>10.0678</v>
+      </c>
+      <c r="M37" s="54">
+        <v>13.8</v>
+      </c>
+      <c r="N37" s="54">
+        <v>9.66</v>
+      </c>
+      <c r="O37" s="54">
+        <v>7.01</v>
+      </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A38" s="51">
         <v>314838</v>
       </c>
+      <c r="B38" s="54">
+        <v>34.28</v>
+      </c>
+      <c r="C38" s="54">
+        <v>6.6515740000000001</v>
+      </c>
+      <c r="D38" s="54">
+        <v>6.24</v>
+      </c>
+      <c r="E38" s="54">
+        <v>19.37</v>
+      </c>
+      <c r="F38" s="54">
+        <v>21.4</v>
+      </c>
+      <c r="G38" s="54">
+        <v>15.8</v>
+      </c>
+      <c r="H38" s="54">
+        <v>13.07</v>
+      </c>
+      <c r="I38" s="54">
+        <v>3.4433799999999999</v>
+      </c>
+      <c r="J38" s="54">
+        <v>25.28</v>
+      </c>
+      <c r="K38" s="54">
+        <v>19.239999999999998</v>
+      </c>
+      <c r="L38" s="54">
+        <v>11.645099999999999</v>
+      </c>
+      <c r="M38" s="54">
+        <v>16.100000000000001</v>
+      </c>
+      <c r="N38" s="54">
+        <v>11.26</v>
+      </c>
+      <c r="O38" s="54">
+        <v>8.18</v>
+      </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A39" s="51">
         <v>359814</v>
       </c>
+      <c r="B39" s="54">
+        <v>39.26</v>
+      </c>
+      <c r="C39" s="54">
+        <v>7.5901430000000003</v>
+      </c>
+      <c r="D39" s="54">
+        <v>7.14</v>
+      </c>
+      <c r="E39" s="54">
+        <v>22.18</v>
+      </c>
+      <c r="F39" s="54">
+        <v>24.45</v>
+      </c>
+      <c r="G39" s="54">
+        <v>18.059999999999999</v>
+      </c>
+      <c r="H39" s="54">
+        <v>14.93</v>
+      </c>
+      <c r="I39" s="54">
+        <v>3.9345300000000001</v>
+      </c>
+      <c r="J39" s="54">
+        <v>28.97</v>
+      </c>
+      <c r="K39" s="54">
+        <v>21.99</v>
+      </c>
+      <c r="L39" s="54">
+        <v>13.3462</v>
+      </c>
+      <c r="M39" s="54">
+        <v>18.41</v>
+      </c>
+      <c r="N39" s="54">
+        <v>12.88</v>
+      </c>
+      <c r="O39" s="54">
+        <v>9.36</v>
+      </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A40" s="51">
         <v>404787</v>
       </c>
+      <c r="B40" s="54">
+        <v>44.16</v>
+      </c>
+      <c r="C40" s="54">
+        <v>8.4808819999999994</v>
+      </c>
+      <c r="D40" s="54">
+        <v>8.0299999999999994</v>
+      </c>
+      <c r="E40" s="54">
+        <v>24.95</v>
+      </c>
+      <c r="F40" s="54">
+        <v>27.5</v>
+      </c>
+      <c r="G40" s="54">
+        <v>20.309999999999999</v>
+      </c>
+      <c r="H40" s="54">
+        <v>16.77</v>
+      </c>
+      <c r="I40" s="54">
+        <v>4.4217500000000003</v>
+      </c>
+      <c r="J40" s="54">
+        <v>32.590000000000003</v>
+      </c>
+      <c r="K40" s="54">
+        <v>24.74</v>
+      </c>
+      <c r="L40" s="54">
+        <v>14.882400000000001</v>
+      </c>
+      <c r="M40" s="54">
+        <v>20.71</v>
+      </c>
+      <c r="N40" s="54">
+        <v>14.49</v>
+      </c>
+      <c r="O40" s="54">
+        <v>10.52</v>
+      </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A41" s="51">
         <v>449757</v>
+      </c>
+      <c r="B41" s="54">
+        <v>49.07</v>
+      </c>
+      <c r="C41" s="54">
+        <v>9.3969310000000004</v>
+      </c>
+      <c r="D41" s="54">
+        <v>8.92</v>
+      </c>
+      <c r="E41" s="54">
+        <v>27.72</v>
+      </c>
+      <c r="F41" s="54">
+        <v>30.54</v>
+      </c>
+      <c r="G41" s="54">
+        <v>22.56</v>
+      </c>
+      <c r="H41" s="54">
+        <v>18.64</v>
+      </c>
+      <c r="I41" s="54">
+        <v>4.9102100000000002</v>
+      </c>
+      <c r="J41" s="54">
+        <v>36.159999999999997</v>
+      </c>
+      <c r="K41" s="54">
+        <v>27.48</v>
+      </c>
+      <c r="L41" s="54">
+        <v>16.627600000000001</v>
+      </c>
+      <c r="M41" s="54">
+        <v>23</v>
+      </c>
+      <c r="N41" s="54">
+        <v>16.09</v>
+      </c>
+      <c r="O41" s="54">
+        <v>11.69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated exported spreadsheet with some corrections on missing headers calculations
</commit_message>
<xml_diff>
--- a/results/cptVSsd_cpt.xlsx
+++ b/results/cptVSsd_cpt.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="26440" windowHeight="18000" tabRatio="500" firstSheet="8" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="26440" windowHeight="16640" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="All RAW Data" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="134">
   <si>
     <t>Trie Node Number</t>
   </si>
@@ -430,6 +430,24 @@
   <si>
     <t>Elias-Fano 128</t>
   </si>
+  <si>
+    <t>I copied over below the exported memory results; then I added up missing header memory calculations</t>
+  </si>
+  <si>
+    <t>This memory headers were not added up during memory exports at runtime</t>
+  </si>
+  <si>
+    <t>The missing memory header was from II for 8 bytes per row and an overall header for II table of 8 bytes.</t>
+  </si>
+  <si>
+    <t>All this is negiclible but I added for the sake of being consistent with Thesis wriging and arguments</t>
+  </si>
+  <si>
+    <t>EF::II MB with missing headers; this column will be used to add-up the headers</t>
+  </si>
+  <si>
+    <t>PT has one extra int per node (extra than PAKDD and Ipredict framework specifies); this is exported in memory results and should be adapted. However, scalability and comparisons should not be affected since is a consistent overload</t>
+  </si>
 </sst>
 </file>
 
@@ -567,7 +585,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="27">
+  <cellStyleXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -595,8 +613,42 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -657,8 +709,11 @@
     <xf numFmtId="1" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="27">
+  <cellStyles count="61">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -672,6 +727,23 @@
     <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -685,6 +757,23 @@
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1174,11 +1263,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-166200416"/>
-        <c:axId val="-167712560"/>
+        <c:axId val="873247040"/>
+        <c:axId val="836324032"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-166200416"/>
+        <c:axId val="873247040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1281,7 +1370,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-167712560"/>
+        <c:crossAx val="836324032"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1289,7 +1378,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-167712560"/>
+        <c:axId val="836324032"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -1396,7 +1485,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-166200416"/>
+        <c:crossAx val="873247040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2018,11 +2107,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-162760592"/>
-        <c:axId val="-210403232"/>
+        <c:axId val="873435648"/>
+        <c:axId val="873439920"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-162760592"/>
+        <c:axId val="873435648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2120,7 +2209,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-210403232"/>
+        <c:crossAx val="873439920"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2128,7 +2217,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-210403232"/>
+        <c:axId val="873439920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2234,7 +2323,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-162760592"/>
+        <c:crossAx val="873435648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3136,11 +3225,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-166604704"/>
-        <c:axId val="-166601312"/>
+        <c:axId val="835905584"/>
+        <c:axId val="835908976"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-166604704"/>
+        <c:axId val="835905584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3238,7 +3327,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-166601312"/>
+        <c:crossAx val="835908976"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3246,7 +3335,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-166601312"/>
+        <c:axId val="835908976"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -3353,7 +3442,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-166604704"/>
+        <c:crossAx val="835905584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3525,7 +3614,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -3673,7 +3761,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -3824,7 +3911,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -3914,11 +4000,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-167632368"/>
-        <c:axId val="-167600704"/>
+        <c:axId val="873952032"/>
+        <c:axId val="873956576"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-167632368"/>
+        <c:axId val="873952032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3950,7 +4036,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4017,7 +4102,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-167600704"/>
+        <c:crossAx val="873956576"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4025,7 +4110,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-167600704"/>
+        <c:axId val="873956576"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -4072,7 +4157,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4133,7 +4217,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-167632368"/>
+        <c:crossAx val="873952032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4147,7 +4231,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4295,9 +4378,7 @@
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000000-F3D7-0A4B-B57A-C85E738D3E45}"/>
                 </c:ext>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -4319,9 +4400,7 @@
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000001-F3D7-0A4B-B57A-C85E738D3E45}"/>
                 </c:ext>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -4343,9 +4422,7 @@
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000002-F3D7-0A4B-B57A-C85E738D3E45}"/>
                 </c:ext>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -4367,9 +4444,7 @@
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000003-F3D7-0A4B-B57A-C85E738D3E45}"/>
                 </c:ext>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -4391,9 +4466,7 @@
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000004-F3D7-0A4B-B57A-C85E738D3E45}"/>
                 </c:ext>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -4415,9 +4488,7 @@
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000005-F3D7-0A4B-B57A-C85E738D3E45}"/>
                 </c:ext>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:numFmt formatCode="#,##0.00" sourceLinked="0"/>
@@ -4587,9 +4658,7 @@
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000007-F3D7-0A4B-B57A-C85E738D3E45}"/>
                 </c:ext>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -4611,9 +4680,7 @@
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000008-F3D7-0A4B-B57A-C85E738D3E45}"/>
                 </c:ext>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -4635,9 +4702,7 @@
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000009-F3D7-0A4B-B57A-C85E738D3E45}"/>
                 </c:ext>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -4659,9 +4724,7 @@
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{0000000A-F3D7-0A4B-B57A-C85E738D3E45}"/>
                 </c:ext>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -4683,9 +4746,7 @@
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{0000000B-F3D7-0A4B-B57A-C85E738D3E45}"/>
                 </c:ext>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -4707,9 +4768,7 @@
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{0000000C-F3D7-0A4B-B57A-C85E738D3E45}"/>
                 </c:ext>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:numFmt formatCode="#,##0.00" sourceLinked="0"/>
@@ -4879,9 +4938,7 @@
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{0000000F-F3D7-0A4B-B57A-C85E738D3E45}"/>
                 </c:ext>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -4903,9 +4960,7 @@
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000010-F3D7-0A4B-B57A-C85E738D3E45}"/>
                 </c:ext>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:numFmt formatCode="#,##0.00" sourceLinked="0"/>
@@ -4948,7 +5003,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -5038,11 +5092,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-166496800"/>
-        <c:axId val="-166492896"/>
+        <c:axId val="831001952"/>
+        <c:axId val="831005856"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-166496800"/>
+        <c:axId val="831001952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5074,7 +5128,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -5141,7 +5194,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-166492896"/>
+        <c:crossAx val="831005856"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5149,7 +5202,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-166492896"/>
+        <c:axId val="831005856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5195,7 +5248,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -5256,7 +5308,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-166496800"/>
+        <c:crossAx val="831001952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:minorUnit val="0.01"/>
@@ -5271,7 +5323,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5438,7 +5489,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -5587,7 +5637,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -5640,22 +5689,22 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>10.418</c:v>
+                  <c:v>10.4218</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>11.543</c:v>
+                  <c:v>11.550344</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12.314</c:v>
+                  <c:v>12.324464</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>12.589</c:v>
+                  <c:v>12.602648</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>12.794</c:v>
+                  <c:v>12.810144</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>12.929</c:v>
+                  <c:v>12.929008</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5738,7 +5787,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -5828,11 +5876,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-322384800"/>
-        <c:axId val="-321960496"/>
+        <c:axId val="874002144"/>
+        <c:axId val="808668496"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-322384800"/>
+        <c:axId val="874002144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5864,7 +5912,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -5931,7 +5978,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-321960496"/>
+        <c:crossAx val="808668496"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5939,7 +5986,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-321960496"/>
+        <c:axId val="808668496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5985,7 +6032,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -6046,7 +6092,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-322384800"/>
+        <c:crossAx val="874002144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6060,7 +6106,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6227,7 +6272,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -6364,7 +6408,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -6501,7 +6544,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -6579,11 +6621,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-162746208"/>
-        <c:axId val="-162742304"/>
+        <c:axId val="808718304"/>
+        <c:axId val="874032000"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-162746208"/>
+        <c:axId val="808718304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6615,7 +6657,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -6682,7 +6723,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-162742304"/>
+        <c:crossAx val="874032000"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6690,7 +6731,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-162742304"/>
+        <c:axId val="874032000"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -6737,7 +6778,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -6798,7 +6838,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-162746208"/>
+        <c:crossAx val="808718304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6812,7 +6852,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6960,9 +6999,7 @@
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000000-08F2-4040-8635-654A70E2FB51}"/>
                 </c:ext>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -6984,9 +7021,7 @@
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000001-08F2-4040-8635-654A70E2FB51}"/>
                 </c:ext>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -7008,9 +7043,7 @@
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000002-08F2-4040-8635-654A70E2FB51}"/>
                 </c:ext>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -7032,9 +7065,7 @@
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000003-08F2-4040-8635-654A70E2FB51}"/>
                 </c:ext>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:numFmt formatCode="#,##0.00" sourceLinked="0"/>
@@ -7192,9 +7223,7 @@
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000005-08F2-4040-8635-654A70E2FB51}"/>
                 </c:ext>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -7216,9 +7245,7 @@
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000006-08F2-4040-8635-654A70E2FB51}"/>
                 </c:ext>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -7240,9 +7267,7 @@
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000007-08F2-4040-8635-654A70E2FB51}"/>
                 </c:ext>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -7264,9 +7289,7 @@
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000008-08F2-4040-8635-654A70E2FB51}"/>
                 </c:ext>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:numFmt formatCode="#,##0.00" sourceLinked="0"/>
@@ -7445,7 +7468,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -7523,11 +7545,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-167538720"/>
-        <c:axId val="-167534816"/>
+        <c:axId val="835922480"/>
+        <c:axId val="874058512"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-167538720"/>
+        <c:axId val="835922480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7559,7 +7581,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -7626,7 +7647,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-167534816"/>
+        <c:crossAx val="874058512"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7634,7 +7655,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-167534816"/>
+        <c:axId val="874058512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7680,7 +7701,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -7741,7 +7761,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-167538720"/>
+        <c:crossAx val="835922480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7755,7 +7775,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7921,7 +7940,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -8057,7 +8075,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -8101,19 +8118,19 @@
             <c:numRef>
               <c:f>'Scalability sCPT  HYBRID'!$B$10:$E$10</c:f>
               <c:numCache>
-                <c:formatCode>0.0</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>16.196</c:v>
+                  <c:v>16.203344</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>15.041</c:v>
+                  <c:v>15.048344</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11.543</c:v>
+                  <c:v>11.550344</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.9244</c:v>
+                  <c:v>6.931744</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8193,7 +8210,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -8271,11 +8287,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-322945296"/>
-        <c:axId val="-322941392"/>
+        <c:axId val="809453424"/>
+        <c:axId val="809428992"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-322945296"/>
+        <c:axId val="809453424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8307,7 +8323,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -8374,7 +8389,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-322941392"/>
+        <c:crossAx val="809428992"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8382,7 +8397,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-322941392"/>
+        <c:axId val="809428992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8428,7 +8443,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -8489,7 +8503,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-322945296"/>
+        <c:crossAx val="809453424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8503,7 +8517,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -8651,9 +8664,7 @@
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000000-BAE4-2C41-9E09-D86358EE871D}"/>
                 </c:ext>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -8675,9 +8686,7 @@
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000001-BAE4-2C41-9E09-D86358EE871D}"/>
                 </c:ext>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -8699,9 +8708,7 @@
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000002-BAE4-2C41-9E09-D86358EE871D}"/>
                 </c:ext>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -8723,9 +8730,7 @@
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000003-BAE4-2C41-9E09-D86358EE871D}"/>
                 </c:ext>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -8747,9 +8752,7 @@
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000004-BAE4-2C41-9E09-D86358EE871D}"/>
                 </c:ext>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:numFmt formatCode="#,##0" sourceLinked="0"/>
@@ -8946,7 +8949,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -9105,7 +9107,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -9179,11 +9180,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-163506544"/>
-        <c:axId val="-163503152"/>
+        <c:axId val="874099776"/>
+        <c:axId val="874103536"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-163506544"/>
+        <c:axId val="874099776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9215,7 +9216,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -9282,7 +9282,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-163503152"/>
+        <c:crossAx val="874103536"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9290,7 +9290,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-163503152"/>
+        <c:axId val="874103536"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -9337,7 +9337,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -9400,7 +9399,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-163506544"/>
+        <c:crossAx val="874099776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9414,7 +9413,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -9562,9 +9560,7 @@
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000000-B427-6747-8744-9B91A4BA03E5}"/>
                 </c:ext>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -9586,9 +9582,7 @@
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000001-B427-6747-8744-9B91A4BA03E5}"/>
                 </c:ext>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -9610,9 +9604,7 @@
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000002-B427-6747-8744-9B91A4BA03E5}"/>
                 </c:ext>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -9634,9 +9626,7 @@
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000014-B427-6747-8744-9B91A4BA03E5}"/>
                 </c:ext>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -9658,9 +9648,7 @@
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000013-B427-6747-8744-9B91A4BA03E5}"/>
                 </c:ext>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:numFmt formatCode="#,##0.00" sourceLinked="0"/>
@@ -9838,9 +9826,7 @@
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000005-B427-6747-8744-9B91A4BA03E5}"/>
                 </c:ext>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -9862,9 +9848,7 @@
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000006-B427-6747-8744-9B91A4BA03E5}"/>
                 </c:ext>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -9886,9 +9870,7 @@
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000007-B427-6747-8744-9B91A4BA03E5}"/>
                 </c:ext>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -9910,9 +9892,7 @@
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000008-B427-6747-8744-9B91A4BA03E5}"/>
                 </c:ext>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -9934,9 +9914,7 @@
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000009-B427-6747-8744-9B91A4BA03E5}"/>
                 </c:ext>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -10113,9 +10091,7 @@
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{0000000E-B427-6747-8744-9B91A4BA03E5}"/>
                 </c:ext>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -10137,9 +10113,7 @@
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{0000000F-B427-6747-8744-9B91A4BA03E5}"/>
                 </c:ext>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -10161,9 +10135,7 @@
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000010-B427-6747-8744-9B91A4BA03E5}"/>
                 </c:ext>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -10185,9 +10157,7 @@
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000011-B427-6747-8744-9B91A4BA03E5}"/>
                 </c:ext>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -10209,9 +10179,7 @@
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000012-B427-6747-8744-9B91A4BA03E5}"/>
                 </c:ext>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:numFmt formatCode="#,##0.00" sourceLinked="0"/>
@@ -10325,11 +10293,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-163446480"/>
-        <c:axId val="-163443088"/>
+        <c:axId val="831042784"/>
+        <c:axId val="809406416"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-163446480"/>
+        <c:axId val="831042784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10361,7 +10329,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -10428,7 +10395,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-163443088"/>
+        <c:crossAx val="809406416"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10436,7 +10403,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-163443088"/>
+        <c:axId val="809406416"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -10483,7 +10450,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -10544,7 +10510,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-163446480"/>
+        <c:crossAx val="831042784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10558,7 +10524,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -11376,11 +11341,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-167390240"/>
-        <c:axId val="-167032400"/>
+        <c:axId val="873789680"/>
+        <c:axId val="873793536"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-167390240"/>
+        <c:axId val="873789680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11478,7 +11443,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-167032400"/>
+        <c:crossAx val="873793536"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11486,7 +11451,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-167032400"/>
+        <c:axId val="873793536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11592,7 +11557,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-167390240"/>
+        <c:crossAx val="873789680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:minorUnit val="0.01"/>
@@ -11754,9 +11719,7 @@
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{0000000A-3370-374A-8692-2C19D9AA7FC9}"/>
                 </c:ext>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -11778,9 +11741,7 @@
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000008-3370-374A-8692-2C19D9AA7FC9}"/>
                 </c:ext>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -11802,9 +11763,7 @@
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000007-3370-374A-8692-2C19D9AA7FC9}"/>
                 </c:ext>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -11826,9 +11785,7 @@
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000000-3370-374A-8692-2C19D9AA7FC9}"/>
                 </c:ext>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:numFmt formatCode="#,##0" sourceLinked="0"/>
@@ -11869,7 +11826,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -11993,9 +11949,7 @@
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000002-3370-374A-8692-2C19D9AA7FC9}"/>
                 </c:ext>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -12017,9 +11971,7 @@
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000005-3370-374A-8692-2C19D9AA7FC9}"/>
                 </c:ext>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -12041,9 +11993,7 @@
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000006-3370-374A-8692-2C19D9AA7FC9}"/>
                 </c:ext>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:numFmt formatCode="#,##0" sourceLinked="0"/>
@@ -12084,7 +12034,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -12131,22 +12080,22 @@
             <c:numRef>
               <c:f>'Scalability sCPT  HYBRID'!$B$15:$F$15</c:f>
               <c:numCache>
-                <c:formatCode>0.0</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>4.982</c:v>
+                  <c:v>4.989344</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.8733</c:v>
+                  <c:v>9.880644</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>19.581</c:v>
+                  <c:v>19.588344</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>39.14</c:v>
+                  <c:v>39.147344</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>78.849</c:v>
+                  <c:v>78.85634400000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12208,9 +12157,7 @@
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000009-3370-374A-8692-2C19D9AA7FC9}"/>
                 </c:ext>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:numFmt formatCode="#,##0" sourceLinked="0"/>
@@ -12251,7 +12198,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -12311,11 +12257,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-163401216"/>
-        <c:axId val="-163397312"/>
+        <c:axId val="809334000"/>
+        <c:axId val="809337904"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-163401216"/>
+        <c:axId val="809334000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12347,7 +12293,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -12414,7 +12359,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-163397312"/>
+        <c:crossAx val="809337904"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12422,7 +12367,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-163397312"/>
+        <c:axId val="809337904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12468,7 +12413,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -12529,7 +12473,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-163401216"/>
+        <c:crossAx val="809334000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -12543,7 +12487,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -13155,11 +13098,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-163363488"/>
-        <c:axId val="-163359584"/>
+        <c:axId val="835973520"/>
+        <c:axId val="835977424"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-163363488"/>
+        <c:axId val="835973520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13257,7 +13200,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-163359584"/>
+        <c:crossAx val="835977424"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13265,7 +13208,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-163359584"/>
+        <c:axId val="835977424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13371,7 +13314,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-163363488"/>
+        <c:crossAx val="835973520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -14725,11 +14668,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-167195744"/>
-        <c:axId val="-167193616"/>
+        <c:axId val="809371520"/>
+        <c:axId val="874110832"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-167195744"/>
+        <c:axId val="809371520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14828,7 +14771,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-167193616"/>
+        <c:crossAx val="874110832"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -14837,7 +14780,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-167193616"/>
+        <c:axId val="874110832"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -14950,7 +14893,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-167195744"/>
+        <c:crossAx val="809371520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -15327,11 +15270,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="28"/>
-        <c:axId val="-167651088"/>
-        <c:axId val="-167649040"/>
+        <c:axId val="836041408"/>
+        <c:axId val="836043728"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-167651088"/>
+        <c:axId val="836041408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15374,7 +15317,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-167649040"/>
+        <c:crossAx val="836043728"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -15382,7 +15325,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-167649040"/>
+        <c:axId val="836043728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15495,7 +15438,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-167651088"/>
+        <c:crossAx val="836041408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -16308,11 +16251,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-167669712"/>
-        <c:axId val="-167666048"/>
+        <c:axId val="836091920"/>
+        <c:axId val="836095552"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-167669712"/>
+        <c:axId val="836091920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16411,7 +16354,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-167666048"/>
+        <c:crossAx val="836095552"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -16420,7 +16363,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-167666048"/>
+        <c:axId val="836095552"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -16533,7 +16476,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-167669712"/>
+        <c:crossAx val="836091920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -17096,11 +17039,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-167208640"/>
-        <c:axId val="-163331232"/>
+        <c:axId val="874142432"/>
+        <c:axId val="874146192"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-167208640"/>
+        <c:axId val="874142432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -17199,7 +17142,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-163331232"/>
+        <c:crossAx val="874146192"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -17208,7 +17151,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-163331232"/>
+        <c:axId val="874146192"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -17321,7 +17264,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-167208640"/>
+        <c:crossAx val="874142432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -17743,11 +17686,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="28"/>
-        <c:axId val="-210669488"/>
-        <c:axId val="-210667168"/>
+        <c:axId val="809386432"/>
+        <c:axId val="809233216"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-210669488"/>
+        <c:axId val="809386432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -17790,7 +17733,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-210667168"/>
+        <c:crossAx val="809233216"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -17798,7 +17741,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-210667168"/>
+        <c:axId val="809233216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -17911,7 +17854,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-210669488"/>
+        <c:crossAx val="809386432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.5"/>
@@ -18359,22 +18302,22 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>10.418</c:v>
+                  <c:v>10.4218</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>11.543</c:v>
+                  <c:v>11.550344</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12.314</c:v>
+                  <c:v>12.324464</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>12.589</c:v>
+                  <c:v>12.602648</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>12.794</c:v>
+                  <c:v>12.810144</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>12.929</c:v>
+                  <c:v>12.929008</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -18487,11 +18430,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-166815824"/>
-        <c:axId val="-210479712"/>
+        <c:axId val="830954576"/>
+        <c:axId val="835801216"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-166815824"/>
+        <c:axId val="830954576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -18589,7 +18532,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-210479712"/>
+        <c:crossAx val="835801216"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -18597,7 +18540,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-210479712"/>
+        <c:axId val="835801216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -18703,7 +18646,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-166815824"/>
+        <c:crossAx val="830954576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -19240,11 +19183,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-322131280"/>
-        <c:axId val="-166422064"/>
+        <c:axId val="873835904"/>
+        <c:axId val="873326128"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-322131280"/>
+        <c:axId val="873835904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -19342,7 +19285,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-166422064"/>
+        <c:crossAx val="873326128"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -19350,7 +19293,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-166422064"/>
+        <c:axId val="873326128"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -19457,7 +19400,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-322131280"/>
+        <c:crossAx val="873835904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -20162,11 +20105,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-163060832"/>
-        <c:axId val="-163056960"/>
+        <c:axId val="873345280"/>
+        <c:axId val="873349136"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-163060832"/>
+        <c:axId val="873345280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -20264,7 +20207,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-163056960"/>
+        <c:crossAx val="873349136"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -20272,7 +20215,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-163056960"/>
+        <c:axId val="873349136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -20378,7 +20321,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-163060832"/>
+        <c:crossAx val="873345280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -20794,19 +20737,19 @@
             <c:numRef>
               <c:f>'Scalability sCPT  HYBRID'!$B$10:$E$10</c:f>
               <c:numCache>
-                <c:formatCode>0.0</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>16.196</c:v>
+                  <c:v>16.203344</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>15.041</c:v>
+                  <c:v>15.048344</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11.543</c:v>
+                  <c:v>11.550344</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.9244</c:v>
+                  <c:v>6.931744</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -20907,11 +20850,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-162843680"/>
-        <c:axId val="-162840048"/>
+        <c:axId val="835844224"/>
+        <c:axId val="835847856"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-162843680"/>
+        <c:axId val="835844224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -21009,7 +20952,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-162840048"/>
+        <c:crossAx val="835847856"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -21017,7 +20960,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-162840048"/>
+        <c:axId val="835847856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -21123,7 +21066,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-162843680"/>
+        <c:crossAx val="835844224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -21794,11 +21737,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-378649664"/>
-        <c:axId val="-378646272"/>
+        <c:axId val="835859392"/>
+        <c:axId val="835862784"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-378649664"/>
+        <c:axId val="835859392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -21896,7 +21839,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-378646272"/>
+        <c:crossAx val="835862784"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -21904,7 +21847,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-378646272"/>
+        <c:axId val="835862784"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -22013,7 +21956,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-378649664"/>
+        <c:crossAx val="835859392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -22755,11 +22698,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-162800304"/>
-        <c:axId val="-162796912"/>
+        <c:axId val="873384720"/>
+        <c:axId val="873388480"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-162800304"/>
+        <c:axId val="873384720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -22857,7 +22800,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-162796912"/>
+        <c:crossAx val="873388480"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -22865,7 +22808,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-162796912"/>
+        <c:axId val="873388480"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -22972,7 +22915,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-162800304"/>
+        <c:crossAx val="873384720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -23437,22 +23380,22 @@
             <c:numRef>
               <c:f>'Scalability sCPT  HYBRID'!$B$15:$F$15</c:f>
               <c:numCache>
-                <c:formatCode>0.0</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>4.982</c:v>
+                  <c:v>4.989344</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.8733</c:v>
+                  <c:v>9.880644</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>19.581</c:v>
+                  <c:v>19.588344</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>39.14</c:v>
+                  <c:v>39.147344</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>78.849</c:v>
+                  <c:v>78.85634400000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -23535,11 +23478,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-323169472"/>
-        <c:axId val="-381435872"/>
+        <c:axId val="873902272"/>
+        <c:axId val="873906544"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-323169472"/>
+        <c:axId val="873902272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -23637,7 +23580,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-381435872"/>
+        <c:crossAx val="873906544"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -23645,7 +23588,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-381435872"/>
+        <c:axId val="873906544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -23751,7 +23694,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-323169472"/>
+        <c:crossAx val="873902272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -37980,7 +37923,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BDD37540-7869-CC44-AD8E-7785C3220739}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{BDD37540-7869-CC44-AD8E-7785C3220739}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -38018,7 +37961,7 @@
         <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5804CB95-1DE4-914E-B325-A834C0A2C2B1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{5804CB95-1DE4-914E-B325-A834C0A2C2B1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -38056,7 +37999,7 @@
         <xdr:cNvPr id="4" name="Chart 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A9AF7D88-9F81-FB4F-ACE8-B0448487158A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A9AF7D88-9F81-FB4F-ACE8-B0448487158A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -38094,7 +38037,7 @@
         <xdr:cNvPr id="5" name="Chart 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DAAB4B1F-B8EB-6042-917C-7A3C4D6A2E63}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{DAAB4B1F-B8EB-6042-917C-7A3C4D6A2E63}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -38132,7 +38075,7 @@
         <xdr:cNvPr id="6" name="Chart 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A9D2C9FA-83DD-A04E-AA7A-A99060986607}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A9D2C9FA-83DD-A04E-AA7A-A99060986607}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -38170,7 +38113,7 @@
         <xdr:cNvPr id="7" name="Chart 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1CEC4ADE-EE65-5943-994C-6EDEE463FAF0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{1CEC4ADE-EE65-5943-994C-6EDEE463FAF0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -38208,7 +38151,7 @@
         <xdr:cNvPr id="8" name="Chart 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B392B203-30BA-BC4B-8191-CD527C17FC57}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{B392B203-30BA-BC4B-8191-CD527C17FC57}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -38246,7 +38189,7 @@
         <xdr:cNvPr id="9" name="Chart 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{20429BD7-D26A-2A4D-9BC3-AA68737B7E88}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{20429BD7-D26A-2A4D-9BC3-AA68737B7E88}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -38284,7 +38227,7 @@
         <xdr:cNvPr id="10" name="Chart 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BDD7CFD4-4571-1D49-A7CD-4B10ABE01D3C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{BDD7CFD4-4571-1D49-A7CD-4B10ABE01D3C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -38322,7 +38265,7 @@
         <xdr:cNvPr id="11" name="Chart 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{184B5225-4C5D-F943-B871-01DB11EBB05E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{184B5225-4C5D-F943-B871-01DB11EBB05E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -38365,7 +38308,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DD8CD7BA-2E25-7C45-9947-E5E3F23F30F6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{DD8CD7BA-2E25-7C45-9947-E5E3F23F30F6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -38408,7 +38351,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{91FCB375-F451-9D45-BC19-B7E4BBC0AA92}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{91FCB375-F451-9D45-BC19-B7E4BBC0AA92}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -38446,7 +38389,7 @@
         <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{253B8090-3C7B-6A40-8F24-3863BA4E3805}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{253B8090-3C7B-6A40-8F24-3863BA4E3805}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -38484,7 +38427,7 @@
         <xdr:cNvPr id="4" name="Chart 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{24FDA3D5-2A31-6145-9F77-B32BC9E82EC5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{24FDA3D5-2A31-6145-9F77-B32BC9E82EC5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -38522,7 +38465,7 @@
         <xdr:cNvPr id="5" name="Chart 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E02EBD22-BD9C-9C4A-AC02-577620246B59}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E02EBD22-BD9C-9C4A-AC02-577620246B59}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -38560,7 +38503,7 @@
         <xdr:cNvPr id="6" name="Chart 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{58E7568E-EBFE-2345-A49E-17D5D79BEB63}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{58E7568E-EBFE-2345-A49E-17D5D79BEB63}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -38598,7 +38541,7 @@
         <xdr:cNvPr id="7" name="Chart 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{632563F3-670C-BC4B-9418-51C102FCCC47}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{632563F3-670C-BC4B-9418-51C102FCCC47}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -38636,7 +38579,7 @@
         <xdr:cNvPr id="8" name="Chart 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{54266E2A-938E-5549-AEF5-2937056460A7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{54266E2A-938E-5549-AEF5-2937056460A7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -38674,7 +38617,7 @@
         <xdr:cNvPr id="9" name="Chart 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D83B7A2D-35A0-3746-89C1-73DC3788E8C7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D83B7A2D-35A0-3746-89C1-73DC3788E8C7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -38712,7 +38655,7 @@
         <xdr:cNvPr id="10" name="Chart 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{465E8062-82DD-354D-866E-725AACBBFB23}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{465E8062-82DD-354D-866E-725AACBBFB23}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -38750,7 +38693,7 @@
         <xdr:cNvPr id="11" name="Chart 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0B19DCC6-97CA-D94A-99B5-AB9153A08F76}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0B19DCC6-97CA-D94A-99B5-AB9153A08F76}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -38793,7 +38736,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{91FCB375-F451-9D45-BC19-B7E4BBC0AA92}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{91FCB375-F451-9D45-BC19-B7E4BBC0AA92}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -38831,7 +38774,7 @@
         <xdr:cNvPr id="4" name="Chart 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{91FCB375-F451-9D45-BC19-B7E4BBC0AA92}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{91FCB375-F451-9D45-BC19-B7E4BBC0AA92}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -38869,7 +38812,7 @@
         <xdr:cNvPr id="5" name="Chart 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{91FCB375-F451-9D45-BC19-B7E4BBC0AA92}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{91FCB375-F451-9D45-BC19-B7E4BBC0AA92}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -38907,7 +38850,7 @@
         <xdr:cNvPr id="6" name="Chart 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{91FCB375-F451-9D45-BC19-B7E4BBC0AA92}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{91FCB375-F451-9D45-BC19-B7E4BBC0AA92}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -38945,7 +38888,7 @@
         <xdr:cNvPr id="7" name="Chart 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{91FCB375-F451-9D45-BC19-B7E4BBC0AA92}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{91FCB375-F451-9D45-BC19-B7E4BBC0AA92}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -39233,8 +39176,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AP70"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D56" sqref="D56"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R19" sqref="R19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -39431,18 +39374,20 @@
       <c r="J2" s="5">
         <v>3.7136</v>
       </c>
-      <c r="K2" s="5">
-        <v>0.16261</v>
-      </c>
-      <c r="L2" s="5">
-        <v>0.16256000000000001</v>
+      <c r="K2" s="12">
+        <f>(8+8*D2)*0.000001+B18</f>
+        <v>0.16659399999999999</v>
+      </c>
+      <c r="L2" s="12">
+        <f>(8+8*D2)*0.000001+C18</f>
+        <v>0.166544</v>
       </c>
       <c r="M2" s="5">
-        <f>0.18184-L2</f>
+        <f>0.18184-C18</f>
         <v>1.9279999999999992E-2</v>
       </c>
       <c r="N2" s="5">
-        <f>0.21355-L2</f>
+        <f>0.21355-C18</f>
         <v>5.098999999999998E-2</v>
       </c>
       <c r="O2" s="5">
@@ -39568,18 +39513,20 @@
       <c r="J3" s="5">
         <v>32.438099999999999</v>
       </c>
-      <c r="K3" s="5">
-        <v>0.51053999999999999</v>
-      </c>
-      <c r="L3" s="5">
-        <v>0.58145999999999998</v>
+      <c r="K3" s="12">
+        <f t="shared" ref="K3:K11" si="7">(8+8*D3)*0.000001+B19</f>
+        <v>0.53726799999999997</v>
+      </c>
+      <c r="L3" s="12">
+        <f t="shared" ref="L3:L11" si="8">(8+8*D3)*0.000001+C19</f>
+        <v>0.60818799999999995</v>
       </c>
       <c r="M3" s="5">
-        <f>0.66967-L3</f>
+        <f>0.66967-C19</f>
         <v>8.8210000000000011E-2</v>
       </c>
       <c r="N3" s="5">
-        <f>0.89558-L3</f>
+        <f>0.89558-C19</f>
         <v>0.31412000000000007</v>
       </c>
       <c r="O3" s="5">
@@ -39631,14 +39578,14 @@
         <v>0.24426</v>
       </c>
       <c r="AD3" s="7">
-        <f t="shared" ref="AD3:AD11" si="7">1000*AC3</f>
+        <f t="shared" ref="AD3:AD11" si="9">1000*AC3</f>
         <v>244.26</v>
       </c>
       <c r="AE3" s="5">
         <v>0.17918999999999999</v>
       </c>
       <c r="AF3" s="7">
-        <f t="shared" ref="AF3:AF11" si="8">1000*AE3</f>
+        <f t="shared" ref="AF3:AF11" si="10">1000*AE3</f>
         <v>179.19</v>
       </c>
       <c r="AG3" s="5">
@@ -39652,7 +39599,7 @@
         <v>0.18373</v>
       </c>
       <c r="AJ3" s="7">
-        <f t="shared" ref="AJ3:AJ11" si="9">1000*AI3</f>
+        <f t="shared" ref="AJ3:AJ11" si="11">1000*AI3</f>
         <v>183.73000000000002</v>
       </c>
       <c r="AK3" s="5">
@@ -39705,18 +39652,20 @@
       <c r="J4" s="5">
         <v>185.399</v>
       </c>
-      <c r="K4" s="5">
-        <v>1.19672</v>
-      </c>
-      <c r="L4" s="5">
-        <v>1.3414900000000001</v>
+      <c r="K4" s="12">
+        <f t="shared" si="7"/>
+        <v>1.36588</v>
+      </c>
+      <c r="L4" s="12">
+        <f t="shared" si="8"/>
+        <v>1.51065</v>
       </c>
       <c r="M4" s="5">
-        <f>1.8452-L4</f>
+        <f>1.8452-C20</f>
         <v>0.50370999999999988</v>
       </c>
       <c r="N4" s="5">
-        <f>2.71807-L4</f>
+        <f>2.71807-C20</f>
         <v>1.3765799999999999</v>
       </c>
       <c r="O4" s="5">
@@ -39768,14 +39717,14 @@
         <v>0.47705599999999998</v>
       </c>
       <c r="AD4" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>477.05599999999998</v>
       </c>
       <c r="AE4" s="5">
         <v>0.52105000000000001</v>
       </c>
       <c r="AF4" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>521.05000000000007</v>
       </c>
       <c r="AG4" s="5">
@@ -39789,7 +39738,7 @@
         <v>0.53049999999999997</v>
       </c>
       <c r="AJ4" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>530.5</v>
       </c>
       <c r="AK4" s="5">
@@ -39842,18 +39791,20 @@
       <c r="J5" s="5">
         <v>2.9919999999999999E-2</v>
       </c>
-      <c r="K5" s="5">
-        <v>2.205E-2</v>
-      </c>
-      <c r="L5" s="5">
-        <v>4.6969999999999998E-2</v>
+      <c r="K5" s="12">
+        <f t="shared" si="7"/>
+        <v>2.4194E-2</v>
+      </c>
+      <c r="L5" s="12">
+        <f t="shared" si="8"/>
+        <v>4.9113999999999998E-2</v>
       </c>
       <c r="M5" s="5">
-        <f>0.05502-L5</f>
+        <f>0.05502-C21</f>
         <v>8.0500000000000016E-3</v>
       </c>
       <c r="N5" s="5">
-        <f>0.07157-L5</f>
+        <f>0.07157-C21</f>
         <v>2.4599999999999997E-2</v>
       </c>
       <c r="O5" s="5">
@@ -39905,14 +39856,14 @@
         <v>0.20355400000000001</v>
       </c>
       <c r="AD5" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>203.554</v>
       </c>
       <c r="AE5" s="5">
         <v>0.31065999999999999</v>
       </c>
       <c r="AF5" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>310.65999999999997</v>
       </c>
       <c r="AG5" s="5">
@@ -39926,7 +39877,7 @@
         <v>0.31697999999999998</v>
       </c>
       <c r="AJ5" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>316.97999999999996</v>
       </c>
       <c r="AK5" s="5">
@@ -39979,18 +39930,20 @@
       <c r="J6" s="5">
         <v>63.522599999999997</v>
       </c>
-      <c r="K6" s="5">
-        <v>0.91413999999999995</v>
-      </c>
-      <c r="L6" s="5">
-        <v>1.2390099999999999</v>
+      <c r="K6" s="12">
+        <f t="shared" si="7"/>
+        <v>1.025388</v>
+      </c>
+      <c r="L6" s="12">
+        <f t="shared" si="8"/>
+        <v>1.350258</v>
       </c>
       <c r="M6" s="5">
-        <f>1.59382-L6</f>
+        <f>1.59382-C22</f>
         <v>0.35481000000000007</v>
       </c>
       <c r="N6" s="5">
-        <f>2.15563-L6</f>
+        <f>2.15563-C22</f>
         <v>0.91661999999999999</v>
       </c>
       <c r="O6" s="5">
@@ -40042,14 +39995,14 @@
         <v>0.34389399999999998</v>
       </c>
       <c r="AD6" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>343.89400000000001</v>
       </c>
       <c r="AE6" s="5">
         <v>0.41846</v>
       </c>
       <c r="AF6" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>418.46</v>
       </c>
       <c r="AG6" s="5">
@@ -40063,7 +40016,7 @@
         <v>0.40916000000000002</v>
       </c>
       <c r="AJ6" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>409.16</v>
       </c>
       <c r="AK6" s="5">
@@ -40116,18 +40069,20 @@
       <c r="J7" s="5">
         <v>6.7868199999999996</v>
       </c>
-      <c r="K7" s="5">
-        <v>0.37228</v>
-      </c>
-      <c r="L7" s="5">
-        <v>0.46009</v>
+      <c r="K7" s="12">
+        <f t="shared" si="7"/>
+        <v>0.44448799999999999</v>
+      </c>
+      <c r="L7" s="12">
+        <f t="shared" si="8"/>
+        <v>0.53229799999999994</v>
       </c>
       <c r="M7" s="5">
-        <f>0.67252-L7</f>
+        <f>0.67252-C23</f>
         <v>0.21243000000000001</v>
       </c>
       <c r="N7" s="5">
-        <f>1.01119-L7</f>
+        <f>1.01119-C23</f>
         <v>0.55110000000000003</v>
       </c>
       <c r="O7" s="5">
@@ -40179,14 +40134,14 @@
         <v>0.100912</v>
       </c>
       <c r="AD7" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>100.91200000000001</v>
       </c>
       <c r="AE7" s="5">
         <v>0.12305000000000001</v>
       </c>
       <c r="AF7" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>123.05000000000001</v>
       </c>
       <c r="AG7" s="5">
@@ -40200,7 +40155,7 @@
         <v>0.12254</v>
       </c>
       <c r="AJ7" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>122.53999999999999</v>
       </c>
       <c r="AK7" s="5">
@@ -40253,18 +40208,20 @@
       <c r="J8" s="10">
         <v>6.7879999999999996E-2</v>
       </c>
-      <c r="K8" s="10">
-        <v>6.8650000000000003E-2</v>
-      </c>
-      <c r="L8" s="5">
-        <v>0.12561</v>
+      <c r="K8" s="12">
+        <f t="shared" si="7"/>
+        <v>6.8794000000000008E-2</v>
+      </c>
+      <c r="L8" s="12">
+        <f t="shared" si="8"/>
+        <v>0.125754</v>
       </c>
       <c r="M8" s="10">
-        <f>0.13825-L8</f>
+        <f>0.13825-C24</f>
         <v>1.2640000000000012E-2</v>
       </c>
       <c r="N8" s="10">
-        <f>0.13332-L8</f>
+        <f>0.13332-C24</f>
         <v>7.7099999999999946E-3</v>
       </c>
       <c r="O8" s="10">
@@ -40316,14 +40273,14 @@
         <v>11.638400000000001</v>
       </c>
       <c r="AD8" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>11638.400000000001</v>
       </c>
       <c r="AE8" s="10">
         <v>11.8131</v>
       </c>
       <c r="AF8" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>11813.1</v>
       </c>
       <c r="AG8" s="10">
@@ -40337,7 +40294,7 @@
         <v>11.2453</v>
       </c>
       <c r="AJ8" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>11245.300000000001</v>
       </c>
       <c r="AK8" s="5">
@@ -40390,18 +40347,20 @@
       <c r="J9" s="5">
         <v>7.7022599999999999</v>
       </c>
-      <c r="K9" s="5">
-        <v>0.52495000000000003</v>
-      </c>
-      <c r="L9" s="5">
-        <v>0.95254000000000005</v>
+      <c r="K9" s="12">
+        <f t="shared" si="7"/>
+        <v>0.54887799999999998</v>
+      </c>
+      <c r="L9" s="12">
+        <f t="shared" si="8"/>
+        <v>0.976468</v>
       </c>
       <c r="M9" s="5">
-        <f>1.0663-L9</f>
+        <f>1.0663-C25</f>
         <v>0.11375999999999997</v>
       </c>
       <c r="N9" s="5">
-        <f>1.20981-L9</f>
+        <f>1.20981-C25</f>
         <v>0.25727</v>
       </c>
       <c r="O9" s="5">
@@ -40453,14 +40412,14 @@
         <v>13.6942</v>
       </c>
       <c r="AD9" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>13694.2</v>
       </c>
       <c r="AE9" s="5">
         <v>17.8782</v>
       </c>
       <c r="AF9" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>17878.2</v>
       </c>
       <c r="AG9" s="5">
@@ -40474,7 +40433,7 @@
         <v>17.973400000000002</v>
       </c>
       <c r="AJ9" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>17973.400000000001</v>
       </c>
       <c r="AK9" s="5">
@@ -40527,18 +40486,20 @@
       <c r="J10" s="10">
         <v>35.615600000000001</v>
       </c>
-      <c r="K10" s="10">
-        <v>0.42069000000000001</v>
-      </c>
-      <c r="L10" s="5">
-        <v>0.48945</v>
+      <c r="K10" s="12">
+        <f t="shared" si="7"/>
+        <v>0.45284200000000002</v>
+      </c>
+      <c r="L10" s="12">
+        <f t="shared" si="8"/>
+        <v>0.52160200000000001</v>
       </c>
       <c r="M10" s="10">
-        <f>0.6043-L10</f>
+        <f>0.6043-C26</f>
         <v>0.11484999999999995</v>
       </c>
       <c r="N10" s="10">
-        <f>0.7534-L10</f>
+        <f>0.7534-C26</f>
         <v>0.26394999999999996</v>
       </c>
       <c r="O10" s="10">
@@ -40590,14 +40551,14 @@
         <v>0.98205900000000002</v>
       </c>
       <c r="AD10" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>982.05899999999997</v>
       </c>
       <c r="AE10" s="10">
         <v>1.0914999999999999</v>
       </c>
       <c r="AF10" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>1091.5</v>
       </c>
       <c r="AG10" s="10">
@@ -40611,7 +40572,7 @@
         <v>1.0933900000000001</v>
       </c>
       <c r="AJ10" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>1093.3900000000001</v>
       </c>
       <c r="AK10" s="5">
@@ -40664,18 +40625,20 @@
       <c r="J11" s="10">
         <v>51.860300000000002</v>
       </c>
-      <c r="K11" s="10">
-        <v>0.53468000000000004</v>
-      </c>
-      <c r="L11" s="5">
-        <v>0.63880000000000003</v>
+      <c r="K11" s="12">
+        <f t="shared" si="7"/>
+        <v>0.57244000000000006</v>
+      </c>
+      <c r="L11" s="12">
+        <f t="shared" si="8"/>
+        <v>0.67656000000000005</v>
       </c>
       <c r="M11" s="10">
-        <f>0.77918-L11</f>
+        <f>0.77918-C27</f>
         <v>0.14037999999999995</v>
       </c>
       <c r="N11" s="10">
-        <f>0.94281-L11</f>
+        <f>0.94281-C27</f>
         <v>0.30401</v>
       </c>
       <c r="O11" s="10">
@@ -40727,14 +40690,14 @@
         <v>1.1633</v>
       </c>
       <c r="AD11" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>1163.3</v>
       </c>
       <c r="AE11" s="10">
         <v>1.4539</v>
       </c>
       <c r="AF11" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>1453.8999999999999</v>
       </c>
       <c r="AG11" s="10">
@@ -40748,7 +40711,7 @@
         <v>1.44573</v>
       </c>
       <c r="AJ11" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>1445.73</v>
       </c>
       <c r="AK11" s="5">
@@ -40809,12 +40772,24 @@
       <c r="Y16" s="5"/>
       <c r="Z16" s="5"/>
     </row>
-    <row r="17" spans="4:30" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:30" ht="48" x14ac:dyDescent="0.2">
+      <c r="B17" s="56" t="s">
+        <v>132</v>
+      </c>
+      <c r="C17" t="s">
+        <v>29</v>
+      </c>
       <c r="W17" s="5"/>
       <c r="Y17" s="5"/>
       <c r="Z17" s="5"/>
     </row>
-    <row r="18" spans="4:30" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:30" ht="96" x14ac:dyDescent="0.2">
+      <c r="B18" s="5">
+        <v>0.16261</v>
+      </c>
+      <c r="C18" s="5">
+        <v>0.16256000000000001</v>
+      </c>
       <c r="E18" t="s">
         <v>20</v>
       </c>
@@ -40835,35 +40810,44 @@
       </c>
       <c r="M18" t="s">
         <v>54</v>
+      </c>
+      <c r="R18" s="56" t="s">
+        <v>133</v>
       </c>
       <c r="W18" s="5"/>
       <c r="Y18" s="5"/>
       <c r="Z18" s="5"/>
       <c r="AD18" s="16"/>
     </row>
-    <row r="19" spans="4:30" x14ac:dyDescent="0.2">
-      <c r="E19" s="3">
-        <f t="shared" ref="E19:E28" si="10">W2/I2</f>
-        <v>1.2895530294294386</v>
+    <row r="19" spans="2:30" x14ac:dyDescent="0.2">
+      <c r="B19" s="5">
+        <v>0.51053999999999999</v>
+      </c>
+      <c r="C19" s="5">
+        <v>0.58145999999999998</v>
+      </c>
+      <c r="E19" s="3" t="e">
+        <f>#REF!/I2</f>
+        <v>#REF!</v>
       </c>
       <c r="F19" s="3" t="e">
         <f>#REF!/I2</f>
         <v>#REF!</v>
       </c>
       <c r="G19" s="3">
-        <f t="shared" ref="G19:G28" si="11">Z2/I2</f>
+        <f t="shared" ref="G19:G28" si="12">Z2/I2</f>
         <v>24.264797099689254</v>
       </c>
       <c r="H19" s="3" t="e">
-        <f t="shared" ref="H19:H28" si="12">F19/E19</f>
+        <f t="shared" ref="H19:H28" si="13">F19/E19</f>
         <v>#REF!</v>
       </c>
       <c r="J19" s="3">
-        <f t="shared" ref="J19:J28" si="13">J2/I2</f>
+        <f t="shared" ref="J19:J28" si="14">J2/I2</f>
         <v>15.169337905539091</v>
       </c>
       <c r="K19" s="3">
-        <f t="shared" ref="K19:K28" si="14">L2/I2</f>
+        <f>C18/I2</f>
         <v>0.66402616596414121</v>
       </c>
       <c r="L19" s="13">
@@ -40871,36 +40855,42 @@
         <v>0.62515824233837736</v>
       </c>
       <c r="M19" s="5">
-        <f>L2+O2</f>
+        <f>C18+O2</f>
         <v>0.63937600000000006</v>
       </c>
       <c r="W19" s="5"/>
       <c r="Y19" s="5"/>
       <c r="Z19" s="5"/>
     </row>
-    <row r="20" spans="4:30" x14ac:dyDescent="0.2">
-      <c r="E20" s="3">
-        <f t="shared" si="10"/>
-        <v>2.0396103242388945</v>
+    <row r="20" spans="2:30" x14ac:dyDescent="0.2">
+      <c r="B20" s="5">
+        <v>1.19672</v>
+      </c>
+      <c r="C20" s="5">
+        <v>1.3414900000000001</v>
+      </c>
+      <c r="E20" s="3" t="e">
+        <f>#REF!/I3</f>
+        <v>#REF!</v>
       </c>
       <c r="F20" s="3">
         <f t="shared" ref="F20:F28" si="16">V3/I3</f>
         <v>62.274144550429618</v>
       </c>
       <c r="G20" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>57.018778377279844</v>
       </c>
-      <c r="H20" s="3">
-        <f t="shared" si="12"/>
-        <v>30.532373664890116</v>
+      <c r="H20" s="3" t="e">
+        <f t="shared" si="13"/>
+        <v>#REF!</v>
       </c>
       <c r="J20" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>47.71495803279533</v>
       </c>
       <c r="K20" s="3">
-        <f t="shared" si="14"/>
+        <f>C19/I3</f>
         <v>0.85530100399681774</v>
       </c>
       <c r="L20" s="13">
@@ -40908,7 +40898,7 @@
         <v>0.83682883763444871</v>
       </c>
       <c r="M20" s="5">
-        <f t="shared" ref="M20:M28" si="17">L3+O3</f>
+        <f>C19+O3</f>
         <v>1.2015639999999999</v>
       </c>
       <c r="V20" s="5"/>
@@ -40916,29 +40906,35 @@
       <c r="Y20" s="5"/>
       <c r="Z20" s="5"/>
     </row>
-    <row r="21" spans="4:30" x14ac:dyDescent="0.2">
-      <c r="E21" s="3">
-        <f t="shared" si="10"/>
-        <v>3.3362321551483389</v>
+    <row r="21" spans="2:30" x14ac:dyDescent="0.2">
+      <c r="B21" s="5">
+        <v>2.205E-2</v>
+      </c>
+      <c r="C21" s="5">
+        <v>4.6969999999999998E-2</v>
+      </c>
+      <c r="E21" s="3" t="e">
+        <f>#REF!/I4</f>
+        <v>#REF!</v>
       </c>
       <c r="F21" s="3">
         <f t="shared" si="16"/>
         <v>166.79357173204767</v>
       </c>
       <c r="G21" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>158.96988669295519</v>
       </c>
-      <c r="H21" s="3">
-        <f t="shared" si="12"/>
-        <v>49.9945938937908</v>
+      <c r="H21" s="3" t="e">
+        <f t="shared" si="13"/>
+        <v>#REF!</v>
       </c>
       <c r="J21" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>151.3059306531963</v>
       </c>
       <c r="K21" s="3">
-        <f t="shared" si="14"/>
+        <f>C20/I4</f>
         <v>1.094803062109053</v>
       </c>
       <c r="L21" s="13">
@@ -40946,7 +40942,7 @@
         <v>0.95178988801469322</v>
       </c>
       <c r="M21" s="5">
-        <f t="shared" si="17"/>
+        <f>C20+O4</f>
         <v>1.9014900000000001</v>
       </c>
       <c r="V21" s="5"/>
@@ -40955,29 +40951,35 @@
       <c r="Z21" s="5"/>
       <c r="AD21" s="16"/>
     </row>
-    <row r="22" spans="4:30" x14ac:dyDescent="0.2">
-      <c r="E22" s="3">
-        <f t="shared" si="10"/>
-        <v>2.8260270195754069</v>
+    <row r="22" spans="2:30" x14ac:dyDescent="0.2">
+      <c r="B22" s="5">
+        <v>0.91413999999999995</v>
+      </c>
+      <c r="C22" s="5">
+        <v>1.2390099999999999</v>
+      </c>
+      <c r="E22" s="3" t="e">
+        <f>#REF!/I5</f>
+        <v>#REF!</v>
       </c>
       <c r="F22" s="3">
         <f t="shared" si="16"/>
         <v>33.344291036598726</v>
       </c>
       <c r="G22" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>14.460810304482758</v>
       </c>
-      <c r="H22" s="3">
-        <f t="shared" si="12"/>
-        <v>11.798999374609128</v>
+      <c r="H22" s="3" t="e">
+        <f t="shared" si="13"/>
+        <v>#REF!</v>
       </c>
       <c r="J22" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.66099693891257161</v>
       </c>
       <c r="K22" s="3">
-        <f t="shared" si="14"/>
+        <f>C21/I5</f>
         <v>1.0376679886605444</v>
       </c>
       <c r="L22" s="13">
@@ -40985,37 +40987,41 @@
         <v>4.5709536671514658E-2</v>
       </c>
       <c r="M22" s="5">
-        <f t="shared" si="17"/>
+        <f>C21+O5</f>
         <v>5.2817999999999997E-2</v>
       </c>
       <c r="V22" s="5"/>
-      <c r="W22" s="5"/>
-      <c r="Y22" s="5"/>
       <c r="Z22" s="5"/>
     </row>
-    <row r="23" spans="4:30" x14ac:dyDescent="0.2">
-      <c r="E23" s="3">
-        <f t="shared" si="10"/>
-        <v>2.5642716049366241</v>
+    <row r="23" spans="2:30" x14ac:dyDescent="0.2">
+      <c r="B23" s="5">
+        <v>0.37228</v>
+      </c>
+      <c r="C23" s="5">
+        <v>0.46009</v>
+      </c>
+      <c r="E23" s="3" t="e">
+        <f>#REF!/I6</f>
+        <v>#REF!</v>
       </c>
       <c r="F23" s="3">
         <f t="shared" si="16"/>
         <v>60.191410719381956</v>
       </c>
       <c r="G23" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>52.021346921369386</v>
       </c>
-      <c r="H23" s="3">
-        <f t="shared" si="12"/>
-        <v>23.473102694544554</v>
+      <c r="H23" s="3" t="e">
+        <f t="shared" si="13"/>
+        <v>#REF!</v>
       </c>
       <c r="J23" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>42.386499811797499</v>
       </c>
       <c r="K23" s="3">
-        <f t="shared" si="14"/>
+        <f>C22/I6</f>
         <v>0.82674980450761171</v>
       </c>
       <c r="L23" s="13">
@@ -41023,37 +41029,41 @@
         <v>0.81479051043920447</v>
       </c>
       <c r="M23" s="5">
-        <f t="shared" si="17"/>
+        <f>C22+O6</f>
         <v>1.5299700000000001</v>
       </c>
       <c r="V23" s="5"/>
-      <c r="W23" s="5"/>
-      <c r="Y23" s="5"/>
       <c r="Z23" s="5"/>
     </row>
-    <row r="24" spans="4:30" x14ac:dyDescent="0.2">
-      <c r="E24" s="3">
-        <f t="shared" si="10"/>
-        <v>4.2673356876769235</v>
+    <row r="24" spans="2:30" x14ac:dyDescent="0.2">
+      <c r="B24" s="10">
+        <v>6.8650000000000003E-2</v>
+      </c>
+      <c r="C24" s="5">
+        <v>0.12561</v>
+      </c>
+      <c r="E24" s="3" t="e">
+        <f>#REF!/I7</f>
+        <v>#REF!</v>
       </c>
       <c r="F24" s="3">
         <f t="shared" si="16"/>
         <v>38.314872216932926</v>
       </c>
       <c r="G24" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>27.323426259832193</v>
       </c>
-      <c r="H24" s="3">
-        <f t="shared" si="12"/>
-        <v>8.9786403088881421</v>
+      <c r="H24" s="3" t="e">
+        <f t="shared" si="13"/>
+        <v>#REF!</v>
       </c>
       <c r="J24" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>18.361877923145371</v>
       </c>
       <c r="K24" s="3">
-        <f t="shared" si="14"/>
+        <f>C23/I7</f>
         <v>1.2447827426777127</v>
       </c>
       <c r="L24" s="13">
@@ -41061,37 +41071,41 @@
         <v>0.67201959770831976</v>
       </c>
       <c r="M24" s="5">
-        <f t="shared" si="17"/>
+        <f>C23+O7</f>
         <v>0.50676999999999994</v>
       </c>
       <c r="V24" s="5"/>
-      <c r="W24" s="5"/>
-      <c r="Y24" s="5"/>
       <c r="Z24" s="5"/>
     </row>
-    <row r="25" spans="4:30" x14ac:dyDescent="0.2">
-      <c r="E25" s="3">
-        <f t="shared" si="10"/>
-        <v>1.1217525181692833</v>
+    <row r="25" spans="2:30" x14ac:dyDescent="0.2">
+      <c r="B25" s="5">
+        <v>0.52495000000000003</v>
+      </c>
+      <c r="C25" s="5">
+        <v>0.95254000000000005</v>
+      </c>
+      <c r="E25" s="3" t="e">
+        <f>#REF!/I8</f>
+        <v>#REF!</v>
       </c>
       <c r="F25" s="3">
         <f t="shared" si="16"/>
         <v>33.075231183255049</v>
       </c>
       <c r="G25" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>15.560720915554242</v>
       </c>
-      <c r="H25" s="3">
-        <f t="shared" si="12"/>
-        <v>29.485319308428487</v>
+      <c r="H25" s="3" t="e">
+        <f t="shared" si="13"/>
+        <v>#REF!</v>
       </c>
       <c r="J25" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.22923301833492674</v>
       </c>
       <c r="K25" s="3">
-        <f t="shared" si="14"/>
+        <f>C24/I8</f>
         <v>0.42418914898423904</v>
       </c>
       <c r="L25" s="13">
@@ -41099,37 +41113,41 @@
         <v>1.4731516590969069E-2</v>
       </c>
       <c r="M25" s="5">
-        <f t="shared" si="17"/>
+        <f>C24+O8</f>
         <v>0.379938</v>
       </c>
       <c r="V25" s="5"/>
-      <c r="W25" s="5"/>
-      <c r="Y25" s="5"/>
       <c r="Z25" s="5"/>
     </row>
-    <row r="26" spans="4:30" x14ac:dyDescent="0.2">
-      <c r="E26" s="3">
-        <f t="shared" si="10"/>
-        <v>2.0512194253104141</v>
+    <row r="26" spans="2:30" x14ac:dyDescent="0.2">
+      <c r="B26" s="10">
+        <v>0.42069000000000001</v>
+      </c>
+      <c r="C26" s="5">
+        <v>0.48945</v>
+      </c>
+      <c r="E26" s="3" t="e">
+        <f>#REF!/I9</f>
+        <v>#REF!</v>
       </c>
       <c r="F26" s="3">
         <f t="shared" si="16"/>
         <v>29.355981443587911</v>
       </c>
       <c r="G26" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>17.027217179933643</v>
       </c>
-      <c r="H26" s="3">
-        <f t="shared" si="12"/>
-        <v>14.311477885475576</v>
+      <c r="H26" s="3" t="e">
+        <f t="shared" si="13"/>
+        <v>#REF!</v>
       </c>
       <c r="J26" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>6.4833537137100175</v>
       </c>
       <c r="K26" s="3">
-        <f t="shared" si="14"/>
+        <f>C25/I9</f>
         <v>0.80179762127704601</v>
       </c>
       <c r="L26" s="13">
@@ -41137,39 +41155,42 @@
         <v>0.38076414044630652</v>
       </c>
       <c r="M26" s="5">
-        <f t="shared" si="17"/>
+        <f>C25+O9</f>
         <v>1.1161480000000001</v>
       </c>
       <c r="V26" s="5"/>
-      <c r="W26" s="5"/>
-      <c r="X26" s="5"/>
-      <c r="Y26" s="5"/>
       <c r="Z26" s="5"/>
       <c r="AD26" s="16"/>
     </row>
-    <row r="27" spans="4:30" x14ac:dyDescent="0.2">
-      <c r="E27" s="3">
-        <f t="shared" si="10"/>
-        <v>1.6084011158957625</v>
+    <row r="27" spans="2:30" x14ac:dyDescent="0.2">
+      <c r="B27" s="10">
+        <v>0.53468000000000004</v>
+      </c>
+      <c r="C27" s="5">
+        <v>0.63880000000000003</v>
+      </c>
+      <c r="E27" s="3" t="e">
+        <f>#REF!/I10</f>
+        <v>#REF!</v>
       </c>
       <c r="F27" s="3">
         <f t="shared" si="16"/>
         <v>58.327108057300777</v>
       </c>
       <c r="G27" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>54.328551296431378</v>
       </c>
-      <c r="H27" s="3">
-        <f t="shared" si="12"/>
-        <v>36.264031080839445</v>
+      <c r="H27" s="3" t="e">
+        <f t="shared" si="13"/>
+        <v>#REF!</v>
       </c>
       <c r="J27" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>46.559626431146775</v>
       </c>
       <c r="K27" s="3">
-        <f t="shared" si="14"/>
+        <f>C26/I10</f>
         <v>0.63984908738656066</v>
       </c>
       <c r="L27" s="13">
@@ -41177,41 +41198,38 @@
         <v>0.85700106702836165</v>
       </c>
       <c r="M27" s="5">
-        <f t="shared" si="17"/>
+        <f>C26+O10</f>
         <v>1.0552980000000001</v>
       </c>
       <c r="V27" s="5"/>
-      <c r="W27" s="5"/>
-      <c r="X27" s="5"/>
-      <c r="Y27" s="5"/>
       <c r="Z27" s="5"/>
     </row>
-    <row r="28" spans="4:30" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:30" x14ac:dyDescent="0.2">
       <c r="D28" t="s">
         <v>49</v>
       </c>
-      <c r="E28" s="3">
-        <f t="shared" si="10"/>
-        <v>1.4649188558349382</v>
+      <c r="E28" s="3" t="e">
+        <f>#REF!/I11</f>
+        <v>#REF!</v>
       </c>
       <c r="F28" s="3">
         <f t="shared" si="16"/>
         <v>58.351781815122095</v>
       </c>
       <c r="G28" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>53.961724828739655</v>
       </c>
-      <c r="H28" s="3">
-        <f t="shared" si="12"/>
-        <v>39.832774069840333</v>
+      <c r="H28" s="3" t="e">
+        <f t="shared" si="13"/>
+        <v>#REF!</v>
       </c>
       <c r="J28" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>46.689978329619237</v>
       </c>
       <c r="K28" s="3">
-        <f t="shared" si="14"/>
+        <f>C27/I11</f>
         <v>0.57511349060766648</v>
       </c>
       <c r="L28" s="13">
@@ -41219,37 +41237,28 @@
         <v>0.86524251175812061</v>
       </c>
       <c r="M28" s="5">
-        <f t="shared" si="17"/>
+        <f>C27+O11</f>
         <v>1.3408</v>
       </c>
       <c r="V28" s="5"/>
-      <c r="W28" s="5"/>
-      <c r="X28" s="5"/>
-      <c r="Y28" s="5"/>
       <c r="Z28" s="5"/>
     </row>
-    <row r="29" spans="4:30" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:30" x14ac:dyDescent="0.2">
       <c r="D29" t="s">
         <v>50</v>
       </c>
       <c r="V29" s="5"/>
-      <c r="W29" s="5"/>
-      <c r="X29" s="5"/>
-      <c r="Y29" s="5"/>
       <c r="Z29" s="5"/>
     </row>
-    <row r="30" spans="4:30" x14ac:dyDescent="0.2">
-      <c r="W30" s="5"/>
-      <c r="X30" s="5"/>
-      <c r="Y30" s="5"/>
+    <row r="30" spans="2:30" x14ac:dyDescent="0.2">
       <c r="Z30" s="5"/>
     </row>
-    <row r="31" spans="4:30" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:30" x14ac:dyDescent="0.2">
       <c r="D31" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="32" spans="4:30" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:30" x14ac:dyDescent="0.2">
       <c r="D32" t="s">
         <v>36</v>
       </c>
@@ -41317,12 +41326,12 @@
         <v>15.169337905539091</v>
       </c>
       <c r="I45" s="49">
-        <f>K2/I2</f>
-        <v>0.66423040629570007</v>
+        <f>L2/I2</f>
+        <v>0.68030003558275054</v>
       </c>
       <c r="J45" s="50">
-        <f>(K2+M2+N2)/I2</f>
-        <v>0.95126976826851128</v>
+        <f>(L2+M2+N2)/I2</f>
+        <v>0.96733939755556175</v>
       </c>
       <c r="K45" s="29"/>
       <c r="L45" s="28"/>
@@ -41336,16 +41345,16 @@
         <v>3</v>
       </c>
       <c r="H46" s="49">
-        <f t="shared" ref="H46:H54" si="18">J3/I3</f>
+        <f t="shared" ref="H46:H54" si="17">J3/I3</f>
         <v>47.71495803279533</v>
       </c>
       <c r="I46" s="49">
-        <f t="shared" ref="I46:I54" si="19">K3/I3</f>
-        <v>0.75098093519852671</v>
+        <f t="shared" ref="I46:I54" si="18">L3/I3</f>
+        <v>0.89461666669902751</v>
       </c>
       <c r="J46" s="50">
-        <f t="shared" ref="J46:J54" si="20">(K3+M3+N3)/I3</f>
-        <v>1.3427899210927237</v>
+        <f t="shared" ref="J46:J54" si="19">(L3+M3+N3)/I3</f>
+        <v>1.4864256525932245</v>
       </c>
       <c r="K46" s="29"/>
       <c r="L46" s="28"/>
@@ -41359,16 +41368,16 @@
         <v>16</v>
       </c>
       <c r="H47" s="49">
+        <f t="shared" si="17"/>
+        <v>151.3059306531963</v>
+      </c>
+      <c r="I47" s="49">
         <f t="shared" si="18"/>
-        <v>151.3059306531963</v>
-      </c>
-      <c r="I47" s="49">
+        <v>1.2328561866096956</v>
+      </c>
+      <c r="J47" s="50">
         <f t="shared" si="19"/>
-        <v>0.97665485429421439</v>
-      </c>
-      <c r="J47" s="50">
-        <f t="shared" si="20"/>
-        <v>2.5111778471253428</v>
+        <v>2.767379179440824</v>
       </c>
       <c r="K47" s="29"/>
       <c r="L47" s="28"/>
@@ -41382,16 +41391,16 @@
         <v>4</v>
       </c>
       <c r="H48" s="49">
+        <f t="shared" si="17"/>
+        <v>0.66099693891257161</v>
+      </c>
+      <c r="I48" s="49">
         <f t="shared" si="18"/>
-        <v>0.66099693891257161</v>
-      </c>
-      <c r="I48" s="49">
+        <v>1.085033544710964</v>
+      </c>
+      <c r="J48" s="50">
         <f t="shared" si="19"/>
-        <v>0.48713176814913789</v>
-      </c>
-      <c r="J48" s="50">
-        <f t="shared" si="20"/>
-        <v>1.2084402593087455</v>
+        <v>1.806342035870572</v>
       </c>
       <c r="K48" s="29"/>
       <c r="L48" s="28"/>
@@ -41405,16 +41414,16 @@
         <v>7</v>
       </c>
       <c r="H49" s="49">
+        <f t="shared" si="17"/>
+        <v>42.386499811797499</v>
+      </c>
+      <c r="I49" s="49">
         <f t="shared" si="18"/>
-        <v>42.386499811797499</v>
-      </c>
-      <c r="I49" s="49">
+        <v>0.90098186256352963</v>
+      </c>
+      <c r="J49" s="50">
         <f t="shared" si="19"/>
-        <v>0.60997495281925751</v>
-      </c>
-      <c r="J49" s="50">
-        <f t="shared" si="20"/>
-        <v>1.458357535643539</v>
+        <v>1.7493644453878108</v>
       </c>
       <c r="K49" s="29"/>
       <c r="L49" s="28"/>
@@ -41428,16 +41437,16 @@
         <v>8</v>
       </c>
       <c r="H50" s="49">
+        <f t="shared" si="17"/>
+        <v>18.361877923145371</v>
+      </c>
+      <c r="I50" s="49">
         <f t="shared" si="18"/>
-        <v>18.361877923145371</v>
-      </c>
-      <c r="I50" s="49">
+        <v>1.4401429380379078</v>
+      </c>
+      <c r="J50" s="50">
         <f t="shared" si="19"/>
-        <v>1.0072110227217694</v>
-      </c>
-      <c r="J50" s="50">
-        <f t="shared" si="20"/>
-        <v>3.0729567844568955</v>
+        <v>3.5058886997730339</v>
       </c>
       <c r="K50" s="29"/>
       <c r="L50" s="28"/>
@@ -41451,16 +41460,16 @@
         <v>5</v>
       </c>
       <c r="H51" s="49">
+        <f t="shared" si="17"/>
+        <v>0.22923301833492674</v>
+      </c>
+      <c r="I51" s="49">
         <f t="shared" si="18"/>
-        <v>0.22923301833492674</v>
-      </c>
-      <c r="I51" s="49">
+        <v>0.42467544177504979</v>
+      </c>
+      <c r="J51" s="50">
         <f t="shared" si="19"/>
-        <v>0.23183333395245612</v>
-      </c>
-      <c r="J51" s="50">
-        <f t="shared" si="20"/>
-        <v>0.30055596098716092</v>
+        <v>0.49339806880975456</v>
       </c>
       <c r="K51" s="29"/>
       <c r="L51" s="28"/>
@@ -41474,16 +41483,16 @@
         <v>6</v>
       </c>
       <c r="H52" s="49">
+        <f t="shared" si="17"/>
+        <v>6.4833537137100175</v>
+      </c>
+      <c r="I52" s="49">
         <f t="shared" si="18"/>
-        <v>6.4833537137100175</v>
-      </c>
-      <c r="I52" s="49">
+        <v>0.82193894183252625</v>
+      </c>
+      <c r="J52" s="50">
         <f t="shared" si="19"/>
-        <v>0.4418750512203008</v>
-      </c>
-      <c r="J52" s="50">
-        <f t="shared" si="20"/>
-        <v>0.75418841488211275</v>
+        <v>1.1342523054943381</v>
       </c>
       <c r="K52" s="29"/>
       <c r="L52" s="28"/>
@@ -41497,16 +41506,16 @@
         <v>9</v>
       </c>
       <c r="H53" s="49">
+        <f t="shared" si="17"/>
+        <v>46.559626431146775</v>
+      </c>
+      <c r="I53" s="49">
         <f t="shared" si="18"/>
-        <v>46.559626431146775</v>
-      </c>
-      <c r="I53" s="49">
+        <v>0.68188081250179755</v>
+      </c>
+      <c r="J53" s="50">
         <f t="shared" si="19"/>
-        <v>0.54996038936081759</v>
-      </c>
-      <c r="J53" s="50">
-        <f t="shared" si="20"/>
-        <v>1.0451587432315481</v>
+        <v>1.1770791663725282</v>
       </c>
       <c r="K53" s="29"/>
       <c r="L53" s="28"/>
@@ -41520,16 +41529,16 @@
         <v>10</v>
       </c>
       <c r="H54" s="49">
+        <f t="shared" si="17"/>
+        <v>46.689978329619237</v>
+      </c>
+      <c r="I54" s="49">
         <f t="shared" si="18"/>
-        <v>46.689978329619237</v>
-      </c>
-      <c r="I54" s="49">
+        <v>0.60910892799862693</v>
+      </c>
+      <c r="J54" s="50">
         <f t="shared" si="19"/>
-        <v>0.48137395297136371</v>
-      </c>
-      <c r="J54" s="50">
-        <f t="shared" si="20"/>
-        <v>0.88145955737202264</v>
+        <v>1.0091945323992859</v>
       </c>
       <c r="K54" s="29"/>
       <c r="L54" s="28"/>
@@ -41630,11 +41639,11 @@
         <v>3</v>
       </c>
       <c r="H62" s="31" t="e">
-        <f t="shared" ref="H62:H70" si="21">H46/K46</f>
+        <f t="shared" ref="H62:H70" si="20">H46/K46</f>
         <v>#DIV/0!</v>
       </c>
       <c r="I62" s="32" t="e">
-        <f t="shared" ref="I62:I70" si="22">I46/K46</f>
+        <f t="shared" ref="I62:I70" si="21">I46/K46</f>
         <v>#DIV/0!</v>
       </c>
       <c r="J62" s="32" t="e">
@@ -41651,15 +41660,15 @@
         <v>16</v>
       </c>
       <c r="H63" s="31" t="e">
+        <f t="shared" si="20"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I63" s="32" t="e">
         <f t="shared" si="21"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I63" s="32" t="e">
-        <f t="shared" si="22"/>
-        <v>#DIV/0!</v>
-      </c>
       <c r="J63" s="32" t="e">
-        <f t="shared" ref="J63:J70" si="23">J47/K47</f>
+        <f t="shared" ref="J63:J70" si="22">J47/K47</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K63" s="29"/>
@@ -41672,15 +41681,15 @@
         <v>4</v>
       </c>
       <c r="H64" s="31" t="e">
+        <f t="shared" si="20"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I64" s="32" t="e">
         <f t="shared" si="21"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I64" s="32" t="e">
+      <c r="J64" s="32" t="e">
         <f t="shared" si="22"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J64" s="32" t="e">
-        <f t="shared" si="23"/>
         <v>#DIV/0!</v>
       </c>
       <c r="K64" s="29"/>
@@ -41693,15 +41702,15 @@
         <v>7</v>
       </c>
       <c r="H65" s="31" t="e">
+        <f t="shared" si="20"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I65" s="32" t="e">
         <f t="shared" si="21"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I65" s="32" t="e">
+      <c r="J65" s="32" t="e">
         <f t="shared" si="22"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J65" s="32" t="e">
-        <f t="shared" si="23"/>
         <v>#DIV/0!</v>
       </c>
       <c r="K65" s="29"/>
@@ -41714,15 +41723,15 @@
         <v>8</v>
       </c>
       <c r="H66" s="31" t="e">
+        <f t="shared" si="20"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I66" s="32" t="e">
         <f t="shared" si="21"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I66" s="32" t="e">
+      <c r="J66" s="32" t="e">
         <f t="shared" si="22"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J66" s="32" t="e">
-        <f t="shared" si="23"/>
         <v>#DIV/0!</v>
       </c>
       <c r="K66" s="29"/>
@@ -41735,15 +41744,15 @@
         <v>5</v>
       </c>
       <c r="H67" s="31" t="e">
+        <f t="shared" si="20"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I67" s="32" t="e">
         <f t="shared" si="21"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I67" s="32" t="e">
+      <c r="J67" s="32" t="e">
         <f t="shared" si="22"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J67" s="32" t="e">
-        <f t="shared" si="23"/>
         <v>#DIV/0!</v>
       </c>
       <c r="K67" s="29"/>
@@ -41756,15 +41765,15 @@
         <v>6</v>
       </c>
       <c r="H68" s="31" t="e">
+        <f t="shared" si="20"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I68" s="32" t="e">
         <f t="shared" si="21"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I68" s="32" t="e">
+      <c r="J68" s="32" t="e">
         <f t="shared" si="22"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J68" s="32" t="e">
-        <f t="shared" si="23"/>
         <v>#DIV/0!</v>
       </c>
       <c r="K68" s="29"/>
@@ -41777,15 +41786,15 @@
         <v>9</v>
       </c>
       <c r="H69" s="31" t="e">
+        <f t="shared" si="20"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I69" s="32" t="e">
         <f t="shared" si="21"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I69" s="32" t="e">
+      <c r="J69" s="32" t="e">
         <f t="shared" si="22"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J69" s="32" t="e">
-        <f t="shared" si="23"/>
         <v>#DIV/0!</v>
       </c>
       <c r="K69" s="29"/>
@@ -41798,15 +41807,15 @@
         <v>10</v>
       </c>
       <c r="H70" s="31" t="e">
+        <f t="shared" si="20"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I70" s="32" t="e">
         <f t="shared" si="21"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I70" s="32" t="e">
+      <c r="J70" s="32" t="e">
         <f t="shared" si="22"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J70" s="32" t="e">
-        <f t="shared" si="23"/>
         <v>#DIV/0!</v>
       </c>
       <c r="K70" s="29"/>
@@ -41826,7 +41835,7 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="67" workbookViewId="0">
+    <sheetView zoomScale="67" workbookViewId="0">
       <selection activeCell="AJ58" sqref="Y31:AJ58"/>
     </sheetView>
   </sheetViews>
@@ -41844,7 +41853,7 @@
   <dimension ref="A1:R34"/>
   <sheetViews>
     <sheetView zoomScale="119" zoomScaleNormal="142" zoomScalePageLayoutView="142" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23:H23"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -42962,10 +42971,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M19"/>
+  <dimension ref="A1:Q20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H41" sqref="H41"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -42974,7 +42983,7 @@
     <col min="6" max="6" width="13.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" s="20" t="s">
         <v>84</v>
       </c>
@@ -42996,8 +43005,11 @@
       <c r="G1" s="20" t="s">
         <v>75</v>
       </c>
+      <c r="L1" t="s">
+        <v>128</v>
+      </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>85</v>
       </c>
@@ -43019,8 +43031,11 @@
       <c r="G2" s="12">
         <v>11.860200000000001</v>
       </c>
+      <c r="L2" t="s">
+        <v>129</v>
+      </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>86</v>
       </c>
@@ -43042,31 +43057,61 @@
       <c r="G3" s="12">
         <v>0.52500000000000002</v>
       </c>
+      <c r="K3" s="12"/>
+      <c r="L3" s="12"/>
+      <c r="M3" s="12"/>
+      <c r="N3" s="12"/>
+      <c r="O3" s="12"/>
+      <c r="P3" s="12"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>87</v>
       </c>
       <c r="B4" s="12">
+        <f>(8+8*'Datasets Attributes, Notes'!D13)*0.000001+L4</f>
+        <v>10.421799999999999</v>
+      </c>
+      <c r="C4" s="12">
+        <f>(8+8*'Datasets Attributes, Notes'!D14)*0.000001+M4</f>
+        <v>11.550343999999999</v>
+      </c>
+      <c r="D4" s="12">
+        <f>(8+8*'Datasets Attributes, Notes'!D15)*0.000001+N4</f>
+        <v>12.324464000000001</v>
+      </c>
+      <c r="E4" s="12">
+        <f>(8+8*'Datasets Attributes, Notes'!D16)*0.000001+O4</f>
+        <v>12.602648</v>
+      </c>
+      <c r="F4" s="12">
+        <f>(8+8*'Datasets Attributes, Notes'!D17)*0.000001+P4</f>
+        <v>12.810144000000001</v>
+      </c>
+      <c r="G4" s="12">
+        <f>(8+8*'Datasets Attributes, Notes'!ID18)*0.000001+Q4</f>
+        <v>12.929008</v>
+      </c>
+      <c r="L4" s="12">
         <v>10.417999999999999</v>
       </c>
-      <c r="C4" s="12">
+      <c r="M4" s="12">
         <v>11.542999999999999</v>
       </c>
-      <c r="D4" s="12">
+      <c r="N4" s="12">
         <v>12.314</v>
       </c>
-      <c r="E4" s="12">
+      <c r="O4" s="12">
         <v>12.589</v>
       </c>
-      <c r="F4" s="12">
+      <c r="P4" s="12">
         <v>12.794</v>
       </c>
-      <c r="G4" s="12">
+      <c r="Q4" s="12">
         <v>12.929</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" s="20" t="s">
         <v>88</v>
       </c>
@@ -43083,7 +43128,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>85</v>
       </c>
@@ -43100,7 +43145,7 @@
         <v>13.843</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>86</v>
       </c>
@@ -43116,25 +43161,45 @@
       <c r="E9" s="3">
         <v>1.2593000000000001</v>
       </c>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>87</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="12">
+        <f>(8+8*'Datasets Attributes, Notes'!$D$20)*0.000001+L10</f>
+        <v>16.203344000000001</v>
+      </c>
+      <c r="C10" s="12">
+        <f>(8+8*'Datasets Attributes, Notes'!$D$20)*0.000001+M10</f>
+        <v>15.048344</v>
+      </c>
+      <c r="D10" s="12">
+        <f>(8+8*'Datasets Attributes, Notes'!$D$20)*0.000001+N10</f>
+        <v>11.550343999999999</v>
+      </c>
+      <c r="E10" s="12">
+        <f>(8+8*'Datasets Attributes, Notes'!$D$20)*0.000001+O10</f>
+        <v>6.9317440000000001</v>
+      </c>
+      <c r="L10" s="3">
         <v>16.196000000000002</v>
       </c>
-      <c r="C10" s="3">
+      <c r="M10" s="3">
         <v>15.041</v>
       </c>
-      <c r="D10" s="3">
+      <c r="N10" s="3">
         <v>11.542999999999999</v>
       </c>
-      <c r="E10" s="3">
+      <c r="O10" s="3">
         <v>6.9244000000000003</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" s="42" t="s">
         <v>89</v>
       </c>
@@ -43154,7 +43219,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" s="19" t="s">
         <v>85</v>
       </c>
@@ -43179,7 +43244,7 @@
       <c r="L13" s="3"/>
       <c r="M13" s="3"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" s="19" t="s">
         <v>86</v>
       </c>
@@ -43198,28 +43263,53 @@
       <c r="F14" s="3">
         <v>35.579599999999999</v>
       </c>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
+      <c r="N14" s="3"/>
+      <c r="O14" s="3"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B15" s="12">
+        <f>(8+8*'Datasets Attributes, Notes'!$D$25)*0.000001+L15</f>
+        <v>4.989344</v>
+      </c>
+      <c r="C15" s="12">
+        <f>(8+8*'Datasets Attributes, Notes'!$D$25)*0.000001+M15</f>
+        <v>9.8806440000000002</v>
+      </c>
+      <c r="D15" s="12">
+        <f>(8+8*'Datasets Attributes, Notes'!$D$25)*0.000001+N15</f>
+        <v>19.588343999999999</v>
+      </c>
+      <c r="E15" s="12">
+        <f>(8+8*'Datasets Attributes, Notes'!$D$25)*0.000001+O15</f>
+        <v>39.147344000000004</v>
+      </c>
+      <c r="F15" s="12">
+        <f>(8+8*'Datasets Attributes, Notes'!$D$25)*0.000001+P15</f>
+        <v>78.856344000000007</v>
+      </c>
+      <c r="L15" s="3">
         <v>4.9820000000000002</v>
       </c>
-      <c r="C15" s="3">
+      <c r="M15" s="3">
         <v>9.8733000000000004</v>
       </c>
-      <c r="D15" s="3">
+      <c r="N15" s="3">
         <v>19.581</v>
       </c>
-      <c r="E15" s="3">
+      <c r="O15" s="3">
         <v>39.14</v>
       </c>
-      <c r="F15" s="3">
+      <c r="P15" s="3">
         <v>78.849000000000004</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" s="21" t="s">
         <v>90</v>
       </c>
@@ -43233,7 +43323,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" s="19" t="s">
         <v>91</v>
       </c>
@@ -43245,6 +43335,14 @@
       </c>
       <c r="D19" s="12">
         <v>0.27705099999999999</v>
+      </c>
+      <c r="L19" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L20" t="s">
+        <v>131</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
rough calculations and exports
</commit_message>
<xml_diff>
--- a/results/cptVSsd_cpt.xlsx
+++ b/results/cptVSsd_cpt.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="26440" windowHeight="16640" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="All RAW Data" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="133">
   <si>
     <t>Trie Node Number</t>
   </si>
@@ -335,28 +335,10 @@
     <t>QUEST1600K</t>
   </si>
   <si>
-    <t>sCPT-H to CPT+</t>
-  </si>
-  <si>
-    <t>sCPT-F to CPT+</t>
-  </si>
-  <si>
-    <t>sCPT-S to CPT+</t>
-  </si>
-  <si>
     <t>Draft Calculations</t>
   </si>
   <si>
     <t>CPTPlus to sCPT</t>
-  </si>
-  <si>
-    <t>II</t>
-  </si>
-  <si>
-    <t>sII</t>
-  </si>
-  <si>
-    <t>sII+Dict</t>
   </si>
   <si>
     <t xml:space="preserve">Alphabet size: 1000 @@ -447,6 +429,21 @@
   </si>
   <si>
     <t>PT has one extra int per node (extra than PAKDD and Ipredict framework specifies); this is exported in memory results and should be adapted. However, scalability and comparisons should not be affected since is a consistent overload</t>
+  </si>
+  <si>
+    <t>sII(nodes) to sII</t>
+  </si>
+  <si>
+    <t>sII+LT to SII</t>
+  </si>
+  <si>
+    <t>nodes</t>
+  </si>
+  <si>
+    <t>sPT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PT </t>
   </si>
 </sst>
 </file>
@@ -585,7 +582,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="61">
+  <cellStyleXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -647,8 +644,30 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -702,8 +721,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
@@ -713,7 +730,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="61">
+  <cellStyles count="83">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -744,6 +761,17 @@
     <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -774,6 +802,17 @@
     <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -39174,10 +39213,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AP70"/>
+  <dimension ref="A1:AP85"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R19" sqref="R19"/>
+    <sheetView tabSelected="1" topLeftCell="F28" workbookViewId="0">
+      <selection activeCell="G44" sqref="G44:K54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -40773,8 +40812,8 @@
       <c r="Z16" s="5"/>
     </row>
     <row r="17" spans="2:30" ht="48" x14ac:dyDescent="0.2">
-      <c r="B17" s="56" t="s">
-        <v>132</v>
+      <c r="B17" s="54" t="s">
+        <v>126</v>
       </c>
       <c r="C17" t="s">
         <v>29</v>
@@ -40811,8 +40850,8 @@
       <c r="M18" t="s">
         <v>54</v>
       </c>
-      <c r="R18" s="56" t="s">
-        <v>133</v>
+      <c r="R18" s="54" t="s">
+        <v>127</v>
       </c>
       <c r="W18" s="5"/>
       <c r="Y18" s="5"/>
@@ -41270,7 +41309,7 @@
     </row>
     <row r="42" spans="4:15" x14ac:dyDescent="0.2">
       <c r="F42" s="25" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="G42" s="25"/>
       <c r="H42" s="25"/>
@@ -41293,7 +41332,7 @@
         <v>1</v>
       </c>
       <c r="O43" s="25" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="44" spans="4:15" x14ac:dyDescent="0.2">
@@ -41302,15 +41341,14 @@
         <v>1</v>
       </c>
       <c r="H44" s="19" t="s">
-        <v>102</v>
-      </c>
-      <c r="I44" s="19" t="s">
-        <v>103</v>
+        <v>130</v>
+      </c>
+      <c r="I44" s="25" t="s">
+        <v>132</v>
       </c>
       <c r="J44" s="25" t="s">
-        <v>104</v>
-      </c>
-      <c r="K44" s="25"/>
+        <v>131</v>
+      </c>
       <c r="L44" s="26"/>
       <c r="M44" s="25"/>
       <c r="N44" s="27"/>
@@ -41321,19 +41359,17 @@
       <c r="G45" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="H45" s="49">
-        <f>J2/I2</f>
-        <v>15.169337905539091</v>
-      </c>
-      <c r="I45" s="49">
-        <f>L2/I2</f>
-        <v>0.68030003558275054</v>
-      </c>
-      <c r="J45" s="50">
-        <f>(L2+M2+N2)/I2</f>
-        <v>0.96733939755556175</v>
-      </c>
-      <c r="K45" s="29"/>
+      <c r="H45" s="6">
+        <v>59088</v>
+      </c>
+      <c r="I45" s="3">
+        <f>N59/I2</f>
+        <v>3.2140892496753497</v>
+      </c>
+      <c r="J45" s="3">
+        <f>O59/I2</f>
+        <v>0.36784500675075565</v>
+      </c>
       <c r="L45" s="28"/>
       <c r="M45" s="25"/>
       <c r="N45" s="27"/>
@@ -41344,19 +41380,17 @@
       <c r="G46" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="H46" s="49">
-        <f t="shared" ref="H46:H54" si="17">J3/I3</f>
-        <v>47.71495803279533</v>
-      </c>
-      <c r="I46" s="49">
-        <f t="shared" ref="I46:I54" si="18">L3/I3</f>
-        <v>0.89461666669902751</v>
-      </c>
-      <c r="J46" s="50">
-        <f t="shared" ref="J46:J54" si="19">(L3+M3+N3)/I3</f>
-        <v>1.4864256525932245</v>
-      </c>
-      <c r="K46" s="29"/>
+      <c r="H46" s="6">
+        <v>231942</v>
+      </c>
+      <c r="I46" s="3">
+        <f>N60/I3</f>
+        <v>3.0947698695163637</v>
+      </c>
+      <c r="J46" s="3">
+        <f t="shared" ref="J46:J54" si="17">O60/I3</f>
+        <v>0.60843370977403732</v>
+      </c>
       <c r="L46" s="28"/>
       <c r="M46" s="25"/>
       <c r="N46" s="27"/>
@@ -41367,19 +41401,17 @@
       <c r="G47" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="H47" s="49">
+      <c r="H47" s="6">
+        <v>460435</v>
+      </c>
+      <c r="I47" s="3">
+        <f>N61/I4</f>
+        <v>1.735734850513994</v>
+      </c>
+      <c r="J47" s="3">
         <f t="shared" si="17"/>
-        <v>151.3059306531963</v>
-      </c>
-      <c r="I47" s="49">
-        <f t="shared" si="18"/>
-        <v>1.2328561866096956</v>
-      </c>
-      <c r="J47" s="50">
-        <f t="shared" si="19"/>
-        <v>2.767379179440824</v>
-      </c>
-      <c r="K47" s="29"/>
+        <v>0.72037925599191854</v>
+      </c>
       <c r="L47" s="28"/>
       <c r="M47" s="25"/>
       <c r="N47" s="27"/>
@@ -41390,19 +41422,17 @@
       <c r="G48" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="H48" s="49">
+      <c r="H48" s="6">
+        <v>36839</v>
+      </c>
+      <c r="I48" s="3">
+        <f>N62/I5</f>
+        <v>0.7908987437523417</v>
+      </c>
+      <c r="J48" s="3">
         <f t="shared" si="17"/>
-        <v>0.66099693891257161</v>
-      </c>
-      <c r="I48" s="49">
-        <f t="shared" si="18"/>
-        <v>1.085033544710964</v>
-      </c>
-      <c r="J48" s="50">
-        <f t="shared" si="19"/>
-        <v>1.806342035870572</v>
-      </c>
-      <c r="K48" s="29"/>
+        <v>1.1098209299201856</v>
+      </c>
       <c r="L48" s="28"/>
       <c r="M48" s="25"/>
       <c r="N48" s="27"/>
@@ -41413,19 +41443,17 @@
       <c r="G49" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="H49" s="49">
+      <c r="H49" s="6">
+        <v>659811</v>
+      </c>
+      <c r="I49" s="3">
+        <f>N63/I6</f>
+        <v>1.1799406092823301</v>
+      </c>
+      <c r="J49" s="3">
         <f t="shared" si="17"/>
-        <v>42.386499811797499</v>
-      </c>
-      <c r="I49" s="49">
-        <f t="shared" si="18"/>
-        <v>0.90098186256352963</v>
-      </c>
-      <c r="J49" s="50">
-        <f t="shared" si="19"/>
-        <v>1.7493644453878108</v>
-      </c>
-      <c r="K49" s="29"/>
+        <v>0.90899039449926899</v>
+      </c>
       <c r="L49" s="28"/>
       <c r="M49" s="25"/>
       <c r="N49" s="27"/>
@@ -41436,19 +41464,17 @@
       <c r="G50" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="H50" s="49">
+      <c r="H50" s="7">
+        <v>183206</v>
+      </c>
+      <c r="I50" s="3">
+        <f>N64/I7</f>
+        <v>0.75927716078391905</v>
+      </c>
+      <c r="J50" s="3">
         <f t="shared" si="17"/>
-        <v>18.361877923145371</v>
-      </c>
-      <c r="I50" s="49">
-        <f t="shared" si="18"/>
-        <v>1.4401429380379078</v>
-      </c>
-      <c r="J50" s="50">
-        <f t="shared" si="19"/>
-        <v>3.5058886997730339</v>
-      </c>
-      <c r="K50" s="29"/>
+        <v>0.9702130353581716</v>
+      </c>
       <c r="L50" s="28"/>
       <c r="M50" s="25"/>
       <c r="N50" s="26"/>
@@ -41459,19 +41485,17 @@
       <c r="G51" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="H51" s="49">
+      <c r="H51" s="9">
+        <v>236799</v>
+      </c>
+      <c r="I51" s="3">
+        <f>N65/I8</f>
+        <v>4.7906593961391737</v>
+      </c>
+      <c r="J51" s="3">
         <f t="shared" si="17"/>
-        <v>0.22923301833492674</v>
-      </c>
-      <c r="I51" s="49">
-        <f t="shared" si="18"/>
-        <v>0.42467544177504979</v>
-      </c>
-      <c r="J51" s="50">
-        <f t="shared" si="19"/>
-        <v>0.49339806880975456</v>
-      </c>
-      <c r="K51" s="29"/>
+        <v>0.66016272572512502</v>
+      </c>
       <c r="L51" s="28"/>
       <c r="M51" s="25"/>
       <c r="N51" s="27"/>
@@ -41482,19 +41506,17 @@
       <c r="G52" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="H52" s="49">
+      <c r="H52" s="7">
+        <v>675229</v>
+      </c>
+      <c r="I52" s="3">
+        <f>N66/I9</f>
+        <v>0.78497951760358819</v>
+      </c>
+      <c r="J52" s="3">
         <f t="shared" si="17"/>
-        <v>6.4833537137100175</v>
-      </c>
-      <c r="I52" s="49">
-        <f t="shared" si="18"/>
-        <v>0.82193894183252625</v>
-      </c>
-      <c r="J52" s="50">
-        <f t="shared" si="19"/>
-        <v>1.1342523054943381</v>
-      </c>
-      <c r="K52" s="29"/>
+        <v>0.96705779616242871</v>
+      </c>
       <c r="L52" s="28"/>
       <c r="M52" s="25"/>
       <c r="N52" s="26"/>
@@ -41505,19 +41527,17 @@
       <c r="G53" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="H53" s="49">
+      <c r="H53" s="9">
+        <v>210891</v>
+      </c>
+      <c r="I53" s="3">
+        <f>N67/I10</f>
+        <v>2.3007637140399453</v>
+      </c>
+      <c r="J53" s="3">
         <f t="shared" si="17"/>
-        <v>46.559626431146775</v>
-      </c>
-      <c r="I53" s="49">
-        <f t="shared" si="18"/>
-        <v>0.68188081250179755</v>
-      </c>
-      <c r="J53" s="50">
-        <f t="shared" si="19"/>
-        <v>1.1770791663725282</v>
-      </c>
-      <c r="K53" s="29"/>
+        <v>0.49736190528481744</v>
+      </c>
       <c r="L53" s="28"/>
       <c r="M53" s="25"/>
       <c r="N53" s="30"/>
@@ -41528,19 +41548,17 @@
       <c r="G54" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="H54" s="49">
+      <c r="H54" s="9">
+        <v>306281</v>
+      </c>
+      <c r="I54" s="3">
+        <f>N68/I11</f>
+        <v>2.0031739458391642</v>
+      </c>
+      <c r="J54" s="3">
         <f t="shared" si="17"/>
-        <v>46.689978329619237</v>
-      </c>
-      <c r="I54" s="49">
-        <f t="shared" si="18"/>
-        <v>0.60910892799862693</v>
-      </c>
-      <c r="J54" s="50">
-        <f t="shared" si="19"/>
-        <v>1.0091945323992859</v>
-      </c>
-      <c r="K54" s="29"/>
+        <v>0.5129925907142272</v>
+      </c>
       <c r="L54" s="28"/>
       <c r="M54" s="25"/>
     </row>
@@ -41592,235 +41610,360 @@
       <c r="J59" s="25"/>
       <c r="K59" s="25"/>
       <c r="L59" s="25"/>
-      <c r="M59" s="25"/>
+      <c r="M59" s="5">
+        <v>2.3635199999999998</v>
+      </c>
+      <c r="N59" s="5">
+        <v>0.78683999999999998</v>
+      </c>
+      <c r="O59" s="5">
+        <v>9.0051999999999993E-2</v>
+      </c>
     </row>
     <row r="60" spans="6:15" x14ac:dyDescent="0.2">
       <c r="F60" s="25"/>
       <c r="G60" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="H60" s="25" t="s">
-        <v>97</v>
-      </c>
-      <c r="I60" s="25" t="s">
-        <v>98</v>
-      </c>
-      <c r="J60" s="25" t="s">
-        <v>99</v>
-      </c>
+      <c r="H60" s="25"/>
+      <c r="I60" s="25"/>
+      <c r="J60" s="25"/>
       <c r="K60" s="25"/>
       <c r="L60" s="26"/>
-      <c r="M60" s="25"/>
+      <c r="M60" s="5">
+        <v>9.2776800000000001</v>
+      </c>
+      <c r="N60" s="5">
+        <v>2.10392</v>
+      </c>
+      <c r="O60" s="5">
+        <v>0.413632</v>
+      </c>
     </row>
     <row r="61" spans="6:15" x14ac:dyDescent="0.2">
       <c r="F61" s="25"/>
       <c r="G61" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="H61" s="31" t="e">
-        <f>H45/K45</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I61" s="32" t="e">
-        <f>I45/K45</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J61" s="32" t="e">
-        <f>J45/K45</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="H61" s="31"/>
+      <c r="I61" s="32"/>
+      <c r="J61" s="32"/>
       <c r="K61" s="29"/>
       <c r="L61" s="28"/>
-      <c r="M61" s="25"/>
+      <c r="M61" s="5">
+        <v>18.417400000000001</v>
+      </c>
+      <c r="N61" s="5">
+        <v>2.1268400000000001</v>
+      </c>
+      <c r="O61" s="5">
+        <v>0.88269900000000001</v>
+      </c>
     </row>
     <row r="62" spans="6:15" x14ac:dyDescent="0.2">
       <c r="F62" s="25"/>
       <c r="G62" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="H62" s="31" t="e">
-        <f t="shared" ref="H62:H70" si="20">H46/K46</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I62" s="32" t="e">
-        <f t="shared" ref="I62:I70" si="21">I46/K46</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J62" s="32" t="e">
-        <f>J46/K46</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="H62" s="31"/>
+      <c r="I62" s="32"/>
+      <c r="J62" s="32"/>
       <c r="K62" s="29"/>
       <c r="L62" s="28"/>
-      <c r="M62" s="25"/>
+      <c r="M62" s="5">
+        <v>1.47356</v>
+      </c>
+      <c r="N62" s="5">
+        <v>3.5799999999999998E-2</v>
+      </c>
+      <c r="O62" s="5">
+        <v>5.0236000000000003E-2</v>
+      </c>
     </row>
     <row r="63" spans="6:15" x14ac:dyDescent="0.2">
       <c r="F63" s="25"/>
       <c r="G63" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="H63" s="31" t="e">
-        <f t="shared" si="20"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I63" s="32" t="e">
-        <f t="shared" si="21"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J63" s="32" t="e">
-        <f t="shared" ref="J63:J70" si="22">J47/K47</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="H63" s="31"/>
+      <c r="I63" s="32"/>
+      <c r="J63" s="32"/>
       <c r="K63" s="29"/>
       <c r="L63" s="28"/>
-      <c r="M63" s="25"/>
+      <c r="M63" s="5">
+        <v>26.392399999999999</v>
+      </c>
+      <c r="N63" s="5">
+        <v>1.7683199999999999</v>
+      </c>
+      <c r="O63" s="5">
+        <v>1.36226</v>
+      </c>
     </row>
     <row r="64" spans="6:15" x14ac:dyDescent="0.2">
       <c r="F64" s="25"/>
       <c r="G64" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="H64" s="31" t="e">
-        <f t="shared" si="20"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I64" s="32" t="e">
-        <f t="shared" si="21"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J64" s="32" t="e">
-        <f t="shared" si="22"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="H64" s="31"/>
+      <c r="I64" s="32"/>
+      <c r="J64" s="32"/>
       <c r="K64" s="29"/>
       <c r="L64" s="28"/>
-      <c r="M64" s="25"/>
+      <c r="M64" s="5">
+        <v>7.3282400000000001</v>
+      </c>
+      <c r="N64" s="5">
+        <v>0.28064</v>
+      </c>
+      <c r="O64" s="5">
+        <v>0.35860500000000001</v>
+      </c>
     </row>
-    <row r="65" spans="6:13" x14ac:dyDescent="0.2">
+    <row r="65" spans="6:15" x14ac:dyDescent="0.2">
       <c r="F65" s="25"/>
       <c r="G65" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="H65" s="31" t="e">
-        <f t="shared" si="20"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I65" s="32" t="e">
-        <f t="shared" si="21"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J65" s="32" t="e">
-        <f t="shared" si="22"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="H65" s="31"/>
+      <c r="I65" s="32"/>
+      <c r="J65" s="32"/>
       <c r="K65" s="29"/>
       <c r="L65" s="28"/>
-      <c r="M65" s="25"/>
+      <c r="M65" s="10">
+        <v>9.4719599999999993</v>
+      </c>
+      <c r="N65" s="10">
+        <v>1.4186000000000001</v>
+      </c>
+      <c r="O65" s="5">
+        <v>0.19548599999999999</v>
+      </c>
     </row>
-    <row r="66" spans="6:13" x14ac:dyDescent="0.2">
+    <row r="66" spans="6:15" x14ac:dyDescent="0.2">
       <c r="F66" s="25"/>
       <c r="G66" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="H66" s="31" t="e">
-        <f t="shared" si="20"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I66" s="32" t="e">
-        <f t="shared" si="21"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J66" s="32" t="e">
-        <f t="shared" si="22"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="H66" s="31"/>
+      <c r="I66" s="32"/>
+      <c r="J66" s="32"/>
       <c r="K66" s="29"/>
       <c r="L66" s="28"/>
-      <c r="M66" s="25"/>
+      <c r="M66" s="5">
+        <v>27.0092</v>
+      </c>
+      <c r="N66" s="5">
+        <v>0.93255999999999994</v>
+      </c>
+      <c r="O66" s="5">
+        <v>1.1488700000000001</v>
+      </c>
     </row>
-    <row r="67" spans="6:13" x14ac:dyDescent="0.2">
+    <row r="67" spans="6:15" x14ac:dyDescent="0.2">
       <c r="F67" s="25"/>
       <c r="G67" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="H67" s="31" t="e">
-        <f t="shared" si="20"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I67" s="32" t="e">
-        <f t="shared" si="21"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J67" s="32" t="e">
-        <f t="shared" si="22"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="H67" s="31"/>
+      <c r="I67" s="32"/>
+      <c r="J67" s="32"/>
       <c r="K67" s="29"/>
       <c r="L67" s="28"/>
-      <c r="M67" s="25"/>
+      <c r="M67" s="10">
+        <v>8.4356399999999994</v>
+      </c>
+      <c r="N67" s="10">
+        <v>1.75996</v>
+      </c>
+      <c r="O67" s="5">
+        <v>0.38045499999999999</v>
+      </c>
     </row>
-    <row r="68" spans="6:13" x14ac:dyDescent="0.2">
+    <row r="68" spans="6:15" x14ac:dyDescent="0.2">
       <c r="F68" s="25"/>
       <c r="G68" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="H68" s="31" t="e">
-        <f t="shared" si="20"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I68" s="32" t="e">
-        <f t="shared" si="21"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J68" s="32" t="e">
-        <f t="shared" si="22"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="H68" s="31"/>
+      <c r="I68" s="32"/>
+      <c r="J68" s="32"/>
       <c r="K68" s="29"/>
       <c r="L68" s="28"/>
-      <c r="M68" s="25"/>
+      <c r="M68" s="10">
+        <v>12.251200000000001</v>
+      </c>
+      <c r="N68" s="10">
+        <v>2.2250000000000001</v>
+      </c>
+      <c r="O68" s="5">
+        <v>0.56979999999999997</v>
+      </c>
     </row>
-    <row r="69" spans="6:13" x14ac:dyDescent="0.2">
+    <row r="69" spans="6:15" x14ac:dyDescent="0.2">
       <c r="F69" s="25"/>
       <c r="G69" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="H69" s="31" t="e">
-        <f t="shared" si="20"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I69" s="32" t="e">
-        <f t="shared" si="21"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J69" s="32" t="e">
-        <f t="shared" si="22"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="H69" s="31"/>
+      <c r="I69" s="32"/>
+      <c r="J69" s="32"/>
       <c r="K69" s="29"/>
       <c r="L69" s="28"/>
       <c r="M69" s="25"/>
     </row>
-    <row r="70" spans="6:13" x14ac:dyDescent="0.2">
+    <row r="70" spans="6:15" x14ac:dyDescent="0.2">
       <c r="F70" s="25"/>
       <c r="G70" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="H70" s="31" t="e">
-        <f t="shared" si="20"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I70" s="32" t="e">
-        <f t="shared" si="21"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J70" s="32" t="e">
-        <f t="shared" si="22"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="H70" s="31"/>
+      <c r="I70" s="32"/>
+      <c r="J70" s="32"/>
       <c r="K70" s="29"/>
       <c r="L70" s="28"/>
       <c r="M70" s="25"/>
+    </row>
+    <row r="75" spans="6:15" x14ac:dyDescent="0.2">
+      <c r="G75" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="H75" t="s">
+        <v>128</v>
+      </c>
+      <c r="I75" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="76" spans="6:15" x14ac:dyDescent="0.2">
+      <c r="G76" s="27" t="s">
+        <v>2</v>
+      </c>
+      <c r="H76" s="12">
+        <f>L2/K2</f>
+        <v>0.9996998691429464</v>
+      </c>
+      <c r="I76" s="3">
+        <f>(K2+O2)/K2</f>
+        <v>3.8621438947381064</v>
+      </c>
+    </row>
+    <row r="77" spans="6:15" x14ac:dyDescent="0.2">
+      <c r="G77" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="H77" s="12">
+        <f t="shared" ref="H77:H85" si="18">L3/K3</f>
+        <v>1.1320011614315388</v>
+      </c>
+      <c r="I77" s="3">
+        <f t="shared" ref="I77:I85" si="19">(K3+O3)/K3</f>
+        <v>2.1541800367786657</v>
+      </c>
+    </row>
+    <row r="78" spans="6:15" x14ac:dyDescent="0.2">
+      <c r="G78" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="H78" s="12">
+        <f t="shared" si="18"/>
+        <v>1.1059902773303658</v>
+      </c>
+      <c r="I78" s="3">
+        <f t="shared" si="19"/>
+        <v>1.4099920930096348</v>
+      </c>
+    </row>
+    <row r="79" spans="6:15" x14ac:dyDescent="0.2">
+      <c r="G79" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="H79" s="12">
+        <f t="shared" si="18"/>
+        <v>2.0300074398611225</v>
+      </c>
+      <c r="I79" s="3">
+        <f t="shared" si="19"/>
+        <v>1.2417128213606679</v>
+      </c>
+    </row>
+    <row r="80" spans="6:15" x14ac:dyDescent="0.2">
+      <c r="G80" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="H80" s="12">
+        <f t="shared" si="18"/>
+        <v>1.3168264110756123</v>
+      </c>
+      <c r="I80" s="3">
+        <f t="shared" si="19"/>
+        <v>1.283756002605843</v>
+      </c>
+    </row>
+    <row r="81" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="G81" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="H81" s="12">
+        <f t="shared" si="18"/>
+        <v>1.1975531397923003</v>
+      </c>
+      <c r="I81" s="3">
+        <f t="shared" si="19"/>
+        <v>1.1050197080686093</v>
+      </c>
+    </row>
+    <row r="82" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="G82" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="H82" s="12">
+        <f t="shared" si="18"/>
+        <v>1.8279791842311828</v>
+      </c>
+      <c r="I82" s="3">
+        <f t="shared" si="19"/>
+        <v>4.6969503154344849</v>
+      </c>
+    </row>
+    <row r="83" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="G83" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="H83" s="12">
+        <f t="shared" si="18"/>
+        <v>1.7790255758110183</v>
+      </c>
+      <c r="I83" s="3">
+        <f t="shared" si="19"/>
+        <v>1.2980771683324892</v>
+      </c>
+    </row>
+    <row r="84" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="G84" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="H84" s="12">
+        <f t="shared" si="18"/>
+        <v>1.1518410394795535</v>
+      </c>
+      <c r="I84" s="3">
+        <f t="shared" si="19"/>
+        <v>2.2495484076123682</v>
+      </c>
+    </row>
+    <row r="85" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="G85" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="H85" s="12">
+        <f t="shared" si="18"/>
+        <v>1.1818880581370974</v>
+      </c>
+      <c r="I85" s="3">
+        <f t="shared" si="19"/>
+        <v>2.2263293969673676</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -43006,7 +43149,7 @@
         <v>75</v>
       </c>
       <c r="L1" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
@@ -43032,7 +43175,7 @@
         <v>11.860200000000001</v>
       </c>
       <c r="L2" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
@@ -43337,12 +43480,12 @@
         <v>0.27705099999999999</v>
       </c>
       <c r="L19" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="L20" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -43827,544 +43970,544 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>105</v>
-      </c>
-      <c r="K1" s="52" t="s">
-        <v>120</v>
+        <v>99</v>
+      </c>
+      <c r="K1" s="50" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="K2" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="K3" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A6" s="51" t="s">
+      <c r="A6" s="49" t="s">
+        <v>101</v>
+      </c>
+      <c r="B6" t="s">
+        <v>102</v>
+      </c>
+      <c r="C6" t="s">
+        <v>103</v>
+      </c>
+      <c r="D6" t="s">
+        <v>104</v>
+      </c>
+      <c r="E6" t="s">
+        <v>105</v>
+      </c>
+      <c r="F6" t="s">
+        <v>106</v>
+      </c>
+      <c r="G6" t="s">
         <v>107</v>
       </c>
-      <c r="B6" t="s">
+      <c r="H6" t="s">
         <v>108</v>
       </c>
-      <c r="C6" t="s">
-        <v>109</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="I6" t="s">
+        <v>118</v>
+      </c>
+      <c r="J6" t="s">
+        <v>120</v>
+      </c>
+      <c r="K6" t="s">
+        <v>121</v>
+      </c>
+      <c r="L6" t="s">
         <v>110</v>
       </c>
-      <c r="E6" t="s">
+      <c r="M6" t="s">
         <v>111</v>
       </c>
-      <c r="F6" t="s">
+      <c r="N6" t="s">
         <v>112</v>
       </c>
-      <c r="G6" t="s">
+      <c r="O6" t="s">
         <v>113</v>
-      </c>
-      <c r="H6" t="s">
-        <v>114</v>
-      </c>
-      <c r="I6" t="s">
-        <v>124</v>
-      </c>
-      <c r="J6" t="s">
-        <v>126</v>
-      </c>
-      <c r="K6" t="s">
-        <v>127</v>
-      </c>
-      <c r="L6" t="s">
-        <v>116</v>
-      </c>
-      <c r="M6" t="s">
-        <v>117</v>
-      </c>
-      <c r="N6" t="s">
-        <v>118</v>
-      </c>
-      <c r="O6" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A7" s="51">
+      <c r="A7" s="49">
         <v>44972</v>
       </c>
-      <c r="B7" s="55">
+      <c r="B7" s="53">
         <v>2.6</v>
       </c>
-      <c r="C7" s="53">
+      <c r="C7" s="51">
         <v>17500</v>
       </c>
-      <c r="D7" s="55">
+      <c r="D7" s="53">
         <v>504</v>
       </c>
-      <c r="E7" s="55">
+      <c r="E7" s="53">
         <v>19.399999999999999</v>
       </c>
-      <c r="F7" s="55">
+      <c r="F7" s="53">
         <v>10.1</v>
       </c>
-      <c r="G7" s="55">
+      <c r="G7" s="53">
         <v>20.2</v>
       </c>
-      <c r="H7" s="55">
+      <c r="H7" s="53">
         <v>261</v>
       </c>
-      <c r="I7" s="55">
+      <c r="I7" s="53">
         <v>87.626400000000004</v>
       </c>
-      <c r="J7" s="55">
+      <c r="J7" s="53">
         <v>2.78</v>
       </c>
-      <c r="K7" s="55">
+      <c r="K7" s="53">
         <v>5.07</v>
       </c>
-      <c r="L7" s="55">
+      <c r="L7" s="53">
         <v>44.8962</v>
       </c>
-      <c r="M7" s="55">
+      <c r="M7" s="53">
         <v>5.21</v>
       </c>
-      <c r="N7" s="55">
+      <c r="N7" s="53">
         <v>10.4</v>
       </c>
-      <c r="O7" s="55">
+      <c r="O7" s="53">
         <v>20.2</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A8" s="51">
+      <c r="A8" s="49">
         <v>89937</v>
       </c>
-      <c r="B8" s="55">
+      <c r="B8" s="53">
         <v>5.0999999999999996</v>
       </c>
-      <c r="C8" s="53">
+      <c r="C8" s="51">
         <v>29600</v>
       </c>
-      <c r="D8" s="55">
+      <c r="D8" s="53">
         <v>1010</v>
       </c>
-      <c r="E8" s="55">
+      <c r="E8" s="53">
         <v>78.900000000000006</v>
       </c>
-      <c r="F8" s="55">
+      <c r="F8" s="53">
         <v>22.8</v>
       </c>
-      <c r="G8" s="55">
+      <c r="G8" s="53">
         <v>45.4</v>
       </c>
-      <c r="H8" s="55">
+      <c r="H8" s="53">
         <v>484</v>
       </c>
-      <c r="I8" s="55">
+      <c r="I8" s="53">
         <v>148.56299999999999</v>
       </c>
-      <c r="J8" s="55">
+      <c r="J8" s="53">
         <v>5.0599999999999996</v>
       </c>
-      <c r="K8" s="55">
+      <c r="K8" s="53">
         <v>32</v>
       </c>
-      <c r="L8" s="55">
+      <c r="L8" s="53">
         <v>79.006799999999998</v>
       </c>
-      <c r="M8" s="55">
+      <c r="M8" s="53">
         <v>10.6</v>
       </c>
-      <c r="N8" s="55">
+      <c r="N8" s="53">
         <v>21.8</v>
       </c>
-      <c r="O8" s="55">
+      <c r="O8" s="53">
         <v>42.2</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A9" s="51">
+      <c r="A9" s="49">
         <v>134921</v>
       </c>
-      <c r="B9" s="55">
+      <c r="B9" s="53">
         <v>7.7</v>
       </c>
-      <c r="C9" s="53">
+      <c r="C9" s="51">
         <v>75300</v>
       </c>
-      <c r="D9" s="55">
+      <c r="D9" s="53">
         <v>2040</v>
       </c>
-      <c r="E9" s="55">
+      <c r="E9" s="53">
         <v>73.5</v>
       </c>
-      <c r="F9" s="55">
+      <c r="F9" s="53">
         <v>34.700000000000003</v>
       </c>
-      <c r="G9" s="55">
+      <c r="G9" s="53">
         <v>84.3</v>
       </c>
-      <c r="H9" s="55">
+      <c r="H9" s="53">
         <v>1170</v>
       </c>
-      <c r="I9" s="55">
+      <c r="I9" s="53">
         <v>397.91300000000001</v>
       </c>
-      <c r="J9" s="55">
+      <c r="J9" s="53">
         <v>7.77</v>
       </c>
-      <c r="K9" s="55">
+      <c r="K9" s="53">
         <v>7.56</v>
       </c>
-      <c r="L9" s="55">
+      <c r="L9" s="53">
         <v>71.266400000000004</v>
       </c>
-      <c r="M9" s="55">
+      <c r="M9" s="53">
         <v>16.7</v>
       </c>
-      <c r="N9" s="55">
+      <c r="N9" s="53">
         <v>33.700000000000003</v>
       </c>
-      <c r="O9" s="55">
+      <c r="O9" s="53">
         <v>65.900000000000006</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A10" s="51">
+      <c r="A10" s="49">
         <v>179903</v>
       </c>
-      <c r="B10" s="55">
+      <c r="B10" s="53">
         <v>11</v>
       </c>
-      <c r="C10" s="53">
+      <c r="C10" s="51">
         <v>63000</v>
       </c>
-      <c r="D10" s="55">
+      <c r="D10" s="53">
         <v>2300</v>
       </c>
-      <c r="E10" s="55">
+      <c r="E10" s="53">
         <v>186</v>
       </c>
-      <c r="F10" s="55">
+      <c r="F10" s="53">
         <v>58.3</v>
       </c>
-      <c r="G10" s="55">
+      <c r="G10" s="53">
         <v>105</v>
       </c>
-      <c r="H10" s="55">
+      <c r="H10" s="53">
         <v>1120</v>
       </c>
-      <c r="I10" s="55">
+      <c r="I10" s="53">
         <v>348.62700000000001</v>
       </c>
-      <c r="J10" s="55">
+      <c r="J10" s="53">
         <v>7.05</v>
       </c>
-      <c r="K10" s="55">
+      <c r="K10" s="53">
         <v>62.2</v>
       </c>
-      <c r="L10" s="55">
+      <c r="L10" s="53">
         <v>253.42099999999999</v>
       </c>
-      <c r="M10" s="55">
+      <c r="M10" s="53">
         <v>22.2</v>
       </c>
-      <c r="N10" s="55">
+      <c r="N10" s="53">
         <v>45</v>
       </c>
-      <c r="O10" s="55">
+      <c r="O10" s="53">
         <v>86.5</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A11" s="51">
+      <c r="A11" s="49">
         <v>224883</v>
       </c>
-      <c r="B11" s="55">
+      <c r="B11" s="53">
         <v>14</v>
       </c>
-      <c r="C11" s="53">
+      <c r="C11" s="51">
         <v>103000</v>
       </c>
-      <c r="D11" s="55">
+      <c r="D11" s="53">
         <v>3010</v>
       </c>
-      <c r="E11" s="55">
+      <c r="E11" s="53">
         <v>139</v>
       </c>
-      <c r="F11" s="55">
+      <c r="F11" s="53">
         <v>58.5</v>
       </c>
-      <c r="G11" s="55">
+      <c r="G11" s="53">
         <v>128</v>
       </c>
-      <c r="H11" s="55">
+      <c r="H11" s="53">
         <v>1790</v>
       </c>
-      <c r="I11" s="55">
+      <c r="I11" s="53">
         <v>548.89800000000002</v>
       </c>
-      <c r="J11" s="55">
+      <c r="J11" s="53">
         <v>18.899999999999999</v>
       </c>
-      <c r="K11" s="55">
+      <c r="K11" s="53">
         <v>48.1</v>
       </c>
-      <c r="L11" s="55">
+      <c r="L11" s="53">
         <v>294.65100000000001</v>
       </c>
-      <c r="M11" s="55">
+      <c r="M11" s="53">
         <v>26.6</v>
       </c>
-      <c r="N11" s="55">
+      <c r="N11" s="53">
         <v>53.5</v>
       </c>
-      <c r="O11" s="55">
+      <c r="O11" s="53">
         <v>105</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A12" s="51">
+      <c r="A12" s="49">
         <v>269860</v>
       </c>
-      <c r="B12" s="55">
+      <c r="B12" s="53">
         <v>17</v>
       </c>
-      <c r="C12" s="53">
+      <c r="C12" s="51">
         <v>138000</v>
       </c>
-      <c r="D12" s="55">
+      <c r="D12" s="53">
         <v>4200</v>
       </c>
-      <c r="E12" s="55">
+      <c r="E12" s="53">
         <v>99.4</v>
       </c>
-      <c r="F12" s="55">
+      <c r="F12" s="53">
         <v>75.5</v>
       </c>
-      <c r="G12" s="55">
+      <c r="G12" s="53">
         <v>164</v>
       </c>
-      <c r="H12" s="55">
+      <c r="H12" s="53">
         <v>2350</v>
       </c>
-      <c r="I12" s="55">
+      <c r="I12" s="53">
         <v>884.90599999999995</v>
       </c>
-      <c r="J12" s="55">
+      <c r="J12" s="53">
         <v>18.7</v>
       </c>
-      <c r="K12" s="55">
+      <c r="K12" s="53">
         <v>18.7</v>
       </c>
-      <c r="L12" s="55">
+      <c r="L12" s="53">
         <v>389.85899999999998</v>
       </c>
-      <c r="M12" s="55">
+      <c r="M12" s="53">
         <v>34.700000000000003</v>
       </c>
-      <c r="N12" s="55">
+      <c r="N12" s="53">
         <v>68.8</v>
       </c>
-      <c r="O12" s="55">
+      <c r="O12" s="53">
         <v>135</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A13" s="51">
+      <c r="A13" s="49">
         <v>314838</v>
       </c>
-      <c r="B13" s="55">
+      <c r="B13" s="53">
         <v>20</v>
       </c>
-      <c r="C13" s="53">
+      <c r="C13" s="51">
         <v>148000</v>
       </c>
-      <c r="D13" s="55">
+      <c r="D13" s="53">
         <v>4210</v>
       </c>
-      <c r="E13" s="55">
+      <c r="E13" s="53">
         <v>345</v>
       </c>
-      <c r="F13" s="55">
+      <c r="F13" s="53">
         <v>88.1</v>
       </c>
-      <c r="G13" s="55">
+      <c r="G13" s="53">
         <v>187</v>
       </c>
-      <c r="H13" s="55">
+      <c r="H13" s="53">
         <v>2440</v>
       </c>
-      <c r="I13" s="55">
+      <c r="I13" s="53">
         <v>885.56700000000001</v>
       </c>
-      <c r="J13" s="55">
+      <c r="J13" s="53">
         <v>13.1</v>
       </c>
-      <c r="K13" s="55">
+      <c r="K13" s="53">
         <v>111</v>
       </c>
-      <c r="L13" s="55">
+      <c r="L13" s="53">
         <v>383.44600000000003</v>
       </c>
-      <c r="M13" s="55">
+      <c r="M13" s="53">
         <v>38.1</v>
       </c>
-      <c r="N13" s="55">
+      <c r="N13" s="53">
         <v>77.5</v>
       </c>
-      <c r="O13" s="55">
+      <c r="O13" s="53">
         <v>152</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A14" s="51">
+      <c r="A14" s="49">
         <v>359814</v>
       </c>
-      <c r="B14" s="55">
+      <c r="B14" s="53">
         <v>23</v>
       </c>
-      <c r="C14" s="53">
+      <c r="C14" s="51">
         <v>95300</v>
       </c>
-      <c r="D14" s="55">
+      <c r="D14" s="53">
         <v>4090</v>
       </c>
-      <c r="E14" s="55">
+      <c r="E14" s="53">
         <v>522</v>
       </c>
-      <c r="F14" s="55">
+      <c r="F14" s="53">
         <v>95.3</v>
       </c>
-      <c r="G14" s="55">
+      <c r="G14" s="53">
         <v>190</v>
       </c>
-      <c r="H14" s="55">
+      <c r="H14" s="53">
         <v>1750</v>
       </c>
-      <c r="I14" s="55">
+      <c r="I14" s="53">
         <v>587.96</v>
       </c>
-      <c r="J14" s="55">
+      <c r="J14" s="53">
         <v>66.5</v>
       </c>
-      <c r="K14" s="55">
+      <c r="K14" s="53">
         <v>178</v>
       </c>
-      <c r="L14" s="55">
+      <c r="L14" s="53">
         <v>229.12899999999999</v>
       </c>
-      <c r="M14" s="55">
+      <c r="M14" s="53">
         <v>44</v>
       </c>
-      <c r="N14" s="55">
+      <c r="N14" s="53">
         <v>88.1</v>
       </c>
-      <c r="O14" s="55">
+      <c r="O14" s="53">
         <v>170</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A15" s="51">
+      <c r="A15" s="49">
         <v>404787</v>
       </c>
-      <c r="B15" s="55">
+      <c r="B15" s="53">
         <v>25</v>
       </c>
-      <c r="C15" s="53">
+      <c r="C15" s="51">
         <v>118000</v>
       </c>
-      <c r="D15" s="55">
+      <c r="D15" s="53">
         <v>5100</v>
       </c>
-      <c r="E15" s="55">
+      <c r="E15" s="53">
         <v>361</v>
       </c>
-      <c r="F15" s="55">
+      <c r="F15" s="53">
         <v>110</v>
       </c>
-      <c r="G15" s="55">
+      <c r="G15" s="53">
         <v>225</v>
       </c>
-      <c r="H15" s="55">
+      <c r="H15" s="53">
         <v>2270</v>
       </c>
-      <c r="I15" s="55">
+      <c r="I15" s="53">
         <v>656.274</v>
       </c>
-      <c r="J15" s="55">
+      <c r="J15" s="53">
         <v>54.3</v>
       </c>
-      <c r="K15" s="55">
+      <c r="K15" s="53">
         <v>143</v>
       </c>
-      <c r="L15" s="55">
+      <c r="L15" s="53">
         <v>456.24299999999999</v>
       </c>
-      <c r="M15" s="55">
+      <c r="M15" s="53">
         <v>49.3</v>
       </c>
-      <c r="N15" s="55">
+      <c r="N15" s="53">
         <v>99.4</v>
       </c>
-      <c r="O15" s="55">
+      <c r="O15" s="53">
         <v>195</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A16" s="51">
+      <c r="A16" s="49">
         <v>449757</v>
       </c>
-      <c r="B16" s="55">
+      <c r="B16" s="53">
         <v>28</v>
       </c>
-      <c r="C16" s="53">
+      <c r="C16" s="51">
         <v>199000</v>
       </c>
-      <c r="D16" s="55">
+      <c r="D16" s="53">
         <v>6280</v>
       </c>
-      <c r="E16" s="55">
+      <c r="E16" s="53">
         <v>286</v>
       </c>
-      <c r="F16" s="55">
+      <c r="F16" s="53">
         <v>122</v>
       </c>
-      <c r="G16" s="55">
+      <c r="G16" s="53">
         <v>277</v>
       </c>
-      <c r="H16" s="55">
+      <c r="H16" s="53">
         <v>3280</v>
       </c>
-      <c r="I16" s="55">
+      <c r="I16" s="53">
         <v>1164.77</v>
       </c>
-      <c r="J16" s="55">
+      <c r="J16" s="53">
         <v>65.2</v>
       </c>
-      <c r="K16" s="55">
+      <c r="K16" s="53">
         <v>105</v>
       </c>
-      <c r="L16" s="55">
+      <c r="L16" s="53">
         <v>439.85700000000003</v>
       </c>
-      <c r="M16" s="55">
+      <c r="M16" s="53">
         <v>55.7</v>
       </c>
-      <c r="N16" s="55">
+      <c r="N16" s="53">
         <v>129</v>
       </c>
-      <c r="O16" s="55">
+      <c r="O16" s="53">
         <v>231</v>
       </c>
     </row>
@@ -44374,525 +44517,525 @@
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A31" s="51" t="s">
+      <c r="A31" s="49" t="s">
+        <v>101</v>
+      </c>
+      <c r="B31" t="s">
+        <v>102</v>
+      </c>
+      <c r="C31" t="s">
+        <v>103</v>
+      </c>
+      <c r="D31" t="s">
+        <v>104</v>
+      </c>
+      <c r="E31" t="s">
+        <v>105</v>
+      </c>
+      <c r="F31" t="s">
+        <v>106</v>
+      </c>
+      <c r="G31" t="s">
         <v>107</v>
       </c>
-      <c r="B31" t="s">
+      <c r="H31" t="s">
         <v>108</v>
       </c>
-      <c r="C31" t="s">
+      <c r="I31" t="s">
+        <v>118</v>
+      </c>
+      <c r="J31" t="s">
         <v>109</v>
       </c>
-      <c r="D31" t="s">
+      <c r="K31" t="s">
+        <v>121</v>
+      </c>
+      <c r="L31" t="s">
         <v>110</v>
       </c>
-      <c r="E31" t="s">
+      <c r="M31" t="s">
         <v>111</v>
       </c>
-      <c r="F31" t="s">
+      <c r="N31" t="s">
         <v>112</v>
       </c>
-      <c r="G31" t="s">
+      <c r="O31" t="s">
         <v>113</v>
-      </c>
-      <c r="H31" t="s">
-        <v>114</v>
-      </c>
-      <c r="I31" t="s">
-        <v>124</v>
-      </c>
-      <c r="J31" t="s">
-        <v>115</v>
-      </c>
-      <c r="K31" t="s">
-        <v>127</v>
-      </c>
-      <c r="L31" t="s">
-        <v>116</v>
-      </c>
-      <c r="M31" t="s">
-        <v>117</v>
-      </c>
-      <c r="N31" t="s">
-        <v>118</v>
-      </c>
-      <c r="O31" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A32" s="51">
+      <c r="A32" s="49">
         <v>44972</v>
       </c>
-      <c r="B32" s="54">
+      <c r="B32" s="52">
         <v>4.8899999999999997</v>
       </c>
-      <c r="C32" s="54">
+      <c r="C32" s="52">
         <v>0.92841099999999999</v>
       </c>
-      <c r="D32" s="54">
+      <c r="D32" s="52">
         <v>0.93</v>
       </c>
-      <c r="E32" s="54">
+      <c r="E32" s="52">
         <v>2.78</v>
       </c>
-      <c r="F32" s="54">
+      <c r="F32" s="52">
         <v>3.06</v>
       </c>
-      <c r="G32" s="54">
+      <c r="G32" s="52">
         <v>2.2599999999999998</v>
       </c>
-      <c r="H32" s="54">
+      <c r="H32" s="52">
         <v>1.6</v>
       </c>
-      <c r="I32" s="54">
+      <c r="I32" s="52">
         <v>0.509718</v>
       </c>
-      <c r="J32" s="54">
+      <c r="J32" s="52">
         <v>3.6</v>
       </c>
-      <c r="K32" s="54">
+      <c r="K32" s="52">
         <v>2.76</v>
       </c>
-      <c r="L32" s="54">
+      <c r="L32" s="52">
         <v>1.69208</v>
       </c>
-      <c r="M32" s="54">
+      <c r="M32" s="52">
         <v>2.31</v>
       </c>
-      <c r="N32" s="54">
+      <c r="N32" s="52">
         <v>1.62</v>
       </c>
-      <c r="O32" s="54">
+      <c r="O32" s="52">
         <v>1.18</v>
       </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A33" s="51">
+      <c r="A33" s="49">
         <v>89937</v>
       </c>
-      <c r="B33" s="54">
+      <c r="B33" s="52">
         <v>9.77</v>
       </c>
-      <c r="C33" s="54">
+      <c r="C33" s="52">
         <v>1.9160489999999999</v>
       </c>
-      <c r="D33" s="54">
+      <c r="D33" s="52">
         <v>1.8</v>
       </c>
-      <c r="E33" s="54">
+      <c r="E33" s="52">
         <v>5.53</v>
       </c>
-      <c r="F33" s="54">
+      <c r="F33" s="52">
         <v>6.12</v>
       </c>
-      <c r="G33" s="54">
+      <c r="G33" s="52">
         <v>4.5199999999999996</v>
       </c>
-      <c r="H33" s="54">
+      <c r="H33" s="52">
         <v>3.36</v>
       </c>
-      <c r="I33" s="54">
+      <c r="I33" s="52">
         <v>0.99899099999999996</v>
       </c>
-      <c r="J33" s="54">
+      <c r="J33" s="52">
         <v>7.25</v>
       </c>
-      <c r="K33" s="54">
+      <c r="K33" s="52">
         <v>5.49</v>
       </c>
-      <c r="L33" s="54">
+      <c r="L33" s="52">
         <v>3.3683200000000002</v>
       </c>
-      <c r="M33" s="54">
+      <c r="M33" s="52">
         <v>4.6100000000000003</v>
       </c>
-      <c r="N33" s="54">
+      <c r="N33" s="52">
         <v>3.23</v>
       </c>
-      <c r="O33" s="54">
+      <c r="O33" s="52">
         <v>2.34</v>
       </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A34" s="51">
+      <c r="A34" s="49">
         <v>134921</v>
       </c>
-      <c r="B34" s="54">
+      <c r="B34" s="52">
         <v>14.65</v>
       </c>
-      <c r="C34" s="54">
+      <c r="C34" s="52">
         <v>2.9083640000000002</v>
       </c>
-      <c r="D34" s="54">
+      <c r="D34" s="52">
         <v>2.69</v>
       </c>
-      <c r="E34" s="54">
+      <c r="E34" s="52">
         <v>8.2899999999999991</v>
       </c>
-      <c r="F34" s="54">
+      <c r="F34" s="52">
         <v>9.18</v>
       </c>
-      <c r="G34" s="54">
+      <c r="G34" s="52">
         <v>6.78</v>
       </c>
-      <c r="H34" s="54">
+      <c r="H34" s="52">
         <v>5.32</v>
       </c>
-      <c r="I34" s="54">
+      <c r="I34" s="52">
         <v>1.4875100000000001</v>
       </c>
-      <c r="J34" s="54">
+      <c r="J34" s="52">
         <v>10.89</v>
       </c>
-      <c r="K34" s="54">
+      <c r="K34" s="52">
         <v>8.2100000000000009</v>
       </c>
-      <c r="L34" s="54">
+      <c r="L34" s="52">
         <v>5.0148900000000003</v>
       </c>
-      <c r="M34" s="54">
+      <c r="M34" s="52">
         <v>6.91</v>
       </c>
-      <c r="N34" s="54">
+      <c r="N34" s="52">
         <v>4.83</v>
       </c>
-      <c r="O34" s="54">
+      <c r="O34" s="52">
         <v>3.51</v>
       </c>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A35" s="51">
+      <c r="A35" s="49">
         <v>179903</v>
       </c>
-      <c r="B35" s="54">
+      <c r="B35" s="52">
         <v>19.54</v>
       </c>
-      <c r="C35" s="54">
+      <c r="C35" s="52">
         <v>3.8546860000000001</v>
       </c>
-      <c r="D35" s="54">
+      <c r="D35" s="52">
         <v>3.57</v>
       </c>
-      <c r="E35" s="54">
+      <c r="E35" s="52">
         <v>11.05</v>
       </c>
-      <c r="F35" s="54">
+      <c r="F35" s="52">
         <v>12.23</v>
       </c>
-      <c r="G35" s="54">
+      <c r="G35" s="52">
         <v>9.0299999999999994</v>
       </c>
-      <c r="H35" s="54">
+      <c r="H35" s="52">
         <v>7.09</v>
       </c>
-      <c r="I35" s="54">
+      <c r="I35" s="52">
         <v>1.9766600000000001</v>
       </c>
-      <c r="J35" s="54">
+      <c r="J35" s="52">
         <v>14.51</v>
       </c>
-      <c r="K35" s="54">
+      <c r="K35" s="52">
         <v>11</v>
       </c>
-      <c r="L35" s="54">
+      <c r="L35" s="52">
         <v>6.6793899999999997</v>
       </c>
-      <c r="M35" s="54">
+      <c r="M35" s="52">
         <v>9.2100000000000009</v>
       </c>
-      <c r="N35" s="54">
+      <c r="N35" s="52">
         <v>6.44</v>
       </c>
-      <c r="O35" s="54">
+      <c r="O35" s="52">
         <v>4.68</v>
       </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A36" s="51">
+      <c r="A36" s="49">
         <v>224883</v>
       </c>
-      <c r="B36" s="54">
+      <c r="B36" s="52">
         <v>24.43</v>
       </c>
-      <c r="C36" s="54">
+      <c r="C36" s="52">
         <v>4.8074339999999998</v>
       </c>
-      <c r="D36" s="54">
+      <c r="D36" s="52">
         <v>4.45</v>
       </c>
-      <c r="E36" s="54">
+      <c r="E36" s="52">
         <v>13.81</v>
       </c>
-      <c r="F36" s="54">
+      <c r="F36" s="52">
         <v>15.28</v>
       </c>
-      <c r="G36" s="54">
+      <c r="G36" s="52">
         <v>11.29</v>
       </c>
-      <c r="H36" s="54">
+      <c r="H36" s="52">
         <v>8.84</v>
       </c>
-      <c r="I36" s="54">
+      <c r="I36" s="52">
         <v>2.4655999999999998</v>
       </c>
-      <c r="J36" s="54">
+      <c r="J36" s="52">
         <v>18.11</v>
       </c>
-      <c r="K36" s="54">
+      <c r="K36" s="52">
         <v>13.77</v>
       </c>
-      <c r="L36" s="54">
+      <c r="L36" s="52">
         <v>8.3453999999999997</v>
       </c>
-      <c r="M36" s="54">
+      <c r="M36" s="52">
         <v>11.5</v>
       </c>
-      <c r="N36" s="54">
+      <c r="N36" s="52">
         <v>8.0500000000000007</v>
       </c>
-      <c r="O36" s="54">
+      <c r="O36" s="52">
         <v>5.84</v>
       </c>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A37" s="51">
+      <c r="A37" s="49">
         <v>269860</v>
       </c>
-      <c r="B37" s="54">
+      <c r="B37" s="52">
         <v>29.35</v>
       </c>
-      <c r="C37" s="54">
+      <c r="C37" s="52">
         <v>5.7389200000000002</v>
       </c>
-      <c r="D37" s="54">
+      <c r="D37" s="52">
         <v>5.35</v>
       </c>
-      <c r="E37" s="54">
+      <c r="E37" s="52">
         <v>16.600000000000001</v>
       </c>
-      <c r="F37" s="54">
+      <c r="F37" s="52">
         <v>18.329999999999998</v>
       </c>
-      <c r="G37" s="54">
+      <c r="G37" s="52">
         <v>13.54</v>
       </c>
-      <c r="H37" s="54">
+      <c r="H37" s="52">
         <v>11.19</v>
       </c>
-      <c r="I37" s="54">
+      <c r="I37" s="52">
         <v>2.95438</v>
       </c>
-      <c r="J37" s="54">
+      <c r="J37" s="52">
         <v>21.73</v>
       </c>
-      <c r="K37" s="54">
+      <c r="K37" s="52">
         <v>16.489999999999998</v>
       </c>
-      <c r="L37" s="54">
+      <c r="L37" s="52">
         <v>10.0678</v>
       </c>
-      <c r="M37" s="54">
+      <c r="M37" s="52">
         <v>13.8</v>
       </c>
-      <c r="N37" s="54">
+      <c r="N37" s="52">
         <v>9.66</v>
       </c>
-      <c r="O37" s="54">
+      <c r="O37" s="52">
         <v>7.01</v>
       </c>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A38" s="51">
+      <c r="A38" s="49">
         <v>314838</v>
       </c>
-      <c r="B38" s="54">
+      <c r="B38" s="52">
         <v>34.28</v>
       </c>
-      <c r="C38" s="54">
+      <c r="C38" s="52">
         <v>6.6515740000000001</v>
       </c>
-      <c r="D38" s="54">
+      <c r="D38" s="52">
         <v>6.24</v>
       </c>
-      <c r="E38" s="54">
+      <c r="E38" s="52">
         <v>19.37</v>
       </c>
-      <c r="F38" s="54">
+      <c r="F38" s="52">
         <v>21.4</v>
       </c>
-      <c r="G38" s="54">
+      <c r="G38" s="52">
         <v>15.8</v>
       </c>
-      <c r="H38" s="54">
+      <c r="H38" s="52">
         <v>13.07</v>
       </c>
-      <c r="I38" s="54">
+      <c r="I38" s="52">
         <v>3.4433799999999999</v>
       </c>
-      <c r="J38" s="54">
+      <c r="J38" s="52">
         <v>25.28</v>
       </c>
-      <c r="K38" s="54">
+      <c r="K38" s="52">
         <v>19.239999999999998</v>
       </c>
-      <c r="L38" s="54">
+      <c r="L38" s="52">
         <v>11.645099999999999</v>
       </c>
-      <c r="M38" s="54">
+      <c r="M38" s="52">
         <v>16.100000000000001</v>
       </c>
-      <c r="N38" s="54">
+      <c r="N38" s="52">
         <v>11.26</v>
       </c>
-      <c r="O38" s="54">
+      <c r="O38" s="52">
         <v>8.18</v>
       </c>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A39" s="51">
+      <c r="A39" s="49">
         <v>359814</v>
       </c>
-      <c r="B39" s="54">
+      <c r="B39" s="52">
         <v>39.26</v>
       </c>
-      <c r="C39" s="54">
+      <c r="C39" s="52">
         <v>7.5901430000000003</v>
       </c>
-      <c r="D39" s="54">
+      <c r="D39" s="52">
         <v>7.14</v>
       </c>
-      <c r="E39" s="54">
+      <c r="E39" s="52">
         <v>22.18</v>
       </c>
-      <c r="F39" s="54">
+      <c r="F39" s="52">
         <v>24.45</v>
       </c>
-      <c r="G39" s="54">
+      <c r="G39" s="52">
         <v>18.059999999999999</v>
       </c>
-      <c r="H39" s="54">
+      <c r="H39" s="52">
         <v>14.93</v>
       </c>
-      <c r="I39" s="54">
+      <c r="I39" s="52">
         <v>3.9345300000000001</v>
       </c>
-      <c r="J39" s="54">
+      <c r="J39" s="52">
         <v>28.97</v>
       </c>
-      <c r="K39" s="54">
+      <c r="K39" s="52">
         <v>21.99</v>
       </c>
-      <c r="L39" s="54">
+      <c r="L39" s="52">
         <v>13.3462</v>
       </c>
-      <c r="M39" s="54">
+      <c r="M39" s="52">
         <v>18.41</v>
       </c>
-      <c r="N39" s="54">
+      <c r="N39" s="52">
         <v>12.88</v>
       </c>
-      <c r="O39" s="54">
+      <c r="O39" s="52">
         <v>9.36</v>
       </c>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A40" s="51">
+      <c r="A40" s="49">
         <v>404787</v>
       </c>
-      <c r="B40" s="54">
+      <c r="B40" s="52">
         <v>44.16</v>
       </c>
-      <c r="C40" s="54">
+      <c r="C40" s="52">
         <v>8.4808819999999994</v>
       </c>
-      <c r="D40" s="54">
+      <c r="D40" s="52">
         <v>8.0299999999999994</v>
       </c>
-      <c r="E40" s="54">
+      <c r="E40" s="52">
         <v>24.95</v>
       </c>
-      <c r="F40" s="54">
+      <c r="F40" s="52">
         <v>27.5</v>
       </c>
-      <c r="G40" s="54">
+      <c r="G40" s="52">
         <v>20.309999999999999</v>
       </c>
-      <c r="H40" s="54">
+      <c r="H40" s="52">
         <v>16.77</v>
       </c>
-      <c r="I40" s="54">
+      <c r="I40" s="52">
         <v>4.4217500000000003</v>
       </c>
-      <c r="J40" s="54">
+      <c r="J40" s="52">
         <v>32.590000000000003</v>
       </c>
-      <c r="K40" s="54">
+      <c r="K40" s="52">
         <v>24.74</v>
       </c>
-      <c r="L40" s="54">
+      <c r="L40" s="52">
         <v>14.882400000000001</v>
       </c>
-      <c r="M40" s="54">
+      <c r="M40" s="52">
         <v>20.71</v>
       </c>
-      <c r="N40" s="54">
+      <c r="N40" s="52">
         <v>14.49</v>
       </c>
-      <c r="O40" s="54">
+      <c r="O40" s="52">
         <v>10.52</v>
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A41" s="51">
+      <c r="A41" s="49">
         <v>449757</v>
       </c>
-      <c r="B41" s="54">
+      <c r="B41" s="52">
         <v>49.07</v>
       </c>
-      <c r="C41" s="54">
+      <c r="C41" s="52">
         <v>9.3969310000000004</v>
       </c>
-      <c r="D41" s="54">
+      <c r="D41" s="52">
         <v>8.92</v>
       </c>
-      <c r="E41" s="54">
+      <c r="E41" s="52">
         <v>27.72</v>
       </c>
-      <c r="F41" s="54">
+      <c r="F41" s="52">
         <v>30.54</v>
       </c>
-      <c r="G41" s="54">
+      <c r="G41" s="52">
         <v>22.56</v>
       </c>
-      <c r="H41" s="54">
+      <c r="H41" s="52">
         <v>18.64</v>
       </c>
-      <c r="I41" s="54">
+      <c r="I41" s="52">
         <v>4.9102100000000002</v>
       </c>
-      <c r="J41" s="54">
+      <c r="J41" s="52">
         <v>36.159999999999997</v>
       </c>
-      <c r="K41" s="54">
+      <c r="K41" s="52">
         <v>27.48</v>
       </c>
-      <c r="L41" s="54">
+      <c r="L41" s="52">
         <v>16.627600000000001</v>
       </c>
-      <c r="M41" s="54">
+      <c r="M41" s="52">
         <v>23</v>
       </c>
-      <c r="N41" s="54">
+      <c r="N41" s="52">
         <v>16.09</v>
       </c>
-      <c r="O41" s="54">
+      <c r="O41" s="52">
         <v>11.69</v>
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="B44">
         <v>1</v>

</xml_diff>